<commit_message>
Iniziato CM 0.09, riorganizzazione struttura cartelle
</commit_message>
<xml_diff>
--- a/Documentazione/Attività sul progetto/DocAttivProg.xlsx
+++ b/Documentazione/Attività sul progetto/DocAttivProg.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\UniUD\Laurea Magistrale\Ingegneria del Software 2\Progetto-Ingegneria-Del-Sw-2\Documentazione\Attività sul progetto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8730122-F086-4D2B-B615-1AF2481A7B2F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06B13CFE-2F32-40B6-A574-BE1DAB8F5C20}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8988" xr2:uid="{CEC92F1B-94C4-4157-8A2A-4E219C7CE5A5}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="8">
   <si>
     <t>PERSONA</t>
   </si>
@@ -104,6 +104,9 @@
   </si>
   <si>
     <t>DATA</t>
+  </si>
+  <si>
+    <t>Interno</t>
   </si>
 </sst>
 </file>
@@ -473,10 +476,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AD9522E-E308-412F-92AE-20147EFE7ABE}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -537,6 +540,34 @@
         <v>43493</v>
       </c>
     </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6">
+        <v>135</v>
+      </c>
+      <c r="D6" s="2">
+        <v>43494</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7">
+        <v>53</v>
+      </c>
+      <c r="D7" s="2">
+        <v>43494</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Modifica proposta di progetto, creazione PDF mancanti
</commit_message>
<xml_diff>
--- a/Documentazione/Attività sul progetto/DocAttivProg.xlsx
+++ b/Documentazione/Attività sul progetto/DocAttivProg.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\UniUD\Laurea Magistrale\Ingegneria del Software 2\Progetto-Ingegneria-Del-Sw-2\Documentazione\Attività sul progetto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10605EA5-0387-407A-A56C-251CD223D2B7}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67943B0F-959F-4ECE-8927-5882BBA41E56}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8988" xr2:uid="{CEC92F1B-94C4-4157-8A2A-4E219C7CE5A5}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="8">
   <si>
     <t>PERSONA</t>
   </si>
@@ -476,10 +476,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AD9522E-E308-412F-92AE-20147EFE7ABE}">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -582,6 +582,20 @@
         <v>43495</v>
       </c>
     </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9">
+        <v>74</v>
+      </c>
+      <c r="D9" s="2">
+        <v>43495</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Piccole modifiche al sommario
</commit_message>
<xml_diff>
--- a/Documentazione/Attività sul progetto/DocAttivProg.xlsx
+++ b/Documentazione/Attività sul progetto/DocAttivProg.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\UniUD\Laurea Magistrale\Ingegneria del Software 2\Progetto-Ingegneria-Del-Sw-2\Documentazione\Attività sul progetto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67943B0F-959F-4ECE-8927-5882BBA41E56}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9FAB876-6EC9-4ADD-9990-7C6AB4C777A3}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8988" xr2:uid="{CEC92F1B-94C4-4157-8A2A-4E219C7CE5A5}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="8">
   <si>
     <t>PERSONA</t>
   </si>
@@ -476,10 +476,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AD9522E-E308-412F-92AE-20147EFE7ABE}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -596,6 +596,20 @@
         <v>43495</v>
       </c>
     </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10">
+        <v>32</v>
+      </c>
+      <c r="D10" s="2">
+        <v>43499</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Nuova versione glossario, CM v 0.10
</commit_message>
<xml_diff>
--- a/Documentazione/Attività sul progetto/DocAttivProg.xlsx
+++ b/Documentazione/Attività sul progetto/DocAttivProg.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\UniUD\Laurea Magistrale\Ingegneria del Software 2\Progetto-Ingegneria-Del-Sw-2\Documentazione\Attività sul progetto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9FAB876-6EC9-4ADD-9990-7C6AB4C777A3}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8EF97FF-2506-4D9C-9021-6FA7787E698D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8988" xr2:uid="{CEC92F1B-94C4-4157-8A2A-4E219C7CE5A5}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{CEC92F1B-94C4-4157-8A2A-4E219C7CE5A5}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="8">
   <si>
     <t>PERSONA</t>
   </si>
@@ -476,10 +476,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AD9522E-E308-412F-92AE-20147EFE7ABE}">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -610,6 +610,20 @@
         <v>43499</v>
       </c>
     </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11">
+        <v>127</v>
+      </c>
+      <c r="D11" s="2">
+        <v>43505</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Aggiunte test chain e risultati test
</commit_message>
<xml_diff>
--- a/Documentazione/Attività sul progetto/DocAttivProg.xlsx
+++ b/Documentazione/Attività sul progetto/DocAttivProg.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\UniUD\Laurea Magistrale\Ingegneria del Software 2\Progetto-Ingegneria-Del-Sw-2\Documentazione\Attività sul progetto\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LUCA\Documents\Università\INGEGNERIA DEL SOFTWARE\Progetto\Documentazione\Attività sul progetto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A428A9E-6931-4A33-818A-1ECCE13BF0DB}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{CEC92F1B-94C4-4157-8A2A-4E219C7CE5A5}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="9">
   <si>
     <t>PERSONA</t>
   </si>
@@ -108,11 +107,14 @@
   <si>
     <t>Interno</t>
   </si>
+  <si>
+    <t>Luca</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -475,30 +477,30 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AD9522E-E308-412F-92AE-20147EFE7ABE}">
-  <dimension ref="A1:D12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="15.5546875" customWidth="1"/>
-    <col min="4" max="4" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="3" width="15.5703125" customWidth="1"/>
+    <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -512,7 +514,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -526,7 +528,7 @@
         <v>43484</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -540,7 +542,7 @@
         <v>43493</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -554,7 +556,7 @@
         <v>43494</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -568,7 +570,7 @@
         <v>43494</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -582,7 +584,7 @@
         <v>43495</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -596,7 +598,7 @@
         <v>43495</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>4</v>
       </c>
@@ -610,7 +612,7 @@
         <v>43499</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>4</v>
       </c>
@@ -624,7 +626,7 @@
         <v>43505</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>4</v>
       </c>
@@ -636,6 +638,20 @@
       </c>
       <c r="D12" s="2">
         <v>43509</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13">
+        <v>195</v>
+      </c>
+      <c r="D13" s="2">
+        <v>43521</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update DocReq, modifica minore su DocProg
</commit_message>
<xml_diff>
--- a/Documentazione/Attività sul progetto/DocAttivProg.xlsx
+++ b/Documentazione/Attività sul progetto/DocAttivProg.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vik\Documents\GitHub\Progetto\Documentazione\Attività sul progetto\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LUCA\Documents\Università\INGEGNERIA DEL SOFTWARE\Progetto\Documentazione\Attività sul progetto\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="11">
   <si>
     <r>
       <rPr>
@@ -114,7 +114,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mm/dd/yy"/>
   </numFmts>
@@ -448,10 +448,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D25"/>
+  <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -793,6 +793,20 @@
         <v>43530</v>
       </c>
     </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>8</v>
+      </c>
+      <c r="B26" t="s">
+        <v>6</v>
+      </c>
+      <c r="C26">
+        <v>15</v>
+      </c>
+      <c r="D26" s="2">
+        <v>43532</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
Caricamento screenshot (file .zip)
</commit_message>
<xml_diff>
--- a/Documentazione/Attività sul progetto/DocAttivProg.xlsx
+++ b/Documentazione/Attività sul progetto/DocAttivProg.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\UniUD\Laurea Magistrale\Ingegneria del Software 2\Progetto-Ingegneria-Del-Sw-2\Documentazione\Attività sul progetto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{656670EA-89EC-4B54-A398-DAF6572AADCB}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD0E2A77-8D19-4246-9A58-433025423DA4}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -452,7 +452,7 @@
   <dimension ref="A1:D27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -816,7 +816,7 @@
         <v>6</v>
       </c>
       <c r="C27">
-        <v>33</v>
+        <v>47</v>
       </c>
       <c r="D27" s="2">
         <v>43532</v>

</xml_diff>

<commit_message>
Attività per calcolo COCOMO
</commit_message>
<xml_diff>
--- a/Documentazione/Attività sul progetto/DocAttivProg.xlsx
+++ b/Documentazione/Attività sul progetto/DocAttivProg.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LUCA\Documents\Università\INGEGNERIA DEL SOFTWARE\Progetto\Documentazione\Attività sul progetto\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LUCA\Documents\Universita\INGEGNERIA DEL SOFTWARE\Progetto\Documentazione\Attività sul progetto\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="32">
   <si>
     <t>PERSONA</t>
   </si>
@@ -123,6 +123,9 @@
   </si>
   <si>
     <t>12/16/2018</t>
+  </si>
+  <si>
+    <t>04/16/2019</t>
   </si>
 </sst>
 </file>
@@ -542,10 +545,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M50"/>
+  <dimension ref="A1:M52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C50" sqref="C50"/>
+    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H50" sqref="H50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -945,7 +948,7 @@
       </c>
       <c r="J19" s="9">
         <f>SUMIFS(C4:C61,B4:B61,"Documentazione interna",A4:A61,"Luca")</f>
-        <v>562</v>
+        <v>632</v>
       </c>
       <c r="K19" s="9">
         <f>SUMIFS(C4:C37,B4:B37,"Manuale",A4:A37,"Luca")</f>
@@ -1415,6 +1418,34 @@
       </c>
       <c r="D50" s="4">
         <v>43528</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>7</v>
+      </c>
+      <c r="B51" t="s">
+        <v>12</v>
+      </c>
+      <c r="C51">
+        <v>70</v>
+      </c>
+      <c r="D51" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>8</v>
+      </c>
+      <c r="B52" t="s">
+        <v>12</v>
+      </c>
+      <c r="C52">
+        <v>70</v>
+      </c>
+      <c r="D52" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Aggiunti documenti calcoli FP e COCOMO
Documenti non formalizzati nel CM
</commit_message>
<xml_diff>
--- a/Documentazione/Attività sul progetto/DocAttivProg.xlsx
+++ b/Documentazione/Attività sul progetto/DocAttivProg.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="33">
   <si>
     <t>PERSONA</t>
   </si>
@@ -126,6 +126,9 @@
   </si>
   <si>
     <t>04/16/2019</t>
+  </si>
+  <si>
+    <t>04/17/2019</t>
   </si>
 </sst>
 </file>
@@ -545,10 +548,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M52"/>
+  <dimension ref="A1:M53"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A33" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H50" sqref="H50"/>
+      <selection activeCell="D54" sqref="D54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -948,7 +951,7 @@
       </c>
       <c r="J19" s="9">
         <f>SUMIFS(C4:C61,B4:B61,"Documentazione interna",A4:A61,"Luca")</f>
-        <v>632</v>
+        <v>752</v>
       </c>
       <c r="K19" s="9">
         <f>SUMIFS(C4:C37,B4:B37,"Manuale",A4:A37,"Luca")</f>
@@ -1446,6 +1449,20 @@
       </c>
       <c r="D52" t="s">
         <v>31</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>7</v>
+      </c>
+      <c r="B53" t="s">
+        <v>12</v>
+      </c>
+      <c r="C53">
+        <v>120</v>
+      </c>
+      <c r="D53" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix date da mm/dd/yyyy a dd/mm/yyyy
</commit_message>
<xml_diff>
--- a/Documentazione/Attività sul progetto/DocAttivProg.xlsx
+++ b/Documentazione/Attività sul progetto/DocAttivProg.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="25">
   <si>
     <t>PERSONA</t>
   </si>
@@ -105,40 +105,12 @@
   </si>
   <si>
     <t>Attività per persona (minuti)</t>
-  </si>
-  <si>
-    <t>03/29/2019</t>
-  </si>
-  <si>
-    <t>01/16/2019</t>
-  </si>
-  <si>
-    <t>12/14/2018</t>
-  </si>
-  <si>
-    <t>01/13/2019</t>
-  </si>
-  <si>
-    <t>12/15/2018</t>
-  </si>
-  <si>
-    <t>12/16/2018</t>
-  </si>
-  <si>
-    <t>04/16/2019</t>
-  </si>
-  <si>
-    <t>04/17/2019</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="m/d/yyyy"/>
-    <numFmt numFmtId="165" formatCode="mm/dd/yy"/>
-  </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -203,11 +175,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -548,10 +518,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M53"/>
+  <dimension ref="A1:M112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D54" sqref="D54"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F53" sqref="F53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -593,7 +563,7 @@
       <c r="D3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="H3" s="6"/>
+      <c r="H3" s="4"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -608,10 +578,10 @@
       <c r="D4" s="2">
         <v>43484</v>
       </c>
-      <c r="H4" s="8" t="s">
+      <c r="H4" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="I4" s="5"/>
+      <c r="I4" s="3"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -626,10 +596,10 @@
       <c r="D5" s="2">
         <v>43493</v>
       </c>
-      <c r="H5" s="7" t="s">
+      <c r="H5" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="I5" s="14" t="s">
+      <c r="I5" s="12" t="s">
         <v>18</v>
       </c>
     </row>
@@ -646,10 +616,10 @@
       <c r="D6" s="2">
         <v>43494</v>
       </c>
-      <c r="H6" s="5" t="s">
+      <c r="H6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="I6" s="15">
+      <c r="I6" s="13">
         <f>SUMIF(B4:B37,"Analisi codice",C4:C37)</f>
         <v>0</v>
       </c>
@@ -667,10 +637,10 @@
       <c r="D7" s="2">
         <v>43494</v>
       </c>
-      <c r="H7" s="5" t="s">
+      <c r="H7" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="I7" s="15">
+      <c r="I7" s="13">
         <f>SUMIF(B4:B37,"Documentazione esterna",C4:C37)</f>
         <v>476</v>
       </c>
@@ -688,10 +658,10 @@
       <c r="D8" s="2">
         <v>43495</v>
       </c>
-      <c r="H8" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="I8" s="15">
+      <c r="H8" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I8" s="13">
         <f>SUMIF(B4:B37,"Documentazione interna",C4:C37)</f>
         <v>627</v>
       </c>
@@ -709,10 +679,10 @@
       <c r="D9" s="2">
         <v>43495</v>
       </c>
-      <c r="H9" s="5" t="s">
+      <c r="H9" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="I9" s="15">
+      <c r="I9" s="13">
         <f>SUMIF(B4:B37,"Manuale",C4:C37)</f>
         <v>174</v>
       </c>
@@ -730,10 +700,10 @@
       <c r="D10" s="2">
         <v>43499</v>
       </c>
-      <c r="H10" s="5" t="s">
+      <c r="H10" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="I10" s="15">
+      <c r="I10" s="13">
         <f>SUMIF(B4:B37,"Sviluppo",C4:C37)</f>
         <v>0</v>
       </c>
@@ -751,10 +721,10 @@
       <c r="D11" s="2">
         <v>43505</v>
       </c>
-      <c r="H11" s="5" t="s">
+      <c r="H11" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="I11" s="15">
+      <c r="I11" s="13">
         <f>SUMIF(B4:B37,"Testing",C4:C37)</f>
         <v>0</v>
       </c>
@@ -811,17 +781,17 @@
       <c r="C15">
         <v>30</v>
       </c>
-      <c r="D15" s="3">
+      <c r="D15" s="2">
         <v>43519</v>
       </c>
-      <c r="H15" s="11" t="s">
+      <c r="H15" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="I15" s="9"/>
-      <c r="J15" s="9"/>
-      <c r="K15" s="9"/>
-      <c r="L15" s="9"/>
-      <c r="M15" s="9"/>
+      <c r="I15" s="7"/>
+      <c r="J15" s="7"/>
+      <c r="K15" s="7"/>
+      <c r="L15" s="7"/>
+      <c r="M15" s="7"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
@@ -833,25 +803,25 @@
       <c r="C16">
         <v>100</v>
       </c>
-      <c r="D16" s="3">
+      <c r="D16" s="2">
         <v>43520</v>
       </c>
-      <c r="H16" s="12" t="s">
+      <c r="H16" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="I16" s="10" t="s">
+      <c r="I16" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="J16" s="10" t="s">
+      <c r="J16" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="K16" s="10" t="s">
+      <c r="K16" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="L16" s="10" t="s">
+      <c r="L16" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="M16" s="10" t="s">
+      <c r="M16" s="8" t="s">
         <v>16</v>
       </c>
     </row>
@@ -865,29 +835,29 @@
       <c r="C17">
         <v>125</v>
       </c>
-      <c r="D17" s="3">
+      <c r="D17" s="2">
         <v>43522</v>
       </c>
-      <c r="H17" s="13" t="s">
+      <c r="H17" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="I17" s="9">
+      <c r="I17" s="7">
         <f>SUMIFS(C4:C37,B4:B37,"Documentazione esterna",A4:A37,"Giovanni")</f>
         <v>461</v>
       </c>
-      <c r="J17" s="9">
+      <c r="J17" s="7">
         <f>SUMIFS(C4:C37,B4:B37,"Documentazione interna",A4:A37,"Giovanni")</f>
         <v>317</v>
       </c>
-      <c r="K17" s="9">
+      <c r="K17" s="7">
         <f>SUMIFS(C4:C37,B4:B37,"Manuale",A4:A37,"Giovanni")</f>
         <v>174</v>
       </c>
-      <c r="L17" s="9">
+      <c r="L17" s="7">
         <f>SUMIFS(C4:C37,B4:B37,"Sviluppo",A4:A37,"Giovanni")</f>
         <v>0</v>
       </c>
-      <c r="M17" s="9">
+      <c r="M17" s="7">
         <f>SUMIFS(C4:C37,B4:B37,"Testing",A4:A37,"Giovanni")</f>
         <v>0</v>
       </c>
@@ -902,29 +872,29 @@
       <c r="C18">
         <v>170</v>
       </c>
-      <c r="D18" s="3">
+      <c r="D18" s="2">
         <v>43523</v>
       </c>
-      <c r="H18" s="13" t="s">
+      <c r="H18" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="I18" s="9">
+      <c r="I18" s="7">
         <f>SUMIFS(C4:C37,B4:B37,"Documentazione esterna",A4:A37,"Hristina")</f>
         <v>0</v>
       </c>
-      <c r="J18" s="9">
+      <c r="J18" s="7">
         <f>SUMIFS(C4:C37,B4:B37,"Documentazione interna",A4:A37,"Hristina")</f>
         <v>10</v>
       </c>
-      <c r="K18" s="9">
+      <c r="K18" s="7">
         <f>SUMIFS(C4:C37,B4:B37,"Manuale",A4:A37,"Hristina")</f>
         <v>0</v>
       </c>
-      <c r="L18" s="9">
+      <c r="L18" s="7">
         <f>SUMIFS(C4:C37,B4:B37,"Sviluppo",A4:A37,"Hristina")</f>
         <v>0</v>
       </c>
-      <c r="M18" s="9">
+      <c r="M18" s="7">
         <f>SUMIFS(C4:C37,B4:B37,"Testing",A4:A37,"Hristina")</f>
         <v>0</v>
       </c>
@@ -939,29 +909,29 @@
       <c r="C19">
         <v>65</v>
       </c>
-      <c r="D19" s="3">
+      <c r="D19" s="2">
         <v>43524</v>
       </c>
-      <c r="H19" s="13" t="s">
+      <c r="H19" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="I19" s="9">
+      <c r="I19" s="7">
         <f>SUMIFS(C4:C59,B4:B59,"Documentazione esterna",A4:A59,"Luca")</f>
         <v>585</v>
       </c>
-      <c r="J19" s="9">
+      <c r="J19" s="7">
         <f>SUMIFS(C4:C61,B4:B61,"Documentazione interna",A4:A61,"Luca")</f>
-        <v>752</v>
-      </c>
-      <c r="K19" s="9">
+        <v>852</v>
+      </c>
+      <c r="K19" s="7">
         <f>SUMIFS(C4:C37,B4:B37,"Manuale",A4:A37,"Luca")</f>
         <v>0</v>
       </c>
-      <c r="L19" s="9">
+      <c r="L19" s="7">
         <f>SUMIFS(C4:C37,B4:B37,"Sviluppo",A4:A37,"Luca")</f>
         <v>0</v>
       </c>
-      <c r="M19" s="9">
+      <c r="M19" s="7">
         <f>SUMIFS(C4:C37,B4:B37,"Testing",A4:A37,"Luca")</f>
         <v>0</v>
       </c>
@@ -979,26 +949,26 @@
       <c r="D20" s="2">
         <v>43487</v>
       </c>
-      <c r="H20" s="13" t="s">
+      <c r="H20" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="I20" s="9">
+      <c r="I20" s="7">
         <f>SUMIFS(C4:C37,B4:B37,"Documentazione esterna",A4:A37,"Viktorija")</f>
         <v>0</v>
       </c>
-      <c r="J20" s="9">
+      <c r="J20" s="7">
         <f>SUMIFS(C4:C37,B4:B37,"Documentazione interna",A4:A37,"Viktorija")</f>
         <v>0</v>
       </c>
-      <c r="K20" s="9">
+      <c r="K20" s="7">
         <f>SUMIFS(C4:C37,B4:B37,"Manuale",A4:A37,"Viktorija")</f>
         <v>0</v>
       </c>
-      <c r="L20" s="9">
+      <c r="L20" s="7">
         <f>SUMIFS(C4:C37,B4:B37,"Sviluppo",A4:A37,"Viktorija")</f>
         <v>0</v>
       </c>
-      <c r="M20" s="9">
+      <c r="M20" s="7">
         <f>SUMIFS(C4:C37,B4:B37,"Testing",A4:A37,"Viktorija")</f>
         <v>0</v>
       </c>
@@ -1111,7 +1081,7 @@
       <c r="C28">
         <v>15</v>
       </c>
-      <c r="D28" s="3">
+      <c r="D28" s="2">
         <v>43532</v>
       </c>
     </row>
@@ -1125,7 +1095,7 @@
       <c r="C29">
         <v>55</v>
       </c>
-      <c r="D29" s="3">
+      <c r="D29" s="2">
         <v>43531</v>
       </c>
     </row>
@@ -1139,7 +1109,7 @@
       <c r="C30">
         <v>68</v>
       </c>
-      <c r="D30" s="3">
+      <c r="D30" s="2">
         <v>43532</v>
       </c>
     </row>
@@ -1153,7 +1123,7 @@
       <c r="C31">
         <v>129</v>
       </c>
-      <c r="D31" s="3">
+      <c r="D31" s="2">
         <v>43533</v>
       </c>
     </row>
@@ -1167,7 +1137,7 @@
       <c r="C32">
         <v>95</v>
       </c>
-      <c r="D32" s="3">
+      <c r="D32" s="2">
         <v>43534</v>
       </c>
     </row>
@@ -1181,7 +1151,7 @@
       <c r="C33">
         <v>74</v>
       </c>
-      <c r="D33" s="4">
+      <c r="D33" s="2">
         <v>43546</v>
       </c>
     </row>
@@ -1195,7 +1165,7 @@
       <c r="C34">
         <v>52</v>
       </c>
-      <c r="D34" s="4">
+      <c r="D34" s="2">
         <v>43546</v>
       </c>
     </row>
@@ -1209,7 +1179,7 @@
       <c r="C35">
         <v>196</v>
       </c>
-      <c r="D35" s="4">
+      <c r="D35" s="2">
         <v>43376</v>
       </c>
     </row>
@@ -1223,7 +1193,7 @@
       <c r="C36">
         <v>115</v>
       </c>
-      <c r="D36" s="4">
+      <c r="D36" s="2">
         <v>43407</v>
       </c>
     </row>
@@ -1237,7 +1207,7 @@
       <c r="C37">
         <v>10</v>
       </c>
-      <c r="D37" s="4">
+      <c r="D37" s="2">
         <v>43546</v>
       </c>
     </row>
@@ -1251,8 +1221,8 @@
       <c r="C38">
         <v>60</v>
       </c>
-      <c r="D38" s="4" t="s">
-        <v>25</v>
+      <c r="D38" s="2">
+        <v>43553</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -1265,8 +1235,8 @@
       <c r="C39">
         <v>60</v>
       </c>
-      <c r="D39" s="4" t="s">
-        <v>25</v>
+      <c r="D39" s="2">
+        <v>43553</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -1279,8 +1249,8 @@
       <c r="C40">
         <v>60</v>
       </c>
-      <c r="D40" s="4" t="s">
-        <v>25</v>
+      <c r="D40" s="2">
+        <v>43553</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -1293,8 +1263,8 @@
       <c r="C41">
         <v>60</v>
       </c>
-      <c r="D41" t="s">
-        <v>26</v>
+      <c r="D41" s="2">
+        <v>43481</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -1307,8 +1277,8 @@
       <c r="C42">
         <v>150</v>
       </c>
-      <c r="D42" s="4">
-        <v>43324</v>
+      <c r="D42" s="2">
+        <v>43442</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -1321,8 +1291,8 @@
       <c r="C43">
         <v>180</v>
       </c>
-      <c r="D43" s="4" t="s">
-        <v>27</v>
+      <c r="D43" s="2">
+        <v>43448</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -1335,8 +1305,8 @@
       <c r="C44">
         <v>180</v>
       </c>
-      <c r="D44" s="4">
-        <v>43525</v>
+      <c r="D44" s="2">
+        <v>43468</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -1349,8 +1319,8 @@
       <c r="C45">
         <v>120</v>
       </c>
-      <c r="D45" s="4" t="s">
-        <v>28</v>
+      <c r="D45" s="2">
+        <v>43478</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -1363,8 +1333,8 @@
       <c r="C46">
         <v>300</v>
       </c>
-      <c r="D46" s="4" t="s">
-        <v>29</v>
+      <c r="D46" s="2">
+        <v>43449</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
@@ -1377,8 +1347,8 @@
       <c r="C47">
         <v>150</v>
       </c>
-      <c r="D47" s="4" t="s">
-        <v>30</v>
+      <c r="D47" s="2">
+        <v>43450</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
@@ -1391,8 +1361,8 @@
       <c r="C48">
         <v>82</v>
       </c>
-      <c r="D48" s="4">
-        <v>43528</v>
+      <c r="D48" s="2">
+        <v>43558</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -1405,8 +1375,8 @@
       <c r="C49">
         <v>82</v>
       </c>
-      <c r="D49" s="4">
-        <v>43528</v>
+      <c r="D49" s="2">
+        <v>43558</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
@@ -1419,8 +1389,8 @@
       <c r="C50">
         <v>82</v>
       </c>
-      <c r="D50" s="4">
-        <v>43528</v>
+      <c r="D50" s="2">
+        <v>43558</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -1433,8 +1403,8 @@
       <c r="C51">
         <v>70</v>
       </c>
-      <c r="D51" t="s">
-        <v>31</v>
+      <c r="D51" s="2">
+        <v>43571</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
@@ -1447,8 +1417,8 @@
       <c r="C52">
         <v>70</v>
       </c>
-      <c r="D52" t="s">
-        <v>31</v>
+      <c r="D52" s="2">
+        <v>43571</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
@@ -1461,9 +1431,197 @@
       <c r="C53">
         <v>120</v>
       </c>
-      <c r="D53" t="s">
-        <v>32</v>
-      </c>
+      <c r="D53" s="2">
+        <v>43572</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>7</v>
+      </c>
+      <c r="B54" t="s">
+        <v>12</v>
+      </c>
+      <c r="C54">
+        <v>100</v>
+      </c>
+      <c r="D54" s="2">
+        <v>43574</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D55" s="2"/>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D56" s="2"/>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D57" s="2"/>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D58" s="2"/>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D59" s="2"/>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D60" s="2"/>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D61" s="2"/>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D62" s="2"/>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D63" s="2"/>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D64" s="2"/>
+    </row>
+    <row r="65" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D65" s="2"/>
+    </row>
+    <row r="66" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D66" s="2"/>
+    </row>
+    <row r="67" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D67" s="2"/>
+    </row>
+    <row r="68" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D68" s="2"/>
+    </row>
+    <row r="69" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D69" s="2"/>
+    </row>
+    <row r="70" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D70" s="2"/>
+    </row>
+    <row r="71" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D71" s="2"/>
+    </row>
+    <row r="72" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D72" s="2"/>
+    </row>
+    <row r="73" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D73" s="2"/>
+    </row>
+    <row r="74" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D74" s="2"/>
+    </row>
+    <row r="75" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D75" s="2"/>
+    </row>
+    <row r="76" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D76" s="2"/>
+    </row>
+    <row r="77" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D77" s="2"/>
+    </row>
+    <row r="78" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D78" s="2"/>
+    </row>
+    <row r="79" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D79" s="2"/>
+    </row>
+    <row r="80" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D80" s="2"/>
+    </row>
+    <row r="81" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D81" s="2"/>
+    </row>
+    <row r="82" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D82" s="2"/>
+    </row>
+    <row r="83" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D83" s="2"/>
+    </row>
+    <row r="84" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D84" s="2"/>
+    </row>
+    <row r="85" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D85" s="2"/>
+    </row>
+    <row r="86" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D86" s="2"/>
+    </row>
+    <row r="87" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D87" s="2"/>
+    </row>
+    <row r="88" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D88" s="2"/>
+    </row>
+    <row r="89" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D89" s="2"/>
+    </row>
+    <row r="90" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D90" s="2"/>
+    </row>
+    <row r="91" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D91" s="2"/>
+    </row>
+    <row r="92" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D92" s="2"/>
+    </row>
+    <row r="93" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D93" s="2"/>
+    </row>
+    <row r="94" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D94" s="2"/>
+    </row>
+    <row r="95" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D95" s="2"/>
+    </row>
+    <row r="96" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D96" s="2"/>
+    </row>
+    <row r="97" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D97" s="2"/>
+    </row>
+    <row r="98" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D98" s="2"/>
+    </row>
+    <row r="99" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D99" s="2"/>
+    </row>
+    <row r="100" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D100" s="2"/>
+    </row>
+    <row r="101" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D101" s="2"/>
+    </row>
+    <row r="102" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D102" s="2"/>
+    </row>
+    <row r="103" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D103" s="2"/>
+    </row>
+    <row r="104" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D104" s="2"/>
+    </row>
+    <row r="105" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D105" s="2"/>
+    </row>
+    <row r="106" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D106" s="2"/>
+    </row>
+    <row r="107" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D107" s="2"/>
+    </row>
+    <row r="108" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D108" s="2"/>
+    </row>
+    <row r="109" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D109" s="2"/>
+    </row>
+    <row r="110" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D110" s="2"/>
+    </row>
+    <row r="111" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D111" s="2"/>
+    </row>
+    <row r="112" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D112" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>

<commit_message>
CMv0.14, aggiunta cartella dei Costi e della Maturità
</commit_message>
<xml_diff>
--- a/Documentazione/Attività sul progetto/DocAttivProg.xlsx
+++ b/Documentazione/Attività sul progetto/DocAttivProg.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LUCA\Documents\Universita\INGEGNERIA DEL SOFTWARE\Progetto\Documentazione\Attività sul progetto\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\UniUD\Laurea Magistrale\Ingegneria del Software 2\Progetto-Ingegneria-Del-Sw-2\Documentazione\Attività sul progetto\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8004B22A-FEDE-4B73-A172-A71E93A5AD94}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" tabRatio="500"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="26">
   <si>
     <t>PERSONA</t>
   </si>
@@ -105,12 +106,15 @@
   </si>
   <si>
     <t>Attività per persona (minuti)</t>
+  </si>
+  <si>
+    <t>Documentazione GDPR</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -517,27 +521,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F53" sqref="F53"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.5703125" customWidth="1"/>
-    <col min="2" max="2" width="23.42578125" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" customWidth="1"/>
-    <col min="4" max="4" width="10.85546875" customWidth="1"/>
-    <col min="5" max="7" width="8.7109375" customWidth="1"/>
-    <col min="8" max="8" width="23.5703125" customWidth="1"/>
-    <col min="9" max="11" width="17.28515625" customWidth="1"/>
-    <col min="12" max="13" width="17.42578125" customWidth="1"/>
-    <col min="14" max="1025" width="8.7109375" customWidth="1"/>
+    <col min="1" max="1" width="15.5546875" customWidth="1"/>
+    <col min="2" max="2" width="23.44140625" customWidth="1"/>
+    <col min="3" max="3" width="15.5546875" customWidth="1"/>
+    <col min="4" max="4" width="10.88671875" customWidth="1"/>
+    <col min="5" max="7" width="8.6640625" customWidth="1"/>
+    <col min="8" max="8" width="23.5546875" customWidth="1"/>
+    <col min="9" max="11" width="17.33203125" customWidth="1"/>
+    <col min="12" max="13" width="17.44140625" customWidth="1"/>
+    <col min="14" max="1025" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -545,12 +549,12 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -565,7 +569,7 @@
       </c>
       <c r="H3" s="4"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -583,7 +587,7 @@
       </c>
       <c r="I4" s="3"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -603,7 +607,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -620,11 +624,11 @@
         <v>14</v>
       </c>
       <c r="I6" s="13">
-        <f>SUMIF(B4:B37,"Analisi codice",C4:C37)</f>
+        <f>SUMIF(B4:B56,"Analisi codice",C4:C56)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -641,11 +645,11 @@
         <v>11</v>
       </c>
       <c r="I7" s="13">
-        <f>SUMIF(B4:B37,"Documentazione esterna",C4:C37)</f>
-        <v>476</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+        <f>SUMIF(B4:B56,"Documentazione esterna",C4:C56)</f>
+        <v>1196</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -662,11 +666,11 @@
         <v>12</v>
       </c>
       <c r="I8" s="13">
-        <f>SUMIF(B4:B37,"Documentazione interna",C4:C37)</f>
-        <v>627</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+        <f>SUMIF(B4:B56,"Documentazione interna",C4:C56)</f>
+        <v>1930</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -683,11 +687,11 @@
         <v>10</v>
       </c>
       <c r="I9" s="13">
-        <f>SUMIF(B4:B37,"Manuale",C4:C37)</f>
+        <f>SUMIF(B4:B56,"Manuale",C4:C56)</f>
         <v>174</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>4</v>
       </c>
@@ -704,11 +708,11 @@
         <v>15</v>
       </c>
       <c r="I10" s="13">
-        <f>SUMIF(B4:B37,"Sviluppo",C4:C37)</f>
+        <f>SUMIF(B4:B56,"Sviluppo",C4:C56)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>4</v>
       </c>
@@ -725,11 +729,11 @@
         <v>16</v>
       </c>
       <c r="I11" s="13">
-        <f>SUMIF(B4:B37,"Testing",C4:C37)</f>
+        <f>SUMIF(B4:B56,"Testing",C4:C56)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>4</v>
       </c>
@@ -743,7 +747,7 @@
         <v>43509</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>7</v>
       </c>
@@ -757,7 +761,7 @@
         <v>43521</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>7</v>
       </c>
@@ -771,7 +775,7 @@
         <v>43523</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>8</v>
       </c>
@@ -793,7 +797,7 @@
       <c r="L15" s="7"/>
       <c r="M15" s="7"/>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>8</v>
       </c>
@@ -825,7 +829,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>8</v>
       </c>
@@ -842,27 +846,27 @@
         <v>4</v>
       </c>
       <c r="I17" s="7">
-        <f>SUMIFS(C4:C37,B4:B37,"Documentazione esterna",A4:A37,"Giovanni")</f>
-        <v>461</v>
+        <f>SUMIFS(C4:C56,B4:B56,"Documentazione esterna",A4:A56,"Giovanni")</f>
+        <v>611</v>
       </c>
       <c r="J17" s="7">
-        <f>SUMIFS(C4:C37,B4:B37,"Documentazione interna",A4:A37,"Giovanni")</f>
-        <v>317</v>
+        <f>SUMIFS(C4:C56,B4:B56,"Documentazione interna",A4:A56,"Giovanni")</f>
+        <v>796</v>
       </c>
       <c r="K17" s="7">
-        <f>SUMIFS(C4:C37,B4:B37,"Manuale",A4:A37,"Giovanni")</f>
+        <f>SUMIFS(C4:C56,B4:B56,"Manuale",A4:A56,"Giovanni")</f>
         <v>174</v>
       </c>
       <c r="L17" s="7">
-        <f>SUMIFS(C4:C37,B4:B37,"Sviluppo",A4:A37,"Giovanni")</f>
+        <f>SUMIFS(C4:C56,B4:B56,"Sviluppo",A4:A56,"Giovanni")</f>
         <v>0</v>
       </c>
       <c r="M17" s="7">
-        <f>SUMIFS(C4:C37,B4:B37,"Testing",A4:A37,"Giovanni")</f>
+        <f>SUMIFS(C4:C56,B4:B56,"Testing",A4:A56,"Giovanni")</f>
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>8</v>
       </c>
@@ -879,15 +883,15 @@
         <v>8</v>
       </c>
       <c r="I18" s="7">
-        <f>SUMIFS(C4:C37,B4:B37,"Documentazione esterna",A4:A37,"Hristina")</f>
+        <f>SUMIFS(C4:C56,B4:B56,"Documentazione esterna",A4:A56,"Hristina")</f>
         <v>0</v>
       </c>
       <c r="J18" s="7">
-        <f>SUMIFS(C4:C37,B4:B37,"Documentazione interna",A4:A37,"Hristina")</f>
-        <v>10</v>
+        <f>SUMIFS(C4:C56,B4:B56,"Documentazione interna",A4:A56,"Hristina")</f>
+        <v>222</v>
       </c>
       <c r="K18" s="7">
-        <f>SUMIFS(C4:C37,B4:B37,"Manuale",A4:A37,"Hristina")</f>
+        <f>SUMIFS(C4:C56,B4:B56,"Manuale",A4:A56,"Hristina")</f>
         <v>0</v>
       </c>
       <c r="L18" s="7">
@@ -899,7 +903,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>8</v>
       </c>
@@ -916,15 +920,15 @@
         <v>7</v>
       </c>
       <c r="I19" s="7">
-        <f>SUMIFS(C4:C59,B4:B59,"Documentazione esterna",A4:A59,"Luca")</f>
+        <f>SUMIFS(C4:C56,B4:B56,"Documentazione esterna",A4:A56,"Luca")</f>
         <v>585</v>
       </c>
       <c r="J19" s="7">
-        <f>SUMIFS(C4:C61,B4:B61,"Documentazione interna",A4:A61,"Luca")</f>
+        <f>SUMIFS(C4:C56,B4:B56,"Documentazione interna",A4:A56,"Luca")</f>
         <v>852</v>
       </c>
       <c r="K19" s="7">
-        <f>SUMIFS(C4:C37,B4:B37,"Manuale",A4:A37,"Luca")</f>
+        <f>SUMIFS(C4:C56,B4:B56,"Manuale",A4:A56,"Luca")</f>
         <v>0</v>
       </c>
       <c r="L19" s="7">
@@ -936,7 +940,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>9</v>
       </c>
@@ -953,15 +957,15 @@
         <v>9</v>
       </c>
       <c r="I20" s="7">
-        <f>SUMIFS(C4:C37,B4:B37,"Documentazione esterna",A4:A37,"Viktorija")</f>
+        <f>SUMIFS(C4:C56,B4:B56,"Documentazione esterna",A4:A56,"Viktorija")</f>
         <v>0</v>
       </c>
       <c r="J20" s="7">
-        <f>SUMIFS(C4:C37,B4:B37,"Documentazione interna",A4:A37,"Viktorija")</f>
-        <v>0</v>
+        <f>SUMIFS(C4:C56,B4:B56,"Documentazione interna",A4:A56,"Viktorija")</f>
+        <v>60</v>
       </c>
       <c r="K20" s="7">
-        <f>SUMIFS(C4:C37,B4:B37,"Manuale",A4:A37,"Viktorija")</f>
+        <f>SUMIFS(C4:C56,B4:B56,"Manuale",A4:A56,"Viktorija")</f>
         <v>0</v>
       </c>
       <c r="L20" s="7">
@@ -973,7 +977,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>9</v>
       </c>
@@ -987,7 +991,7 @@
         <v>43506</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>9</v>
       </c>
@@ -1001,7 +1005,7 @@
         <v>43520</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>9</v>
       </c>
@@ -1015,7 +1019,7 @@
         <v>43523</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>9</v>
       </c>
@@ -1029,7 +1033,7 @@
         <v>43524</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>9</v>
       </c>
@@ -1043,7 +1047,7 @@
         <v>43530</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>7</v>
       </c>
@@ -1057,7 +1061,7 @@
         <v>43532</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>4</v>
       </c>
@@ -1071,7 +1075,7 @@
         <v>43532</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>8</v>
       </c>
@@ -1085,7 +1089,7 @@
         <v>43532</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>8</v>
       </c>
@@ -1099,7 +1103,7 @@
         <v>43531</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>8</v>
       </c>
@@ -1113,7 +1117,7 @@
         <v>43532</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>8</v>
       </c>
@@ -1127,7 +1131,7 @@
         <v>43533</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>8</v>
       </c>
@@ -1141,7 +1145,7 @@
         <v>43534</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>4</v>
       </c>
@@ -1155,7 +1159,7 @@
         <v>43546</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>4</v>
       </c>
@@ -1169,7 +1173,7 @@
         <v>43546</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>9</v>
       </c>
@@ -1183,7 +1187,7 @@
         <v>43376</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>9</v>
       </c>
@@ -1197,7 +1201,7 @@
         <v>43407</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>8</v>
       </c>
@@ -1211,7 +1215,7 @@
         <v>43546</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>7</v>
       </c>
@@ -1225,7 +1229,7 @@
         <v>43553</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>8</v>
       </c>
@@ -1239,7 +1243,7 @@
         <v>43553</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>9</v>
       </c>
@@ -1253,7 +1257,7 @@
         <v>43553</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>7</v>
       </c>
@@ -1267,7 +1271,7 @@
         <v>43481</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>7</v>
       </c>
@@ -1281,7 +1285,7 @@
         <v>43442</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>7</v>
       </c>
@@ -1295,7 +1299,7 @@
         <v>43448</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>7</v>
       </c>
@@ -1309,7 +1313,7 @@
         <v>43468</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>7</v>
       </c>
@@ -1323,7 +1327,7 @@
         <v>43478</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>4</v>
       </c>
@@ -1337,7 +1341,7 @@
         <v>43449</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>4</v>
       </c>
@@ -1351,7 +1355,7 @@
         <v>43450</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>7</v>
       </c>
@@ -1365,7 +1369,7 @@
         <v>43558</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>8</v>
       </c>
@@ -1379,7 +1383,7 @@
         <v>43558</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>4</v>
       </c>
@@ -1393,7 +1397,7 @@
         <v>43558</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>7</v>
       </c>
@@ -1407,7 +1411,7 @@
         <v>43571</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>8</v>
       </c>
@@ -1421,7 +1425,7 @@
         <v>43571</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>7</v>
       </c>
@@ -1435,7 +1439,7 @@
         <v>43572</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>7</v>
       </c>
@@ -1449,178 +1453,200 @@
         <v>43574</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D55" s="2"/>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D56" s="2"/>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>4</v>
+      </c>
+      <c r="B55" t="s">
+        <v>25</v>
+      </c>
+      <c r="C55">
+        <v>42</v>
+      </c>
+      <c r="D55" s="2">
+        <v>43577</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>4</v>
+      </c>
+      <c r="B56" t="s">
+        <v>12</v>
+      </c>
+      <c r="C56">
+        <v>97</v>
+      </c>
+      <c r="D56" s="2">
+        <v>43578</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D57" s="2"/>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D58" s="2"/>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D59" s="2"/>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D60" s="2"/>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D61" s="2"/>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D62" s="2"/>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D63" s="2"/>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D64" s="2"/>
     </row>
-    <row r="65" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D65" s="2"/>
     </row>
-    <row r="66" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D66" s="2"/>
     </row>
-    <row r="67" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D67" s="2"/>
     </row>
-    <row r="68" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D68" s="2"/>
     </row>
-    <row r="69" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D69" s="2"/>
     </row>
-    <row r="70" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D70" s="2"/>
     </row>
-    <row r="71" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D71" s="2"/>
     </row>
-    <row r="72" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="72" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D72" s="2"/>
     </row>
-    <row r="73" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D73" s="2"/>
     </row>
-    <row r="74" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="74" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D74" s="2"/>
     </row>
-    <row r="75" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="75" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D75" s="2"/>
     </row>
-    <row r="76" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="76" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D76" s="2"/>
     </row>
-    <row r="77" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="77" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D77" s="2"/>
     </row>
-    <row r="78" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="78" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D78" s="2"/>
     </row>
-    <row r="79" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="79" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D79" s="2"/>
     </row>
-    <row r="80" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="80" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D80" s="2"/>
     </row>
-    <row r="81" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="81" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D81" s="2"/>
     </row>
-    <row r="82" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="82" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D82" s="2"/>
     </row>
-    <row r="83" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="83" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D83" s="2"/>
     </row>
-    <row r="84" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="84" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D84" s="2"/>
     </row>
-    <row r="85" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="85" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D85" s="2"/>
     </row>
-    <row r="86" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="86" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D86" s="2"/>
     </row>
-    <row r="87" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="87" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D87" s="2"/>
     </row>
-    <row r="88" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="88" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D88" s="2"/>
     </row>
-    <row r="89" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="89" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D89" s="2"/>
     </row>
-    <row r="90" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="90" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D90" s="2"/>
     </row>
-    <row r="91" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="91" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D91" s="2"/>
     </row>
-    <row r="92" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="92" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D92" s="2"/>
     </row>
-    <row r="93" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="93" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D93" s="2"/>
     </row>
-    <row r="94" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="94" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D94" s="2"/>
     </row>
-    <row r="95" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="95" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D95" s="2"/>
     </row>
-    <row r="96" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="96" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D96" s="2"/>
     </row>
-    <row r="97" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="97" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D97" s="2"/>
     </row>
-    <row r="98" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="98" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D98" s="2"/>
     </row>
-    <row r="99" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="99" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D99" s="2"/>
     </row>
-    <row r="100" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="100" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D100" s="2"/>
     </row>
-    <row r="101" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="101" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D101" s="2"/>
     </row>
-    <row r="102" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="102" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D102" s="2"/>
     </row>
-    <row r="103" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="103" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D103" s="2"/>
     </row>
-    <row r="104" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="104" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D104" s="2"/>
     </row>
-    <row r="105" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="105" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D105" s="2"/>
     </row>
-    <row r="106" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="106" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D106" s="2"/>
     </row>
-    <row r="107" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="107" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D107" s="2"/>
     </row>
-    <row r="108" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="108" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D108" s="2"/>
     </row>
-    <row r="109" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="109" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D109" s="2"/>
     </row>
-    <row r="110" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="110" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D110" s="2"/>
     </row>
-    <row r="111" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="111" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D111" s="2"/>
     </row>
-    <row r="112" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="112" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D112" s="2"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modifica documento delle attività
Ho aggiunto 2 attività (Documentazione esterna) per i 2 verbali esterni che ho fatto all'inizio.
</commit_message>
<xml_diff>
--- a/Documentazione/Attività sul progetto/DocAttivProg.xlsx
+++ b/Documentazione/Attività sul progetto/DocAttivProg.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\UniUD\Laurea Magistrale\Ingegneria del Software 2\Progetto-Ingegneria-Del-Sw-2\Documentazione\Attività sul progetto\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vik\Documents\GitHub\Progetto\Documentazione\Attività sul progetto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B253E8BC-05F4-49D5-AAFF-850A8041A669}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" iterateDelta="1E-4"/>
+  <calcPr calcId="152511" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -31,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="24">
   <si>
     <t>PERSONA</t>
   </si>
@@ -108,7 +107,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yyyy"/>
   </numFmts>
@@ -519,27 +518,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M112"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M114"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M21" sqref="M21"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.5546875" customWidth="1"/>
-    <col min="2" max="2" width="23.44140625" customWidth="1"/>
-    <col min="3" max="3" width="15.5546875" customWidth="1"/>
-    <col min="4" max="4" width="10.88671875" customWidth="1"/>
-    <col min="5" max="7" width="8.6640625" customWidth="1"/>
-    <col min="8" max="8" width="23.5546875" customWidth="1"/>
-    <col min="9" max="11" width="17.33203125" customWidth="1"/>
-    <col min="12" max="13" width="17.44140625" customWidth="1"/>
-    <col min="14" max="1025" width="8.6640625" customWidth="1"/>
+    <col min="1" max="1" width="15.5703125" customWidth="1"/>
+    <col min="2" max="2" width="23.42578125" customWidth="1"/>
+    <col min="3" max="3" width="15.5703125" customWidth="1"/>
+    <col min="4" max="4" width="10.85546875" customWidth="1"/>
+    <col min="5" max="7" width="8.7109375" customWidth="1"/>
+    <col min="8" max="8" width="23.5703125" customWidth="1"/>
+    <col min="9" max="11" width="17.28515625" customWidth="1"/>
+    <col min="12" max="13" width="17.42578125" customWidth="1"/>
+    <col min="14" max="1025" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
@@ -547,12 +546,12 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -567,7 +566,7 @@
       </c>
       <c r="H3" s="4"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -585,7 +584,7 @@
       </c>
       <c r="I4" s="3"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -605,7 +604,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -622,11 +621,11 @@
         <v>13</v>
       </c>
       <c r="I6" s="13">
-        <f>SUMIF(B4:B57,"Analisi codice",C4:C57)</f>
+        <f>SUMIF(B4:B59,"Analisi codice",C4:C59)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -643,11 +642,11 @@
         <v>10</v>
       </c>
       <c r="I7" s="13">
-        <f>SUMIF(B4:B57,"Documentazione esterna",C4:C57)</f>
-        <v>1238</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+        <f>SUMIF(B4:B59,"Documentazione esterna",C4:C59)</f>
+        <v>1313</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -664,11 +663,11 @@
         <v>11</v>
       </c>
       <c r="I8" s="13">
-        <f>SUMIF(B4:B57,"Documentazione interna",C4:C57)</f>
+        <f>SUMIF(B4:B59,"Documentazione interna",C4:C59)</f>
         <v>1930</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -685,11 +684,11 @@
         <v>9</v>
       </c>
       <c r="I9" s="13">
-        <f>SUMIF(B4:B57,"Manuale",C4:C57)</f>
+        <f>SUMIF(B4:B59,"Manuale",C4:C59)</f>
         <v>174</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>4</v>
       </c>
@@ -706,11 +705,11 @@
         <v>14</v>
       </c>
       <c r="I10" s="13">
-        <f>SUMIF(B4:B57,"Sviluppo",C4:C57)</f>
+        <f>SUMIF(B4:B59,"Sviluppo",C4:C59)</f>
         <v>1706</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>4</v>
       </c>
@@ -727,11 +726,11 @@
         <v>15</v>
       </c>
       <c r="I11" s="13">
-        <f>SUMIF(B4:B57,"Testing",C4:C57)</f>
+        <f>SUMIF(B4:B59,"Testing",C4:C59)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>4</v>
       </c>
@@ -745,46 +744,46 @@
         <v>43509</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13">
+        <v>45</v>
+      </c>
+      <c r="D13" s="2">
+        <v>43511</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14">
+        <v>30</v>
+      </c>
+      <c r="D14" s="2">
+        <v>43514</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>6</v>
       </c>
-      <c r="B13" t="s">
-        <v>11</v>
-      </c>
-      <c r="C13">
+      <c r="B15" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15">
         <v>195</v>
       </c>
-      <c r="D13" s="2">
+      <c r="D15" s="2">
         <v>43521</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>6</v>
-      </c>
-      <c r="B14" t="s">
-        <v>11</v>
-      </c>
-      <c r="C14">
-        <v>105</v>
-      </c>
-      <c r="D14" s="2">
-        <v>43523</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>7</v>
-      </c>
-      <c r="B15" t="s">
-        <v>5</v>
-      </c>
-      <c r="C15">
-        <v>30</v>
-      </c>
-      <c r="D15" s="2">
-        <v>43519</v>
       </c>
       <c r="H15" s="9" t="s">
         <v>23</v>
@@ -795,18 +794,18 @@
       <c r="L15" s="7"/>
       <c r="M15" s="7"/>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B16" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C16">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="D16" s="2">
-        <v>43520</v>
+        <v>43523</v>
       </c>
       <c r="H16" s="10" t="s">
         <v>19</v>
@@ -827,44 +826,44 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>7</v>
       </c>
       <c r="B17" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="C17">
-        <v>125</v>
+        <v>30</v>
       </c>
       <c r="D17" s="2">
-        <v>43522</v>
+        <v>43519</v>
       </c>
       <c r="H17" s="11" t="s">
         <v>4</v>
       </c>
       <c r="I17" s="7">
-        <f>SUMIFS(C4:C58,B4:B58,"Documentazione esterna",A4:A58,"Giovanni")</f>
+        <f>SUMIFS(C4:C60,B4:B60,"Documentazione esterna",A4:A60,"Giovanni")</f>
         <v>653</v>
       </c>
       <c r="J17" s="7">
-        <f>SUMIFS(C4:C58,B4:B58,"Documentazione interna",A4:A58,"Giovanni")</f>
+        <f>SUMIFS(C4:C60,B4:B60,"Documentazione interna",A4:A60,"Giovanni")</f>
         <v>796</v>
       </c>
       <c r="K17" s="7">
-        <f>SUMIFS(C4:C58,B4:B58,"Manuale",A4:A58,"Giovanni")</f>
+        <f>SUMIFS(C4:C60,B4:B60,"Manuale",A4:A60,"Giovanni")</f>
         <v>174</v>
       </c>
       <c r="L17" s="7">
-        <f>SUMIFS(C4:C58,B4:B58,"Sviluppo",A4:A58,"Giovanni")</f>
+        <f>SUMIFS(C4:C60,B4:B60,"Sviluppo",A4:A60,"Giovanni")</f>
         <v>0</v>
       </c>
       <c r="M17" s="7">
-        <f>SUMIFS(C4:C58,B4:B58,"Testing",A4:A58,"Giovanni")</f>
+        <f>SUMIFS(C4:C60,B4:B60,"Testing",A4:A60,"Giovanni")</f>
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>7</v>
       </c>
@@ -872,36 +871,36 @@
         <v>14</v>
       </c>
       <c r="C18">
-        <v>170</v>
+        <v>100</v>
       </c>
       <c r="D18" s="2">
-        <v>43523</v>
+        <v>43520</v>
       </c>
       <c r="H18" s="11" t="s">
         <v>7</v>
       </c>
       <c r="I18" s="7">
-        <f>SUMIFS(C4:C58,B4:B58,"Documentazione esterna",A4:A58,"Hristina")</f>
+        <f>SUMIFS(C4:C60,B4:B60,"Documentazione esterna",A4:A60,"Hristina")</f>
         <v>0</v>
       </c>
       <c r="J18" s="7">
-        <f>SUMIFS(C4:C58,B4:B58,"Documentazione interna",A4:A58,"Hristina")</f>
+        <f>SUMIFS(C4:C60,B4:B60,"Documentazione interna",A4:A60,"Hristina")</f>
         <v>252</v>
       </c>
       <c r="K18" s="7">
-        <f>SUMIFS(C4:C58,B4:B58,"Manuale",A4:A58,"Hristina")</f>
+        <f>SUMIFS(C4:C60,B4:B60,"Manuale",A4:A60,"Hristina")</f>
         <v>0</v>
       </c>
       <c r="L18" s="7">
-        <f>SUMIFS(C4:C58,B4:B58,"Sviluppo",A4:A58,"Hristina")</f>
+        <f>SUMIFS(C4:C60,B4:B60,"Sviluppo",A4:A60,"Hristina")</f>
         <v>892</v>
       </c>
       <c r="M18" s="7">
-        <f>SUMIFS(C4:C58,B4:B58,"Testing",A4:A58,"Hristina")</f>
+        <f>SUMIFS(C4:C60,B4:B60,"Testing",A4:A60,"Hristina")</f>
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>7</v>
       </c>
@@ -909,87 +908,87 @@
         <v>14</v>
       </c>
       <c r="C19">
-        <v>65</v>
+        <v>125</v>
       </c>
       <c r="D19" s="2">
-        <v>43524</v>
+        <v>43522</v>
       </c>
       <c r="H19" s="11" t="s">
         <v>6</v>
       </c>
       <c r="I19" s="7">
-        <f>SUMIFS(C4:C58,B4:B58,"Documentazione esterna",A4:A58,"Luca")</f>
+        <f>SUMIFS(C4:C60,B4:B60,"Documentazione esterna",A4:A60,"Luca")</f>
         <v>585</v>
       </c>
       <c r="J19" s="7">
-        <f>SUMIFS(C4:C58,B4:B58,"Documentazione interna",A4:A58,"Luca")</f>
+        <f>SUMIFS(C4:C60,B4:B60,"Documentazione interna",A4:A60,"Luca")</f>
         <v>852</v>
       </c>
       <c r="K19" s="7">
-        <f>SUMIFS(C4:C58,B4:B58,"Manuale",A4:A58,"Luca")</f>
+        <f>SUMIFS(C4:C60,B4:B60,"Manuale",A4:A60,"Luca")</f>
         <v>0</v>
       </c>
       <c r="L19" s="7">
-        <f>SUMIFS(C4:C58,B4:B58,"Sviluppo",A4:A58,"Luca")</f>
+        <f>SUMIFS(C4:C60,B4:B60,"Sviluppo",A4:A60,"Luca")</f>
         <v>0</v>
       </c>
       <c r="M19" s="7">
-        <f>SUMIFS(C4:C58,B4:B58,"Testing",A4:A58,"Luca")</f>
+        <f>SUMIFS(C4:C60,B4:B60,"Testing",A4:A60,"Luca")</f>
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B20" t="s">
         <v>14</v>
       </c>
       <c r="C20">
-        <v>60</v>
+        <v>170</v>
       </c>
       <c r="D20" s="2">
-        <v>43487</v>
+        <v>43523</v>
       </c>
       <c r="H20" s="11" t="s">
         <v>8</v>
       </c>
       <c r="I20" s="7">
-        <f>SUMIFS(C4:C58,B4:B58,"Documentazione esterna",A4:A58,"Viktorija")</f>
+        <f>SUMIFS(C4:C60,B4:B60,"Documentazione esterna",A4:A60,"Viktorija")</f>
+        <v>75</v>
+      </c>
+      <c r="J20" s="7">
+        <f>SUMIFS(C4:C60,B4:B60,"Documentazione interna",A4:A60,"Viktorija")</f>
+        <v>60</v>
+      </c>
+      <c r="K20" s="7">
+        <f>SUMIFS(C4:C60,B4:B60,"Manuale",A4:A60,"Viktorija")</f>
         <v>0</v>
       </c>
-      <c r="J20" s="7">
-        <f>SUMIFS(C4:C58,B4:B58,"Documentazione interna",A4:A58,"Viktorija")</f>
-        <v>60</v>
-      </c>
-      <c r="K20" s="7">
-        <f>SUMIFS(C4:C58,B4:B58,"Manuale",A4:A58,"Viktorija")</f>
+      <c r="L20" s="7">
+        <f>SUMIFS(C4:C60,B4:B60,"Sviluppo",A4:A60,"Viktorija")</f>
+        <v>814</v>
+      </c>
+      <c r="M20" s="7">
+        <f>SUMIFS(C4:C60,B4:B60,"Testing",A4:A60,"Viktorija")</f>
         <v>0</v>
       </c>
-      <c r="L20" s="7">
-        <f>SUMIFS(C4:C58,B4:B58,"Sviluppo",A4:A58,"Viktorija")</f>
-        <v>814</v>
-      </c>
-      <c r="M20" s="7">
-        <f>SUMIFS(C4:C58,B4:B58,"Testing",A4:A58,"Viktorija")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B21" t="s">
         <v>14</v>
       </c>
       <c r="C21">
-        <v>103</v>
+        <v>65</v>
       </c>
       <c r="D21" s="2">
-        <v>43506</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+        <v>43524</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>8</v>
       </c>
@@ -997,13 +996,13 @@
         <v>14</v>
       </c>
       <c r="C22">
-        <v>100</v>
+        <v>60</v>
       </c>
       <c r="D22" s="2">
-        <v>43520</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+        <v>43487</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>8</v>
       </c>
@@ -1011,13 +1010,13 @@
         <v>14</v>
       </c>
       <c r="C23">
-        <v>170</v>
+        <v>103</v>
       </c>
       <c r="D23" s="2">
-        <v>43523</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+        <v>43506</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>8</v>
       </c>
@@ -1025,13 +1024,13 @@
         <v>14</v>
       </c>
       <c r="C24">
-        <v>45</v>
+        <v>100</v>
       </c>
       <c r="D24" s="2">
-        <v>43524</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+        <v>43520</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>8</v>
       </c>
@@ -1039,46 +1038,46 @@
         <v>14</v>
       </c>
       <c r="C25">
+        <v>170</v>
+      </c>
+      <c r="D25" s="2">
+        <v>43523</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>8</v>
+      </c>
+      <c r="B26" t="s">
+        <v>14</v>
+      </c>
+      <c r="C26">
+        <v>45</v>
+      </c>
+      <c r="D26" s="2">
+        <v>43524</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>8</v>
+      </c>
+      <c r="B27" t="s">
+        <v>14</v>
+      </c>
+      <c r="C27">
         <v>25</v>
       </c>
-      <c r="D25" s="2">
+      <c r="D27" s="2">
         <v>43530</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>6</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B28" t="s">
         <v>10</v>
-      </c>
-      <c r="C26">
-        <v>15</v>
-      </c>
-      <c r="D26" s="2">
-        <v>43532</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
-        <v>4</v>
-      </c>
-      <c r="B27" t="s">
-        <v>9</v>
-      </c>
-      <c r="C27">
-        <v>47</v>
-      </c>
-      <c r="D27" s="2">
-        <v>43532</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
-        <v>7</v>
-      </c>
-      <c r="B28" t="s">
-        <v>5</v>
       </c>
       <c r="C28">
         <v>15</v>
@@ -1087,35 +1086,35 @@
         <v>43532</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B29" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C29">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="D29" s="2">
-        <v>43531</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+        <v>43532</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>7</v>
       </c>
       <c r="B30" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="C30">
-        <v>68</v>
+        <v>15</v>
       </c>
       <c r="D30" s="2">
         <v>43532</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>7</v>
       </c>
@@ -1123,13 +1122,13 @@
         <v>14</v>
       </c>
       <c r="C31">
-        <v>129</v>
+        <v>55</v>
       </c>
       <c r="D31" s="2">
-        <v>43533</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+        <v>43531</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>7</v>
       </c>
@@ -1137,97 +1136,97 @@
         <v>14</v>
       </c>
       <c r="C32">
+        <v>68</v>
+      </c>
+      <c r="D32" s="2">
+        <v>43532</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>7</v>
+      </c>
+      <c r="B33" t="s">
+        <v>14</v>
+      </c>
+      <c r="C33">
+        <v>129</v>
+      </c>
+      <c r="D33" s="2">
+        <v>43533</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>7</v>
+      </c>
+      <c r="B34" t="s">
+        <v>14</v>
+      </c>
+      <c r="C34">
         <v>95</v>
       </c>
-      <c r="D32" s="2">
+      <c r="D34" s="2">
         <v>43534</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
         <v>4</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B35" t="s">
         <v>10</v>
       </c>
-      <c r="C33">
+      <c r="C35">
         <v>74</v>
       </c>
-      <c r="D33" s="2">
+      <c r="D35" s="2">
         <v>43546</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>4</v>
       </c>
-      <c r="B34" t="s">
-        <v>11</v>
-      </c>
-      <c r="C34">
+      <c r="B36" t="s">
+        <v>11</v>
+      </c>
+      <c r="C36">
         <v>52</v>
       </c>
-      <c r="D34" s="2">
+      <c r="D36" s="2">
         <v>43546</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>8</v>
       </c>
-      <c r="B35" t="s">
-        <v>14</v>
-      </c>
-      <c r="C35">
+      <c r="B37" t="s">
+        <v>14</v>
+      </c>
+      <c r="C37">
         <v>196</v>
       </c>
-      <c r="D35" s="2">
+      <c r="D37" s="2">
         <v>43376</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
         <v>8</v>
       </c>
-      <c r="B36" t="s">
-        <v>14</v>
-      </c>
-      <c r="C36">
+      <c r="B38" t="s">
+        <v>14</v>
+      </c>
+      <c r="C38">
         <v>115</v>
       </c>
-      <c r="D36" s="2">
+      <c r="D38" s="2">
         <v>43407</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
-        <v>7</v>
-      </c>
-      <c r="B37" t="s">
-        <v>11</v>
-      </c>
-      <c r="C37">
-        <v>10</v>
-      </c>
-      <c r="D37" s="2">
-        <v>43546</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
-        <v>6</v>
-      </c>
-      <c r="B38" t="s">
-        <v>11</v>
-      </c>
-      <c r="C38">
-        <v>60</v>
-      </c>
-      <c r="D38" s="2">
-        <v>43553</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>7</v>
       </c>
@@ -1235,15 +1234,15 @@
         <v>11</v>
       </c>
       <c r="C39">
-        <v>60</v>
+        <v>10</v>
       </c>
       <c r="D39" s="2">
-        <v>43553</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+        <v>43546</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B40" t="s">
         <v>11</v>
@@ -1255,35 +1254,35 @@
         <v>43553</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B41" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C41">
         <v>60</v>
       </c>
       <c r="D41" s="2">
-        <v>43481</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+        <v>43553</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B42" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C42">
-        <v>150</v>
+        <v>60</v>
       </c>
       <c r="D42" s="2">
-        <v>43442</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+        <v>43553</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>6</v>
       </c>
@@ -1291,13 +1290,13 @@
         <v>10</v>
       </c>
       <c r="C43">
-        <v>180</v>
+        <v>60</v>
       </c>
       <c r="D43" s="2">
-        <v>43448</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+        <v>43481</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>6</v>
       </c>
@@ -1305,85 +1304,85 @@
         <v>10</v>
       </c>
       <c r="C44">
-        <v>180</v>
+        <v>150</v>
       </c>
       <c r="D44" s="2">
-        <v>43468</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+        <v>43442</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>6</v>
       </c>
       <c r="B45" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C45">
+        <v>180</v>
+      </c>
+      <c r="D45" s="2">
+        <v>43448</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>6</v>
+      </c>
+      <c r="B46" t="s">
+        <v>10</v>
+      </c>
+      <c r="C46">
+        <v>180</v>
+      </c>
+      <c r="D46" s="2">
+        <v>43468</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>6</v>
+      </c>
+      <c r="B47" t="s">
+        <v>11</v>
+      </c>
+      <c r="C47">
         <v>120</v>
       </c>
-      <c r="D45" s="2">
+      <c r="D47" s="2">
         <v>43478</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A46" t="s">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
         <v>4</v>
       </c>
-      <c r="B46" t="s">
-        <v>11</v>
-      </c>
-      <c r="C46">
+      <c r="B48" t="s">
+        <v>11</v>
+      </c>
+      <c r="C48">
         <v>300</v>
       </c>
-      <c r="D46" s="2">
+      <c r="D48" s="2">
         <v>43449</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A47" t="s">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
         <v>4</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B49" t="s">
         <v>10</v>
       </c>
-      <c r="C47">
+      <c r="C49">
         <v>150</v>
       </c>
-      <c r="D47" s="2">
+      <c r="D49" s="2">
         <v>43450</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A48" t="s">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
         <v>6</v>
-      </c>
-      <c r="B48" t="s">
-        <v>11</v>
-      </c>
-      <c r="C48">
-        <v>82</v>
-      </c>
-      <c r="D48" s="2">
-        <v>43558</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A49" t="s">
-        <v>7</v>
-      </c>
-      <c r="B49" t="s">
-        <v>11</v>
-      </c>
-      <c r="C49">
-        <v>82</v>
-      </c>
-      <c r="D49" s="2">
-        <v>43558</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A50" t="s">
-        <v>4</v>
       </c>
       <c r="B50" t="s">
         <v>11</v>
@@ -1395,49 +1394,49 @@
         <v>43558</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>7</v>
       </c>
       <c r="B51" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C51">
-        <v>85</v>
-      </c>
-      <c r="D51" s="14">
-        <v>43559</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+        <v>82</v>
+      </c>
+      <c r="D51" s="2">
+        <v>43558</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B52" t="s">
         <v>11</v>
       </c>
       <c r="C52">
-        <v>70</v>
+        <v>82</v>
       </c>
       <c r="D52" s="2">
-        <v>43571</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+        <v>43558</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>7</v>
       </c>
       <c r="B53" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C53">
-        <v>70</v>
-      </c>
-      <c r="D53" s="2">
-        <v>43571</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+        <v>85</v>
+      </c>
+      <c r="D53" s="14">
+        <v>43559</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>6</v>
       </c>
@@ -1445,229 +1444,257 @@
         <v>11</v>
       </c>
       <c r="C54">
+        <v>70</v>
+      </c>
+      <c r="D54" s="2">
+        <v>43571</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>7</v>
+      </c>
+      <c r="B55" t="s">
+        <v>11</v>
+      </c>
+      <c r="C55">
+        <v>70</v>
+      </c>
+      <c r="D55" s="2">
+        <v>43571</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>6</v>
+      </c>
+      <c r="B56" t="s">
+        <v>11</v>
+      </c>
+      <c r="C56">
         <v>120</v>
       </c>
-      <c r="D54" s="2">
+      <c r="D56" s="2">
         <v>43572</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A55" t="s">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
         <v>6</v>
       </c>
-      <c r="B55" t="s">
-        <v>11</v>
-      </c>
-      <c r="C55">
+      <c r="B57" t="s">
+        <v>11</v>
+      </c>
+      <c r="C57">
         <v>100</v>
       </c>
-      <c r="D55" s="2">
+      <c r="D57" s="2">
         <v>43574</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A56" t="s">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
         <v>4</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B58" t="s">
         <v>10</v>
       </c>
-      <c r="C56">
+      <c r="C58">
         <v>42</v>
       </c>
-      <c r="D56" s="2">
+      <c r="D58" s="2">
         <v>43577</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A57" t="s">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
         <v>4</v>
       </c>
-      <c r="B57" t="s">
-        <v>11</v>
-      </c>
-      <c r="C57">
+      <c r="B59" t="s">
+        <v>11</v>
+      </c>
+      <c r="C59">
         <v>97</v>
       </c>
-      <c r="D57" s="2">
+      <c r="D59" s="2">
         <v>43578</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A58" t="s">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
         <v>7</v>
       </c>
-      <c r="B58" t="s">
-        <v>11</v>
-      </c>
-      <c r="C58">
+      <c r="B60" t="s">
+        <v>11</v>
+      </c>
+      <c r="C60">
         <v>30</v>
       </c>
-      <c r="D58" s="14">
+      <c r="D60" s="14">
         <v>43578</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="D59" s="2"/>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="D60" s="2"/>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D61" s="2"/>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D62" s="2"/>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D63" s="2"/>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D64" s="2"/>
     </row>
-    <row r="65" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="65" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D65" s="2"/>
     </row>
-    <row r="66" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="66" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D66" s="2"/>
     </row>
-    <row r="67" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="67" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D67" s="2"/>
     </row>
-    <row r="68" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="68" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D68" s="2"/>
     </row>
-    <row r="69" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="69" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D69" s="2"/>
     </row>
-    <row r="70" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="70" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D70" s="2"/>
     </row>
-    <row r="71" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="71" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D71" s="2"/>
     </row>
-    <row r="72" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="72" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D72" s="2"/>
     </row>
-    <row r="73" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="73" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D73" s="2"/>
     </row>
-    <row r="74" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="74" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D74" s="2"/>
     </row>
-    <row r="75" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="75" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D75" s="2"/>
     </row>
-    <row r="76" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="76" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D76" s="2"/>
     </row>
-    <row r="77" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="77" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D77" s="2"/>
     </row>
-    <row r="78" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="78" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D78" s="2"/>
     </row>
-    <row r="79" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="79" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D79" s="2"/>
     </row>
-    <row r="80" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="80" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D80" s="2"/>
     </row>
-    <row r="81" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="81" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D81" s="2"/>
     </row>
-    <row r="82" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="82" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D82" s="2"/>
     </row>
-    <row r="83" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="83" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D83" s="2"/>
     </row>
-    <row r="84" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="84" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D84" s="2"/>
     </row>
-    <row r="85" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="85" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D85" s="2"/>
     </row>
-    <row r="86" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="86" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D86" s="2"/>
     </row>
-    <row r="87" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="87" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D87" s="2"/>
     </row>
-    <row r="88" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="88" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D88" s="2"/>
     </row>
-    <row r="89" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="89" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D89" s="2"/>
     </row>
-    <row r="90" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="90" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D90" s="2"/>
     </row>
-    <row r="91" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="91" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D91" s="2"/>
     </row>
-    <row r="92" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="92" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D92" s="2"/>
     </row>
-    <row r="93" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="93" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D93" s="2"/>
     </row>
-    <row r="94" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="94" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D94" s="2"/>
     </row>
-    <row r="95" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="95" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D95" s="2"/>
     </row>
-    <row r="96" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="96" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D96" s="2"/>
     </row>
-    <row r="97" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="97" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D97" s="2"/>
     </row>
-    <row r="98" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="98" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D98" s="2"/>
     </row>
-    <row r="99" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="99" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D99" s="2"/>
     </row>
-    <row r="100" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="100" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D100" s="2"/>
     </row>
-    <row r="101" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="101" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D101" s="2"/>
     </row>
-    <row r="102" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="102" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D102" s="2"/>
     </row>
-    <row r="103" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="103" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D103" s="2"/>
     </row>
-    <row r="104" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="104" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D104" s="2"/>
     </row>
-    <row r="105" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="105" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D105" s="2"/>
     </row>
-    <row r="106" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="106" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D106" s="2"/>
     </row>
-    <row r="107" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="107" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D107" s="2"/>
     </row>
-    <row r="108" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="108" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D108" s="2"/>
     </row>
-    <row r="109" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="109" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D109" s="2"/>
     </row>
-    <row r="110" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="110" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D110" s="2"/>
     </row>
-    <row r="111" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="111" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D111" s="2"/>
     </row>
-    <row r="112" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="112" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D112" s="2"/>
+    </row>
+    <row r="113" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D113" s="2"/>
+    </row>
+    <row r="114" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D114" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>

<commit_message>
Modifica per possibili errori COCOMO
</commit_message>
<xml_diff>
--- a/Documentazione/Attività sul progetto/DocAttivProg.xlsx
+++ b/Documentazione/Attività sul progetto/DocAttivProg.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\UniUD\Laurea Magistrale\Ingegneria del Software 2\Progetto-Ingegneria-Del-Sw-2\Documentazione\Attività sul progetto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1AEA2DC-DF67-4FBA-A840-5A1B0214E391}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E703D01-6344-4EEE-9BA4-99197C42C907}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="27">
   <si>
     <t>PERSONA</t>
   </si>
@@ -189,7 +189,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -212,28 +212,49 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -241,27 +262,8 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -271,6 +273,46 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -590,8 +632,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O112"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C60" sqref="C60"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C61" sqref="C61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -601,1188 +643,1196 @@
     <col min="3" max="3" width="15.5546875" customWidth="1"/>
     <col min="4" max="4" width="10.88671875" customWidth="1"/>
     <col min="5" max="7" width="8.6640625" customWidth="1"/>
-    <col min="8" max="8" width="23.5546875" customWidth="1"/>
+    <col min="8" max="8" width="26.33203125" customWidth="1"/>
     <col min="9" max="11" width="17.33203125" customWidth="1"/>
     <col min="12" max="14" width="17.44140625" customWidth="1"/>
     <col min="15" max="1025" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="F1" s="25" t="s">
+      <c r="F1" s="14" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
-      <c r="F2" s="26" t="s">
+      <c r="F2" s="15" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A3" s="21" t="s">
+      <c r="A3" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="21" t="s">
+      <c r="B3" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="21" t="s">
+      <c r="C3" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="21" t="s">
+      <c r="D3" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="H3" s="4"/>
+      <c r="H3" s="3"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A4" s="22" t="s">
+      <c r="A4" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="22" t="s">
+      <c r="B4" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="C4" s="22">
+      <c r="C4" s="11">
         <v>98</v>
       </c>
-      <c r="D4" s="23">
+      <c r="D4" s="12">
         <v>43484</v>
       </c>
-      <c r="H4" s="6" t="s">
+      <c r="H4" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
+      <c r="I4" s="21"/>
+      <c r="J4" s="21"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A5" s="22" t="s">
+      <c r="A5" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="22" t="s">
+      <c r="B5" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="22">
+      <c r="C5" s="11">
         <v>149</v>
       </c>
-      <c r="D5" s="23">
+      <c r="D5" s="12">
         <v>43493</v>
       </c>
-      <c r="H5" s="5" t="s">
+      <c r="H5" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="I5" s="12" t="s">
+      <c r="I5" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="J5" s="12" t="s">
+      <c r="J5" s="24" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A6" s="22" t="s">
+      <c r="A6" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="22" t="s">
-        <v>24</v>
-      </c>
-      <c r="C6" s="22">
+      <c r="B6" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="11">
         <v>135</v>
       </c>
-      <c r="D6" s="23">
+      <c r="D6" s="12">
         <v>43494</v>
       </c>
-      <c r="H6" s="3" t="s">
+      <c r="H6" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="I6" s="13">
+      <c r="I6" s="26">
         <f>SUMIF(B4:B59,"Ispezione codice",C4:C59)</f>
         <v>0</v>
       </c>
-      <c r="J6" s="17">
+      <c r="J6" s="27">
         <f>(I6/I12)*100</f>
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A7" s="22" t="s">
+      <c r="A7" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="22" t="s">
+      <c r="B7" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="C7" s="22">
+      <c r="C7" s="11">
         <v>53</v>
       </c>
-      <c r="D7" s="23">
+      <c r="D7" s="12">
         <v>43494</v>
       </c>
-      <c r="H7" s="3" t="s">
+      <c r="H7" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="I7" s="13">
+      <c r="I7" s="26">
         <f>SUMIF(B:B,"Documenti di progetto",C:C)</f>
-        <v>1238</v>
-      </c>
-      <c r="J7" s="18">
+        <v>1277</v>
+      </c>
+      <c r="J7" s="28">
         <f>(I7/I12)*100</f>
-        <v>24.15609756097561</v>
+        <v>24.728892331525948</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A8" s="22" t="s">
+      <c r="A8" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="22" t="s">
+      <c r="B8" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="C8" s="22">
+      <c r="C8" s="11">
         <v>87</v>
       </c>
-      <c r="D8" s="23">
+      <c r="D8" s="12">
         <v>43495</v>
       </c>
-      <c r="H8" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="I8" s="13">
+      <c r="H8" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="I8" s="26">
         <f>SUMIF(B:B,"Documenti di processo",C:C)</f>
         <v>2067</v>
       </c>
-      <c r="J8" s="18">
+      <c r="J8" s="28">
         <f>(I8/I12)*100</f>
-        <v>40.331707317073175</v>
+        <v>40.027110766847407</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A9" s="22" t="s">
+      <c r="A9" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="22" t="s">
-        <v>24</v>
-      </c>
-      <c r="C9" s="22">
+      <c r="B9" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" s="11">
         <v>74</v>
       </c>
-      <c r="D9" s="23">
+      <c r="D9" s="12">
         <v>43495</v>
       </c>
-      <c r="H9" s="3" t="s">
+      <c r="H9" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="I9" s="13">
+      <c r="I9" s="26">
         <f>SUMIF(B:B,"Manuale",C:C)</f>
         <v>174</v>
       </c>
-      <c r="J9" s="18">
+      <c r="J9" s="28">
         <f>(I9/I12)*100</f>
-        <v>3.3951219512195125</v>
+        <v>3.3694810224632068</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A10" s="22" t="s">
+      <c r="A10" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B10" s="22" t="s">
-        <v>24</v>
-      </c>
-      <c r="C10" s="22">
+      <c r="B10" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" s="11">
         <v>32</v>
       </c>
-      <c r="D10" s="23">
+      <c r="D10" s="12">
         <v>43499</v>
       </c>
-      <c r="H10" s="3" t="s">
+      <c r="H10" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="I10" s="13">
+      <c r="I10" s="26">
         <f>SUMIF(B:B,"Sviluppo",C:C)</f>
         <v>1646</v>
       </c>
-      <c r="J10" s="18">
+      <c r="J10" s="28">
         <f>(I10/I12)*100</f>
-        <v>32.117073170731707</v>
+        <v>31.87451587916344</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A11" s="22" t="s">
+      <c r="A11" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B11" s="22" t="s">
+      <c r="B11" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="22">
+      <c r="C11" s="11">
         <v>127</v>
       </c>
-      <c r="D11" s="23">
+      <c r="D11" s="12">
         <v>43505</v>
       </c>
-      <c r="H11" s="3" t="s">
+      <c r="H11" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="I11" s="13">
+      <c r="I11" s="30">
         <f>SUMIF(B:B,"Testing",C:C)</f>
         <v>0</v>
       </c>
-      <c r="J11" s="19">
+      <c r="J11" s="31">
         <f>(I11/I12)*100</f>
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A12" s="22" t="s">
+      <c r="A12" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B12" s="22" t="s">
-        <v>24</v>
-      </c>
-      <c r="C12" s="22">
-        <v>24</v>
-      </c>
-      <c r="D12" s="23">
+      <c r="B12" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" s="11">
+        <v>24</v>
+      </c>
+      <c r="D12" s="12">
         <v>43509</v>
       </c>
-      <c r="H12" s="5" t="s">
+      <c r="H12" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="I12" s="13">
+      <c r="I12" s="17">
         <f>SUM(I6:I11)</f>
-        <v>5125</v>
-      </c>
-      <c r="J12" s="20">
+        <v>5164</v>
+      </c>
+      <c r="J12" s="18">
         <f>SUM(J6:J11)</f>
         <v>100</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A13" s="22" t="s">
+      <c r="A13" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B13" s="22" t="s">
-        <v>24</v>
-      </c>
-      <c r="C13" s="22">
+      <c r="B13" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" s="11">
         <v>195</v>
       </c>
-      <c r="D13" s="23">
+      <c r="D13" s="12">
         <v>43521</v>
       </c>
-      <c r="H13" s="15"/>
-      <c r="I13" s="16"/>
-      <c r="J13" s="16"/>
+      <c r="H13" s="8"/>
+      <c r="I13" s="9"/>
+      <c r="J13" s="9"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A14" s="22" t="s">
+      <c r="A14" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B14" s="22" t="s">
-        <v>24</v>
-      </c>
-      <c r="C14" s="22">
+      <c r="B14" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" s="11">
         <v>105</v>
       </c>
-      <c r="D14" s="23">
+      <c r="D14" s="12">
         <v>43523</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A15" s="22" t="s">
+      <c r="A15" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B15" s="22" t="s">
+      <c r="B15" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="C15" s="22">
+      <c r="C15" s="11">
         <v>30</v>
       </c>
-      <c r="D15" s="23">
+      <c r="D15" s="12">
         <v>43519</v>
       </c>
-      <c r="H15" s="9" t="s">
+      <c r="H15" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="I15" s="7"/>
-      <c r="J15" s="7"/>
-      <c r="K15" s="7"/>
-      <c r="L15" s="7"/>
-      <c r="M15" s="7"/>
-      <c r="N15" s="14"/>
-      <c r="O15" s="14"/>
+      <c r="I15" s="22"/>
+      <c r="J15" s="22"/>
+      <c r="K15" s="22"/>
+      <c r="L15" s="22"/>
+      <c r="M15" s="22"/>
+      <c r="N15" s="22"/>
+      <c r="O15" s="22"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A16" s="22" t="s">
+      <c r="A16" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="22" t="s">
+      <c r="B16" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="C16" s="22">
+      <c r="C16" s="11">
         <v>100</v>
       </c>
-      <c r="D16" s="23">
+      <c r="D16" s="12">
         <v>43520</v>
       </c>
-      <c r="H16" s="10" t="s">
+      <c r="H16" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="I16" s="8" t="s">
+      <c r="I16" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="J16" s="8" t="s">
+      <c r="J16" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="K16" s="8" t="s">
+      <c r="K16" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="L16" s="8" t="s">
+      <c r="L16" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="M16" s="8" t="s">
+      <c r="M16" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="N16" s="8" t="s">
+      <c r="N16" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="O16" s="8" t="s">
+      <c r="O16" s="19" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A17" s="22" t="s">
+      <c r="A17" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B17" s="22" t="s">
+      <c r="B17" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="C17" s="22">
+      <c r="C17" s="11">
         <v>125</v>
       </c>
-      <c r="D17" s="23">
+      <c r="D17" s="12">
         <v>43522</v>
       </c>
-      <c r="H17" s="11" t="s">
+      <c r="H17" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="I17" s="7">
+      <c r="I17" s="4">
         <f>SUMIFS(C:C,B:B,"Documenti di progetto",A:A,"Giovanni")</f>
-        <v>653</v>
-      </c>
-      <c r="J17" s="7">
+        <v>692</v>
+      </c>
+      <c r="J17" s="4">
         <f>SUMIFS(C:C,B:B,"Documenti di processo",A:A,"Giovanni")</f>
         <v>903</v>
       </c>
-      <c r="K17" s="7">
+      <c r="K17" s="4">
         <f>SUMIFS(C:C,B:B,"Manuale",A:A,"Giovanni")</f>
         <v>174</v>
       </c>
-      <c r="L17" s="7">
+      <c r="L17" s="4">
         <f>SUMIFS(C:C,B:B,"Sviluppo",A:A,"Giovanni")</f>
         <v>0</v>
       </c>
-      <c r="M17" s="7">
+      <c r="M17" s="4">
         <f>SUMIFS(C:C,B:B,"Testing",A:A,"Giovanni")</f>
         <v>0</v>
       </c>
-      <c r="N17" s="7">
+      <c r="N17" s="4">
         <f>SUMIFS(C:C,B:B,"Ispezione codice",A:A,"Giovanni")</f>
         <v>0</v>
       </c>
-      <c r="O17" s="7">
+      <c r="O17" s="20">
         <f>SUM(I17:M17)</f>
-        <v>1730</v>
+        <v>1769</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A18" s="22" t="s">
+      <c r="A18" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B18" s="22" t="s">
+      <c r="B18" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="C18" s="22">
+      <c r="C18" s="11">
         <v>170</v>
       </c>
-      <c r="D18" s="23">
+      <c r="D18" s="12">
         <v>43523</v>
       </c>
-      <c r="H18" s="11" t="s">
+      <c r="H18" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="I18" s="7">
+      <c r="I18" s="4">
         <f>SUMIFS(C:C,B:B,"Documenti di progetto",A:A,"Hristina")</f>
         <v>0</v>
       </c>
-      <c r="J18" s="7">
+      <c r="J18" s="4">
         <f>SUMIFS(C:C,B:B,"Documenti di processo",A:A,"Hristina")</f>
         <v>252</v>
       </c>
-      <c r="K18" s="7">
+      <c r="K18" s="4">
         <f>SUMIFS(C:C,B:B,"Manuale",A:A,"Hristina")</f>
         <v>0</v>
       </c>
-      <c r="L18" s="7">
+      <c r="L18" s="4">
         <f>SUMIFS(C:C,B:B,"Sviluppo",A:A,"Hristina")</f>
         <v>892</v>
       </c>
-      <c r="M18" s="7">
+      <c r="M18" s="4">
         <f>SUMIFS(C:C,B:B,"Testing",A:A,"Hristina")</f>
         <v>0</v>
       </c>
-      <c r="N18" s="7">
+      <c r="N18" s="4">
         <f>SUMIFS(C:C,B:B,"Ispezione codice",A:A,"Hristina")</f>
         <v>0</v>
       </c>
-      <c r="O18" s="7">
+      <c r="O18" s="20">
         <f>SUM(I18:M18)</f>
         <v>1144</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A19" s="22" t="s">
+      <c r="A19" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B19" s="22" t="s">
+      <c r="B19" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="C19" s="22">
+      <c r="C19" s="11">
         <v>65</v>
       </c>
-      <c r="D19" s="23">
+      <c r="D19" s="12">
         <v>43524</v>
       </c>
-      <c r="H19" s="11" t="s">
+      <c r="H19" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="I19" s="7">
+      <c r="I19" s="4">
         <f>SUMIFS(C:C,B:B,"Documenti di progetto",A:A,"Luca")</f>
         <v>585</v>
       </c>
-      <c r="J19" s="7">
+      <c r="J19" s="4">
         <f>SUMIFS(C:C,B:B,"Documenti di processo",A:A,"Luca")</f>
         <v>852</v>
       </c>
-      <c r="K19" s="7">
+      <c r="K19" s="4">
         <f>SUMIFS(C:C,B:B,"Manuale",A:A,"Luca")</f>
         <v>0</v>
       </c>
-      <c r="L19" s="7">
+      <c r="L19" s="4">
         <f>SUMIFS(C:C,B:B,"Sviluppo",A:A,"Luca")</f>
         <v>0</v>
       </c>
-      <c r="M19" s="7">
+      <c r="M19" s="4">
         <f>SUMIFS(C:C,B:B,"Testing",A:A,"Luca")</f>
         <v>0</v>
       </c>
-      <c r="N19" s="7">
+      <c r="N19" s="4">
         <f>SUMIFS(C:C,B:B,"Ispezione codice",A:A,"Luca")</f>
         <v>0</v>
       </c>
-      <c r="O19" s="7">
+      <c r="O19" s="20">
         <f>SUM(I19:M19)</f>
         <v>1437</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A20" s="22" t="s">
+      <c r="A20" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="B20" s="22" t="s">
+      <c r="B20" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="C20" s="22">
+      <c r="C20" s="11">
         <v>60</v>
       </c>
-      <c r="D20" s="23">
+      <c r="D20" s="12">
         <v>43487</v>
       </c>
-      <c r="H20" s="11" t="s">
+      <c r="H20" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="I20" s="7">
+      <c r="I20" s="4">
         <f>SUMIFS(C:C,B:B,"Documenti di progetto",A:A,"Viktorija")</f>
         <v>0</v>
       </c>
-      <c r="J20" s="7">
+      <c r="J20" s="4">
         <f>SUMIFS(C:C,B:B,"Documenti di processo",A:A,"Viktorija")</f>
         <v>60</v>
       </c>
-      <c r="K20" s="7">
+      <c r="K20" s="4">
         <f>SUMIFS(C:C,B:B,"Manuale",A:A,"Viktorija")</f>
         <v>0</v>
       </c>
-      <c r="L20" s="7">
+      <c r="L20" s="4">
         <f>SUMIFS(C:C,B:B,"Sviluppo",A:A,"Viktorija")</f>
         <v>754</v>
       </c>
-      <c r="M20" s="7">
+      <c r="M20" s="4">
         <f>SUMIFS(C:C,B:B,"Testing",A:A,"Viktorija")</f>
         <v>0</v>
       </c>
-      <c r="N20" s="7">
+      <c r="N20" s="4">
         <f>SUMIFS(C:C,B:B,"Ispezione codice",A:A,"Viktorija")</f>
         <v>0</v>
       </c>
-      <c r="O20" s="7">
+      <c r="O20" s="20">
         <f>SUM(I20:M20)</f>
         <v>814</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A21" s="22" t="s">
+      <c r="A21" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="B21" s="22" t="s">
+      <c r="B21" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="C21" s="22">
+      <c r="C21" s="11">
         <v>103</v>
       </c>
-      <c r="D21" s="23">
+      <c r="D21" s="12">
         <v>43506</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A22" s="22" t="s">
+      <c r="A22" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="B22" s="22" t="s">
+      <c r="B22" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="C22" s="22">
+      <c r="C22" s="11">
         <v>100</v>
       </c>
-      <c r="D22" s="23">
+      <c r="D22" s="12">
         <v>43520</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A23" s="22" t="s">
+      <c r="A23" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="B23" s="22" t="s">
+      <c r="B23" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="C23" s="22">
+      <c r="C23" s="11">
         <v>170</v>
       </c>
-      <c r="D23" s="23">
+      <c r="D23" s="12">
         <v>43523</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A24" s="22" t="s">
+      <c r="A24" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="B24" s="22" t="s">
+      <c r="B24" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="C24" s="22">
+      <c r="C24" s="11">
         <v>45</v>
       </c>
-      <c r="D24" s="23">
+      <c r="D24" s="12">
         <v>43524</v>
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A25" s="22" t="s">
+      <c r="A25" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="B25" s="22" t="s">
+      <c r="B25" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="C25" s="22">
+      <c r="C25" s="11">
         <v>25</v>
       </c>
-      <c r="D25" s="23">
+      <c r="D25" s="12">
         <v>43530</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A26" s="22" t="s">
+      <c r="A26" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B26" s="22" t="s">
+      <c r="B26" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="C26" s="22">
+      <c r="C26" s="11">
         <v>15</v>
       </c>
-      <c r="D26" s="23">
+      <c r="D26" s="12">
         <v>43532</v>
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A27" s="22" t="s">
+      <c r="A27" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B27" s="22" t="s">
+      <c r="B27" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C27" s="22">
+      <c r="C27" s="11">
         <v>47</v>
       </c>
-      <c r="D27" s="23">
+      <c r="D27" s="12">
         <v>43532</v>
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A28" s="22" t="s">
+      <c r="A28" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B28" s="22" t="s">
+      <c r="B28" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="C28" s="22">
+      <c r="C28" s="11">
         <v>15</v>
       </c>
-      <c r="D28" s="23">
+      <c r="D28" s="12">
         <v>43532</v>
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A29" s="22" t="s">
+      <c r="A29" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B29" s="22" t="s">
+      <c r="B29" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="C29" s="22">
+      <c r="C29" s="11">
         <v>55</v>
       </c>
-      <c r="D29" s="23">
+      <c r="D29" s="12">
         <v>43531</v>
       </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A30" s="22" t="s">
+      <c r="A30" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B30" s="22" t="s">
+      <c r="B30" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="C30" s="22">
+      <c r="C30" s="11">
         <v>68</v>
       </c>
-      <c r="D30" s="23">
+      <c r="D30" s="12">
         <v>43532</v>
       </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A31" s="22" t="s">
+      <c r="A31" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B31" s="22" t="s">
+      <c r="B31" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="C31" s="22">
+      <c r="C31" s="11">
         <v>129</v>
       </c>
-      <c r="D31" s="23">
+      <c r="D31" s="12">
         <v>43533</v>
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A32" s="22" t="s">
+      <c r="A32" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B32" s="22" t="s">
+      <c r="B32" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="C32" s="22">
+      <c r="C32" s="11">
         <v>95</v>
       </c>
-      <c r="D32" s="23">
+      <c r="D32" s="12">
         <v>43534</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A33" s="22" t="s">
+      <c r="A33" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B33" s="22" t="s">
+      <c r="B33" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="C33" s="22">
+      <c r="C33" s="11">
         <v>74</v>
       </c>
-      <c r="D33" s="23">
+      <c r="D33" s="12">
         <v>43546</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A34" s="22" t="s">
+      <c r="A34" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B34" s="22" t="s">
-        <v>24</v>
-      </c>
-      <c r="C34" s="22">
+      <c r="B34" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C34" s="11">
         <v>52</v>
       </c>
-      <c r="D34" s="23">
+      <c r="D34" s="12">
         <v>43546</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A35" s="22" t="s">
+      <c r="A35" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="B35" s="22" t="s">
+      <c r="B35" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="C35" s="22">
+      <c r="C35" s="11">
         <v>196</v>
       </c>
-      <c r="D35" s="23">
+      <c r="D35" s="12">
         <v>43376</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A36" s="22" t="s">
+      <c r="A36" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="B36" s="22" t="s">
+      <c r="B36" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="C36" s="22">
+      <c r="C36" s="11">
         <v>115</v>
       </c>
-      <c r="D36" s="23">
+      <c r="D36" s="12">
         <v>43407</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A37" s="22" t="s">
+      <c r="A37" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B37" s="22" t="s">
-        <v>24</v>
-      </c>
-      <c r="C37" s="22">
+      <c r="B37" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C37" s="11">
         <v>10</v>
       </c>
-      <c r="D37" s="23">
+      <c r="D37" s="12">
         <v>43546</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A38" s="22" t="s">
+      <c r="A38" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B38" s="22" t="s">
-        <v>24</v>
-      </c>
-      <c r="C38" s="22">
+      <c r="B38" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C38" s="11">
         <v>60</v>
       </c>
-      <c r="D38" s="23">
+      <c r="D38" s="12">
         <v>43553</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A39" s="22" t="s">
+      <c r="A39" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B39" s="22" t="s">
-        <v>24</v>
-      </c>
-      <c r="C39" s="22">
+      <c r="B39" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C39" s="11">
         <v>60</v>
       </c>
-      <c r="D39" s="23">
+      <c r="D39" s="12">
         <v>43553</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A40" s="22" t="s">
+      <c r="A40" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="B40" s="22" t="s">
-        <v>24</v>
-      </c>
-      <c r="C40" s="22">
+      <c r="B40" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C40" s="11">
         <v>60</v>
       </c>
-      <c r="D40" s="23">
+      <c r="D40" s="12">
         <v>43553</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A41" s="22" t="s">
+      <c r="A41" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B41" s="22" t="s">
+      <c r="B41" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="C41" s="22">
+      <c r="C41" s="11">
         <v>60</v>
       </c>
-      <c r="D41" s="23">
+      <c r="D41" s="12">
         <v>43481</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A42" s="22" t="s">
+      <c r="A42" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B42" s="22" t="s">
+      <c r="B42" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="C42" s="22">
+      <c r="C42" s="11">
         <v>150</v>
       </c>
-      <c r="D42" s="23">
+      <c r="D42" s="12">
         <v>43442</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A43" s="22" t="s">
+      <c r="A43" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B43" s="22" t="s">
+      <c r="B43" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="C43" s="22">
+      <c r="C43" s="11">
         <v>180</v>
       </c>
-      <c r="D43" s="23">
+      <c r="D43" s="12">
         <v>43448</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A44" s="22" t="s">
+      <c r="A44" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B44" s="22" t="s">
+      <c r="B44" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="C44" s="22">
+      <c r="C44" s="11">
         <v>180</v>
       </c>
-      <c r="D44" s="23">
+      <c r="D44" s="12">
         <v>43468</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A45" s="22" t="s">
+      <c r="A45" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B45" s="22" t="s">
-        <v>24</v>
-      </c>
-      <c r="C45" s="22">
+      <c r="B45" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C45" s="11">
         <v>120</v>
       </c>
-      <c r="D45" s="23">
+      <c r="D45" s="12">
         <v>43478</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A46" s="22" t="s">
+      <c r="A46" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B46" s="22" t="s">
-        <v>24</v>
-      </c>
-      <c r="C46" s="22">
+      <c r="B46" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C46" s="11">
         <v>300</v>
       </c>
-      <c r="D46" s="23">
+      <c r="D46" s="12">
         <v>43449</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A47" s="22" t="s">
+      <c r="A47" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B47" s="22" t="s">
+      <c r="B47" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="C47" s="22">
+      <c r="C47" s="11">
         <v>150</v>
       </c>
-      <c r="D47" s="23">
+      <c r="D47" s="12">
         <v>43450</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A48" s="22" t="s">
+      <c r="A48" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B48" s="22" t="s">
-        <v>24</v>
-      </c>
-      <c r="C48" s="22">
+      <c r="B48" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C48" s="11">
         <v>82</v>
       </c>
-      <c r="D48" s="23">
+      <c r="D48" s="12">
         <v>43558</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A49" s="22" t="s">
+      <c r="A49" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B49" s="22" t="s">
-        <v>24</v>
-      </c>
-      <c r="C49" s="22">
+      <c r="B49" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C49" s="11">
         <v>82</v>
       </c>
-      <c r="D49" s="23">
+      <c r="D49" s="12">
         <v>43558</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A50" s="22" t="s">
+      <c r="A50" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B50" s="22" t="s">
-        <v>24</v>
-      </c>
-      <c r="C50" s="22">
+      <c r="B50" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C50" s="11">
         <v>82</v>
       </c>
-      <c r="D50" s="23">
+      <c r="D50" s="12">
         <v>43558</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A51" s="22" t="s">
+      <c r="A51" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B51" s="22" t="s">
+      <c r="B51" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="C51" s="22">
+      <c r="C51" s="11">
         <v>85</v>
       </c>
-      <c r="D51" s="24">
+      <c r="D51" s="13">
         <v>43559</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A52" s="22" t="s">
+      <c r="A52" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B52" s="22" t="s">
-        <v>24</v>
-      </c>
-      <c r="C52" s="22">
+      <c r="B52" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C52" s="11">
         <v>70</v>
       </c>
-      <c r="D52" s="23">
+      <c r="D52" s="12">
         <v>43571</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A53" s="22" t="s">
+      <c r="A53" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B53" s="22" t="s">
-        <v>24</v>
-      </c>
-      <c r="C53" s="22">
+      <c r="B53" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C53" s="11">
         <v>70</v>
       </c>
-      <c r="D53" s="23">
+      <c r="D53" s="12">
         <v>43571</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A54" s="22" t="s">
+      <c r="A54" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B54" s="22" t="s">
-        <v>24</v>
-      </c>
-      <c r="C54" s="22">
+      <c r="B54" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C54" s="11">
         <v>120</v>
       </c>
-      <c r="D54" s="23">
+      <c r="D54" s="12">
         <v>43572</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A55" s="22" t="s">
+      <c r="A55" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B55" s="22" t="s">
-        <v>24</v>
-      </c>
-      <c r="C55" s="22">
+      <c r="B55" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C55" s="11">
         <v>100</v>
       </c>
-      <c r="D55" s="23">
+      <c r="D55" s="12">
         <v>43574</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A56" s="22" t="s">
+      <c r="A56" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B56" s="22" t="s">
+      <c r="B56" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="C56" s="22">
+      <c r="C56" s="11">
         <v>42</v>
       </c>
-      <c r="D56" s="23">
+      <c r="D56" s="12">
         <v>43577</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A57" s="22" t="s">
+      <c r="A57" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B57" s="22" t="s">
-        <v>24</v>
-      </c>
-      <c r="C57" s="22">
+      <c r="B57" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C57" s="11">
         <v>97</v>
       </c>
-      <c r="D57" s="23">
+      <c r="D57" s="12">
         <v>43578</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A58" s="22" t="s">
+      <c r="A58" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B58" s="22" t="s">
-        <v>24</v>
-      </c>
-      <c r="C58" s="22">
+      <c r="B58" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C58" s="11">
         <v>30</v>
       </c>
-      <c r="D58" s="23">
+      <c r="D58" s="12">
         <v>43578</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A59" s="22" t="s">
+      <c r="A59" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B59" s="22" t="s">
-        <v>24</v>
-      </c>
-      <c r="C59" s="22">
+      <c r="B59" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C59" s="11">
         <v>107</v>
       </c>
-      <c r="D59" s="23">
+      <c r="D59" s="12">
         <v>43581</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A60" s="22"/>
-      <c r="B60" s="22"/>
-      <c r="C60" s="22"/>
-      <c r="D60" s="23"/>
+      <c r="A60" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B60" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C60" s="11">
+        <v>39</v>
+      </c>
+      <c r="D60" s="12">
+        <v>43584</v>
+      </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A61" s="22"/>
-      <c r="B61" s="22"/>
-      <c r="C61" s="22"/>
-      <c r="D61" s="23"/>
+      <c r="A61" s="11"/>
+      <c r="B61" s="11"/>
+      <c r="C61" s="11"/>
+      <c r="D61" s="12"/>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A62" s="22"/>
-      <c r="B62" s="22"/>
-      <c r="C62" s="22"/>
-      <c r="D62" s="23"/>
+      <c r="A62" s="11"/>
+      <c r="B62" s="11"/>
+      <c r="C62" s="11"/>
+      <c r="D62" s="12"/>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A63" s="22"/>
-      <c r="B63" s="22"/>
-      <c r="C63" s="22"/>
-      <c r="D63" s="23"/>
+      <c r="A63" s="11"/>
+      <c r="B63" s="11"/>
+      <c r="C63" s="11"/>
+      <c r="D63" s="12"/>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A64" s="22"/>
-      <c r="B64" s="22"/>
-      <c r="C64" s="22"/>
-      <c r="D64" s="23"/>
+      <c r="A64" s="11"/>
+      <c r="B64" s="11"/>
+      <c r="C64" s="11"/>
+      <c r="D64" s="12"/>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A65" s="22"/>
-      <c r="B65" s="22"/>
-      <c r="C65" s="22"/>
-      <c r="D65" s="23"/>
+      <c r="A65" s="11"/>
+      <c r="B65" s="11"/>
+      <c r="C65" s="11"/>
+      <c r="D65" s="12"/>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A66" s="22"/>
-      <c r="B66" s="22"/>
-      <c r="C66" s="22"/>
-      <c r="D66" s="23"/>
+      <c r="A66" s="11"/>
+      <c r="B66" s="11"/>
+      <c r="C66" s="11"/>
+      <c r="D66" s="12"/>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A67" s="22"/>
-      <c r="B67" s="22"/>
-      <c r="C67" s="22"/>
-      <c r="D67" s="23"/>
+      <c r="A67" s="11"/>
+      <c r="B67" s="11"/>
+      <c r="C67" s="11"/>
+      <c r="D67" s="12"/>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A68" s="22"/>
-      <c r="B68" s="22"/>
-      <c r="C68" s="22"/>
-      <c r="D68" s="23"/>
+      <c r="A68" s="11"/>
+      <c r="B68" s="11"/>
+      <c r="C68" s="11"/>
+      <c r="D68" s="12"/>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A69" s="22"/>
-      <c r="B69" s="22"/>
-      <c r="C69" s="22"/>
-      <c r="D69" s="23"/>
+      <c r="A69" s="11"/>
+      <c r="B69" s="11"/>
+      <c r="C69" s="11"/>
+      <c r="D69" s="12"/>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A70" s="22"/>
-      <c r="B70" s="22"/>
-      <c r="C70" s="22"/>
-      <c r="D70" s="23"/>
+      <c r="A70" s="11"/>
+      <c r="B70" s="11"/>
+      <c r="C70" s="11"/>
+      <c r="D70" s="12"/>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A71" s="22"/>
-      <c r="B71" s="22"/>
-      <c r="C71" s="22"/>
-      <c r="D71" s="23"/>
+      <c r="A71" s="11"/>
+      <c r="B71" s="11"/>
+      <c r="C71" s="11"/>
+      <c r="D71" s="12"/>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A72" s="22"/>
-      <c r="B72" s="22"/>
-      <c r="C72" s="22"/>
-      <c r="D72" s="23"/>
+      <c r="A72" s="11"/>
+      <c r="B72" s="11"/>
+      <c r="C72" s="11"/>
+      <c r="D72" s="12"/>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A73" s="22"/>
-      <c r="B73" s="22"/>
-      <c r="C73" s="22"/>
-      <c r="D73" s="23"/>
+      <c r="A73" s="11"/>
+      <c r="B73" s="11"/>
+      <c r="C73" s="11"/>
+      <c r="D73" s="12"/>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A74" s="22"/>
-      <c r="B74" s="22"/>
-      <c r="C74" s="22"/>
-      <c r="D74" s="23"/>
+      <c r="A74" s="11"/>
+      <c r="B74" s="11"/>
+      <c r="C74" s="11"/>
+      <c r="D74" s="12"/>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A75" s="22"/>
-      <c r="B75" s="22"/>
-      <c r="C75" s="22"/>
-      <c r="D75" s="23"/>
+      <c r="A75" s="11"/>
+      <c r="B75" s="11"/>
+      <c r="C75" s="11"/>
+      <c r="D75" s="12"/>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A76" s="22"/>
-      <c r="B76" s="22"/>
-      <c r="C76" s="22"/>
-      <c r="D76" s="23"/>
+      <c r="A76" s="11"/>
+      <c r="B76" s="11"/>
+      <c r="C76" s="11"/>
+      <c r="D76" s="12"/>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A77" s="22"/>
-      <c r="B77" s="22"/>
-      <c r="C77" s="22"/>
-      <c r="D77" s="23"/>
+      <c r="A77" s="11"/>
+      <c r="B77" s="11"/>
+      <c r="C77" s="11"/>
+      <c r="D77" s="12"/>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A78" s="22"/>
-      <c r="B78" s="22"/>
-      <c r="C78" s="22"/>
-      <c r="D78" s="23"/>
+      <c r="A78" s="11"/>
+      <c r="B78" s="11"/>
+      <c r="C78" s="11"/>
+      <c r="D78" s="12"/>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D79" s="2"/>
@@ -1887,6 +1937,10 @@
       <c r="D112" s="2"/>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="H4:J4"/>
+    <mergeCell ref="H15:O15"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Documenti di progetto - i 2 verbali esterni
</commit_message>
<xml_diff>
--- a/Documentazione/Attività sul progetto/DocAttivProg.xlsx
+++ b/Documentazione/Attività sul progetto/DocAttivProg.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="27">
   <si>
     <t>PERSONA</t>
   </si>
@@ -628,10 +628,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O113"/>
+  <dimension ref="A1:O115"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A56" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E72" sqref="E72"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -733,7 +733,7 @@
         <v>20</v>
       </c>
       <c r="I6" s="23">
-        <f>SUMIF(B4:B59,"Ispezione codice",C4:C59)</f>
+        <f>SUMIF(B4:B61,"Ispezione codice",C4:C61)</f>
         <v>0</v>
       </c>
       <c r="J6" s="24">
@@ -759,11 +759,11 @@
       </c>
       <c r="I7" s="23">
         <f>SUMIF(B:B,"Documenti di progetto",C:C)</f>
-        <v>1371</v>
+        <v>1501</v>
       </c>
       <c r="J7" s="25">
         <f>(I7/I12)*100</f>
-        <v>26.07455306200076</v>
+        <v>27.858203414996286</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
@@ -788,7 +788,7 @@
       </c>
       <c r="J8" s="25">
         <f>(I8/I12)*100</f>
-        <v>39.311525294788893</v>
+        <v>38.363028953229403</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
@@ -813,7 +813,7 @@
       </c>
       <c r="J9" s="25">
         <f>(I9/I12)*100</f>
-        <v>3.3092430581970333</v>
+        <v>3.229398663697105</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
@@ -838,21 +838,21 @@
       </c>
       <c r="J10" s="25">
         <f>(I10/I12)*100</f>
-        <v>31.304678585013313</v>
+        <v>30.549368968077207</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="C11" s="10">
-        <v>127</v>
+        <v>75</v>
       </c>
       <c r="D11" s="11">
-        <v>43505</v>
+        <v>43497</v>
       </c>
       <c r="H11" s="26" t="s">
         <v>11</v>
@@ -868,23 +868,23 @@
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C12" s="10">
-        <v>24</v>
+        <v>55</v>
       </c>
       <c r="D12" s="11">
-        <v>43509</v>
+        <v>43503</v>
       </c>
       <c r="H12" s="15" t="s">
         <v>16</v>
       </c>
       <c r="I12" s="16">
         <f>SUM(I6:I11)</f>
-        <v>5258</v>
+        <v>5388</v>
       </c>
       <c r="J12" s="17">
         <f>SUM(J6:J11)</f>
@@ -893,16 +893,16 @@
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="C13" s="10">
-        <v>195</v>
+        <v>127</v>
       </c>
       <c r="D13" s="11">
-        <v>43521</v>
+        <v>43505</v>
       </c>
       <c r="H13" s="7"/>
       <c r="I13" s="8"/>
@@ -910,30 +910,30 @@
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="10" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B14" s="10" t="s">
         <v>24</v>
       </c>
       <c r="C14" s="10">
-        <v>105</v>
+        <v>24</v>
       </c>
       <c r="D14" s="11">
-        <v>43523</v>
+        <v>43509</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="10" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>5</v>
+        <v>24</v>
       </c>
       <c r="C15" s="10">
-        <v>30</v>
+        <v>195</v>
       </c>
       <c r="D15" s="11">
-        <v>43519</v>
+        <v>43521</v>
       </c>
       <c r="H15" s="30" t="s">
         <v>15</v>
@@ -948,16 +948,16 @@
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="10" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="C16" s="10">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="D16" s="11">
-        <v>43520</v>
+        <v>43523</v>
       </c>
       <c r="H16" s="5" t="s">
         <v>14</v>
@@ -989,13 +989,13 @@
         <v>7</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C17" s="10">
-        <v>125</v>
+        <v>30</v>
       </c>
       <c r="D17" s="11">
-        <v>43522</v>
+        <v>43519</v>
       </c>
       <c r="H17" s="6" t="s">
         <v>4</v>
@@ -1037,10 +1037,10 @@
         <v>10</v>
       </c>
       <c r="C18" s="10">
-        <v>170</v>
+        <v>100</v>
       </c>
       <c r="D18" s="11">
-        <v>43523</v>
+        <v>43520</v>
       </c>
       <c r="H18" s="6" t="s">
         <v>7</v>
@@ -1082,10 +1082,10 @@
         <v>10</v>
       </c>
       <c r="C19" s="10">
-        <v>65</v>
+        <v>125</v>
       </c>
       <c r="D19" s="11">
-        <v>43524</v>
+        <v>43522</v>
       </c>
       <c r="H19" s="6" t="s">
         <v>6</v>
@@ -1121,23 +1121,23 @@
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C20" s="10">
-        <v>60</v>
+        <v>170</v>
       </c>
       <c r="D20" s="11">
-        <v>43487</v>
+        <v>43523</v>
       </c>
       <c r="H20" s="6" t="s">
         <v>8</v>
       </c>
       <c r="I20" s="3">
         <f>SUMIFS(C:C,B:B,"Documenti di progetto",A:A,"Viktorija")</f>
-        <v>25</v>
+        <v>155</v>
       </c>
       <c r="J20" s="3">
         <f>SUMIFS(C:C,B:B,"Documenti di processo",A:A,"Viktorija")</f>
@@ -1161,21 +1161,21 @@
       </c>
       <c r="O20" s="19">
         <f>SUM(I20:M20)</f>
-        <v>839</v>
+        <v>969</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B21" s="10" t="s">
         <v>10</v>
       </c>
       <c r="C21" s="10">
-        <v>103</v>
+        <v>65</v>
       </c>
       <c r="D21" s="11">
-        <v>43506</v>
+        <v>43524</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
@@ -1183,13 +1183,13 @@
         <v>8</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C22" s="10">
-        <v>100</v>
+        <v>60</v>
       </c>
       <c r="D22" s="11">
-        <v>43520</v>
+        <v>43487</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
@@ -1200,10 +1200,10 @@
         <v>10</v>
       </c>
       <c r="C23" s="10">
-        <v>170</v>
+        <v>103</v>
       </c>
       <c r="D23" s="11">
-        <v>43523</v>
+        <v>43506</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
@@ -1214,10 +1214,10 @@
         <v>10</v>
       </c>
       <c r="C24" s="10">
-        <v>45</v>
+        <v>100</v>
       </c>
       <c r="D24" s="11">
-        <v>43524</v>
+        <v>43520</v>
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
@@ -1228,46 +1228,46 @@
         <v>10</v>
       </c>
       <c r="C25" s="10">
-        <v>25</v>
+        <v>170</v>
       </c>
       <c r="D25" s="11">
-        <v>43530</v>
+        <v>43523</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" s="10" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="C26" s="10">
-        <v>15</v>
+        <v>45</v>
       </c>
       <c r="D26" s="11">
-        <v>43532</v>
+        <v>43524</v>
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" s="10" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B27" s="10" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C27" s="10">
-        <v>47</v>
+        <v>25</v>
       </c>
       <c r="D27" s="11">
-        <v>43532</v>
+        <v>43530</v>
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" s="10" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B28" s="10" t="s">
-        <v>5</v>
+        <v>23</v>
       </c>
       <c r="C28" s="10">
         <v>15</v>
@@ -1278,16 +1278,16 @@
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" s="10" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B29" s="10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C29" s="10">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="D29" s="11">
-        <v>43531</v>
+        <v>43532</v>
       </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
@@ -1295,10 +1295,10 @@
         <v>7</v>
       </c>
       <c r="B30" s="10" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C30" s="10">
-        <v>68</v>
+        <v>15</v>
       </c>
       <c r="D30" s="11">
         <v>43532</v>
@@ -1312,10 +1312,10 @@
         <v>10</v>
       </c>
       <c r="C31" s="10">
-        <v>129</v>
+        <v>55</v>
       </c>
       <c r="D31" s="11">
-        <v>43533</v>
+        <v>43531</v>
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
@@ -1326,94 +1326,94 @@
         <v>10</v>
       </c>
       <c r="C32" s="10">
-        <v>95</v>
+        <v>68</v>
       </c>
       <c r="D32" s="11">
-        <v>43534</v>
+        <v>43532</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="10" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B33" s="10" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="C33" s="10">
-        <v>74</v>
+        <v>129</v>
       </c>
       <c r="D33" s="11">
-        <v>43546</v>
+        <v>43533</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="10" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B34" s="10" t="s">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="C34" s="10">
-        <v>52</v>
+        <v>95</v>
       </c>
       <c r="D34" s="11">
-        <v>43546</v>
+        <v>43534</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="10" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B35" s="10" t="s">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="C35" s="10">
-        <v>196</v>
+        <v>74</v>
       </c>
       <c r="D35" s="11">
-        <v>43376</v>
+        <v>43546</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="10" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B36" s="10" t="s">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="C36" s="10">
-        <v>115</v>
+        <v>52</v>
       </c>
       <c r="D36" s="11">
-        <v>43407</v>
+        <v>43546</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="10" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B37" s="10" t="s">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="C37" s="10">
-        <v>10</v>
+        <v>196</v>
       </c>
       <c r="D37" s="11">
-        <v>43546</v>
+        <v>43376</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="10" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B38" s="10" t="s">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="C38" s="10">
-        <v>60</v>
+        <v>115</v>
       </c>
       <c r="D38" s="11">
-        <v>43553</v>
+        <v>43407</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -1424,15 +1424,15 @@
         <v>24</v>
       </c>
       <c r="C39" s="10">
-        <v>60</v>
+        <v>10</v>
       </c>
       <c r="D39" s="11">
-        <v>43553</v>
+        <v>43546</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="10" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B40" s="10" t="s">
         <v>24</v>
@@ -1446,30 +1446,30 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="10" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B41" s="10" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C41" s="10">
         <v>60</v>
       </c>
       <c r="D41" s="11">
-        <v>43481</v>
+        <v>43553</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="10" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B42" s="10" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C42" s="10">
-        <v>150</v>
+        <v>60</v>
       </c>
       <c r="D42" s="11">
-        <v>43442</v>
+        <v>43553</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -1480,10 +1480,10 @@
         <v>23</v>
       </c>
       <c r="C43" s="10">
-        <v>180</v>
+        <v>60</v>
       </c>
       <c r="D43" s="11">
-        <v>43448</v>
+        <v>43481</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -1494,10 +1494,10 @@
         <v>23</v>
       </c>
       <c r="C44" s="10">
-        <v>180</v>
+        <v>150</v>
       </c>
       <c r="D44" s="11">
-        <v>43468</v>
+        <v>43442</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -1505,74 +1505,74 @@
         <v>6</v>
       </c>
       <c r="B45" s="10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C45" s="10">
-        <v>120</v>
+        <v>180</v>
       </c>
       <c r="D45" s="11">
-        <v>43478</v>
+        <v>43448</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="10" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B46" s="10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C46" s="10">
-        <v>300</v>
+        <v>180</v>
       </c>
       <c r="D46" s="11">
-        <v>43449</v>
+        <v>43468</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="10" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B47" s="10" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C47" s="10">
-        <v>150</v>
+        <v>120</v>
       </c>
       <c r="D47" s="11">
-        <v>43450</v>
+        <v>43478</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="10" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B48" s="10" t="s">
         <v>24</v>
       </c>
       <c r="C48" s="10">
-        <v>82</v>
+        <v>300</v>
       </c>
       <c r="D48" s="11">
-        <v>43558</v>
+        <v>43449</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="10" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B49" s="10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C49" s="10">
-        <v>82</v>
+        <v>150</v>
       </c>
       <c r="D49" s="11">
-        <v>43558</v>
+        <v>43450</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="10" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B50" s="10" t="s">
         <v>24</v>
@@ -1589,27 +1589,27 @@
         <v>7</v>
       </c>
       <c r="B51" s="10" t="s">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="C51" s="10">
-        <v>85</v>
-      </c>
-      <c r="D51" s="12">
-        <v>43559</v>
+        <v>82</v>
+      </c>
+      <c r="D51" s="11">
+        <v>43558</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="10" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B52" s="10" t="s">
         <v>24</v>
       </c>
       <c r="C52" s="10">
-        <v>70</v>
+        <v>82</v>
       </c>
       <c r="D52" s="11">
-        <v>43571</v>
+        <v>43558</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
@@ -1617,13 +1617,13 @@
         <v>7</v>
       </c>
       <c r="B53" s="10" t="s">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="C53" s="10">
-        <v>70</v>
-      </c>
-      <c r="D53" s="11">
-        <v>43571</v>
+        <v>85</v>
+      </c>
+      <c r="D53" s="12">
+        <v>43559</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
@@ -1634,66 +1634,66 @@
         <v>24</v>
       </c>
       <c r="C54" s="10">
-        <v>120</v>
+        <v>70</v>
       </c>
       <c r="D54" s="11">
-        <v>43572</v>
+        <v>43571</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="10" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B55" s="10" t="s">
         <v>24</v>
       </c>
       <c r="C55" s="10">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="D55" s="11">
-        <v>43574</v>
+        <v>43571</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="10" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B56" s="10" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C56" s="10">
-        <v>42</v>
+        <v>120</v>
       </c>
       <c r="D56" s="11">
-        <v>43577</v>
+        <v>43572</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="10" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B57" s="10" t="s">
         <v>24</v>
       </c>
       <c r="C57" s="10">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="D57" s="11">
-        <v>43578</v>
+        <v>43574</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="10" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B58" s="10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C58" s="10">
-        <v>30</v>
+        <v>42</v>
       </c>
       <c r="D58" s="11">
-        <v>43578</v>
+        <v>43577</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
@@ -1704,24 +1704,24 @@
         <v>24</v>
       </c>
       <c r="C59" s="10">
-        <v>107</v>
+        <v>97</v>
       </c>
       <c r="D59" s="11">
-        <v>43581</v>
+        <v>43578</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="10" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B60" s="10" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C60" s="10">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="D60" s="11">
-        <v>43584</v>
+        <v>43578</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
@@ -1729,68 +1729,84 @@
         <v>4</v>
       </c>
       <c r="B61" s="10" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C61" s="10">
-        <v>22</v>
+        <v>107</v>
       </c>
       <c r="D61" s="11">
-        <v>43585</v>
+        <v>43581</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="10" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B62" s="10" t="s">
         <v>23</v>
       </c>
       <c r="C62" s="10">
-        <v>22</v>
+        <v>39</v>
       </c>
       <c r="D62" s="11">
-        <v>43585</v>
+        <v>43584</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="10" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B63" s="10" t="s">
         <v>23</v>
       </c>
       <c r="C63" s="10">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D63" s="11">
-        <v>43587</v>
+        <v>43585</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="10" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B64" s="10" t="s">
         <v>23</v>
       </c>
       <c r="C64" s="10">
+        <v>22</v>
+      </c>
+      <c r="D64" s="11">
+        <v>43585</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B65" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C65" s="10">
         <v>25</v>
       </c>
-      <c r="D64" s="11">
+      <c r="D65" s="11">
         <v>43587</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" s="10"/>
-      <c r="B65" s="10"/>
-      <c r="C65" s="10"/>
-      <c r="D65" s="11"/>
-    </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="10"/>
-      <c r="B66" s="10"/>
-      <c r="C66" s="10"/>
-      <c r="D66" s="11"/>
+      <c r="A66" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B66" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C66" s="10">
+        <v>25</v>
+      </c>
+      <c r="D66" s="11">
+        <v>43587</v>
+      </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="10"/>
@@ -2072,7 +2088,19 @@
       <c r="A113" s="10"/>
       <c r="B113" s="10"/>
       <c r="C113" s="10"/>
-      <c r="D113" s="10"/>
+      <c r="D113" s="11"/>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A114" s="10"/>
+      <c r="B114" s="10"/>
+      <c r="C114" s="10"/>
+      <c r="D114" s="11"/>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A115" s="10"/>
+      <c r="B115" s="10"/>
+      <c r="C115" s="10"/>
+      <c r="D115" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Update Attivita' del 08/05
</commit_message>
<xml_diff>
--- a/Documentazione/Attività sul progetto/DocAttivProg.xlsx
+++ b/Documentazione/Attività sul progetto/DocAttivProg.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="27">
   <si>
     <t>PERSONA</t>
   </si>
@@ -630,8 +630,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O115"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F75" sqref="F75"/>
+    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D81" sqref="D81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -759,11 +759,11 @@
       </c>
       <c r="I7" s="23">
         <f>SUMIF(B:B,"Documenti di progetto",C:C)</f>
-        <v>1536</v>
+        <v>1716</v>
       </c>
       <c r="J7" s="25">
         <f>(I7/I12)*100</f>
-        <v>25.325638911788957</v>
+        <v>26.708171206225678</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
@@ -788,7 +788,7 @@
       </c>
       <c r="J8" s="25">
         <f>(I8/I12)*100</f>
-        <v>34.080791426215995</v>
+        <v>32.171206225680933</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
@@ -813,7 +813,7 @@
       </c>
       <c r="J9" s="25">
         <f>(I9/I12)*100</f>
-        <v>2.8689200329760927</v>
+        <v>2.7081712062256806</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
@@ -834,11 +834,11 @@
       </c>
       <c r="I10" s="23">
         <f>SUMIF(B:B,"Sviluppo",C:C)</f>
-        <v>2288</v>
+        <v>2468</v>
       </c>
       <c r="J10" s="25">
         <f>(I10/I12)*100</f>
-        <v>37.724649629018963</v>
+        <v>38.412451361867703</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
@@ -884,7 +884,7 @@
       </c>
       <c r="I12" s="16">
         <f>SUM(I6:I11)</f>
-        <v>6065</v>
+        <v>6425</v>
       </c>
       <c r="J12" s="17">
         <f>SUM(J6:J11)</f>
@@ -1002,7 +1002,7 @@
       </c>
       <c r="I17" s="3">
         <f>SUMIFS(C:C,B:B,"Documenti di progetto",A:A,"Giovanni")</f>
-        <v>714</v>
+        <v>759</v>
       </c>
       <c r="J17" s="3">
         <f>SUMIFS(C:C,B:B,"Documenti di processo",A:A,"Giovanni")</f>
@@ -1026,7 +1026,7 @@
       </c>
       <c r="O17" s="19">
         <f>SUM(I17:M17)</f>
-        <v>1791</v>
+        <v>1836</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
@@ -1047,7 +1047,7 @@
       </c>
       <c r="I18" s="3">
         <f>SUMIFS(C:C,B:B,"Documenti di progetto",A:A,"Hristina")</f>
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="J18" s="3">
         <f>SUMIFS(C:C,B:B,"Documenti di processo",A:A,"Hristina")</f>
@@ -1059,7 +1059,7 @@
       </c>
       <c r="L18" s="3">
         <f>SUMIFS(C:C,B:B,"Sviluppo",A:A,"Hristina")</f>
-        <v>1145</v>
+        <v>1205</v>
       </c>
       <c r="M18" s="3">
         <f>SUMIFS(C:C,B:B,"Testing",A:A,"Hristina")</f>
@@ -1071,7 +1071,7 @@
       </c>
       <c r="O18" s="19">
         <f>SUM(I18:M18)</f>
-        <v>1397</v>
+        <v>1502</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
@@ -1092,7 +1092,7 @@
       </c>
       <c r="I19" s="3">
         <f>SUMIFS(C:C,B:B,"Documenti di progetto",A:A,"Luca")</f>
-        <v>632</v>
+        <v>677</v>
       </c>
       <c r="J19" s="3">
         <f>SUMIFS(C:C,B:B,"Documenti di processo",A:A,"Luca")</f>
@@ -1104,7 +1104,7 @@
       </c>
       <c r="L19" s="3">
         <f>SUMIFS(C:C,B:B,"Sviluppo",A:A,"Luca")</f>
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="M19" s="3">
         <f>SUMIFS(C:C,B:B,"Testing",A:A,"Luca")</f>
@@ -1116,7 +1116,7 @@
       </c>
       <c r="O19" s="19">
         <f>SUM(I19:M19)</f>
-        <v>1484</v>
+        <v>1589</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
@@ -1137,7 +1137,7 @@
       </c>
       <c r="I20" s="3">
         <f>SUMIFS(C:C,B:B,"Documenti di progetto",A:A,"Viktorija")</f>
-        <v>190</v>
+        <v>235</v>
       </c>
       <c r="J20" s="3">
         <f>SUMIFS(C:C,B:B,"Documenti di processo",A:A,"Viktorija")</f>
@@ -1149,7 +1149,7 @@
       </c>
       <c r="L20" s="3">
         <f>SUMIFS(C:C,B:B,"Sviluppo",A:A,"Viktorija")</f>
-        <v>1143</v>
+        <v>1203</v>
       </c>
       <c r="M20" s="3">
         <f>SUMIFS(C:C,B:B,"Testing",A:A,"Viktorija")</f>
@@ -1161,7 +1161,7 @@
       </c>
       <c r="O20" s="19">
         <f>SUM(I20:M20)</f>
-        <v>1393</v>
+        <v>1498</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
@@ -1921,46 +1921,102 @@
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" s="10"/>
-      <c r="B75" s="10"/>
-      <c r="C75" s="10"/>
-      <c r="D75" s="11"/>
+      <c r="A75" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B75" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C75" s="10">
+        <v>45</v>
+      </c>
+      <c r="D75" s="11">
+        <v>43593</v>
+      </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" s="10"/>
-      <c r="B76" s="10"/>
-      <c r="C76" s="10"/>
-      <c r="D76" s="11"/>
+      <c r="A76" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B76" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C76" s="10">
+        <v>45</v>
+      </c>
+      <c r="D76" s="11">
+        <v>43593</v>
+      </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" s="10"/>
-      <c r="B77" s="10"/>
-      <c r="C77" s="10"/>
-      <c r="D77" s="11"/>
+      <c r="A77" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B77" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C77" s="10">
+        <v>45</v>
+      </c>
+      <c r="D77" s="11">
+        <v>43593</v>
+      </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" s="10"/>
-      <c r="B78" s="10"/>
-      <c r="C78" s="10"/>
-      <c r="D78" s="11"/>
+      <c r="A78" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B78" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C78" s="10">
+        <v>45</v>
+      </c>
+      <c r="D78" s="11">
+        <v>43593</v>
+      </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" s="10"/>
-      <c r="B79" s="10"/>
-      <c r="C79" s="10"/>
-      <c r="D79" s="11"/>
+      <c r="A79" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B79" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C79" s="10">
+        <v>60</v>
+      </c>
+      <c r="D79" s="11">
+        <v>43593</v>
+      </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" s="10"/>
-      <c r="B80" s="10"/>
-      <c r="C80" s="10"/>
-      <c r="D80" s="11"/>
+      <c r="A80" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B80" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C80" s="10">
+        <v>60</v>
+      </c>
+      <c r="D80" s="11">
+        <v>43593</v>
+      </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A81" s="10"/>
-      <c r="B81" s="10"/>
-      <c r="C81" s="10"/>
-      <c r="D81" s="11"/>
+      <c r="A81" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B81" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C81" s="10">
+        <v>60</v>
+      </c>
+      <c r="D81" s="11">
+        <v>43593</v>
+      </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="10"/>

</xml_diff>

<commit_message>
Nuova versione CM, cambio nomi cartelle Manuale e Proposta, nuove statistiche documento delle attività
</commit_message>
<xml_diff>
--- a/Documentazione/Attività sul progetto/DocAttivProg.xlsx
+++ b/Documentazione/Attività sul progetto/DocAttivProg.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vik\Documents\GitHub\Progetto\Documentazione\Attività sul progetto\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\UniUD\Laurea Magistrale\Ingegneria del Software 2\Progetto-Ingegneria-Del-Sw-2\Documentazione\Attività sul progetto\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C6818F6-8B26-48EB-BBFC-91F88FADC684}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" tabRatio="500"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511" iterateDelta="1E-4"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="29">
   <si>
     <t>PERSONA</t>
   </si>
@@ -71,15 +72,9 @@
     <t>Attività</t>
   </si>
   <si>
-    <t>Minuti di lavoro per attività</t>
-  </si>
-  <si>
     <t>Persona</t>
   </si>
   <si>
-    <t>Attività per persona (minuti)</t>
-  </si>
-  <si>
     <t>Totale</t>
   </si>
   <si>
@@ -111,15 +106,26 @@
   </si>
   <si>
     <t>Le categorie sono: Ispezione Codice, Documenti di progetto, Documenti di processo, Manuale, Sviluppo, Testing</t>
+  </si>
+  <si>
+    <t>Media</t>
+  </si>
+  <si>
+    <t>Tempo/persona (minuti) per attività e relativa media</t>
+  </si>
+  <si>
+    <t>Percentuale tempo/persona per attività e relativa media</t>
+  </si>
+  <si>
+    <t>Minuti di lavoro per attività e relativa percentuale</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="m/d/yyyy"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="m/d/yyyy"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -168,7 +174,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -187,8 +193,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -238,13 +250,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -265,7 +287,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -276,9 +298,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -293,30 +312,70 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="4" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="4" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="3">
-    <cellStyle name="Migliaia" xfId="1" builtinId="3"/>
+  <cellStyles count="2">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
-    <cellStyle name="Percentuale" xfId="2" builtinId="5"/>
+    <cellStyle name="Percentuale" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -627,39 +686,39 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O115"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A65" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B83" sqref="B83"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Q71" sqref="Q71"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.5703125" customWidth="1"/>
-    <col min="2" max="2" width="23.42578125" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" customWidth="1"/>
-    <col min="4" max="4" width="10.85546875" customWidth="1"/>
-    <col min="5" max="7" width="8.7109375" customWidth="1"/>
-    <col min="8" max="8" width="26.28515625" customWidth="1"/>
-    <col min="9" max="11" width="17.28515625" customWidth="1"/>
-    <col min="12" max="14" width="17.42578125" customWidth="1"/>
-    <col min="15" max="1025" width="8.7109375" customWidth="1"/>
+    <col min="1" max="1" width="15.5546875" customWidth="1"/>
+    <col min="2" max="2" width="23.44140625" customWidth="1"/>
+    <col min="3" max="3" width="15.5546875" customWidth="1"/>
+    <col min="4" max="4" width="10.88671875" customWidth="1"/>
+    <col min="5" max="7" width="8.6640625" customWidth="1"/>
+    <col min="8" max="8" width="26.33203125" customWidth="1"/>
+    <col min="9" max="11" width="17.33203125" customWidth="1"/>
+    <col min="12" max="14" width="17.44140625" customWidth="1"/>
+    <col min="15" max="1025" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="F1" s="13" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="F2" s="14" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
         <v>0</v>
       </c>
@@ -674,12 +733,12 @@
       </c>
       <c r="H3" s="2"/>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" s="10" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C4" s="10">
         <v>98</v>
@@ -687,18 +746,18 @@
       <c r="D4" s="11">
         <v>43484</v>
       </c>
-      <c r="H4" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="I4" s="29"/>
-      <c r="J4" s="29"/>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="H4" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="I4" s="25"/>
+      <c r="J4" s="25"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" s="10" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C5" s="10">
         <v>149</v>
@@ -706,22 +765,22 @@
       <c r="D5" s="11">
         <v>43493</v>
       </c>
-      <c r="H5" s="20" t="s">
+      <c r="H5" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="I5" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="J5" s="21" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="I5" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="J5" s="20" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" s="10" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C6" s="10">
         <v>135</v>
@@ -729,24 +788,24 @@
       <c r="D6" s="11">
         <v>43494</v>
       </c>
-      <c r="H6" s="22" t="s">
-        <v>20</v>
-      </c>
-      <c r="I6" s="23">
+      <c r="H6" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="I6" s="22">
         <f>SUMIF(B4:B61,"Ispezione codice",C4:C61)</f>
         <v>0</v>
       </c>
-      <c r="J6" s="24">
-        <f>(I6/I12)*100</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J6" s="42">
+        <f>I6/I12</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
         <v>4</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C7" s="10">
         <v>53</v>
@@ -754,24 +813,24 @@
       <c r="D7" s="11">
         <v>43494</v>
       </c>
-      <c r="H7" s="22" t="s">
-        <v>23</v>
-      </c>
-      <c r="I7" s="23">
+      <c r="H7" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="I7" s="22">
         <f>SUMIF(B:B,"Documenti di progetto",C:C)</f>
-        <v>1716</v>
-      </c>
-      <c r="J7" s="25">
-        <f>(I7/I12)*100</f>
-        <v>25.777377196935557</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+        <v>1747</v>
+      </c>
+      <c r="J7" s="42">
+        <f>(I7/I12)</f>
+        <v>0.25939123979213063</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" s="10" t="s">
         <v>4</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C8" s="10">
         <v>87</v>
@@ -779,24 +838,24 @@
       <c r="D8" s="11">
         <v>43495</v>
       </c>
-      <c r="H8" s="22" t="s">
-        <v>24</v>
-      </c>
-      <c r="I8" s="23">
+      <c r="H8" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="I8" s="22">
         <f>SUMIF(B:B,"Documenti di processo",C:C)</f>
-        <v>2067</v>
-      </c>
-      <c r="J8" s="25">
-        <f>(I8/I12)*100</f>
-        <v>31.050022532672372</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+        <v>2114</v>
+      </c>
+      <c r="J8" s="42">
+        <f>I8/I12</f>
+        <v>0.31388270230141052</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" s="10" t="s">
         <v>4</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C9" s="10">
         <v>74</v>
@@ -804,24 +863,24 @@
       <c r="D9" s="11">
         <v>43495</v>
       </c>
-      <c r="H9" s="22" t="s">
+      <c r="H9" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="I9" s="23">
+      <c r="I9" s="22">
         <f>SUMIF(B:B,"Manuale",C:C)</f>
         <v>174</v>
       </c>
-      <c r="J9" s="25">
-        <f>(I9/I12)*100</f>
-        <v>2.6137899954934656</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J9" s="42">
+        <f>I9/I12</f>
+        <v>2.5835189309576838E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" s="10" t="s">
         <v>4</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C10" s="10">
         <v>32</v>
@@ -829,24 +888,24 @@
       <c r="D10" s="11">
         <v>43499</v>
       </c>
-      <c r="H10" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="I10" s="23">
+      <c r="H10" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="I10" s="22">
         <f>SUMIF(B:B,"Sviluppo",C:C)</f>
         <v>2700</v>
       </c>
-      <c r="J10" s="25">
-        <f>(I10/I12)*100</f>
-        <v>40.558810274898605</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J10" s="42">
+        <f>I10/I12</f>
+        <v>0.40089086859688194</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" s="10" t="s">
         <v>8</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C11" s="10">
         <v>75</v>
@@ -854,24 +913,24 @@
       <c r="D11" s="11">
         <v>43497</v>
       </c>
-      <c r="H11" s="26" t="s">
+      <c r="H11" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="I11" s="27">
+      <c r="I11" s="24">
         <f>SUMIF(B:B,"Testing",C:C)</f>
         <v>0</v>
       </c>
-      <c r="J11" s="28">
-        <f>(I11/I12)*100</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J11" s="43">
+        <f>I11/I12</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
         <v>8</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C12" s="10">
         <v>55</v>
@@ -880,18 +939,18 @@
         <v>43503</v>
       </c>
       <c r="H12" s="15" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="I12" s="16">
         <f>SUM(I6:I11)</f>
-        <v>6657</v>
-      </c>
-      <c r="J12" s="17">
+        <v>6735</v>
+      </c>
+      <c r="J12" s="44">
         <f>SUM(J6:J11)</f>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+        <v>0.99999999999999989</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13" s="10" t="s">
         <v>4</v>
       </c>
@@ -908,12 +967,12 @@
       <c r="I13" s="8"/>
       <c r="J13" s="8"/>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14" s="10" t="s">
         <v>4</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C14" s="10">
         <v>24</v>
@@ -922,12 +981,12 @@
         <v>43509</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15" s="10" t="s">
         <v>6</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C15" s="10">
         <v>195</v>
@@ -935,23 +994,23 @@
       <c r="D15" s="11">
         <v>43521</v>
       </c>
-      <c r="H15" s="30" t="s">
-        <v>15</v>
-      </c>
-      <c r="I15" s="30"/>
-      <c r="J15" s="30"/>
-      <c r="K15" s="30"/>
-      <c r="L15" s="30"/>
-      <c r="M15" s="30"/>
-      <c r="N15" s="30"/>
-      <c r="O15" s="30"/>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="H15" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="I15" s="26"/>
+      <c r="J15" s="26"/>
+      <c r="K15" s="26"/>
+      <c r="L15" s="26"/>
+      <c r="M15" s="26"/>
+      <c r="N15" s="26"/>
+      <c r="O15" s="26"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A16" s="10" t="s">
         <v>6</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C16" s="10">
         <v>105</v>
@@ -960,13 +1019,13 @@
         <v>43523</v>
       </c>
       <c r="H16" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I16" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="J16" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="K16" s="4" t="s">
         <v>9</v>
@@ -978,13 +1037,13 @@
         <v>11</v>
       </c>
       <c r="N16" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="O16" s="18" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+      <c r="O16" s="17" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A17" s="10" t="s">
         <v>7</v>
       </c>
@@ -1002,11 +1061,11 @@
       </c>
       <c r="I17" s="3">
         <f>SUMIFS(C:C,B:B,"Documenti di progetto",A:A,"Giovanni")</f>
-        <v>759</v>
+        <v>790</v>
       </c>
       <c r="J17" s="3">
         <f>SUMIFS(C:C,B:B,"Documenti di processo",A:A,"Giovanni")</f>
-        <v>903</v>
+        <v>950</v>
       </c>
       <c r="K17" s="3">
         <f>SUMIFS(C:C,B:B,"Manuale",A:A,"Giovanni")</f>
@@ -1024,12 +1083,12 @@
         <f>SUMIFS(C:C,B:B,"Ispezione codice",A:A,"Giovanni")</f>
         <v>0</v>
       </c>
-      <c r="O17" s="19">
+      <c r="O17" s="18">
         <f>SUM(I17:M17)</f>
-        <v>1836</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+        <v>1914</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A18" s="10" t="s">
         <v>7</v>
       </c>
@@ -1069,12 +1128,12 @@
         <f>SUMIFS(C:C,B:B,"Ispezione codice",A:A,"Hristina")</f>
         <v>0</v>
       </c>
-      <c r="O18" s="19">
+      <c r="O18" s="18">
         <f>SUM(I18:M18)</f>
         <v>1618</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A19" s="10" t="s">
         <v>7</v>
       </c>
@@ -1114,12 +1173,12 @@
         <f>SUMIFS(C:C,B:B,"Ispezione codice",A:A,"Luca")</f>
         <v>0</v>
       </c>
-      <c r="O19" s="19">
+      <c r="O19" s="18">
         <f>SUM(I19:M19)</f>
         <v>1589</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A20" s="10" t="s">
         <v>7</v>
       </c>
@@ -1159,12 +1218,12 @@
         <f>SUMIFS(C:C,B:B,"Ispezione codice",A:A,"Viktorija")</f>
         <v>0</v>
       </c>
-      <c r="O20" s="19">
+      <c r="O20" s="18">
         <f>SUM(I20:M20)</f>
         <v>1614</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A21" s="10" t="s">
         <v>7</v>
       </c>
@@ -1177,8 +1236,36 @@
       <c r="D21" s="11">
         <v>43524</v>
       </c>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="H21" s="36" t="s">
+        <v>25</v>
+      </c>
+      <c r="I21" s="37">
+        <f>AVERAGE(I17:I20)</f>
+        <v>436.75</v>
+      </c>
+      <c r="J21" s="37">
+        <f>AVERAGE(J17:J20)</f>
+        <v>528.5</v>
+      </c>
+      <c r="K21" s="37">
+        <f>AVERAGE(K17:K20)</f>
+        <v>43.5</v>
+      </c>
+      <c r="L21" s="37">
+        <f>AVERAGE(L17:L20)</f>
+        <v>675</v>
+      </c>
+      <c r="M21" s="37">
+        <f>AVERAGE(M17:M20)</f>
+        <v>0</v>
+      </c>
+      <c r="N21" s="38">
+        <f>AVERAGE(N17:N20)</f>
+        <v>0</v>
+      </c>
+      <c r="O21" s="35"/>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A22" s="10" t="s">
         <v>8</v>
       </c>
@@ -1192,7 +1279,7 @@
         <v>43487</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A23" s="10" t="s">
         <v>8</v>
       </c>
@@ -1206,7 +1293,7 @@
         <v>43506</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A24" s="10" t="s">
         <v>8</v>
       </c>
@@ -1219,8 +1306,18 @@
       <c r="D24" s="11">
         <v>43520</v>
       </c>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="H24" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="I24" s="27"/>
+      <c r="J24" s="27"/>
+      <c r="K24" s="27"/>
+      <c r="L24" s="27"/>
+      <c r="M24" s="27"/>
+      <c r="N24" s="27"/>
+      <c r="O24" s="27"/>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A25" s="10" t="s">
         <v>8</v>
       </c>
@@ -1233,8 +1330,32 @@
       <c r="D25" s="11">
         <v>43523</v>
       </c>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="H25" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="I25" s="29" t="s">
+        <v>20</v>
+      </c>
+      <c r="J25" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="K25" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="L25" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="M25" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="N25" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="O25" s="30" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A26" s="10" t="s">
         <v>8</v>
       </c>
@@ -1247,8 +1368,39 @@
       <c r="D26" s="11">
         <v>43524</v>
       </c>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="H26" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="I26" s="32">
+        <f>I17/O17</f>
+        <v>0.41274817136886105</v>
+      </c>
+      <c r="J26" s="32">
+        <f>J17/O17</f>
+        <v>0.49634273772204807</v>
+      </c>
+      <c r="K26" s="32">
+        <f>K17/O17</f>
+        <v>9.0909090909090912E-2</v>
+      </c>
+      <c r="L26" s="32">
+        <f>L17/O17</f>
+        <v>0</v>
+      </c>
+      <c r="M26" s="32">
+        <f>M17/O17</f>
+        <v>0</v>
+      </c>
+      <c r="N26" s="32">
+        <f>N17/17</f>
+        <v>0</v>
+      </c>
+      <c r="O26" s="33">
+        <f>SUM(I26:M26)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A27" s="10" t="s">
         <v>8</v>
       </c>
@@ -1261,13 +1413,44 @@
       <c r="D27" s="11">
         <v>43530</v>
       </c>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="H27" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="I27" s="32">
+        <f>I18/O18</f>
+        <v>2.7812113720642771E-2</v>
+      </c>
+      <c r="J27" s="32">
+        <f>J18/O18</f>
+        <v>0.15574783683559951</v>
+      </c>
+      <c r="K27" s="32">
+        <f>K18/O18</f>
+        <v>0</v>
+      </c>
+      <c r="L27" s="32">
+        <f>L18/O18</f>
+        <v>0.8164400494437577</v>
+      </c>
+      <c r="M27" s="32">
+        <f>M18/O18</f>
+        <v>0</v>
+      </c>
+      <c r="N27" s="32">
+        <f>N18/17</f>
+        <v>0</v>
+      </c>
+      <c r="O27" s="33">
+        <f>SUM(I27:M27)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A28" s="10" t="s">
         <v>6</v>
       </c>
       <c r="B28" s="10" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C28" s="10">
         <v>15</v>
@@ -1275,8 +1458,39 @@
       <c r="D28" s="11">
         <v>43532</v>
       </c>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="H28" s="31" t="s">
+        <v>6</v>
+      </c>
+      <c r="I28" s="32">
+        <f>I19/O19</f>
+        <v>0.42605412208936438</v>
+      </c>
+      <c r="J28" s="32">
+        <f>J19/O19</f>
+        <v>0.53618628067967278</v>
+      </c>
+      <c r="K28" s="32">
+        <f>K19/O19</f>
+        <v>0</v>
+      </c>
+      <c r="L28" s="32">
+        <f>L19/O19</f>
+        <v>3.7759597230962873E-2</v>
+      </c>
+      <c r="M28" s="32">
+        <f>M19/O19</f>
+        <v>0</v>
+      </c>
+      <c r="N28" s="32">
+        <f>N19/17</f>
+        <v>0</v>
+      </c>
+      <c r="O28" s="33">
+        <f>SUM(I28:M28)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A29" s="10" t="s">
         <v>4</v>
       </c>
@@ -1289,8 +1503,39 @@
       <c r="D29" s="11">
         <v>43532</v>
       </c>
-    </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="H29" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="I29" s="32">
+        <f>I20/O20</f>
+        <v>0.14560099132589838</v>
+      </c>
+      <c r="J29" s="32">
+        <f>J20/O20</f>
+        <v>3.717472118959108E-2</v>
+      </c>
+      <c r="K29" s="32">
+        <f>K20/O20</f>
+        <v>0</v>
+      </c>
+      <c r="L29" s="32">
+        <f>L20/O20</f>
+        <v>0.81722428748451048</v>
+      </c>
+      <c r="M29" s="32">
+        <f>M20/O20</f>
+        <v>0</v>
+      </c>
+      <c r="N29" s="32">
+        <f>N20/17</f>
+        <v>0</v>
+      </c>
+      <c r="O29" s="33">
+        <f>SUM(I29:M29)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A30" s="10" t="s">
         <v>7</v>
       </c>
@@ -1303,8 +1548,36 @@
       <c r="D30" s="11">
         <v>43532</v>
       </c>
-    </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="H30" s="39" t="s">
+        <v>25</v>
+      </c>
+      <c r="I30" s="40">
+        <f>AVERAGE(I26:I29)</f>
+        <v>0.25305384962619165</v>
+      </c>
+      <c r="J30" s="40">
+        <f>AVERAGE(J26:J29)</f>
+        <v>0.30636289410672779</v>
+      </c>
+      <c r="K30" s="40">
+        <f>AVERAGE(K26:K29)</f>
+        <v>2.2727272727272728E-2</v>
+      </c>
+      <c r="L30" s="40">
+        <f>AVERAGE(L26:L29)</f>
+        <v>0.4178559835398078</v>
+      </c>
+      <c r="M30" s="40">
+        <f>AVERAGE(M26:M29)</f>
+        <v>0</v>
+      </c>
+      <c r="N30" s="41">
+        <f>AVERAGE(N26:N29)</f>
+        <v>0</v>
+      </c>
+      <c r="O30" s="34"/>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A31" s="10" t="s">
         <v>7</v>
       </c>
@@ -1318,7 +1591,7 @@
         <v>43531</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A32" s="10" t="s">
         <v>7</v>
       </c>
@@ -1332,7 +1605,7 @@
         <v>43532</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="10" t="s">
         <v>7</v>
       </c>
@@ -1346,7 +1619,7 @@
         <v>43533</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="10" t="s">
         <v>7</v>
       </c>
@@ -1360,12 +1633,12 @@
         <v>43534</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="10" t="s">
         <v>4</v>
       </c>
       <c r="B35" s="10" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C35" s="10">
         <v>74</v>
@@ -1374,12 +1647,12 @@
         <v>43546</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="10" t="s">
         <v>4</v>
       </c>
       <c r="B36" s="10" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C36" s="10">
         <v>52</v>
@@ -1388,7 +1661,7 @@
         <v>43546</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" s="10" t="s">
         <v>8</v>
       </c>
@@ -1402,7 +1675,7 @@
         <v>43376</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" s="10" t="s">
         <v>8</v>
       </c>
@@ -1416,12 +1689,12 @@
         <v>43407</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" s="10" t="s">
         <v>7</v>
       </c>
       <c r="B39" s="10" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C39" s="10">
         <v>10</v>
@@ -1430,12 +1703,12 @@
         <v>43546</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" s="10" t="s">
         <v>6</v>
       </c>
       <c r="B40" s="10" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C40" s="10">
         <v>60</v>
@@ -1444,12 +1717,12 @@
         <v>43553</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" s="10" t="s">
         <v>7</v>
       </c>
       <c r="B41" s="10" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C41" s="10">
         <v>60</v>
@@ -1458,12 +1731,12 @@
         <v>43553</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" s="10" t="s">
         <v>8</v>
       </c>
       <c r="B42" s="10" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C42" s="10">
         <v>60</v>
@@ -1472,12 +1745,12 @@
         <v>43553</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" s="10" t="s">
         <v>6</v>
       </c>
       <c r="B43" s="10" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C43" s="10">
         <v>60</v>
@@ -1486,12 +1759,12 @@
         <v>43481</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" s="10" t="s">
         <v>6</v>
       </c>
       <c r="B44" s="10" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C44" s="10">
         <v>150</v>
@@ -1500,12 +1773,12 @@
         <v>43442</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" s="10" t="s">
         <v>6</v>
       </c>
       <c r="B45" s="10" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C45" s="10">
         <v>180</v>
@@ -1514,12 +1787,12 @@
         <v>43448</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" s="10" t="s">
         <v>6</v>
       </c>
       <c r="B46" s="10" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C46" s="10">
         <v>180</v>
@@ -1528,12 +1801,12 @@
         <v>43468</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" s="10" t="s">
         <v>6</v>
       </c>
       <c r="B47" s="10" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C47" s="10">
         <v>120</v>
@@ -1542,12 +1815,12 @@
         <v>43478</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" s="10" t="s">
         <v>4</v>
       </c>
       <c r="B48" s="10" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C48" s="10">
         <v>300</v>
@@ -1556,12 +1829,12 @@
         <v>43449</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" s="10" t="s">
         <v>4</v>
       </c>
       <c r="B49" s="10" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C49" s="10">
         <v>150</v>
@@ -1570,12 +1843,12 @@
         <v>43450</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" s="10" t="s">
         <v>6</v>
       </c>
       <c r="B50" s="10" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C50" s="10">
         <v>82</v>
@@ -1584,12 +1857,12 @@
         <v>43558</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" s="10" t="s">
         <v>7</v>
       </c>
       <c r="B51" s="10" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C51" s="10">
         <v>82</v>
@@ -1598,12 +1871,12 @@
         <v>43558</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" s="10" t="s">
         <v>4</v>
       </c>
       <c r="B52" s="10" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C52" s="10">
         <v>82</v>
@@ -1612,7 +1885,7 @@
         <v>43558</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" s="10" t="s">
         <v>7</v>
       </c>
@@ -1626,12 +1899,12 @@
         <v>43559</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" s="10" t="s">
         <v>6</v>
       </c>
       <c r="B54" s="10" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C54" s="10">
         <v>70</v>
@@ -1640,12 +1913,12 @@
         <v>43571</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" s="10" t="s">
         <v>7</v>
       </c>
       <c r="B55" s="10" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C55" s="10">
         <v>70</v>
@@ -1654,12 +1927,12 @@
         <v>43571</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" s="10" t="s">
         <v>6</v>
       </c>
       <c r="B56" s="10" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C56" s="10">
         <v>120</v>
@@ -1668,12 +1941,12 @@
         <v>43572</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" s="10" t="s">
         <v>6</v>
       </c>
       <c r="B57" s="10" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C57" s="10">
         <v>100</v>
@@ -1682,12 +1955,12 @@
         <v>43574</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" s="10" t="s">
         <v>4</v>
       </c>
       <c r="B58" s="10" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C58" s="10">
         <v>42</v>
@@ -1696,12 +1969,12 @@
         <v>43577</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" s="10" t="s">
         <v>4</v>
       </c>
       <c r="B59" s="10" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C59" s="10">
         <v>97</v>
@@ -1710,12 +1983,12 @@
         <v>43578</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" s="10" t="s">
         <v>7</v>
       </c>
       <c r="B60" s="10" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C60" s="10">
         <v>30</v>
@@ -1724,12 +1997,12 @@
         <v>43578</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" s="10" t="s">
         <v>4</v>
       </c>
       <c r="B61" s="10" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C61" s="10">
         <v>107</v>
@@ -1738,12 +2011,12 @@
         <v>43581</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" s="10" t="s">
         <v>4</v>
       </c>
       <c r="B62" s="10" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C62" s="10">
         <v>39</v>
@@ -1752,12 +2025,12 @@
         <v>43584</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" s="10" t="s">
         <v>4</v>
       </c>
       <c r="B63" s="10" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C63" s="10">
         <v>22</v>
@@ -1766,12 +2039,12 @@
         <v>43585</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" s="10" t="s">
         <v>6</v>
       </c>
       <c r="B64" s="10" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C64" s="10">
         <v>22</v>
@@ -1780,12 +2053,12 @@
         <v>43585</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" s="10" t="s">
         <v>6</v>
       </c>
       <c r="B65" s="10" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C65" s="10">
         <v>25</v>
@@ -1794,12 +2067,12 @@
         <v>43587</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66" s="10" t="s">
         <v>8</v>
       </c>
       <c r="B66" s="10" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C66" s="10">
         <v>25</v>
@@ -1808,7 +2081,7 @@
         <v>43587</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67" s="10" t="s">
         <v>8</v>
       </c>
@@ -1822,12 +2095,12 @@
         <v>43587</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68" s="10" t="s">
         <v>8</v>
       </c>
       <c r="B68" s="10" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C68" s="10">
         <v>35</v>
@@ -1836,7 +2109,7 @@
         <v>43587</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69" s="10" t="s">
         <v>8</v>
       </c>
@@ -1850,7 +2123,7 @@
         <v>43588</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70" s="10" t="s">
         <v>7</v>
       </c>
@@ -1864,7 +2137,7 @@
         <v>43588</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71" s="10" t="s">
         <v>7</v>
       </c>
@@ -1878,7 +2151,7 @@
         <v>43589</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72" s="10" t="s">
         <v>8</v>
       </c>
@@ -1892,7 +2165,7 @@
         <v>43589</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73" s="10" t="s">
         <v>7</v>
       </c>
@@ -1906,7 +2179,7 @@
         <v>43590</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74" s="10" t="s">
         <v>8</v>
       </c>
@@ -1920,12 +2193,12 @@
         <v>43590</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75" s="10" t="s">
         <v>4</v>
       </c>
       <c r="B75" s="10" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C75" s="10">
         <v>45</v>
@@ -1934,12 +2207,12 @@
         <v>43593</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76" s="10" t="s">
         <v>7</v>
       </c>
       <c r="B76" s="10" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C76" s="10">
         <v>45</v>
@@ -1948,12 +2221,12 @@
         <v>43593</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" s="10" t="s">
         <v>6</v>
       </c>
       <c r="B77" s="10" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C77" s="10">
         <v>45</v>
@@ -1962,12 +2235,12 @@
         <v>43593</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A78" s="10" t="s">
         <v>8</v>
       </c>
       <c r="B78" s="10" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C78" s="10">
         <v>45</v>
@@ -1976,7 +2249,7 @@
         <v>43593</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A79" s="10" t="s">
         <v>7</v>
       </c>
@@ -1990,7 +2263,7 @@
         <v>43593</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A80" s="10" t="s">
         <v>6</v>
       </c>
@@ -2004,7 +2277,7 @@
         <v>43593</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A81" s="10" t="s">
         <v>8</v>
       </c>
@@ -2018,7 +2291,7 @@
         <v>43593</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A82" s="10" t="s">
         <v>8</v>
       </c>
@@ -2032,7 +2305,7 @@
         <v>43594</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A83" s="10" t="s">
         <v>7</v>
       </c>
@@ -2046,202 +2319,219 @@
         <v>43594</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A84" s="10"/>
-      <c r="B84" s="10"/>
-      <c r="C84" s="10"/>
-      <c r="D84" s="11"/>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A85" s="10"/>
-      <c r="B85" s="10"/>
-      <c r="C85" s="10"/>
-      <c r="D85" s="11"/>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A84" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B84" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C84" s="10">
+        <v>47</v>
+      </c>
+      <c r="D84" s="11">
+        <v>43598</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A85" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B85" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C85" s="10">
+        <v>31</v>
+      </c>
+      <c r="D85" s="11">
+        <v>43598</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A86" s="10"/>
       <c r="B86" s="10"/>
       <c r="C86" s="10"/>
       <c r="D86" s="11"/>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A87" s="10"/>
       <c r="B87" s="10"/>
       <c r="C87" s="10"/>
       <c r="D87" s="11"/>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A88" s="10"/>
       <c r="B88" s="10"/>
       <c r="C88" s="10"/>
       <c r="D88" s="11"/>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A89" s="10"/>
       <c r="B89" s="10"/>
       <c r="C89" s="10"/>
       <c r="D89" s="11"/>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A90" s="10"/>
       <c r="B90" s="10"/>
       <c r="C90" s="10"/>
       <c r="D90" s="11"/>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A91" s="10"/>
       <c r="B91" s="10"/>
       <c r="C91" s="10"/>
       <c r="D91" s="11"/>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A92" s="10"/>
       <c r="B92" s="10"/>
       <c r="C92" s="10"/>
       <c r="D92" s="11"/>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A93" s="10"/>
       <c r="B93" s="10"/>
       <c r="C93" s="10"/>
       <c r="D93" s="11"/>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A94" s="10"/>
       <c r="B94" s="10"/>
       <c r="C94" s="10"/>
       <c r="D94" s="11"/>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A95" s="10"/>
       <c r="B95" s="10"/>
       <c r="C95" s="10"/>
       <c r="D95" s="11"/>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A96" s="10"/>
       <c r="B96" s="10"/>
       <c r="C96" s="10"/>
       <c r="D96" s="11"/>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A97" s="10"/>
       <c r="B97" s="10"/>
       <c r="C97" s="10"/>
       <c r="D97" s="11"/>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A98" s="10"/>
       <c r="B98" s="10"/>
       <c r="C98" s="10"/>
       <c r="D98" s="11"/>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A99" s="10"/>
       <c r="B99" s="10"/>
       <c r="C99" s="10"/>
       <c r="D99" s="11"/>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A100" s="10"/>
       <c r="B100" s="10"/>
       <c r="C100" s="10"/>
       <c r="D100" s="11"/>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A101" s="10"/>
       <c r="B101" s="10"/>
       <c r="C101" s="10"/>
       <c r="D101" s="11"/>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A102" s="10"/>
       <c r="B102" s="10"/>
       <c r="C102" s="10"/>
       <c r="D102" s="11"/>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A103" s="10"/>
       <c r="B103" s="10"/>
       <c r="C103" s="10"/>
       <c r="D103" s="11"/>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A104" s="10"/>
       <c r="B104" s="10"/>
       <c r="C104" s="10"/>
       <c r="D104" s="11"/>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A105" s="10"/>
       <c r="B105" s="10"/>
       <c r="C105" s="10"/>
       <c r="D105" s="11"/>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A106" s="10"/>
       <c r="B106" s="10"/>
       <c r="C106" s="10"/>
       <c r="D106" s="11"/>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A107" s="10"/>
       <c r="B107" s="10"/>
       <c r="C107" s="10"/>
       <c r="D107" s="11"/>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A108" s="10"/>
       <c r="B108" s="10"/>
       <c r="C108" s="10"/>
       <c r="D108" s="11"/>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A109" s="10"/>
       <c r="B109" s="10"/>
       <c r="C109" s="10"/>
       <c r="D109" s="11"/>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A110" s="10"/>
       <c r="B110" s="10"/>
       <c r="C110" s="10"/>
       <c r="D110" s="11"/>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A111" s="10"/>
       <c r="B111" s="10"/>
       <c r="C111" s="10"/>
       <c r="D111" s="11"/>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A112" s="10"/>
       <c r="B112" s="10"/>
       <c r="C112" s="10"/>
       <c r="D112" s="11"/>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A113" s="10"/>
       <c r="B113" s="10"/>
       <c r="C113" s="10"/>
       <c r="D113" s="11"/>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A114" s="10"/>
       <c r="B114" s="10"/>
       <c r="C114" s="10"/>
       <c r="D114" s="11"/>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A115" s="10"/>
       <c r="B115" s="10"/>
       <c r="C115" s="10"/>
       <c r="D115" s="10"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="H4:J4"/>
     <mergeCell ref="H15:O15"/>
+    <mergeCell ref="H24:O24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Aggiornamento doc di design
</commit_message>
<xml_diff>
--- a/Documentazione/Attività sul progetto/DocAttivProg.xlsx
+++ b/Documentazione/Attività sul progetto/DocAttivProg.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\UniUD\Laurea Magistrale\Ingegneria del Software 2\Progetto-Ingegneria-Del-Sw-2\Documentazione\Attività sul progetto\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vik\Documents\GitHub\Progetto\Documentazione\Attività sul progetto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFA3FDEA-A5FD-465B-89E6-8ED67ECBF2F9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" iterateDelta="1E-4"/>
+  <calcPr calcId="152511" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -31,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="29">
   <si>
     <t>PERSONA</t>
   </si>
@@ -123,7 +122,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yyyy"/>
   </numFmts>
@@ -686,39 +685,39 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O115"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N30" sqref="N30"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F102" sqref="F102"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.5546875" customWidth="1"/>
-    <col min="2" max="2" width="23.44140625" customWidth="1"/>
-    <col min="3" max="3" width="15.5546875" customWidth="1"/>
-    <col min="4" max="4" width="10.88671875" customWidth="1"/>
-    <col min="5" max="7" width="8.6640625" customWidth="1"/>
-    <col min="8" max="8" width="26.33203125" customWidth="1"/>
-    <col min="9" max="11" width="17.33203125" customWidth="1"/>
-    <col min="12" max="14" width="17.44140625" customWidth="1"/>
-    <col min="15" max="1025" width="8.6640625" customWidth="1"/>
+    <col min="1" max="1" width="15.5703125" customWidth="1"/>
+    <col min="2" max="2" width="23.42578125" customWidth="1"/>
+    <col min="3" max="3" width="15.5703125" customWidth="1"/>
+    <col min="4" max="4" width="10.85546875" customWidth="1"/>
+    <col min="5" max="7" width="8.7109375" customWidth="1"/>
+    <col min="8" max="8" width="26.28515625" customWidth="1"/>
+    <col min="9" max="11" width="17.28515625" customWidth="1"/>
+    <col min="12" max="14" width="17.42578125" customWidth="1"/>
+    <col min="15" max="1025" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="F1" s="13" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="F2" s="14" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>0</v>
       </c>
@@ -733,7 +732,7 @@
       </c>
       <c r="H3" s="2"/>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>4</v>
       </c>
@@ -752,7 +751,7 @@
       <c r="I4" s="42"/>
       <c r="J4" s="42"/>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
         <v>4</v>
       </c>
@@ -775,7 +774,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
         <v>4</v>
       </c>
@@ -800,7 +799,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
         <v>4</v>
       </c>
@@ -818,14 +817,14 @@
       </c>
       <c r="I7" s="22">
         <f>SUMIF(B:B,"Documenti di progetto",C:C)</f>
-        <v>1907</v>
+        <v>2067</v>
       </c>
       <c r="J7" s="39">
         <f>(I7/I12)</f>
-        <v>0.24782326185834957</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+        <v>0.26314449395289624</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
         <v>4</v>
       </c>
@@ -847,10 +846,10 @@
       </c>
       <c r="J8" s="39">
         <f>I8/I12</f>
-        <v>0.27472384665367122</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+        <v>0.26912794398472312</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
         <v>4</v>
       </c>
@@ -872,10 +871,10 @@
       </c>
       <c r="J9" s="39">
         <f>I9/I12</f>
-        <v>2.2612085769980507E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+        <v>2.2151495862507958E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
         <v>4</v>
       </c>
@@ -897,10 +896,10 @@
       </c>
       <c r="J10" s="39">
         <f>I10/I12</f>
-        <v>0.45484080571799868</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+        <v>0.44557606619987267</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
         <v>8</v>
       </c>
@@ -925,7 +924,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>8</v>
       </c>
@@ -943,14 +942,14 @@
       </c>
       <c r="I12" s="16">
         <f>SUM(I6:I11)</f>
-        <v>7695</v>
+        <v>7855</v>
       </c>
       <c r="J12" s="41">
         <f>SUM(J6:J11)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
         <v>4</v>
       </c>
@@ -967,7 +966,7 @@
       <c r="I13" s="8"/>
       <c r="J13" s="8"/>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="10" t="s">
         <v>4</v>
       </c>
@@ -981,7 +980,7 @@
         <v>43509</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="10" t="s">
         <v>6</v>
       </c>
@@ -1005,7 +1004,7 @@
       <c r="N15" s="43"/>
       <c r="O15" s="43"/>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="10" t="s">
         <v>6</v>
       </c>
@@ -1043,7 +1042,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="10" t="s">
         <v>7</v>
       </c>
@@ -1088,7 +1087,7 @@
         <v>1954</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="10" t="s">
         <v>7</v>
       </c>
@@ -1133,7 +1132,7 @@
         <v>2058</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="10" t="s">
         <v>7</v>
       </c>
@@ -1178,7 +1177,7 @@
         <v>1629</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="10" t="s">
         <v>7</v>
       </c>
@@ -1196,7 +1195,7 @@
       </c>
       <c r="I20" s="3">
         <f>SUMIFS(C:C,B:B,"Documenti di progetto",A:A,"Viktorija")</f>
-        <v>275</v>
+        <v>435</v>
       </c>
       <c r="J20" s="3">
         <f>SUMIFS(C:C,B:B,"Documenti di processo",A:A,"Viktorija")</f>
@@ -1220,10 +1219,10 @@
       </c>
       <c r="O20" s="18">
         <f>SUM(I20:M20)</f>
-        <v>2054</v>
-      </c>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
+        <v>2214</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="10" t="s">
         <v>7</v>
       </c>
@@ -1241,7 +1240,7 @@
       </c>
       <c r="I21" s="34">
         <f t="shared" ref="I21:N21" si="0">AVERAGE(I17:I20)</f>
-        <v>476.75</v>
+        <v>516.75</v>
       </c>
       <c r="J21" s="34">
         <f t="shared" si="0"/>
@@ -1265,7 +1264,7 @@
       </c>
       <c r="O21" s="32"/>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
         <v>8</v>
       </c>
@@ -1279,7 +1278,7 @@
         <v>43487</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" s="10" t="s">
         <v>8</v>
       </c>
@@ -1293,7 +1292,7 @@
         <v>43506</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" s="10" t="s">
         <v>8</v>
       </c>
@@ -1317,7 +1316,7 @@
       <c r="N24" s="44"/>
       <c r="O24" s="44"/>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" s="10" t="s">
         <v>8</v>
       </c>
@@ -1355,7 +1354,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" s="10" t="s">
         <v>8</v>
       </c>
@@ -1400,7 +1399,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" s="10" t="s">
         <v>8</v>
       </c>
@@ -1445,7 +1444,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" s="10" t="s">
         <v>6</v>
       </c>
@@ -1490,7 +1489,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" s="10" t="s">
         <v>4</v>
       </c>
@@ -1508,11 +1507,11 @@
       </c>
       <c r="I29" s="29">
         <f>I20/O20</f>
-        <v>0.13388510223953262</v>
+        <v>0.19647696476964768</v>
       </c>
       <c r="J29" s="29">
         <f>J20/O20</f>
-        <v>2.9211295034079845E-2</v>
+        <v>2.7100271002710029E-2</v>
       </c>
       <c r="K29" s="29">
         <f>K20/O20</f>
@@ -1520,7 +1519,7 @@
       </c>
       <c r="L29" s="29">
         <f>L20/O20</f>
-        <v>0.83690360272638753</v>
+        <v>0.77642276422764223</v>
       </c>
       <c r="M29" s="29">
         <f>M20/O20</f>
@@ -1528,14 +1527,14 @@
       </c>
       <c r="N29" s="29">
         <f>N20/O20</f>
-        <v>9.7370983446932822E-3</v>
+        <v>9.0334236675700084E-3</v>
       </c>
       <c r="O29" s="30">
         <f>SUM(I29:M29)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" s="10" t="s">
         <v>7</v>
       </c>
@@ -1553,11 +1552,11 @@
       </c>
       <c r="I30" s="37">
         <f t="shared" ref="I30:N30" si="1">AVERAGE(I26:I29)</f>
-        <v>0.26002609256059733</v>
+        <v>0.27567405819312613</v>
       </c>
       <c r="J30" s="37">
         <f t="shared" si="1"/>
-        <v>0.29021568070787868</v>
+        <v>0.28968792470003618</v>
       </c>
       <c r="K30" s="37">
         <f t="shared" si="1"/>
@@ -1565,7 +1564,7 @@
       </c>
       <c r="L30" s="37">
         <f t="shared" si="1"/>
-        <v>0.42749620011944622</v>
+        <v>0.41237599049475993</v>
       </c>
       <c r="M30" s="37">
         <f t="shared" si="1"/>
@@ -1573,11 +1572,11 @@
       </c>
       <c r="N30" s="38">
         <f t="shared" si="1"/>
-        <v>1.0492039175866946E-2</v>
+        <v>1.0316120506586129E-2</v>
       </c>
       <c r="O30" s="31"/>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" s="10" t="s">
         <v>7</v>
       </c>
@@ -1591,7 +1590,7 @@
         <v>43531</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" s="10" t="s">
         <v>7</v>
       </c>
@@ -1605,7 +1604,7 @@
         <v>43532</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="10" t="s">
         <v>7</v>
       </c>
@@ -1619,7 +1618,7 @@
         <v>43533</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="10" t="s">
         <v>7</v>
       </c>
@@ -1633,7 +1632,7 @@
         <v>43534</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="10" t="s">
         <v>4</v>
       </c>
@@ -1647,7 +1646,7 @@
         <v>43546</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="10" t="s">
         <v>4</v>
       </c>
@@ -1661,7 +1660,7 @@
         <v>43546</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="10" t="s">
         <v>8</v>
       </c>
@@ -1675,7 +1674,7 @@
         <v>43376</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="10" t="s">
         <v>8</v>
       </c>
@@ -1689,7 +1688,7 @@
         <v>43407</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="10" t="s">
         <v>7</v>
       </c>
@@ -1703,7 +1702,7 @@
         <v>43546</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="10" t="s">
         <v>6</v>
       </c>
@@ -1717,7 +1716,7 @@
         <v>43553</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="10" t="s">
         <v>7</v>
       </c>
@@ -1731,7 +1730,7 @@
         <v>43553</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="10" t="s">
         <v>8</v>
       </c>
@@ -1745,7 +1744,7 @@
         <v>43553</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="10" t="s">
         <v>6</v>
       </c>
@@ -1759,7 +1758,7 @@
         <v>43481</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="10" t="s">
         <v>6</v>
       </c>
@@ -1773,7 +1772,7 @@
         <v>43442</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="10" t="s">
         <v>6</v>
       </c>
@@ -1787,7 +1786,7 @@
         <v>43448</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="10" t="s">
         <v>6</v>
       </c>
@@ -1801,7 +1800,7 @@
         <v>43468</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="10" t="s">
         <v>6</v>
       </c>
@@ -1815,7 +1814,7 @@
         <v>43478</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="10" t="s">
         <v>4</v>
       </c>
@@ -1829,7 +1828,7 @@
         <v>43449</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="10" t="s">
         <v>4</v>
       </c>
@@ -1843,7 +1842,7 @@
         <v>43450</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="10" t="s">
         <v>6</v>
       </c>
@@ -1857,7 +1856,7 @@
         <v>43558</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="10" t="s">
         <v>7</v>
       </c>
@@ -1871,7 +1870,7 @@
         <v>43558</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="10" t="s">
         <v>4</v>
       </c>
@@ -1885,7 +1884,7 @@
         <v>43558</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="10" t="s">
         <v>7</v>
       </c>
@@ -1899,7 +1898,7 @@
         <v>43559</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="10" t="s">
         <v>6</v>
       </c>
@@ -1913,7 +1912,7 @@
         <v>43571</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="10" t="s">
         <v>7</v>
       </c>
@@ -1927,7 +1926,7 @@
         <v>43571</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="10" t="s">
         <v>6</v>
       </c>
@@ -1941,7 +1940,7 @@
         <v>43572</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="10" t="s">
         <v>6</v>
       </c>
@@ -1955,7 +1954,7 @@
         <v>43574</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="10" t="s">
         <v>4</v>
       </c>
@@ -1969,7 +1968,7 @@
         <v>43577</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="10" t="s">
         <v>4</v>
       </c>
@@ -1983,7 +1982,7 @@
         <v>43578</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="10" t="s">
         <v>7</v>
       </c>
@@ -1997,7 +1996,7 @@
         <v>43578</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="10" t="s">
         <v>4</v>
       </c>
@@ -2011,7 +2010,7 @@
         <v>43581</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="10" t="s">
         <v>4</v>
       </c>
@@ -2025,7 +2024,7 @@
         <v>43584</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="10" t="s">
         <v>4</v>
       </c>
@@ -2039,7 +2038,7 @@
         <v>43585</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="10" t="s">
         <v>6</v>
       </c>
@@ -2053,7 +2052,7 @@
         <v>43585</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="10" t="s">
         <v>6</v>
       </c>
@@ -2067,7 +2066,7 @@
         <v>43587</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="10" t="s">
         <v>8</v>
       </c>
@@ -2081,7 +2080,7 @@
         <v>43587</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="10" t="s">
         <v>8</v>
       </c>
@@ -2095,7 +2094,7 @@
         <v>43587</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="10" t="s">
         <v>8</v>
       </c>
@@ -2109,7 +2108,7 @@
         <v>43587</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="10" t="s">
         <v>8</v>
       </c>
@@ -2123,7 +2122,7 @@
         <v>43588</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="10" t="s">
         <v>7</v>
       </c>
@@ -2137,7 +2136,7 @@
         <v>43588</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="10" t="s">
         <v>7</v>
       </c>
@@ -2151,7 +2150,7 @@
         <v>43589</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="10" t="s">
         <v>8</v>
       </c>
@@ -2165,7 +2164,7 @@
         <v>43589</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="10" t="s">
         <v>7</v>
       </c>
@@ -2179,7 +2178,7 @@
         <v>43590</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="10" t="s">
         <v>8</v>
       </c>
@@ -2193,7 +2192,7 @@
         <v>43590</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="10" t="s">
         <v>4</v>
       </c>
@@ -2207,7 +2206,7 @@
         <v>43593</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="10" t="s">
         <v>7</v>
       </c>
@@ -2221,7 +2220,7 @@
         <v>43593</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="10" t="s">
         <v>6</v>
       </c>
@@ -2235,7 +2234,7 @@
         <v>43593</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="10" t="s">
         <v>8</v>
       </c>
@@ -2249,7 +2248,7 @@
         <v>43593</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="10" t="s">
         <v>7</v>
       </c>
@@ -2263,7 +2262,7 @@
         <v>43593</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="10" t="s">
         <v>6</v>
       </c>
@@ -2277,7 +2276,7 @@
         <v>43593</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="10" t="s">
         <v>8</v>
       </c>
@@ -2291,7 +2290,7 @@
         <v>43593</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="10" t="s">
         <v>8</v>
       </c>
@@ -2305,7 +2304,7 @@
         <v>43594</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="10" t="s">
         <v>7</v>
       </c>
@@ -2319,7 +2318,7 @@
         <v>43594</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="10" t="s">
         <v>4</v>
       </c>
@@ -2333,7 +2332,7 @@
         <v>43598</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" s="10" t="s">
         <v>4</v>
       </c>
@@ -2347,7 +2346,7 @@
         <v>43598</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" s="10" t="s">
         <v>7</v>
       </c>
@@ -2361,7 +2360,7 @@
         <v>43595</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" s="10" t="s">
         <v>8</v>
       </c>
@@ -2375,7 +2374,7 @@
         <v>43595</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" s="10" t="s">
         <v>7</v>
       </c>
@@ -2389,7 +2388,7 @@
         <v>43599</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" s="10" t="s">
         <v>8</v>
       </c>
@@ -2403,7 +2402,7 @@
         <v>43599</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" s="10" t="s">
         <v>4</v>
       </c>
@@ -2417,7 +2416,7 @@
         <v>43600</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" s="10" t="s">
         <v>6</v>
       </c>
@@ -2431,7 +2430,7 @@
         <v>43600</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" s="10" t="s">
         <v>8</v>
       </c>
@@ -2445,7 +2444,7 @@
         <v>43600</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" s="10" t="s">
         <v>7</v>
       </c>
@@ -2459,7 +2458,7 @@
         <v>43600</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" s="10" t="s">
         <v>4</v>
       </c>
@@ -2473,7 +2472,7 @@
         <v>43600</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" s="10" t="s">
         <v>6</v>
       </c>
@@ -2487,7 +2486,7 @@
         <v>43600</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" s="10" t="s">
         <v>8</v>
       </c>
@@ -2501,7 +2500,7 @@
         <v>43600</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" s="10" t="s">
         <v>7</v>
       </c>
@@ -2515,109 +2514,117 @@
         <v>43600</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A98" s="10"/>
-      <c r="B98" s="10"/>
-      <c r="C98" s="10"/>
-      <c r="D98" s="11"/>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A98" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B98" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C98" s="10">
+        <v>160</v>
+      </c>
+      <c r="D98" s="11">
+        <v>43604</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" s="10"/>
       <c r="B99" s="10"/>
       <c r="C99" s="10"/>
       <c r="D99" s="11"/>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" s="10"/>
       <c r="B100" s="10"/>
       <c r="C100" s="10"/>
       <c r="D100" s="11"/>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" s="10"/>
       <c r="B101" s="10"/>
       <c r="C101" s="10"/>
       <c r="D101" s="11"/>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" s="10"/>
       <c r="B102" s="10"/>
       <c r="C102" s="10"/>
       <c r="D102" s="11"/>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" s="10"/>
       <c r="B103" s="10"/>
       <c r="C103" s="10"/>
       <c r="D103" s="11"/>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" s="10"/>
       <c r="B104" s="10"/>
       <c r="C104" s="10"/>
       <c r="D104" s="11"/>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" s="10"/>
       <c r="B105" s="10"/>
       <c r="C105" s="10"/>
       <c r="D105" s="11"/>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" s="10"/>
       <c r="B106" s="10"/>
       <c r="C106" s="10"/>
       <c r="D106" s="11"/>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" s="10"/>
       <c r="B107" s="10"/>
       <c r="C107" s="10"/>
       <c r="D107" s="11"/>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" s="10"/>
       <c r="B108" s="10"/>
       <c r="C108" s="10"/>
       <c r="D108" s="11"/>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" s="10"/>
       <c r="B109" s="10"/>
       <c r="C109" s="10"/>
       <c r="D109" s="11"/>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" s="10"/>
       <c r="B110" s="10"/>
       <c r="C110" s="10"/>
       <c r="D110" s="11"/>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" s="10"/>
       <c r="B111" s="10"/>
       <c r="C111" s="10"/>
       <c r="D111" s="11"/>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" s="10"/>
       <c r="B112" s="10"/>
       <c r="C112" s="10"/>
       <c r="D112" s="11"/>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" s="10"/>
       <c r="B113" s="10"/>
       <c r="C113" s="10"/>
       <c r="D113" s="11"/>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" s="10"/>
       <c r="B114" s="10"/>
       <c r="C114" s="10"/>
       <c r="D114" s="11"/>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" s="10"/>
       <c r="B115" s="10"/>
       <c r="C115" s="10"/>

</xml_diff>

<commit_message>
CMv0.19, DocDBv0.6, altri piccoli cambiamenti
</commit_message>
<xml_diff>
--- a/Documentazione/Attività sul progetto/DocAttivProg.xlsx
+++ b/Documentazione/Attività sul progetto/DocAttivProg.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\UniUD\Laurea Magistrale\Ingegneria del Software 2\Progetto-Ingegneria-Del-Sw-2\Documentazione\Attività sul progetto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94744BFD-8F48-4D14-B78B-B3DE40F39EB5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74757BBA-E144-48D7-B5F1-A7CBEADA6598}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="29">
   <si>
     <t>Le categorie sono: Ispezione Codice, Documenti di progetto, Documenti di processo, Manuale, Sviluppo, Testing</t>
   </si>
@@ -168,7 +168,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -193,8 +193,14 @@
         <bgColor rgb="FFE2F0D9"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -266,12 +272,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -340,9 +357,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="4" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -376,6 +390,13 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -763,8 +784,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O138"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A103" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C128" sqref="C128"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -820,11 +841,11 @@
       <c r="D4" s="6">
         <v>43484</v>
       </c>
-      <c r="H4" s="41" t="s">
+      <c r="H4" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="I4" s="41"/>
-      <c r="J4" s="41"/>
+      <c r="I4" s="40"/>
+      <c r="J4" s="40"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
@@ -869,9 +890,9 @@
         <f>SUMIF(B:B,"Ispezione codice",C:C)</f>
         <v>506</v>
       </c>
-      <c r="J6" s="39">
+      <c r="J6" s="38">
         <f>I6/I12</f>
-        <v>5.2030848329048841E-2</v>
+        <v>5.1178314959037116E-2</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.3">
@@ -892,11 +913,11 @@
       </c>
       <c r="I7" s="10">
         <f>SUMIF(B:B,"Documenti di progetto",C:C)</f>
-        <v>2235</v>
-      </c>
-      <c r="J7" s="39">
+        <v>2333</v>
+      </c>
+      <c r="J7" s="38">
         <f>(I7/I12)</f>
-        <v>0.22982005141388176</v>
+        <v>0.23596642055224032</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.3">
@@ -917,11 +938,11 @@
       </c>
       <c r="I8" s="10">
         <f>SUMIF(B:B,"Documenti di processo",C:C)</f>
-        <v>2272</v>
-      </c>
-      <c r="J8" s="39">
+        <v>2336</v>
+      </c>
+      <c r="J8" s="38">
         <f>I8/I12</f>
-        <v>0.23362467866323908</v>
+        <v>0.23626984929705674</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.3">
@@ -944,9 +965,9 @@
         <f>SUMIF(B:B,"Manuale",C:C)</f>
         <v>174</v>
       </c>
-      <c r="J9" s="39">
+      <c r="J9" s="38">
         <f>I9/I12</f>
-        <v>1.7892030848329049E-2</v>
+        <v>1.7598867199352684E-2</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.3">
@@ -969,9 +990,9 @@
         <f>SUMIF(B:B,"Sviluppo",C:C)</f>
         <v>4538</v>
       </c>
-      <c r="J10" s="39">
+      <c r="J10" s="38">
         <f>I10/I12</f>
-        <v>0.46663239074550128</v>
+        <v>0.45898654799231314</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.3">
@@ -994,7 +1015,7 @@
         <f>SUMIF(B:B,"Testing",C:C)</f>
         <v>0</v>
       </c>
-      <c r="J11" s="40">
+      <c r="J11" s="39">
         <f>I11/I12</f>
         <v>0</v>
       </c>
@@ -1017,7 +1038,7 @@
       </c>
       <c r="I12" s="14">
         <f>SUM(I6:I11)</f>
-        <v>9725</v>
+        <v>9887</v>
       </c>
       <c r="J12" s="15">
         <f>SUM(J6:J11)</f>
@@ -1066,16 +1087,16 @@
       <c r="D15" s="6">
         <v>43521</v>
       </c>
-      <c r="H15" s="42" t="s">
+      <c r="H15" s="41" t="s">
         <v>20</v>
       </c>
-      <c r="I15" s="42"/>
-      <c r="J15" s="42"/>
-      <c r="K15" s="42"/>
-      <c r="L15" s="42"/>
-      <c r="M15" s="42"/>
-      <c r="N15" s="42"/>
-      <c r="O15" s="42"/>
+      <c r="I15" s="41"/>
+      <c r="J15" s="41"/>
+      <c r="K15" s="41"/>
+      <c r="L15" s="41"/>
+      <c r="M15" s="41"/>
+      <c r="N15" s="41"/>
+      <c r="O15" s="41"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
@@ -1133,11 +1154,11 @@
       </c>
       <c r="I17" s="20">
         <f>SUMIFS(C:C,B:B,"Documenti di progetto",A:A,"Giovanni")</f>
-        <v>883</v>
+        <v>981</v>
       </c>
       <c r="J17" s="20">
         <f>SUMIFS(C:C,B:B,"Documenti di processo",A:A,"Giovanni")</f>
-        <v>1048</v>
+        <v>1112</v>
       </c>
       <c r="K17" s="20">
         <f>SUMIFS(C:C,B:B,"Manuale",A:A,"Giovanni")</f>
@@ -1156,8 +1177,8 @@
         <v>134</v>
       </c>
       <c r="O17" s="21">
-        <f>SUM(I17:M17)</f>
-        <v>2105</v>
+        <f>SUM(I17:N17)</f>
+        <v>2401</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.3">
@@ -1201,8 +1222,8 @@
         <v>134</v>
       </c>
       <c r="O18" s="21">
-        <f>SUM(I18:M18)</f>
-        <v>2671</v>
+        <f>SUM(I18:N18)</f>
+        <v>2805</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.3">
@@ -1246,8 +1267,8 @@
         <v>104</v>
       </c>
       <c r="O19" s="21">
-        <f>SUM(I19:M19)</f>
-        <v>1659</v>
+        <f>SUM(I19:N19)</f>
+        <v>1763</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.3">
@@ -1291,8 +1312,8 @@
         <v>134</v>
       </c>
       <c r="O20" s="21">
-        <f>SUM(I20:M20)</f>
-        <v>2784</v>
+        <f>SUM(I20:N20)</f>
+        <v>2918</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.3">
@@ -1313,31 +1334,31 @@
       </c>
       <c r="I21" s="23">
         <f t="shared" ref="I21:N21" si="0">AVERAGE(I17:I20)</f>
-        <v>558.75</v>
-      </c>
-      <c r="J21" s="37">
+        <v>583.25</v>
+      </c>
+      <c r="J21" s="36">
         <f t="shared" si="0"/>
-        <v>568</v>
-      </c>
-      <c r="K21" s="37">
+        <v>584</v>
+      </c>
+      <c r="K21" s="36">
         <f t="shared" si="0"/>
         <v>43.5</v>
       </c>
-      <c r="L21" s="37">
+      <c r="L21" s="36">
         <f t="shared" si="0"/>
         <v>1134.5</v>
       </c>
-      <c r="M21" s="37">
+      <c r="M21" s="36">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="N21" s="38">
+      <c r="N21" s="37">
         <f t="shared" si="0"/>
         <v>126.5</v>
       </c>
-      <c r="O21" s="21">
+      <c r="O21" s="45">
         <f>SUM(O17:O20)</f>
-        <v>9219</v>
+        <v>9887</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.3">
@@ -1381,16 +1402,16 @@
       <c r="D24" s="6">
         <v>43520</v>
       </c>
-      <c r="H24" s="43" t="s">
+      <c r="H24" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="I24" s="43"/>
-      <c r="J24" s="43"/>
-      <c r="K24" s="43"/>
-      <c r="L24" s="43"/>
-      <c r="M24" s="43"/>
-      <c r="N24" s="43"/>
-      <c r="O24" s="43"/>
+      <c r="I24" s="42"/>
+      <c r="J24" s="42"/>
+      <c r="K24" s="42"/>
+      <c r="L24" s="42"/>
+      <c r="M24" s="42"/>
+      <c r="N24" s="42"/>
+      <c r="O24" s="42"/>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A25" s="5" t="s">
@@ -1446,32 +1467,32 @@
       <c r="H26" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="I26" s="35">
+      <c r="I26" s="34">
         <f>I17/O17</f>
-        <v>0.4194774346793349</v>
-      </c>
-      <c r="J26" s="35">
+        <v>0.40857975843398586</v>
+      </c>
+      <c r="J26" s="34">
         <f>J17/O17</f>
-        <v>0.49786223277909741</v>
-      </c>
-      <c r="K26" s="35">
+        <v>0.46314035818408994</v>
+      </c>
+      <c r="K26" s="34">
         <f>K17/O17</f>
-        <v>8.2660332541567696E-2</v>
-      </c>
-      <c r="L26" s="35">
+        <v>7.2469804248229908E-2</v>
+      </c>
+      <c r="L26" s="34">
         <f>L17/O17</f>
         <v>0</v>
       </c>
-      <c r="M26" s="35">
+      <c r="M26" s="34">
         <f>M17/O17</f>
         <v>0</v>
       </c>
-      <c r="N26" s="35">
+      <c r="N26" s="34">
         <f>N17/O17</f>
-        <v>6.3657957244655589E-2</v>
+        <v>5.5810079133694297E-2</v>
       </c>
       <c r="O26" s="28">
-        <f>SUM(I26:M26)</f>
+        <f>SUM(I26:N26)</f>
         <v>1</v>
       </c>
     </row>
@@ -1491,32 +1512,32 @@
       <c r="H27" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="I27" s="35">
+      <c r="I27" s="34">
         <f>I18/O18</f>
-        <v>4.4926993635342569E-2</v>
-      </c>
-      <c r="J27" s="35">
+        <v>4.2780748663101602E-2</v>
+      </c>
+      <c r="J27" s="34">
         <f>J18/O18</f>
-        <v>0.10557843504305503</v>
-      </c>
-      <c r="K27" s="35">
+        <v>0.10053475935828877</v>
+      </c>
+      <c r="K27" s="34">
         <f>K18/O18</f>
         <v>0</v>
       </c>
-      <c r="L27" s="35">
+      <c r="L27" s="34">
         <f>L18/O18</f>
-        <v>0.84949457132160244</v>
-      </c>
-      <c r="M27" s="35">
+        <v>0.80891265597147954</v>
+      </c>
+      <c r="M27" s="34">
         <f>M18/O18</f>
         <v>0</v>
       </c>
-      <c r="N27" s="35">
+      <c r="N27" s="34">
         <f>N18/O18</f>
-        <v>5.0168476226132533E-2</v>
+        <v>4.7771836007130128E-2</v>
       </c>
       <c r="O27" s="28">
-        <f>SUM(I27:M27)</f>
+        <f>SUM(I27:N27)</f>
         <v>1</v>
       </c>
     </row>
@@ -1536,32 +1557,32 @@
       <c r="H28" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="I28" s="35">
+      <c r="I28" s="34">
         <f>I19/O19</f>
-        <v>0.45027124773960214</v>
-      </c>
-      <c r="J28" s="35">
+        <v>0.42370958593306862</v>
+      </c>
+      <c r="J28" s="34">
         <f>J19/O19</f>
-        <v>0.51356238698010848</v>
-      </c>
-      <c r="K28" s="35">
+        <v>0.48326715825297789</v>
+      </c>
+      <c r="K28" s="34">
         <f>K19/O19</f>
         <v>0</v>
       </c>
-      <c r="L28" s="35">
+      <c r="L28" s="34">
         <f>L19/O19</f>
-        <v>3.6166365280289332E-2</v>
-      </c>
-      <c r="M28" s="35">
+        <v>3.4032898468519569E-2</v>
+      </c>
+      <c r="M28" s="34">
         <f>M19/O19</f>
         <v>0</v>
       </c>
-      <c r="N28" s="35">
+      <c r="N28" s="34">
         <f>N19/O19</f>
-        <v>6.268836648583484E-2</v>
+        <v>5.8990357345433918E-2</v>
       </c>
       <c r="O28" s="28">
-        <f>SUM(I28:M28)</f>
+        <f>SUM(I28:N28)</f>
         <v>1</v>
       </c>
     </row>
@@ -1581,32 +1602,32 @@
       <c r="H29" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="I29" s="35">
+      <c r="I29" s="34">
         <f>I20/O20</f>
-        <v>0.17420977011494254</v>
-      </c>
-      <c r="J29" s="35">
+        <v>0.16620973269362577</v>
+      </c>
+      <c r="J29" s="34">
         <f>J20/O20</f>
-        <v>3.2327586206896554E-2</v>
-      </c>
-      <c r="K29" s="35">
+        <v>3.0843043180260453E-2</v>
+      </c>
+      <c r="K29" s="34">
         <f>K20/O20</f>
         <v>0</v>
       </c>
-      <c r="L29" s="35">
+      <c r="L29" s="34">
         <f>L20/O20</f>
-        <v>0.79346264367816088</v>
-      </c>
-      <c r="M29" s="35">
+        <v>0.75702535983550379</v>
+      </c>
+      <c r="M29" s="34">
         <f>M20/O20</f>
         <v>0</v>
       </c>
-      <c r="N29" s="35">
+      <c r="N29" s="34">
         <f>N20/O20</f>
-        <v>4.8132183908045974E-2</v>
-      </c>
-      <c r="O29" s="36">
-        <f>SUM(I29:M29)</f>
+        <v>4.5921864290610008E-2</v>
+      </c>
+      <c r="O29" s="35">
+        <f>SUM(I29:N29)</f>
         <v>1</v>
       </c>
     </row>
@@ -1626,31 +1647,34 @@
       <c r="H30" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="I30" s="33">
+      <c r="I30" s="32">
         <f>AVERAGE(I26:I29)</f>
-        <v>0.27222136154230553</v>
-      </c>
-      <c r="J30" s="33">
+        <v>0.26031995643094546</v>
+      </c>
+      <c r="J30" s="32">
         <f>AVERAGE(J26:J29)</f>
-        <v>0.28733266025228937</v>
-      </c>
-      <c r="K30" s="33">
+        <v>0.26944632974390426</v>
+      </c>
+      <c r="K30" s="32">
         <f>AVERAGE(K26:K29)</f>
-        <v>2.0665083135391924E-2</v>
-      </c>
-      <c r="L30" s="33">
+        <v>1.8117451062057477E-2</v>
+      </c>
+      <c r="L30" s="32">
         <f>AVERAGE(L26:L29)</f>
-        <v>0.41978089507001315</v>
-      </c>
-      <c r="M30" s="33">
+        <v>0.39999272856887569</v>
+      </c>
+      <c r="M30" s="32">
         <f t="shared" ref="M30" si="1">AVERAGE(M26:M29)</f>
         <v>0</v>
       </c>
-      <c r="N30" s="34">
+      <c r="N30" s="33">
         <f>AVERAGE(N26:N29)</f>
-        <v>5.6161745966167229E-2</v>
-      </c>
-      <c r="O30" s="30"/>
+        <v>5.2123534194217093E-2</v>
+      </c>
+      <c r="O30" s="44">
+        <f>SUM(I30:N30)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A31" s="5" t="s">
@@ -2913,13 +2937,13 @@
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A121" s="31" t="s">
-        <v>6</v>
-      </c>
-      <c r="B121" s="31" t="s">
-        <v>7</v>
-      </c>
-      <c r="C121" s="31">
+      <c r="A121" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="B121" s="30" t="s">
+        <v>7</v>
+      </c>
+      <c r="C121" s="30">
         <v>30</v>
       </c>
       <c r="D121" s="6">
@@ -2930,10 +2954,10 @@
       <c r="A122" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B122" s="32" t="s">
+      <c r="B122" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="C122" s="32">
+      <c r="C122" s="31">
         <v>84</v>
       </c>
       <c r="D122" s="6">
@@ -2944,10 +2968,10 @@
       <c r="A123" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B123" s="32" t="s">
+      <c r="B123" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="C123" s="32">
+      <c r="C123" s="31">
         <v>84</v>
       </c>
       <c r="D123" s="6">
@@ -2955,13 +2979,13 @@
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A124" s="31" t="s">
-        <v>6</v>
-      </c>
-      <c r="B124" s="32" t="s">
+      <c r="A124" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="B124" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="C124" s="32">
+      <c r="C124" s="31">
         <v>84</v>
       </c>
       <c r="D124" s="6">
@@ -2969,13 +2993,13 @@
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A125" s="32" t="s">
-        <v>25</v>
-      </c>
-      <c r="B125" s="32" t="s">
+      <c r="A125" s="31" t="s">
+        <v>25</v>
+      </c>
+      <c r="B125" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="C125" s="32">
+      <c r="C125" s="31">
         <v>84</v>
       </c>
       <c r="D125" s="6">
@@ -2983,82 +3007,98 @@
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A126" s="32"/>
-      <c r="B126" s="32"/>
-      <c r="C126" s="32"/>
-      <c r="D126" s="32"/>
+      <c r="A126" s="31" t="s">
+        <v>6</v>
+      </c>
+      <c r="B126" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="C126" s="31">
+        <v>64</v>
+      </c>
+      <c r="D126" s="43">
+        <v>43616</v>
+      </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A127" s="32"/>
-      <c r="B127" s="32"/>
-      <c r="C127" s="32"/>
-      <c r="D127" s="32"/>
+      <c r="A127" s="31" t="s">
+        <v>6</v>
+      </c>
+      <c r="B127" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="C127" s="31">
+        <v>98</v>
+      </c>
+      <c r="D127" s="43">
+        <v>43616</v>
+      </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A128" s="32"/>
-      <c r="B128" s="32"/>
-      <c r="C128" s="32"/>
-      <c r="D128" s="32"/>
+      <c r="A128" s="31"/>
+      <c r="B128" s="31"/>
+      <c r="C128" s="31"/>
+      <c r="D128" s="31"/>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A129" s="32"/>
-      <c r="B129" s="32"/>
-      <c r="C129" s="32"/>
-      <c r="D129" s="32"/>
+      <c r="A129" s="31"/>
+      <c r="B129" s="31"/>
+      <c r="C129" s="31"/>
+      <c r="D129" s="31"/>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A130" s="32"/>
-      <c r="B130" s="32"/>
-      <c r="C130" s="32"/>
-      <c r="D130" s="32"/>
+      <c r="A130" s="31"/>
+      <c r="B130" s="31"/>
+      <c r="C130" s="31"/>
+      <c r="D130" s="31"/>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A131" s="32"/>
-      <c r="B131" s="32"/>
-      <c r="C131" s="32"/>
-      <c r="D131" s="32"/>
+      <c r="A131" s="31"/>
+      <c r="B131" s="31"/>
+      <c r="C131" s="31"/>
+      <c r="D131" s="31"/>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A132" s="32"/>
-      <c r="B132" s="32"/>
-      <c r="C132" s="32"/>
-      <c r="D132" s="32"/>
+      <c r="A132" s="31"/>
+      <c r="B132" s="31"/>
+      <c r="C132" s="31"/>
+      <c r="D132" s="31"/>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A133" s="32"/>
-      <c r="B133" s="32"/>
-      <c r="C133" s="32"/>
-      <c r="D133" s="32"/>
+      <c r="A133" s="31"/>
+      <c r="B133" s="31"/>
+      <c r="C133" s="31"/>
+      <c r="D133" s="31"/>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A134" s="32"/>
-      <c r="B134" s="32"/>
-      <c r="C134" s="32"/>
-      <c r="D134" s="32"/>
+      <c r="A134" s="31"/>
+      <c r="B134" s="31"/>
+      <c r="C134" s="31"/>
+      <c r="D134" s="31"/>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A135" s="32"/>
-      <c r="B135" s="32"/>
-      <c r="C135" s="32"/>
-      <c r="D135" s="32"/>
+      <c r="A135" s="31"/>
+      <c r="B135" s="31"/>
+      <c r="C135" s="31"/>
+      <c r="D135" s="31"/>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A136" s="32"/>
-      <c r="B136" s="32"/>
-      <c r="C136" s="32"/>
-      <c r="D136" s="32"/>
+      <c r="A136" s="31"/>
+      <c r="B136" s="31"/>
+      <c r="C136" s="31"/>
+      <c r="D136" s="31"/>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A137" s="32"/>
-      <c r="B137" s="32"/>
-      <c r="C137" s="32"/>
-      <c r="D137" s="32"/>
+      <c r="A137" s="31"/>
+      <c r="B137" s="31"/>
+      <c r="C137" s="31"/>
+      <c r="D137" s="31"/>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A138" s="32"/>
-      <c r="B138" s="32"/>
-      <c r="C138" s="32"/>
-      <c r="D138" s="32"/>
+      <c r="A138" s="31"/>
+      <c r="B138" s="31"/>
+      <c r="C138" s="31"/>
+      <c r="D138" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
Aggiornate test chain Anagrafica Responsabili e Registro Trattamenti
</commit_message>
<xml_diff>
--- a/Documentazione/Attività sul progetto/DocAttivProg.xlsx
+++ b/Documentazione/Attività sul progetto/DocAttivProg.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\UniUD\Laurea Magistrale\Ingegneria del Software 2\Progetto-Ingegneria-Del-Sw-2\Documentazione\Attività sul progetto\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LUCA\Documents\Universita\INGEGNERIA DEL SOFTWARE\Progetto\Documentazione\Attività sul progetto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74757BBA-E144-48D7-B5F1-A7CBEADA6598}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" iterateDelta="1E-4"/>
+  <calcPr calcId="162913" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -31,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="29">
   <si>
     <t>Le categorie sono: Ispezione Codice, Documenti di progetto, Documenti di processo, Manuale, Sviluppo, Testing</t>
   </si>
@@ -123,7 +122,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yyyy"/>
   </numFmts>
@@ -383,6 +382,13 @@
     <xf numFmtId="10" fontId="0" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -390,13 +396,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="0" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -781,39 +780,39 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O138"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C128" sqref="C128"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G134" sqref="G134"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.5546875" customWidth="1"/>
-    <col min="2" max="2" width="23.44140625" customWidth="1"/>
-    <col min="3" max="3" width="15.5546875" customWidth="1"/>
-    <col min="4" max="4" width="10.88671875" customWidth="1"/>
-    <col min="5" max="7" width="8.6640625" customWidth="1"/>
-    <col min="8" max="8" width="26.33203125" customWidth="1"/>
-    <col min="9" max="11" width="17.33203125" customWidth="1"/>
-    <col min="12" max="14" width="17.44140625" customWidth="1"/>
-    <col min="15" max="1025" width="8.6640625" customWidth="1"/>
+    <col min="1" max="1" width="15.5703125" customWidth="1"/>
+    <col min="2" max="2" width="23.42578125" customWidth="1"/>
+    <col min="3" max="3" width="15.5703125" customWidth="1"/>
+    <col min="4" max="4" width="10.85546875" customWidth="1"/>
+    <col min="5" max="7" width="8.7109375" customWidth="1"/>
+    <col min="8" max="8" width="26.28515625" customWidth="1"/>
+    <col min="9" max="11" width="17.28515625" customWidth="1"/>
+    <col min="12" max="14" width="17.42578125" customWidth="1"/>
+    <col min="15" max="1025" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="F1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="F2" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
@@ -828,7 +827,7 @@
       </c>
       <c r="H3" s="2"/>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>6</v>
       </c>
@@ -841,13 +840,13 @@
       <c r="D4" s="6">
         <v>43484</v>
       </c>
-      <c r="H4" s="40" t="s">
+      <c r="H4" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="I4" s="40"/>
-      <c r="J4" s="40"/>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="I4" s="43"/>
+      <c r="J4" s="43"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>6</v>
       </c>
@@ -870,7 +869,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>6</v>
       </c>
@@ -892,10 +891,10 @@
       </c>
       <c r="J6" s="38">
         <f>I6/I12</f>
-        <v>5.1178314959037116E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+        <v>5.086960892731477E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>6</v>
       </c>
@@ -917,10 +916,10 @@
       </c>
       <c r="J7" s="38">
         <f>(I7/I12)</f>
-        <v>0.23596642055224032</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+        <v>0.23454307831506988</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>6</v>
       </c>
@@ -942,10 +941,10 @@
       </c>
       <c r="J8" s="38">
         <f>I8/I12</f>
-        <v>0.23626984929705674</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+        <v>0.23484467678697094</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>6</v>
       </c>
@@ -967,10 +966,10 @@
       </c>
       <c r="J9" s="38">
         <f>I9/I12</f>
-        <v>1.7598867199352684E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+        <v>1.7492711370262391E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>6</v>
       </c>
@@ -992,10 +991,10 @@
       </c>
       <c r="J10" s="38">
         <f>I10/I12</f>
-        <v>0.45898654799231314</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+        <v>0.45621795516236052</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>16</v>
       </c>
@@ -1013,14 +1012,14 @@
       </c>
       <c r="I11" s="12">
         <f>SUMIF(B:B,"Testing",C:C)</f>
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="J11" s="39">
         <f>I11/I12</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+        <v>6.0319694380215139E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>16</v>
       </c>
@@ -1038,14 +1037,14 @@
       </c>
       <c r="I12" s="14">
         <f>SUM(I6:I11)</f>
-        <v>9887</v>
+        <v>9947</v>
       </c>
       <c r="J12" s="15">
         <f>SUM(J6:J11)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>6</v>
       </c>
@@ -1060,7 +1059,7 @@
       </c>
       <c r="H13" s="2"/>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>6</v>
       </c>
@@ -1074,7 +1073,7 @@
         <v>43509</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>19</v>
       </c>
@@ -1087,18 +1086,18 @@
       <c r="D15" s="6">
         <v>43521</v>
       </c>
-      <c r="H15" s="41" t="s">
+      <c r="H15" s="44" t="s">
         <v>20</v>
       </c>
-      <c r="I15" s="41"/>
-      <c r="J15" s="41"/>
-      <c r="K15" s="41"/>
-      <c r="L15" s="41"/>
-      <c r="M15" s="41"/>
-      <c r="N15" s="41"/>
-      <c r="O15" s="41"/>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="I15" s="44"/>
+      <c r="J15" s="44"/>
+      <c r="K15" s="44"/>
+      <c r="L15" s="44"/>
+      <c r="M15" s="44"/>
+      <c r="N15" s="44"/>
+      <c r="O15" s="44"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>19</v>
       </c>
@@ -1136,7 +1135,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>25</v>
       </c>
@@ -1181,7 +1180,7 @@
         <v>2401</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>25</v>
       </c>
@@ -1226,7 +1225,7 @@
         <v>2805</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>25</v>
       </c>
@@ -1260,7 +1259,7 @@
       </c>
       <c r="M19" s="20">
         <f>SUMIFS(C:C,B:B,"Testing",A:A,"Luca")</f>
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="N19" s="20">
         <f>SUMIFS(C:C,B:B,"Ispezione codice",A:A,"Luca")</f>
@@ -1268,10 +1267,10 @@
       </c>
       <c r="O19" s="21">
         <f>SUM(I19:N19)</f>
-        <v>1763</v>
-      </c>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
+        <v>1823</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>25</v>
       </c>
@@ -1316,7 +1315,7 @@
         <v>2918</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>25</v>
       </c>
@@ -1350,18 +1349,18 @@
       </c>
       <c r="M21" s="36">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="N21" s="37">
         <f t="shared" si="0"/>
         <v>126.5</v>
       </c>
-      <c r="O21" s="45">
+      <c r="O21" s="42">
         <f>SUM(O17:O20)</f>
-        <v>9887</v>
-      </c>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
+        <v>9947</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>16</v>
       </c>
@@ -1375,7 +1374,7 @@
         <v>43487</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
         <v>16</v>
       </c>
@@ -1389,7 +1388,7 @@
         <v>43506</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
         <v>16</v>
       </c>
@@ -1402,18 +1401,18 @@
       <c r="D24" s="6">
         <v>43520</v>
       </c>
-      <c r="H24" s="42" t="s">
+      <c r="H24" s="45" t="s">
         <v>28</v>
       </c>
-      <c r="I24" s="42"/>
-      <c r="J24" s="42"/>
-      <c r="K24" s="42"/>
-      <c r="L24" s="42"/>
-      <c r="M24" s="42"/>
-      <c r="N24" s="42"/>
-      <c r="O24" s="42"/>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="I24" s="45"/>
+      <c r="J24" s="45"/>
+      <c r="K24" s="45"/>
+      <c r="L24" s="45"/>
+      <c r="M24" s="45"/>
+      <c r="N24" s="45"/>
+      <c r="O24" s="45"/>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
         <v>16</v>
       </c>
@@ -1451,7 +1450,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
         <v>16</v>
       </c>
@@ -1496,7 +1495,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
         <v>16</v>
       </c>
@@ -1541,7 +1540,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
         <v>19</v>
       </c>
@@ -1559,11 +1558,11 @@
       </c>
       <c r="I28" s="34">
         <f>I19/O19</f>
-        <v>0.42370958593306862</v>
+        <v>0.4097641250685683</v>
       </c>
       <c r="J28" s="34">
         <f>J19/O19</f>
-        <v>0.48326715825297789</v>
+        <v>0.46736149204607791</v>
       </c>
       <c r="K28" s="34">
         <f>K19/O19</f>
@@ -1571,22 +1570,22 @@
       </c>
       <c r="L28" s="34">
         <f>L19/O19</f>
-        <v>3.4032898468519569E-2</v>
+        <v>3.2912781130005488E-2</v>
       </c>
       <c r="M28" s="34">
         <f>M19/O19</f>
-        <v>0</v>
+        <v>3.2912781130005488E-2</v>
       </c>
       <c r="N28" s="34">
         <f>N19/O19</f>
-        <v>5.8990357345433918E-2</v>
+        <v>5.704882062534284E-2</v>
       </c>
       <c r="O28" s="28">
         <f>SUM(I28:N28)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
         <v>6</v>
       </c>
@@ -1631,7 +1630,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
         <v>25</v>
       </c>
@@ -1649,11 +1648,11 @@
       </c>
       <c r="I30" s="32">
         <f>AVERAGE(I26:I29)</f>
-        <v>0.26031995643094546</v>
+        <v>0.25683359121482041</v>
       </c>
       <c r="J30" s="32">
         <f>AVERAGE(J26:J29)</f>
-        <v>0.26944632974390426</v>
+        <v>0.26546991319217927</v>
       </c>
       <c r="K30" s="32">
         <f>AVERAGE(K26:K29)</f>
@@ -1661,22 +1660,22 @@
       </c>
       <c r="L30" s="32">
         <f>AVERAGE(L26:L29)</f>
-        <v>0.39999272856887569</v>
+        <v>0.39971269923424724</v>
       </c>
       <c r="M30" s="32">
         <f t="shared" ref="M30" si="1">AVERAGE(M26:M29)</f>
-        <v>0</v>
+        <v>8.2281952825013719E-3</v>
       </c>
       <c r="N30" s="33">
         <f>AVERAGE(N26:N29)</f>
-        <v>5.2123534194217093E-2</v>
-      </c>
-      <c r="O30" s="44">
+        <v>5.163815001419432E-2</v>
+      </c>
+      <c r="O30" s="41">
         <f>SUM(I30:N30)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
         <v>25</v>
       </c>
@@ -1690,7 +1689,7 @@
         <v>43531</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
         <v>25</v>
       </c>
@@ -1704,7 +1703,7 @@
         <v>43532</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
         <v>25</v>
       </c>
@@ -1718,7 +1717,7 @@
         <v>43533</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
         <v>25</v>
       </c>
@@ -1732,7 +1731,7 @@
         <v>43534</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
         <v>6</v>
       </c>
@@ -1746,7 +1745,7 @@
         <v>43546</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
         <v>6</v>
       </c>
@@ -1760,7 +1759,7 @@
         <v>43546</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
         <v>16</v>
       </c>
@@ -1774,7 +1773,7 @@
         <v>43376</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
         <v>16</v>
       </c>
@@ -1788,7 +1787,7 @@
         <v>43407</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
         <v>25</v>
       </c>
@@ -1802,7 +1801,7 @@
         <v>43546</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
         <v>19</v>
       </c>
@@ -1816,7 +1815,7 @@
         <v>43553</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
         <v>25</v>
       </c>
@@ -1830,7 +1829,7 @@
         <v>43553</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
         <v>16</v>
       </c>
@@ -1844,7 +1843,7 @@
         <v>43553</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
         <v>19</v>
       </c>
@@ -1858,7 +1857,7 @@
         <v>43481</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
         <v>19</v>
       </c>
@@ -1872,7 +1871,7 @@
         <v>43442</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
         <v>19</v>
       </c>
@@ -1886,7 +1885,7 @@
         <v>43448</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="5" t="s">
         <v>19</v>
       </c>
@@ -1900,7 +1899,7 @@
         <v>43468</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
         <v>19</v>
       </c>
@@ -1914,7 +1913,7 @@
         <v>43478</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
         <v>6</v>
       </c>
@@ -1928,7 +1927,7 @@
         <v>43449</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="5" t="s">
         <v>6</v>
       </c>
@@ -1942,7 +1941,7 @@
         <v>43450</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="5" t="s">
         <v>19</v>
       </c>
@@ -1956,7 +1955,7 @@
         <v>43558</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="5" t="s">
         <v>25</v>
       </c>
@@ -1970,7 +1969,7 @@
         <v>43558</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="5" t="s">
         <v>6</v>
       </c>
@@ -1984,7 +1983,7 @@
         <v>43558</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="5" t="s">
         <v>25</v>
       </c>
@@ -1998,7 +1997,7 @@
         <v>43559</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="5" t="s">
         <v>19</v>
       </c>
@@ -2012,7 +2011,7 @@
         <v>43571</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="5" t="s">
         <v>25</v>
       </c>
@@ -2026,7 +2025,7 @@
         <v>43571</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="5" t="s">
         <v>19</v>
       </c>
@@ -2040,7 +2039,7 @@
         <v>43572</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="5" t="s">
         <v>19</v>
       </c>
@@ -2054,7 +2053,7 @@
         <v>43574</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="5" t="s">
         <v>6</v>
       </c>
@@ -2068,7 +2067,7 @@
         <v>43577</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="5" t="s">
         <v>6</v>
       </c>
@@ -2082,7 +2081,7 @@
         <v>43578</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="5" t="s">
         <v>25</v>
       </c>
@@ -2096,7 +2095,7 @@
         <v>43578</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="5" t="s">
         <v>6</v>
       </c>
@@ -2110,7 +2109,7 @@
         <v>43581</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="5" t="s">
         <v>6</v>
       </c>
@@ -2124,7 +2123,7 @@
         <v>43584</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="5" t="s">
         <v>6</v>
       </c>
@@ -2138,7 +2137,7 @@
         <v>43585</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="5" t="s">
         <v>19</v>
       </c>
@@ -2152,7 +2151,7 @@
         <v>43585</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="5" t="s">
         <v>19</v>
       </c>
@@ -2166,7 +2165,7 @@
         <v>43587</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="5" t="s">
         <v>16</v>
       </c>
@@ -2180,7 +2179,7 @@
         <v>43587</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="5" t="s">
         <v>16</v>
       </c>
@@ -2194,7 +2193,7 @@
         <v>43587</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="5" t="s">
         <v>16</v>
       </c>
@@ -2208,7 +2207,7 @@
         <v>43587</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="5" t="s">
         <v>16</v>
       </c>
@@ -2222,7 +2221,7 @@
         <v>43588</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="5" t="s">
         <v>25</v>
       </c>
@@ -2236,7 +2235,7 @@
         <v>43588</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="5" t="s">
         <v>25</v>
       </c>
@@ -2250,7 +2249,7 @@
         <v>43589</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="5" t="s">
         <v>16</v>
       </c>
@@ -2264,7 +2263,7 @@
         <v>43589</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="5" t="s">
         <v>25</v>
       </c>
@@ -2278,7 +2277,7 @@
         <v>43590</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="5" t="s">
         <v>16</v>
       </c>
@@ -2292,7 +2291,7 @@
         <v>43590</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="5" t="s">
         <v>6</v>
       </c>
@@ -2306,7 +2305,7 @@
         <v>43593</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="5" t="s">
         <v>25</v>
       </c>
@@ -2320,7 +2319,7 @@
         <v>43593</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="5" t="s">
         <v>19</v>
       </c>
@@ -2334,7 +2333,7 @@
         <v>43593</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="5" t="s">
         <v>16</v>
       </c>
@@ -2348,7 +2347,7 @@
         <v>43593</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="5" t="s">
         <v>25</v>
       </c>
@@ -2362,7 +2361,7 @@
         <v>43593</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="5" t="s">
         <v>19</v>
       </c>
@@ -2376,7 +2375,7 @@
         <v>43593</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="5" t="s">
         <v>16</v>
       </c>
@@ -2390,7 +2389,7 @@
         <v>43593</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="5" t="s">
         <v>16</v>
       </c>
@@ -2404,7 +2403,7 @@
         <v>43594</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="5" t="s">
         <v>25</v>
       </c>
@@ -2418,7 +2417,7 @@
         <v>43594</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="5" t="s">
         <v>6</v>
       </c>
@@ -2432,7 +2431,7 @@
         <v>43598</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" s="5" t="s">
         <v>6</v>
       </c>
@@ -2446,7 +2445,7 @@
         <v>43598</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" s="5" t="s">
         <v>25</v>
       </c>
@@ -2460,7 +2459,7 @@
         <v>43595</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" s="5" t="s">
         <v>16</v>
       </c>
@@ -2474,7 +2473,7 @@
         <v>43595</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" s="5" t="s">
         <v>25</v>
       </c>
@@ -2488,7 +2487,7 @@
         <v>43599</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" s="5" t="s">
         <v>16</v>
       </c>
@@ -2502,7 +2501,7 @@
         <v>43599</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" s="5" t="s">
         <v>6</v>
       </c>
@@ -2516,7 +2515,7 @@
         <v>43600</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" s="5" t="s">
         <v>19</v>
       </c>
@@ -2530,7 +2529,7 @@
         <v>43600</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" s="5" t="s">
         <v>16</v>
       </c>
@@ -2544,7 +2543,7 @@
         <v>43600</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" s="5" t="s">
         <v>25</v>
       </c>
@@ -2558,7 +2557,7 @@
         <v>43600</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" s="5" t="s">
         <v>6</v>
       </c>
@@ -2572,7 +2571,7 @@
         <v>43600</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" s="5" t="s">
         <v>19</v>
       </c>
@@ -2586,7 +2585,7 @@
         <v>43600</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" s="5" t="s">
         <v>16</v>
       </c>
@@ -2600,7 +2599,7 @@
         <v>43600</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" s="5" t="s">
         <v>25</v>
       </c>
@@ -2614,7 +2613,7 @@
         <v>43600</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" s="5" t="s">
         <v>25</v>
       </c>
@@ -2628,7 +2627,7 @@
         <v>43603</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" s="5" t="s">
         <v>16</v>
       </c>
@@ -2642,7 +2641,7 @@
         <v>43603</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" s="5" t="s">
         <v>25</v>
       </c>
@@ -2656,7 +2655,7 @@
         <v>43604</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" s="5" t="s">
         <v>16</v>
       </c>
@@ -2670,7 +2669,7 @@
         <v>43604</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" s="5" t="s">
         <v>16</v>
       </c>
@@ -2684,7 +2683,7 @@
         <v>43604</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" s="5" t="s">
         <v>16</v>
       </c>
@@ -2698,7 +2697,7 @@
         <v>43605</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" s="5" t="s">
         <v>25</v>
       </c>
@@ -2712,7 +2711,7 @@
         <v>43606</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" s="5" t="s">
         <v>6</v>
       </c>
@@ -2726,7 +2725,7 @@
         <v>43607</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" s="5" t="s">
         <v>16</v>
       </c>
@@ -2740,7 +2739,7 @@
         <v>43607</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" s="5" t="s">
         <v>25</v>
       </c>
@@ -2754,7 +2753,7 @@
         <v>43607</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" s="5" t="s">
         <v>6</v>
       </c>
@@ -2768,7 +2767,7 @@
         <v>43607</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" s="5" t="s">
         <v>16</v>
       </c>
@@ -2782,7 +2781,7 @@
         <v>43607</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" s="5" t="s">
         <v>25</v>
       </c>
@@ -2796,7 +2795,7 @@
         <v>43607</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" s="5" t="s">
         <v>16</v>
       </c>
@@ -2810,7 +2809,7 @@
         <v>43607</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" s="5" t="s">
         <v>25</v>
       </c>
@@ -2824,7 +2823,7 @@
         <v>43607</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" s="5" t="s">
         <v>25</v>
       </c>
@@ -2838,7 +2837,7 @@
         <v>43607</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" s="5" t="s">
         <v>6</v>
       </c>
@@ -2852,7 +2851,7 @@
         <v>43608</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" s="5" t="s">
         <v>6</v>
       </c>
@@ -2866,7 +2865,7 @@
         <v>43609</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" s="5" t="s">
         <v>16</v>
       </c>
@@ -2880,7 +2879,7 @@
         <v>43608</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" s="5" t="s">
         <v>25</v>
       </c>
@@ -2894,7 +2893,7 @@
         <v>43608</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" s="5" t="s">
         <v>25</v>
       </c>
@@ -2908,7 +2907,7 @@
         <v>43609</v>
       </c>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" s="5" t="s">
         <v>19</v>
       </c>
@@ -2922,7 +2921,7 @@
         <v>43614</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" s="5" t="s">
         <v>16</v>
       </c>
@@ -2936,7 +2935,7 @@
         <v>43614</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" s="30" t="s">
         <v>6</v>
       </c>
@@ -2950,7 +2949,7 @@
         <v>43614</v>
       </c>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" s="5" t="s">
         <v>19</v>
       </c>
@@ -2964,7 +2963,7 @@
         <v>43614</v>
       </c>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" s="5" t="s">
         <v>16</v>
       </c>
@@ -2978,7 +2977,7 @@
         <v>43614</v>
       </c>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" s="30" t="s">
         <v>6</v>
       </c>
@@ -2992,7 +2991,7 @@
         <v>43614</v>
       </c>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" s="31" t="s">
         <v>25</v>
       </c>
@@ -3006,7 +3005,7 @@
         <v>43614</v>
       </c>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" s="31" t="s">
         <v>6</v>
       </c>
@@ -3016,11 +3015,11 @@
       <c r="C126" s="31">
         <v>64</v>
       </c>
-      <c r="D126" s="43">
+      <c r="D126" s="40">
         <v>43616</v>
       </c>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" s="31" t="s">
         <v>6</v>
       </c>
@@ -3030,71 +3029,79 @@
       <c r="C127" s="31">
         <v>98</v>
       </c>
-      <c r="D127" s="43">
+      <c r="D127" s="40">
         <v>43616</v>
       </c>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A128" s="31"/>
-      <c r="B128" s="31"/>
-      <c r="C128" s="31"/>
-      <c r="D128" s="31"/>
-    </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A128" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="B128" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="C128" s="31">
+        <v>60</v>
+      </c>
+      <c r="D128" s="40">
+        <v>43617</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" s="31"/>
       <c r="B129" s="31"/>
       <c r="C129" s="31"/>
       <c r="D129" s="31"/>
     </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" s="31"/>
       <c r="B130" s="31"/>
       <c r="C130" s="31"/>
       <c r="D130" s="31"/>
     </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" s="31"/>
       <c r="B131" s="31"/>
       <c r="C131" s="31"/>
       <c r="D131" s="31"/>
     </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132" s="31"/>
       <c r="B132" s="31"/>
       <c r="C132" s="31"/>
       <c r="D132" s="31"/>
     </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133" s="31"/>
       <c r="B133" s="31"/>
       <c r="C133" s="31"/>
       <c r="D133" s="31"/>
     </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134" s="31"/>
       <c r="B134" s="31"/>
       <c r="C134" s="31"/>
       <c r="D134" s="31"/>
     </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135" s="31"/>
       <c r="B135" s="31"/>
       <c r="C135" s="31"/>
       <c r="D135" s="31"/>
     </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136" s="31"/>
       <c r="B136" s="31"/>
       <c r="C136" s="31"/>
       <c r="D136" s="31"/>
     </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A137" s="31"/>
       <c r="B137" s="31"/>
       <c r="C137" s="31"/>
       <c r="D137" s="31"/>
     </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A138" s="31"/>
       <c r="B138" s="31"/>
       <c r="C138" s="31"/>

</xml_diff>

<commit_message>
Modifica formato date in AA-MM-GG
</commit_message>
<xml_diff>
--- a/Documentazione/Attività sul progetto/DocAttivProg.xlsx
+++ b/Documentazione/Attività sul progetto/DocAttivProg.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="30">
   <si>
     <t>Le categorie sono: Ispezione Codice, Documenti di progetto, Documenti di processo, Manuale, Sviluppo, Testing</t>
   </si>
@@ -281,15 +281,6 @@
   </cellStyleXfs>
   <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -391,6 +382,15 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -742,8 +742,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O138"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E135" sqref="E135"/>
+    <sheetView tabSelected="1" topLeftCell="A115" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B137" sqref="B137"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -760,2367 +760,2375 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="F2" s="6" t="s">
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="F2" s="3" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H3" s="5"/>
+      <c r="H3" s="2"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="8">
+      <c r="A4" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="5">
         <v>98</v>
       </c>
-      <c r="D4" s="9">
+      <c r="D4" s="6">
         <v>43484</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="H4" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
+      <c r="I4" s="44"/>
+      <c r="J4" s="44"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="8">
+      <c r="A5" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="5">
         <v>149</v>
       </c>
-      <c r="D5" s="9">
+      <c r="D5" s="6">
         <v>43493</v>
       </c>
-      <c r="H5" s="10" t="s">
+      <c r="H5" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="I5" s="11" t="s">
+      <c r="I5" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="J5" s="11" t="s">
+      <c r="J5" s="8" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="8" t="s">
+      <c r="A6" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="8">
+      <c r="C6" s="5">
         <v>135</v>
       </c>
-      <c r="D6" s="9">
+      <c r="D6" s="6">
         <v>43494</v>
       </c>
-      <c r="H6" s="12" t="s">
+      <c r="H6" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="I6" s="13">
+      <c r="I6" s="10">
         <f>SUMIF(B:B,"Ispezione codice",C:C)</f>
         <v>536</v>
       </c>
-      <c r="J6" s="14">
+      <c r="J6" s="11">
         <f>I6/I12</f>
-        <v>5.0767190755824969E-2</v>
+        <v>5.0599452468611347E-2</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" s="8">
+      <c r="A7" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="5">
         <v>53</v>
       </c>
-      <c r="D7" s="9">
+      <c r="D7" s="6">
         <v>43494</v>
       </c>
-      <c r="H7" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="I7" s="13">
+      <c r="H7" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="I7" s="10">
         <f>SUMIF(B:B,"Documenti di progetto",C:C)</f>
-        <v>2303</v>
-      </c>
-      <c r="J7" s="14">
+        <v>2338</v>
+      </c>
+      <c r="J7" s="11">
         <f>(I7/I12)</f>
-        <v>0.2181284334154196</v>
+        <v>0.22071179080524875</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" s="8">
+      <c r="A8" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="5">
         <v>87</v>
       </c>
-      <c r="D8" s="9">
+      <c r="D8" s="6">
         <v>43495</v>
       </c>
-      <c r="H8" s="12" t="s">
+      <c r="H8" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="I8" s="13">
+      <c r="I8" s="10">
         <f>SUMIF(B:B,"Documenti di processo",C:C)</f>
         <v>2336</v>
       </c>
-      <c r="J8" s="14">
+      <c r="J8" s="11">
         <f>I8/I12</f>
-        <v>0.22125402538359537</v>
+        <v>0.22052298687812708</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" s="8" t="s">
+      <c r="A9" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="8">
+      <c r="C9" s="5">
         <v>74</v>
       </c>
-      <c r="D9" s="9">
+      <c r="D9" s="6">
         <v>43495</v>
       </c>
-      <c r="H9" s="12" t="s">
+      <c r="H9" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="I9" s="13">
+      <c r="I9" s="10">
         <f>SUMIF(B:B,"Manuale",C:C)</f>
         <v>174</v>
       </c>
-      <c r="J9" s="14">
+      <c r="J9" s="11">
         <f>I9/I12</f>
-        <v>1.6480394014017807E-2</v>
+        <v>1.642594165958652E-2</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B10" s="8" t="s">
+      <c r="A10" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="8">
+      <c r="C10" s="5">
         <v>32</v>
       </c>
-      <c r="D10" s="9">
+      <c r="D10" s="6">
         <v>43499</v>
       </c>
-      <c r="H10" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="I10" s="13">
+      <c r="H10" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="I10" s="10">
         <f>SUMIF(B:B,"Sviluppo",C:C)</f>
         <v>5119</v>
       </c>
-      <c r="J10" s="14">
+      <c r="J10" s="11">
         <f>I10/I12</f>
-        <v>0.48484561469975374</v>
+        <v>0.48324365146795051</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B11" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C11" s="8">
+      <c r="A11" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="5">
         <v>75</v>
       </c>
-      <c r="D11" s="9">
+      <c r="D11" s="6">
         <v>43497</v>
       </c>
-      <c r="H11" s="15" t="s">
+      <c r="H11" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="I11" s="16">
+      <c r="I11" s="13">
         <f>SUMIF(B:B,"Testing",C:C)</f>
         <v>90</v>
       </c>
-      <c r="J11" s="17">
+      <c r="J11" s="14">
         <f>I11/I12</f>
-        <v>8.5243417313885204E-3</v>
+        <v>8.4961767204757861E-3</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B12" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C12" s="8">
+      <c r="A12" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" s="5">
         <v>55</v>
       </c>
-      <c r="D12" s="9">
+      <c r="D12" s="6">
         <v>43503</v>
       </c>
-      <c r="H12" s="18" t="s">
+      <c r="H12" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="I12" s="19">
+      <c r="I12" s="16">
         <f>SUM(I6:I11)</f>
-        <v>10558</v>
-      </c>
-      <c r="J12" s="20">
+        <v>10593</v>
+      </c>
+      <c r="J12" s="17">
         <f>SUM(J6:J11)</f>
-        <v>1</v>
+        <v>0.99999999999999989</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A13" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B13" s="8" t="s">
+      <c r="A13" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="8">
+      <c r="C13" s="5">
         <v>127</v>
       </c>
-      <c r="D13" s="9">
+      <c r="D13" s="6">
         <v>43505</v>
       </c>
-      <c r="H13" s="5"/>
+      <c r="H13" s="2"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A14" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B14" s="8" t="s">
+      <c r="A14" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="8">
+      <c r="C14" s="5">
         <v>24</v>
       </c>
-      <c r="D14" s="9">
+      <c r="D14" s="6">
         <v>43509</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A15" s="8" t="s">
+      <c r="A15" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B15" s="8" t="s">
+      <c r="B15" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="8">
+      <c r="C15" s="5">
         <v>195</v>
       </c>
-      <c r="D15" s="9">
+      <c r="D15" s="6">
         <v>43521</v>
       </c>
-      <c r="H15" s="2" t="s">
+      <c r="H15" s="45" t="s">
         <v>20</v>
       </c>
-      <c r="I15" s="2"/>
-      <c r="J15" s="2"/>
-      <c r="K15" s="2"/>
-      <c r="L15" s="2"/>
-      <c r="M15" s="2"/>
-      <c r="N15" s="2"/>
-      <c r="O15" s="2"/>
+      <c r="I15" s="45"/>
+      <c r="J15" s="45"/>
+      <c r="K15" s="45"/>
+      <c r="L15" s="45"/>
+      <c r="M15" s="45"/>
+      <c r="N15" s="45"/>
+      <c r="O15" s="45"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A16" s="8" t="s">
+      <c r="A16" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="8" t="s">
+      <c r="B16" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C16" s="8">
+      <c r="C16" s="5">
         <v>105</v>
       </c>
-      <c r="D16" s="9">
+      <c r="D16" s="6">
         <v>43523</v>
       </c>
-      <c r="H16" s="21" t="s">
+      <c r="H16" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="I16" s="22" t="s">
+      <c r="I16" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="J16" s="22" t="s">
+      <c r="J16" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="K16" s="22" t="s">
+      <c r="K16" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="L16" s="22" t="s">
-        <v>15</v>
-      </c>
-      <c r="M16" s="22" t="s">
+      <c r="L16" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="M16" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="N16" s="22" t="s">
+      <c r="N16" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="O16" s="23" t="s">
+      <c r="O16" s="20" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A17" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B17" s="8" t="s">
+      <c r="A17" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B17" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C17" s="8">
+      <c r="C17" s="5">
         <v>30</v>
       </c>
-      <c r="D17" s="9">
+      <c r="D17" s="6">
         <v>43519</v>
       </c>
-      <c r="H17" s="24" t="s">
-        <v>6</v>
-      </c>
-      <c r="I17" s="25">
+      <c r="H17" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="I17" s="22">
         <f>SUMIFS(C:C,B:B,"Documenti di progetto",A:A,"Giovanni")</f>
         <v>981</v>
       </c>
-      <c r="J17" s="25">
+      <c r="J17" s="22">
         <f>SUMIFS(C:C,B:B,"Documenti di processo",A:A,"Giovanni")</f>
         <v>1112</v>
       </c>
-      <c r="K17" s="25">
+      <c r="K17" s="22">
         <f>SUMIFS(C:C,B:B,"Manuale",A:A,"Giovanni")</f>
         <v>174</v>
       </c>
-      <c r="L17" s="25">
+      <c r="L17" s="22">
         <f>SUMIFS(C:C,B:B,"Sviluppo",A:A,"Giovanni")</f>
         <v>0</v>
       </c>
-      <c r="M17" s="25">
+      <c r="M17" s="22">
         <f>SUMIFS(C:C,B:B,"Testing",A:A,"Giovanni")</f>
         <v>0</v>
       </c>
-      <c r="N17" s="25">
+      <c r="N17" s="22">
         <f>SUMIFS(C:C,B:B,"Ispezione codice",A:A,"Giovanni")</f>
         <v>134</v>
       </c>
-      <c r="O17" s="26">
+      <c r="O17" s="23">
         <f>SUM(I17:N17)</f>
         <v>2401</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A18" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B18" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C18" s="8">
+      <c r="A18" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18" s="5">
         <v>100</v>
       </c>
-      <c r="D18" s="9">
+      <c r="D18" s="6">
         <v>43520</v>
       </c>
-      <c r="H18" s="24" t="s">
-        <v>25</v>
-      </c>
-      <c r="I18" s="25">
+      <c r="H18" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="I18" s="22">
         <f>SUMIFS(C:C,B:B,"Documenti di progetto",A:A,"Hristina")</f>
         <v>140</v>
       </c>
-      <c r="J18" s="25">
+      <c r="J18" s="22">
         <f>SUMIFS(C:C,B:B,"Documenti di processo",A:A,"Hristina")</f>
         <v>282</v>
       </c>
-      <c r="K18" s="25">
+      <c r="K18" s="22">
         <f>SUMIFS(C:C,B:B,"Manuale",A:A,"Hristina")</f>
         <v>0</v>
       </c>
-      <c r="L18" s="25">
+      <c r="L18" s="22">
         <f>SUMIFS(C:C,B:B,"Sviluppo",A:A,"Hristina")</f>
         <v>2567</v>
       </c>
-      <c r="M18" s="25">
+      <c r="M18" s="22">
         <f>SUMIFS(C:C,B:B,"Testing",A:A,"Hristina")</f>
         <v>0</v>
       </c>
-      <c r="N18" s="25">
+      <c r="N18" s="22">
         <f>SUMIFS(C:C,B:B,"Ispezione codice",A:A,"Hristina")</f>
         <v>134</v>
       </c>
-      <c r="O18" s="26">
+      <c r="O18" s="23">
         <f>SUM(I18:N18)</f>
         <v>3123</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A19" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B19" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C19" s="8">
+      <c r="A19" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C19" s="5">
         <v>125</v>
       </c>
-      <c r="D19" s="9">
+      <c r="D19" s="6">
         <v>43522</v>
       </c>
-      <c r="H19" s="24" t="s">
+      <c r="H19" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="I19" s="25">
+      <c r="I19" s="22">
         <f>SUMIFS(C:C,B:B,"Documenti di progetto",A:A,"Luca")</f>
-        <v>747</v>
-      </c>
-      <c r="J19" s="25">
+        <v>782</v>
+      </c>
+      <c r="J19" s="22">
         <f>SUMIFS(C:C,B:B,"Documenti di processo",A:A,"Luca")</f>
         <v>852</v>
       </c>
-      <c r="K19" s="25">
+      <c r="K19" s="22">
         <f>SUMIFS(C:C,B:B,"Manuale",A:A,"Luca")</f>
         <v>0</v>
       </c>
-      <c r="L19" s="25">
+      <c r="L19" s="22">
         <f>SUMIFS(C:C,B:B,"Sviluppo",A:A,"Luca")</f>
         <v>60</v>
       </c>
-      <c r="M19" s="25">
+      <c r="M19" s="22">
         <f>SUMIFS(C:C,B:B,"Testing",A:A,"Luca")</f>
         <v>90</v>
       </c>
-      <c r="N19" s="25">
+      <c r="N19" s="22">
         <f>SUMIFS(C:C,B:B,"Ispezione codice",A:A,"Luca")</f>
         <v>134</v>
       </c>
-      <c r="O19" s="26">
+      <c r="O19" s="23">
         <f>SUM(I19:N19)</f>
-        <v>1883</v>
+        <v>1918</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A20" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B20" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C20" s="8">
+      <c r="A20" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C20" s="5">
         <v>170</v>
       </c>
-      <c r="D20" s="9">
+      <c r="D20" s="6">
         <v>43523</v>
       </c>
-      <c r="H20" s="24" t="s">
-        <v>16</v>
-      </c>
-      <c r="I20" s="25">
+      <c r="H20" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="I20" s="22">
         <f>SUMIFS(C:C,B:B,"Documenti di progetto",A:A,"Viktorija")</f>
         <v>435</v>
       </c>
-      <c r="J20" s="25">
+      <c r="J20" s="22">
         <f>SUMIFS(C:C,B:B,"Documenti di processo",A:A,"Viktorija")</f>
         <v>90</v>
       </c>
-      <c r="K20" s="25">
+      <c r="K20" s="22">
         <f>SUMIFS(C:C,B:B,"Manuale",A:A,"Viktorija")</f>
         <v>0</v>
       </c>
-      <c r="L20" s="25">
+      <c r="L20" s="22">
         <f>SUMIFS(C:C,B:B,"Sviluppo",A:A,"Viktorija")</f>
         <v>2492</v>
       </c>
-      <c r="M20" s="25">
+      <c r="M20" s="22">
         <f>SUMIFS(C:C,B:B,"Testing",A:A,"Viktorija")</f>
         <v>0</v>
       </c>
-      <c r="N20" s="25">
+      <c r="N20" s="22">
         <f>SUMIFS(C:C,B:B,"Ispezione codice",A:A,"Viktorija")</f>
         <v>134</v>
       </c>
-      <c r="O20" s="26">
+      <c r="O20" s="23">
         <f>SUM(I20:N20)</f>
         <v>3151</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A21" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B21" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C21" s="8">
+      <c r="A21" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C21" s="5">
         <v>65</v>
       </c>
-      <c r="D21" s="9">
+      <c r="D21" s="6">
         <v>43524</v>
       </c>
-      <c r="H21" s="27" t="s">
+      <c r="H21" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="I21" s="28">
+      <c r="I21" s="25">
         <f t="shared" ref="I21:N21" si="0">AVERAGE(I17:I20)</f>
-        <v>575.75</v>
-      </c>
-      <c r="J21" s="29">
+        <v>584.5</v>
+      </c>
+      <c r="J21" s="26">
         <f t="shared" si="0"/>
         <v>584</v>
       </c>
-      <c r="K21" s="29">
+      <c r="K21" s="26">
         <f t="shared" si="0"/>
         <v>43.5</v>
       </c>
-      <c r="L21" s="29">
+      <c r="L21" s="26">
         <f t="shared" si="0"/>
         <v>1279.75</v>
       </c>
-      <c r="M21" s="29">
+      <c r="M21" s="26">
         <f t="shared" si="0"/>
         <v>22.5</v>
       </c>
-      <c r="N21" s="30">
+      <c r="N21" s="27">
         <f t="shared" si="0"/>
         <v>134</v>
       </c>
-      <c r="O21" s="31">
+      <c r="O21" s="28">
         <f>SUM(O17:O20)</f>
-        <v>10558</v>
+        <v>10593</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A22" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B22" s="8" t="s">
+      <c r="A22" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B22" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C22" s="8">
+      <c r="C22" s="5">
         <v>60</v>
       </c>
-      <c r="D22" s="9">
+      <c r="D22" s="6">
         <v>43487</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A23" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B23" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C23" s="8">
+      <c r="A23" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C23" s="5">
         <v>103</v>
       </c>
-      <c r="D23" s="9">
+      <c r="D23" s="6">
         <v>43506</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A24" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B24" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C24" s="8">
+      <c r="A24" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C24" s="5">
         <v>100</v>
       </c>
-      <c r="D24" s="9">
+      <c r="D24" s="6">
         <v>43520</v>
       </c>
-      <c r="H24" s="1" t="s">
+      <c r="H24" s="46" t="s">
         <v>28</v>
       </c>
-      <c r="I24" s="1"/>
-      <c r="J24" s="1"/>
-      <c r="K24" s="1"/>
-      <c r="L24" s="1"/>
-      <c r="M24" s="1"/>
-      <c r="N24" s="1"/>
-      <c r="O24" s="1"/>
+      <c r="I24" s="46"/>
+      <c r="J24" s="46"/>
+      <c r="K24" s="46"/>
+      <c r="L24" s="46"/>
+      <c r="M24" s="46"/>
+      <c r="N24" s="46"/>
+      <c r="O24" s="46"/>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A25" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B25" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C25" s="8">
+      <c r="A25" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C25" s="5">
         <v>170</v>
       </c>
-      <c r="D25" s="9">
+      <c r="D25" s="6">
         <v>43523</v>
       </c>
-      <c r="H25" s="32" t="s">
+      <c r="H25" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="I25" s="33" t="s">
+      <c r="I25" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="J25" s="33" t="s">
+      <c r="J25" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="K25" s="33" t="s">
+      <c r="K25" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="L25" s="33" t="s">
-        <v>15</v>
-      </c>
-      <c r="M25" s="33" t="s">
+      <c r="L25" s="30" t="s">
+        <v>15</v>
+      </c>
+      <c r="M25" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="N25" s="33" t="s">
+      <c r="N25" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="O25" s="34" t="s">
+      <c r="O25" s="31" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A26" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B26" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C26" s="8">
+      <c r="A26" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C26" s="5">
         <v>45</v>
       </c>
-      <c r="D26" s="9">
+      <c r="D26" s="6">
         <v>43524</v>
       </c>
-      <c r="H26" s="35" t="s">
-        <v>6</v>
-      </c>
-      <c r="I26" s="36">
+      <c r="H26" s="32" t="s">
+        <v>6</v>
+      </c>
+      <c r="I26" s="33">
         <f>I17/O17</f>
         <v>0.40857975843398586</v>
       </c>
-      <c r="J26" s="36">
+      <c r="J26" s="33">
         <f>J17/O17</f>
         <v>0.46314035818408994</v>
       </c>
-      <c r="K26" s="36">
+      <c r="K26" s="33">
         <f>K17/O17</f>
         <v>7.2469804248229908E-2</v>
       </c>
-      <c r="L26" s="36">
+      <c r="L26" s="33">
         <f>L17/O17</f>
         <v>0</v>
       </c>
-      <c r="M26" s="36">
+      <c r="M26" s="33">
         <f>M17/O17</f>
         <v>0</v>
       </c>
-      <c r="N26" s="36">
+      <c r="N26" s="33">
         <f>N17/O17</f>
         <v>5.5810079133694297E-2</v>
       </c>
-      <c r="O26" s="37">
+      <c r="O26" s="34">
         <f>SUM(I26:N26)</f>
         <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A27" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B27" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C27" s="8">
-        <v>25</v>
-      </c>
-      <c r="D27" s="9">
+      <c r="A27" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C27" s="5">
+        <v>25</v>
+      </c>
+      <c r="D27" s="6">
         <v>43530</v>
       </c>
-      <c r="H27" s="35" t="s">
-        <v>25</v>
-      </c>
-      <c r="I27" s="36">
+      <c r="H27" s="32" t="s">
+        <v>25</v>
+      </c>
+      <c r="I27" s="33">
         <f>I18/O18</f>
         <v>4.4828690361831569E-2</v>
       </c>
-      <c r="J27" s="36">
+      <c r="J27" s="33">
         <f>J18/O18</f>
         <v>9.0297790585975021E-2</v>
       </c>
-      <c r="K27" s="36">
+      <c r="K27" s="33">
         <f>K18/O18</f>
         <v>0</v>
       </c>
-      <c r="L27" s="36">
+      <c r="L27" s="33">
         <f>L18/O18</f>
         <v>0.82196605827729752</v>
       </c>
-      <c r="M27" s="36">
+      <c r="M27" s="33">
         <f>M18/O18</f>
         <v>0</v>
       </c>
-      <c r="N27" s="36">
+      <c r="N27" s="33">
         <f>N18/O18</f>
         <v>4.2907460774895934E-2</v>
       </c>
-      <c r="O27" s="37">
+      <c r="O27" s="34">
         <f>SUM(I27:N27)</f>
         <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A28" s="8" t="s">
+      <c r="A28" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B28" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C28" s="8">
-        <v>15</v>
-      </c>
-      <c r="D28" s="9">
+      <c r="B28" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C28" s="5">
+        <v>15</v>
+      </c>
+      <c r="D28" s="6">
         <v>43532</v>
       </c>
-      <c r="H28" s="35" t="s">
+      <c r="H28" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="I28" s="36">
+      <c r="I28" s="33">
         <f>I19/O19</f>
-        <v>0.39670738183749338</v>
-      </c>
-      <c r="J28" s="36">
+        <v>0.40771637122002086</v>
+      </c>
+      <c r="J28" s="33">
         <f>J19/O19</f>
-        <v>0.45246946362187995</v>
-      </c>
-      <c r="K28" s="36">
+        <v>0.44421272158498437</v>
+      </c>
+      <c r="K28" s="33">
         <f>K19/O19</f>
         <v>0</v>
       </c>
-      <c r="L28" s="36">
+      <c r="L28" s="33">
         <f>L19/O19</f>
-        <v>3.1864046733935211E-2</v>
-      </c>
-      <c r="M28" s="36">
+        <v>3.1282586027111578E-2</v>
+      </c>
+      <c r="M28" s="33">
         <f>M19/O19</f>
-        <v>4.7796070100902817E-2</v>
-      </c>
-      <c r="N28" s="36">
+        <v>4.692387904066736E-2</v>
+      </c>
+      <c r="N28" s="33">
         <f>N19/O19</f>
-        <v>7.1163037705788634E-2</v>
-      </c>
-      <c r="O28" s="37">
+        <v>6.9864442127215848E-2</v>
+      </c>
+      <c r="O28" s="34">
         <f>SUM(I28:N28)</f>
         <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A29" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B29" s="8" t="s">
+      <c r="A29" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B29" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C29" s="8">
+      <c r="C29" s="5">
         <v>47</v>
       </c>
-      <c r="D29" s="9">
+      <c r="D29" s="6">
         <v>43532</v>
       </c>
-      <c r="H29" s="35" t="s">
-        <v>16</v>
-      </c>
-      <c r="I29" s="36">
+      <c r="H29" s="32" t="s">
+        <v>16</v>
+      </c>
+      <c r="I29" s="33">
         <f>I20/O20</f>
         <v>0.13805141225007933</v>
       </c>
-      <c r="J29" s="36">
+      <c r="J29" s="33">
         <f>J20/O20</f>
         <v>2.8562361155188828E-2</v>
       </c>
-      <c r="K29" s="36">
+      <c r="K29" s="33">
         <f>K20/O20</f>
         <v>0</v>
       </c>
-      <c r="L29" s="36">
+      <c r="L29" s="33">
         <f>L20/O20</f>
         <v>0.79086004443033953</v>
       </c>
-      <c r="M29" s="36">
+      <c r="M29" s="33">
         <f>M20/O20</f>
         <v>0</v>
       </c>
-      <c r="N29" s="36">
+      <c r="N29" s="33">
         <f>N20/O20</f>
         <v>4.2526182164392259E-2</v>
       </c>
-      <c r="O29" s="38">
+      <c r="O29" s="35">
         <f>SUM(I29:N29)</f>
         <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A30" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B30" s="8" t="s">
+      <c r="A30" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B30" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C30" s="8">
-        <v>15</v>
-      </c>
-      <c r="D30" s="9">
+      <c r="C30" s="5">
+        <v>15</v>
+      </c>
+      <c r="D30" s="6">
         <v>43532</v>
       </c>
-      <c r="H30" s="39" t="s">
+      <c r="H30" s="36" t="s">
         <v>27</v>
       </c>
-      <c r="I30" s="40">
+      <c r="I30" s="37">
         <f t="shared" ref="I30:N30" si="1">AVERAGE(I26:I29)</f>
-        <v>0.24704181072084752</v>
-      </c>
-      <c r="J30" s="40">
+        <v>0.24979405806647942</v>
+      </c>
+      <c r="J30" s="37">
         <f t="shared" si="1"/>
-        <v>0.25861749338678341</v>
-      </c>
-      <c r="K30" s="40">
+        <v>0.25655330787755953</v>
+      </c>
+      <c r="K30" s="37">
         <f t="shared" si="1"/>
         <v>1.8117451062057477E-2</v>
       </c>
-      <c r="L30" s="40">
+      <c r="L30" s="37">
         <f t="shared" si="1"/>
-        <v>0.41117253736039305</v>
-      </c>
-      <c r="M30" s="40">
+        <v>0.41102717218368712</v>
+      </c>
+      <c r="M30" s="37">
         <f t="shared" si="1"/>
-        <v>1.1949017525225704E-2</v>
-      </c>
-      <c r="N30" s="41">
+        <v>1.173096976016684E-2</v>
+      </c>
+      <c r="N30" s="38">
         <f t="shared" si="1"/>
-        <v>5.3101689944692776E-2</v>
-      </c>
-      <c r="O30" s="42">
+        <v>5.2777041050049586E-2</v>
+      </c>
+      <c r="O30" s="39">
         <f>SUM(I30:N30)</f>
         <v>0.99999999999999989</v>
       </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A31" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B31" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C31" s="8">
+      <c r="A31" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C31" s="5">
         <v>55</v>
       </c>
-      <c r="D31" s="9">
+      <c r="D31" s="6">
         <v>43531</v>
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A32" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B32" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C32" s="8">
+      <c r="A32" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C32" s="5">
         <v>68</v>
       </c>
-      <c r="D32" s="9">
+      <c r="D32" s="6">
         <v>43532</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B33" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C33" s="8">
+      <c r="A33" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C33" s="5">
         <v>129</v>
       </c>
-      <c r="D33" s="9">
+      <c r="D33" s="6">
         <v>43533</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B34" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C34" s="8">
+      <c r="A34" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C34" s="5">
         <v>95</v>
       </c>
-      <c r="D34" s="9">
+      <c r="D34" s="6">
         <v>43534</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B35" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C35" s="8">
+      <c r="A35" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C35" s="5">
         <v>74</v>
       </c>
-      <c r="D35" s="9">
+      <c r="D35" s="6">
         <v>43546</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B36" s="8" t="s">
+      <c r="A36" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B36" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C36" s="8">
+      <c r="C36" s="5">
         <v>52</v>
       </c>
-      <c r="D36" s="9">
+      <c r="D36" s="6">
         <v>43546</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B37" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C37" s="8">
+      <c r="A37" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C37" s="5">
         <v>196</v>
       </c>
-      <c r="D37" s="9">
+      <c r="D37" s="6">
         <v>43376</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B38" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C38" s="8">
+      <c r="A38" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C38" s="5">
         <v>115</v>
       </c>
-      <c r="D38" s="9">
+      <c r="D38" s="6">
         <v>43407</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B39" s="8" t="s">
+      <c r="A39" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B39" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C39" s="8">
+      <c r="C39" s="5">
         <v>10</v>
       </c>
-      <c r="D39" s="9">
+      <c r="D39" s="6">
         <v>43546</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="8" t="s">
+      <c r="A40" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B40" s="8" t="s">
+      <c r="B40" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C40" s="8">
+      <c r="C40" s="5">
         <v>60</v>
       </c>
-      <c r="D40" s="9">
+      <c r="D40" s="6">
         <v>43553</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B41" s="8" t="s">
+      <c r="A41" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B41" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C41" s="8">
+      <c r="C41" s="5">
         <v>60</v>
       </c>
-      <c r="D41" s="9">
+      <c r="D41" s="6">
         <v>43553</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B42" s="8" t="s">
+      <c r="A42" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B42" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C42" s="8">
+      <c r="C42" s="5">
         <v>60</v>
       </c>
-      <c r="D42" s="9">
+      <c r="D42" s="6">
         <v>43553</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="8" t="s">
+      <c r="A43" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B43" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C43" s="8">
+      <c r="B43" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C43" s="5">
         <v>60</v>
       </c>
-      <c r="D43" s="9">
+      <c r="D43" s="6">
         <v>43481</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="8" t="s">
+      <c r="A44" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B44" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C44" s="8">
+      <c r="B44" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C44" s="5">
         <v>150</v>
       </c>
-      <c r="D44" s="9">
+      <c r="D44" s="6">
         <v>43442</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="8" t="s">
+      <c r="A45" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B45" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C45" s="8">
+      <c r="B45" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C45" s="5">
         <v>180</v>
       </c>
-      <c r="D45" s="9">
+      <c r="D45" s="6">
         <v>43448</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="8" t="s">
+      <c r="A46" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B46" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C46" s="8">
+      <c r="B46" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C46" s="5">
         <v>180</v>
       </c>
-      <c r="D46" s="9">
+      <c r="D46" s="6">
         <v>43468</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="8" t="s">
+      <c r="A47" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B47" s="8" t="s">
+      <c r="B47" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C47" s="8">
+      <c r="C47" s="5">
         <v>120</v>
       </c>
-      <c r="D47" s="9">
+      <c r="D47" s="6">
         <v>43478</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B48" s="8" t="s">
+      <c r="A48" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B48" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C48" s="8">
+      <c r="C48" s="5">
         <v>300</v>
       </c>
-      <c r="D48" s="9">
+      <c r="D48" s="6">
         <v>43449</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B49" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C49" s="8">
+      <c r="A49" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B49" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C49" s="5">
         <v>150</v>
       </c>
-      <c r="D49" s="9">
+      <c r="D49" s="6">
         <v>43450</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="8" t="s">
+      <c r="A50" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B50" s="8" t="s">
+      <c r="B50" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C50" s="8">
+      <c r="C50" s="5">
         <v>82</v>
       </c>
-      <c r="D50" s="9">
+      <c r="D50" s="6">
         <v>43558</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B51" s="8" t="s">
+      <c r="A51" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B51" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C51" s="8">
+      <c r="C51" s="5">
         <v>82</v>
       </c>
-      <c r="D51" s="9">
+      <c r="D51" s="6">
         <v>43558</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B52" s="8" t="s">
+      <c r="A52" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B52" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C52" s="8">
+      <c r="C52" s="5">
         <v>82</v>
       </c>
-      <c r="D52" s="9">
+      <c r="D52" s="6">
         <v>43558</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B53" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C53" s="8">
+      <c r="A53" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B53" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C53" s="5">
         <v>85</v>
       </c>
-      <c r="D53" s="9">
+      <c r="D53" s="6">
         <v>43559</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="8" t="s">
+      <c r="A54" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B54" s="8" t="s">
+      <c r="B54" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C54" s="8">
+      <c r="C54" s="5">
         <v>70</v>
       </c>
-      <c r="D54" s="9">
+      <c r="D54" s="6">
         <v>43571</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B55" s="8" t="s">
+      <c r="A55" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B55" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C55" s="8">
+      <c r="C55" s="5">
         <v>70</v>
       </c>
-      <c r="D55" s="9">
+      <c r="D55" s="6">
         <v>43571</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="8" t="s">
+      <c r="A56" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B56" s="8" t="s">
+      <c r="B56" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C56" s="8">
+      <c r="C56" s="5">
         <v>120</v>
       </c>
-      <c r="D56" s="9">
+      <c r="D56" s="6">
         <v>43572</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="8" t="s">
+      <c r="A57" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B57" s="8" t="s">
+      <c r="B57" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C57" s="8">
+      <c r="C57" s="5">
         <v>100</v>
       </c>
-      <c r="D57" s="9">
+      <c r="D57" s="6">
         <v>43574</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B58" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C58" s="8">
+      <c r="A58" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B58" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C58" s="5">
         <v>42</v>
       </c>
-      <c r="D58" s="9">
+      <c r="D58" s="6">
         <v>43577</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B59" s="8" t="s">
+      <c r="A59" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B59" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C59" s="8">
+      <c r="C59" s="5">
         <v>97</v>
       </c>
-      <c r="D59" s="9">
+      <c r="D59" s="6">
         <v>43578</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B60" s="8" t="s">
+      <c r="A60" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B60" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C60" s="8">
+      <c r="C60" s="5">
         <v>30</v>
       </c>
-      <c r="D60" s="9">
+      <c r="D60" s="6">
         <v>43578</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B61" s="8" t="s">
+      <c r="A61" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B61" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C61" s="8">
+      <c r="C61" s="5">
         <v>107</v>
       </c>
-      <c r="D61" s="9">
+      <c r="D61" s="6">
         <v>43581</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B62" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C62" s="8">
+      <c r="A62" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B62" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C62" s="5">
         <v>39</v>
       </c>
-      <c r="D62" s="9">
+      <c r="D62" s="6">
         <v>43584</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B63" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C63" s="8">
+      <c r="A63" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B63" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C63" s="5">
         <v>22</v>
       </c>
-      <c r="D63" s="9">
+      <c r="D63" s="6">
         <v>43585</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" s="8" t="s">
+      <c r="A64" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B64" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C64" s="8">
+      <c r="B64" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C64" s="5">
         <v>22</v>
       </c>
-      <c r="D64" s="9">
+      <c r="D64" s="6">
         <v>43585</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" s="8" t="s">
+      <c r="A65" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B65" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C65" s="8">
-        <v>25</v>
-      </c>
-      <c r="D65" s="9">
+      <c r="B65" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C65" s="5">
+        <v>25</v>
+      </c>
+      <c r="D65" s="6">
         <v>43587</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B66" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C66" s="8">
-        <v>25</v>
-      </c>
-      <c r="D66" s="9">
+      <c r="A66" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B66" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C66" s="5">
+        <v>25</v>
+      </c>
+      <c r="D66" s="6">
         <v>43587</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B67" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C67" s="8">
+      <c r="A67" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B67" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C67" s="5">
         <v>136</v>
       </c>
-      <c r="D67" s="9">
+      <c r="D67" s="6">
         <v>43587</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B68" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C68" s="8">
+      <c r="A68" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B68" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C68" s="5">
         <v>35</v>
       </c>
-      <c r="D68" s="9">
+      <c r="D68" s="6">
         <v>43587</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B69" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C69" s="8">
+      <c r="A69" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B69" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C69" s="5">
         <v>135</v>
       </c>
-      <c r="D69" s="9">
+      <c r="D69" s="6">
         <v>43588</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A70" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B70" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C70" s="8">
+      <c r="A70" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B70" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C70" s="5">
         <v>135</v>
       </c>
-      <c r="D70" s="9">
+      <c r="D70" s="6">
         <v>43588</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B71" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C71" s="8">
+      <c r="A71" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B71" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C71" s="5">
         <v>40</v>
       </c>
-      <c r="D71" s="9">
+      <c r="D71" s="6">
         <v>43589</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B72" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C72" s="8">
+      <c r="A72" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B72" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C72" s="5">
         <v>40</v>
       </c>
-      <c r="D72" s="9">
+      <c r="D72" s="6">
         <v>43589</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B73" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C73" s="8">
+      <c r="A73" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B73" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C73" s="5">
         <v>78</v>
       </c>
-      <c r="D73" s="9">
+      <c r="D73" s="6">
         <v>43590</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A74" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B74" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C74" s="8">
+      <c r="A74" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B74" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C74" s="5">
         <v>78</v>
       </c>
-      <c r="D74" s="9">
+      <c r="D74" s="6">
         <v>43590</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B75" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C75" s="8">
+      <c r="A75" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B75" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C75" s="5">
         <v>45</v>
       </c>
-      <c r="D75" s="9">
+      <c r="D75" s="6">
         <v>43593</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B76" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C76" s="8">
+      <c r="A76" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B76" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C76" s="5">
         <v>45</v>
       </c>
-      <c r="D76" s="9">
+      <c r="D76" s="6">
         <v>43593</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" s="8" t="s">
+      <c r="A77" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B77" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C77" s="8">
+      <c r="B77" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C77" s="5">
         <v>45</v>
       </c>
-      <c r="D77" s="9">
+      <c r="D77" s="6">
         <v>43593</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B78" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C78" s="8">
+      <c r="A78" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B78" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C78" s="5">
         <v>45</v>
       </c>
-      <c r="D78" s="9">
+      <c r="D78" s="6">
         <v>43593</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B79" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C79" s="8">
+      <c r="A79" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B79" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C79" s="5">
         <v>60</v>
       </c>
-      <c r="D79" s="9">
+      <c r="D79" s="6">
         <v>43593</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" s="8" t="s">
+      <c r="A80" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B80" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C80" s="8">
+      <c r="B80" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C80" s="5">
         <v>60</v>
       </c>
-      <c r="D80" s="9">
+      <c r="D80" s="6">
         <v>43593</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A81" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B81" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C81" s="8">
+      <c r="A81" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B81" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C81" s="5">
         <v>60</v>
       </c>
-      <c r="D81" s="9">
+      <c r="D81" s="6">
         <v>43593</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A82" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B82" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C82" s="8">
+      <c r="A82" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B82" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C82" s="5">
         <v>116</v>
       </c>
-      <c r="D82" s="9">
+      <c r="D82" s="6">
         <v>43594</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A83" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B83" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C83" s="8">
+      <c r="A83" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B83" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C83" s="5">
         <v>116</v>
       </c>
-      <c r="D83" s="9">
+      <c r="D83" s="6">
         <v>43594</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A84" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B84" s="8" t="s">
+      <c r="A84" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B84" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C84" s="8">
+      <c r="C84" s="5">
         <v>47</v>
       </c>
-      <c r="D84" s="9">
+      <c r="D84" s="6">
         <v>43598</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A85" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B85" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C85" s="8">
+      <c r="A85" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B85" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C85" s="5">
         <v>31</v>
       </c>
-      <c r="D85" s="9">
+      <c r="D85" s="6">
         <v>43598</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A86" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B86" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C86" s="8">
+      <c r="A86" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B86" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C86" s="5">
         <v>160</v>
       </c>
-      <c r="D86" s="9">
+      <c r="D86" s="6">
         <v>43595</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A87" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B87" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C87" s="8">
+      <c r="A87" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B87" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C87" s="5">
         <v>160</v>
       </c>
-      <c r="D87" s="9">
+      <c r="D87" s="6">
         <v>43595</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A88" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B88" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C88" s="8">
+      <c r="A88" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B88" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C88" s="5">
         <v>240</v>
       </c>
-      <c r="D88" s="9">
+      <c r="D88" s="6">
         <v>43599</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A89" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B89" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C89" s="8">
+      <c r="A89" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B89" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C89" s="5">
         <v>240</v>
       </c>
-      <c r="D89" s="9">
+      <c r="D89" s="6">
         <v>43599</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A90" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B90" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C90" s="8">
+      <c r="A90" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B90" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C90" s="5">
         <v>40</v>
       </c>
-      <c r="D90" s="9">
+      <c r="D90" s="6">
         <v>43600</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A91" s="8" t="s">
+      <c r="A91" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B91" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C91" s="8">
+      <c r="B91" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C91" s="5">
         <v>40</v>
       </c>
-      <c r="D91" s="9">
+      <c r="D91" s="6">
         <v>43600</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A92" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B92" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C92" s="8">
+      <c r="A92" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B92" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C92" s="5">
         <v>40</v>
       </c>
-      <c r="D92" s="9">
+      <c r="D92" s="6">
         <v>43600</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A93" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B93" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C93" s="8">
+      <c r="A93" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B93" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C93" s="5">
         <v>40</v>
       </c>
-      <c r="D93" s="9">
+      <c r="D93" s="6">
         <v>43600</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A94" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B94" s="8" t="s">
+      <c r="A94" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B94" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C94" s="8">
+      <c r="C94" s="5">
         <v>20</v>
       </c>
-      <c r="D94" s="9">
+      <c r="D94" s="6">
         <v>43600</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A95" s="8" t="s">
+      <c r="A95" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B95" s="8" t="s">
+      <c r="B95" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C95" s="8">
+      <c r="C95" s="5">
         <v>20</v>
       </c>
-      <c r="D95" s="9">
+      <c r="D95" s="6">
         <v>43600</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A96" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B96" s="8" t="s">
+      <c r="A96" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B96" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C96" s="8">
+      <c r="C96" s="5">
         <v>20</v>
       </c>
-      <c r="D96" s="9">
+      <c r="D96" s="6">
         <v>43600</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A97" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B97" s="8" t="s">
+      <c r="A97" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B97" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C97" s="8">
+      <c r="C97" s="5">
         <v>20</v>
       </c>
-      <c r="D97" s="9">
+      <c r="D97" s="6">
         <v>43600</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A98" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B98" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C98" s="8">
+      <c r="A98" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B98" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C98" s="5">
         <v>210</v>
       </c>
-      <c r="D98" s="9">
+      <c r="D98" s="6">
         <v>43603</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A99" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B99" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C99" s="8">
+      <c r="A99" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B99" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C99" s="5">
         <v>210</v>
       </c>
-      <c r="D99" s="9">
+      <c r="D99" s="6">
         <v>43603</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A100" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B100" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C100" s="8">
+      <c r="A100" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B100" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C100" s="5">
         <v>65</v>
       </c>
-      <c r="D100" s="9">
+      <c r="D100" s="6">
         <v>43604</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A101" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B101" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C101" s="8">
+      <c r="A101" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B101" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C101" s="5">
         <v>65</v>
       </c>
-      <c r="D101" s="9">
+      <c r="D101" s="6">
         <v>43604</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A102" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B102" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C102" s="8">
+      <c r="A102" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B102" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C102" s="5">
         <v>110</v>
       </c>
-      <c r="D102" s="9">
+      <c r="D102" s="6">
         <v>43604</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A103" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B103" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C103" s="8">
+      <c r="A103" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B103" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C103" s="5">
         <v>20</v>
       </c>
-      <c r="D103" s="9">
+      <c r="D103" s="6">
         <v>43605</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A104" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B104" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C104" s="8">
-        <v>15</v>
-      </c>
-      <c r="D104" s="9">
+      <c r="A104" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B104" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C104" s="5">
+        <v>15</v>
+      </c>
+      <c r="D104" s="6">
         <v>43606</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A105" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B105" s="8" t="s">
+      <c r="A105" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B105" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C105" s="8">
+      <c r="C105" s="5">
         <v>30</v>
       </c>
-      <c r="D105" s="9">
+      <c r="D105" s="6">
         <v>43607</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A106" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B106" s="8" t="s">
+      <c r="A106" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B106" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C106" s="8">
+      <c r="C106" s="5">
         <v>30</v>
       </c>
-      <c r="D106" s="9">
+      <c r="D106" s="6">
         <v>43607</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A107" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B107" s="8" t="s">
+      <c r="A107" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B107" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C107" s="8">
+      <c r="C107" s="5">
         <v>30</v>
       </c>
-      <c r="D107" s="9">
+      <c r="D107" s="6">
         <v>43607</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A108" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B108" s="8" t="s">
+      <c r="A108" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B108" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C108" s="8">
+      <c r="C108" s="5">
         <v>30</v>
       </c>
-      <c r="D108" s="9">
+      <c r="D108" s="6">
         <v>43607</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A109" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B109" s="8" t="s">
+      <c r="A109" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B109" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C109" s="8">
+      <c r="C109" s="5">
         <v>30</v>
       </c>
-      <c r="D109" s="9">
+      <c r="D109" s="6">
         <v>43607</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A110" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B110" s="8" t="s">
+      <c r="A110" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B110" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C110" s="8">
+      <c r="C110" s="5">
         <v>30</v>
       </c>
-      <c r="D110" s="9">
+      <c r="D110" s="6">
         <v>43607</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A111" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B111" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C111" s="8">
+      <c r="A111" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B111" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C111" s="5">
         <v>130</v>
       </c>
-      <c r="D111" s="9">
+      <c r="D111" s="6">
         <v>43607</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A112" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B112" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C112" s="8">
+      <c r="A112" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B112" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C112" s="5">
         <v>130</v>
       </c>
-      <c r="D112" s="9">
+      <c r="D112" s="6">
         <v>43607</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A113" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B113" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C113" s="8">
+      <c r="A113" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B113" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C113" s="5">
         <v>20</v>
       </c>
-      <c r="D113" s="9">
+      <c r="D113" s="6">
         <v>43607</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A114" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B114" s="8" t="s">
+      <c r="A114" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B114" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C114" s="8">
+      <c r="C114" s="5">
         <v>68</v>
       </c>
-      <c r="D114" s="9">
+      <c r="D114" s="6">
         <v>43608</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A115" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B115" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C115" s="8">
+      <c r="A115" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B115" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C115" s="5">
         <v>23</v>
       </c>
-      <c r="D115" s="9">
+      <c r="D115" s="6">
         <v>43609</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A116" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B116" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C116" s="8">
+      <c r="A116" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B116" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C116" s="5">
         <v>85</v>
       </c>
-      <c r="D116" s="9">
+      <c r="D116" s="6">
         <v>43608</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A117" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B117" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C117" s="8">
+      <c r="A117" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B117" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C117" s="5">
         <v>85</v>
       </c>
-      <c r="D117" s="9">
+      <c r="D117" s="6">
         <v>43608</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A118" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B118" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C118" s="8">
+      <c r="A118" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B118" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C118" s="5">
         <v>73</v>
       </c>
-      <c r="D118" s="9">
+      <c r="D118" s="6">
         <v>43609</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A119" s="8" t="s">
+      <c r="A119" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B119" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C119" s="8">
+      <c r="B119" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C119" s="5">
         <v>30</v>
       </c>
-      <c r="D119" s="9">
+      <c r="D119" s="6">
         <v>43614</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A120" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B120" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C120" s="8">
+      <c r="A120" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B120" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C120" s="5">
         <v>30</v>
       </c>
-      <c r="D120" s="9">
+      <c r="D120" s="6">
         <v>43614</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A121" s="43" t="s">
-        <v>6</v>
-      </c>
-      <c r="B121" s="43" t="s">
-        <v>7</v>
-      </c>
-      <c r="C121" s="43">
+      <c r="A121" s="40" t="s">
+        <v>6</v>
+      </c>
+      <c r="B121" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="C121" s="40">
         <v>30</v>
       </c>
-      <c r="D121" s="9">
+      <c r="D121" s="6">
         <v>43614</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A122" s="8" t="s">
+      <c r="A122" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B122" s="8" t="s">
+      <c r="B122" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C122" s="8">
+      <c r="C122" s="5">
         <v>84</v>
       </c>
-      <c r="D122" s="9">
+      <c r="D122" s="6">
         <v>43614</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A123" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B123" s="8" t="s">
+      <c r="A123" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B123" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C123" s="8">
+      <c r="C123" s="5">
         <v>84</v>
       </c>
-      <c r="D123" s="9">
+      <c r="D123" s="6">
         <v>43614</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A124" s="43" t="s">
-        <v>6</v>
-      </c>
-      <c r="B124" s="8" t="s">
+      <c r="A124" s="40" t="s">
+        <v>6</v>
+      </c>
+      <c r="B124" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C124" s="8">
+      <c r="C124" s="5">
         <v>84</v>
       </c>
-      <c r="D124" s="9">
+      <c r="D124" s="6">
         <v>43614</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A125" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B125" s="8" t="s">
+      <c r="A125" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B125" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C125" s="8">
+      <c r="C125" s="5">
         <v>84</v>
       </c>
-      <c r="D125" s="9">
+      <c r="D125" s="6">
         <v>43614</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A126" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B126" s="8" t="s">
+      <c r="A126" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B126" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C126" s="8">
+      <c r="C126" s="5">
         <v>64</v>
       </c>
-      <c r="D126" s="44" t="s">
+      <c r="D126" s="41" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A127" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B127" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C127" s="8">
+      <c r="A127" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B127" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C127" s="5">
         <v>98</v>
       </c>
-      <c r="D127" s="44" t="s">
+      <c r="D127" s="41" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A128" s="8" t="s">
+      <c r="A128" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B128" s="8" t="s">
+      <c r="B128" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C128" s="8">
+      <c r="C128" s="5">
         <v>60</v>
       </c>
-      <c r="D128" s="44">
+      <c r="D128" s="41">
         <v>43471</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A129" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B129" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C129" s="8">
+      <c r="A129" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B129" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C129" s="5">
         <v>165</v>
       </c>
-      <c r="D129" s="8" t="s">
+      <c r="D129" s="5" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A130" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B130" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C130" s="8">
+      <c r="A130" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B130" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C130" s="5">
         <v>165</v>
       </c>
-      <c r="D130" s="8" t="s">
+      <c r="D130" s="5" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A131" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B131" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C131" s="8">
+      <c r="A131" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B131" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C131" s="5">
         <v>118</v>
       </c>
-      <c r="D131" s="44">
+      <c r="D131" s="41">
         <v>43502</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A132" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B132" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C132" s="8">
+      <c r="A132" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B132" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C132" s="5">
         <v>118</v>
       </c>
-      <c r="D132" s="44">
+      <c r="D132" s="41">
         <v>43502</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A133" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B133" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C133" s="8">
+      <c r="A133" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B133" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C133" s="5">
         <v>20</v>
       </c>
-      <c r="D133" s="45">
+      <c r="D133" s="42">
         <v>43530</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A134" s="8" t="s">
+      <c r="A134" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B134" s="8" t="s">
+      <c r="B134" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C134" s="8">
+      <c r="C134" s="5">
         <v>30</v>
       </c>
-      <c r="D134" s="46">
+      <c r="D134" s="43">
         <v>43619</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A135" s="8" t="s">
+      <c r="A135" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B135" s="8" t="s">
+      <c r="B135" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C135" s="8">
+      <c r="C135" s="5">
         <v>30</v>
       </c>
-      <c r="D135" s="46">
+      <c r="D135" s="43">
         <v>43619</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A136" s="8"/>
-      <c r="B136" s="8"/>
-      <c r="C136" s="8"/>
-      <c r="D136" s="8"/>
+      <c r="A136" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B136" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C136" s="5">
+        <v>35</v>
+      </c>
+      <c r="D136" s="43">
+        <v>43619</v>
+      </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A137" s="8"/>
-      <c r="B137" s="8"/>
-      <c r="C137" s="8"/>
-      <c r="D137" s="8"/>
+      <c r="A137" s="5"/>
+      <c r="B137" s="5"/>
+      <c r="C137" s="5"/>
+      <c r="D137" s="5"/>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A138" s="8"/>
-      <c r="B138" s="8"/>
-      <c r="C138" s="8"/>
-      <c r="D138" s="8"/>
+      <c r="A138" s="5"/>
+      <c r="B138" s="5"/>
+      <c r="C138" s="5"/>
+      <c r="D138" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
CMv0.20, doc Rilascio, modifica doc Requisiti
</commit_message>
<xml_diff>
--- a/Documentazione/Attività sul progetto/DocAttivProg.xlsx
+++ b/Documentazione/Attività sul progetto/DocAttivProg.xlsx
@@ -1,17 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\UniUD\Laurea Magistrale\Ingegneria del Software 2\Progetto-Ingegneria-Del-Sw-2\Documentazione\Attività sul progetto\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFAAB00B-E21F-4780-BAB7-549AAF7CFDD3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Foglio1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
     </ext>
@@ -20,112 +31,103 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="30">
   <si>
-    <t xml:space="preserve">Le categorie sono: Ispezione Codice, Documenti di progetto, Documenti di processo, Manuale, Sviluppo, Testing</t>
+    <t>Le categorie sono: Ispezione Codice, Documenti di progetto, Documenti di processo, Manuale, Sviluppo, Testing</t>
   </si>
   <si>
-    <t xml:space="preserve">Vecchia convenzione: i verbali esterni sono documenti di progetto, quelli interni di processo</t>
+    <t>Vecchia convenzione: i verbali esterni sono documenti di progetto, quelli interni di processo</t>
   </si>
   <si>
-    <t xml:space="preserve">PERSONA</t>
+    <t>PERSONA</t>
   </si>
   <si>
-    <t xml:space="preserve">ATTIVITÀ</t>
+    <t>ATTIVITÀ</t>
   </si>
   <si>
-    <t xml:space="preserve">TEMPO (min)</t>
+    <t>TEMPO (min)</t>
   </si>
   <si>
-    <t xml:space="preserve">DATA</t>
+    <t>DATA</t>
   </si>
   <si>
-    <t xml:space="preserve">Giovanni</t>
+    <t>Giovanni</t>
   </si>
   <si>
-    <t xml:space="preserve">Documenti di progetto</t>
+    <t>Documenti di progetto</t>
   </si>
   <si>
-    <t xml:space="preserve">Minuti di lavoro per attività e relativa percentuale</t>
+    <t>Minuti di lavoro per attività e relativa percentuale</t>
   </si>
   <si>
-    <t xml:space="preserve">Attività</t>
+    <t>Attività</t>
   </si>
   <si>
-    <t xml:space="preserve">Totale minuti</t>
+    <t>Totale minuti</t>
   </si>
   <si>
-    <t xml:space="preserve">Percentuale</t>
+    <t>Percentuale</t>
   </si>
   <si>
-    <t xml:space="preserve">Documenti di processo</t>
+    <t>Documenti di processo</t>
   </si>
   <si>
-    <t xml:space="preserve">Ispezione codice</t>
+    <t>Ispezione codice</t>
   </si>
   <si>
-    <t xml:space="preserve">Manuale</t>
+    <t>Manuale</t>
   </si>
   <si>
-    <t xml:space="preserve">Sviluppo</t>
+    <t>Sviluppo</t>
   </si>
   <si>
-    <t xml:space="preserve">Viktorija</t>
+    <t>Viktorija</t>
   </si>
   <si>
-    <t xml:space="preserve">Testing</t>
+    <t>Testing</t>
   </si>
   <si>
-    <t xml:space="preserve">Totale</t>
+    <t>Totale</t>
   </si>
   <si>
-    <t xml:space="preserve">Luca</t>
+    <t>Luca</t>
   </si>
   <si>
-    <t xml:space="preserve">Tempo/persona (minuti) per attività e relativa media</t>
+    <t>Tempo/persona (minuti) per attività e relativa media</t>
   </si>
   <si>
-    <t xml:space="preserve">Persona</t>
+    <t>Persona</t>
   </si>
   <si>
-    <t xml:space="preserve">Doc. Progetto</t>
+    <t>Doc. Progetto</t>
   </si>
   <si>
-    <t xml:space="preserve">Doc. Processo</t>
+    <t>Doc. Processo</t>
   </si>
   <si>
-    <t xml:space="preserve">Ispezione Codice</t>
+    <t>Ispezione Codice</t>
   </si>
   <si>
-    <t xml:space="preserve">Hristina</t>
+    <t>Hristina</t>
   </si>
   <si>
-    <t xml:space="preserve">Interno</t>
+    <t>Interno</t>
   </si>
   <si>
-    <t xml:space="preserve">Media</t>
+    <t>Media</t>
   </si>
   <si>
-    <t xml:space="preserve">Percentuale tempo/persona per attività e relativa media</t>
+    <t>Percentuale tempo/persona per attività e relativa media</t>
   </si>
   <si>
-    <t xml:space="preserve">05/31/2019</t>
+    <t>05/31/2019</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="7">
-    <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="M/D/YYYY"/>
-    <numFmt numFmtId="166" formatCode="0%"/>
-    <numFmt numFmtId="167" formatCode="0.00%"/>
-    <numFmt numFmtId="168" formatCode="0.00"/>
-    <numFmt numFmtId="169" formatCode="M/D/YYYY"/>
-    <numFmt numFmtId="170" formatCode="MM/DD/YY"/>
-  </numFmts>
-  <fonts count="7">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -134,22 +136,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
+      <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -157,7 +144,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
@@ -165,8 +152,15 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
-      <u val="single"/>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -201,288 +195,210 @@
     </fill>
   </fills>
   <borders count="8">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
-      <bottom style="thin"/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
-      <top style="thin"/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
-      <right style="thin"/>
-      <top style="thin"/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
       <right/>
-      <top style="thin"/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
       <right/>
       <top/>
-      <bottom style="thin"/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+  <cellStyleXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
+  </cellStyleXfs>
+  <cellXfs count="45">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-  </cellStyleXfs>
-  <cellXfs count="47">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="10" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="10" fontId="0" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="9" fontId="0" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="2" borderId="0" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="2" borderId="2" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="2" borderId="3" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="10" fontId="0" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="9" fontId="0" fillId="4" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="9" fontId="0" fillId="4" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="4" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="10" fontId="0" fillId="4" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="9" fontId="0" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="4" borderId="0" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="4" borderId="4" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="4" borderId="7" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="4" borderId="3" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="4" borderId="5" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="4" borderId="0" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+  <cellStyles count="2">
+    <cellStyle name="Normale" xfId="0" builtinId="0"/>
+    <cellStyle name="Percentuale" xfId="1" builtinId="5"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -541,48 +457,356 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema di Office">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4472C4"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:O139"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:O158"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A118" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D139" activeCellId="0" sqref="D139"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="P13" sqref="P13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="10.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="5" style="0" width="8.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="26.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="9" style="0" width="17.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="12" style="0" width="17.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="15" style="0" width="8.71"/>
+    <col min="1" max="1" width="15.5546875" customWidth="1"/>
+    <col min="2" max="2" width="23.44140625" customWidth="1"/>
+    <col min="3" max="3" width="15.5546875" customWidth="1"/>
+    <col min="4" max="4" width="10.88671875" customWidth="1"/>
+    <col min="5" max="7" width="8.6640625" customWidth="1"/>
+    <col min="8" max="8" width="26.33203125" customWidth="1"/>
+    <col min="9" max="11" width="17.33203125" customWidth="1"/>
+    <col min="12" max="14" width="17.44140625" customWidth="1"/>
+    <col min="15" max="1025" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="F1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="F2" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
@@ -597,2379 +821,2557 @@
       </c>
       <c r="H3" s="2"/>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="5" t="n">
+      <c r="C4" s="5">
         <v>98</v>
       </c>
-      <c r="D4" s="6" t="n">
+      <c r="D4" s="40">
         <v>43484</v>
       </c>
-      <c r="H4" s="7" t="s">
+      <c r="H4" s="42" t="s">
         <v>8</v>
       </c>
-      <c r="I4" s="7"/>
-      <c r="J4" s="7"/>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I4" s="42"/>
+      <c r="J4" s="42"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="5" t="n">
+      <c r="C5" s="5">
         <v>149</v>
       </c>
-      <c r="D5" s="6" t="n">
+      <c r="D5" s="40">
         <v>43493</v>
       </c>
-      <c r="H5" s="8" t="s">
+      <c r="H5" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="I5" s="9" t="s">
+      <c r="I5" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="J5" s="9" t="s">
+      <c r="J5" s="7" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>6</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="5" t="n">
+      <c r="C6" s="5">
         <v>135</v>
       </c>
-      <c r="D6" s="6" t="n">
+      <c r="D6" s="40">
         <v>43494</v>
       </c>
-      <c r="H6" s="10" t="s">
+      <c r="H6" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="I6" s="11" t="n">
-        <f aca="false">SUMIF(B:B,"Ispezione codice",C:C)</f>
-        <v>536</v>
-      </c>
-      <c r="J6" s="12" t="n">
-        <f aca="false">I6/I12</f>
-        <v>0.0488917267171395</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I6" s="9">
+        <f>SUMIF(B:B,"Ispezione codice",C:C)</f>
+        <v>756</v>
+      </c>
+      <c r="J6" s="10">
+        <f>I6/I12</f>
+        <v>6.6531725776643486E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="5" t="n">
+      <c r="C7" s="5">
         <v>53</v>
       </c>
-      <c r="D7" s="6" t="n">
+      <c r="D7" s="40">
         <v>43494</v>
       </c>
-      <c r="H7" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="I7" s="11" t="n">
-        <f aca="false">SUMIF(B:B,"Documenti di progetto",C:C)</f>
-        <v>2348</v>
-      </c>
-      <c r="J7" s="12" t="n">
-        <f aca="false">(I7/I12)</f>
-        <v>0.214174952111648</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H7" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="I7" s="9">
+        <f>SUMIF(B:B,"Documenti di progetto",C:C)</f>
+        <v>2528</v>
+      </c>
+      <c r="J7" s="10">
+        <f>(I7/I12)</f>
+        <v>0.22247645868168617</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="5" t="n">
+      <c r="C8" s="5">
         <v>87</v>
       </c>
-      <c r="D8" s="6" t="n">
+      <c r="D8" s="40">
         <v>43495</v>
       </c>
-      <c r="H8" s="10" t="s">
+      <c r="H8" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="I8" s="11" t="n">
-        <f aca="false">SUMIF(B:B,"Documenti di processo",C:C)</f>
+      <c r="I8" s="9">
+        <f>SUMIF(B:B,"Documenti di processo",C:C)</f>
         <v>2336</v>
       </c>
-      <c r="J8" s="12" t="n">
-        <f aca="false">I8/I12</f>
-        <v>0.213080361214996</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J8" s="10">
+        <f>I8/I12</f>
+        <v>0.20557951245269734</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>6</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="5" t="n">
+      <c r="C9" s="5">
         <v>74</v>
       </c>
-      <c r="D9" s="6" t="n">
+      <c r="D9" s="40">
         <v>43495</v>
       </c>
-      <c r="H9" s="10" t="s">
+      <c r="H9" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="I9" s="11" t="n">
-        <f aca="false">SUMIF(B:B,"Manuale",C:C)</f>
+      <c r="I9" s="9">
+        <f>SUMIF(B:B,"Manuale",C:C)</f>
         <v>174</v>
       </c>
-      <c r="J9" s="12" t="n">
-        <f aca="false">I9/I12</f>
-        <v>0.0158715680014595</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J9" s="10">
+        <f>I9/I12</f>
+        <v>1.5312857520021121E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>6</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="5" t="n">
+      <c r="C10" s="5">
         <v>32</v>
       </c>
-      <c r="D10" s="6" t="n">
+      <c r="D10" s="40">
         <v>43499</v>
       </c>
-      <c r="H10" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="I10" s="11" t="n">
-        <f aca="false">SUMIF(B:B,"Sviluppo",C:C)</f>
+      <c r="H10" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="I10" s="9">
+        <f>SUMIF(B:B,"Sviluppo",C:C)</f>
         <v>5479</v>
       </c>
-      <c r="J10" s="12" t="n">
-        <f aca="false">I10/I12</f>
-        <v>0.499771960229864</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J10" s="10">
+        <f>I10/I12</f>
+        <v>0.48217900202411335</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>16</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="5" t="n">
+      <c r="C11" s="5">
         <v>75</v>
       </c>
-      <c r="D11" s="6" t="n">
+      <c r="D11" s="40">
         <v>43497</v>
       </c>
-      <c r="H11" s="13" t="s">
+      <c r="H11" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="I11" s="14" t="n">
-        <f aca="false">SUMIF(B:B,"Testing",C:C)</f>
+      <c r="I11" s="12">
+        <f>SUMIF(B:B,"Testing",C:C)</f>
         <v>90</v>
       </c>
-      <c r="J11" s="15" t="n">
-        <f aca="false">I11/I12</f>
-        <v>0.00820943172489282</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J11" s="13">
+        <f>I11/I12</f>
+        <v>7.9204435448385103E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>16</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C12" s="5" t="n">
+      <c r="C12" s="5">
         <v>55</v>
       </c>
-      <c r="D12" s="6" t="n">
+      <c r="D12" s="40">
         <v>43503</v>
       </c>
-      <c r="H12" s="16" t="s">
+      <c r="H12" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="I12" s="17" t="n">
-        <f aca="false">SUM(I6:I11)</f>
-        <v>10963</v>
-      </c>
-      <c r="J12" s="18" t="n">
-        <f aca="false">SUM(J6:J11)</f>
+      <c r="I12" s="15">
+        <f>SUM(I6:I11)</f>
+        <v>11363</v>
+      </c>
+      <c r="J12" s="16">
+        <f>SUM(J6:J11)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
         <v>6</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="5" t="n">
+      <c r="C13" s="5">
         <v>127</v>
       </c>
-      <c r="D13" s="6" t="n">
+      <c r="D13" s="40">
         <v>43505</v>
       </c>
       <c r="H13" s="2"/>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
         <v>6</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="5" t="n">
+      <c r="C14" s="5">
         <v>24</v>
       </c>
-      <c r="D14" s="6" t="n">
+      <c r="D14" s="40">
         <v>43509</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
         <v>19</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="5" t="n">
+      <c r="C15" s="5">
         <v>195</v>
       </c>
-      <c r="D15" s="6" t="n">
+      <c r="D15" s="40">
         <v>43521</v>
       </c>
-      <c r="H15" s="19" t="s">
+      <c r="H15" s="43" t="s">
         <v>20</v>
       </c>
-      <c r="I15" s="19"/>
-      <c r="J15" s="19"/>
-      <c r="K15" s="19"/>
-      <c r="L15" s="19"/>
-      <c r="M15" s="19"/>
-      <c r="N15" s="19"/>
-      <c r="O15" s="19"/>
-    </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I15" s="43"/>
+      <c r="J15" s="43"/>
+      <c r="K15" s="43"/>
+      <c r="L15" s="43"/>
+      <c r="M15" s="43"/>
+      <c r="N15" s="43"/>
+      <c r="O15" s="43"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
         <v>19</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C16" s="5" t="n">
+      <c r="C16" s="5">
         <v>105</v>
       </c>
-      <c r="D16" s="6" t="n">
+      <c r="D16" s="40">
         <v>43523</v>
       </c>
-      <c r="H16" s="20" t="s">
+      <c r="H16" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="I16" s="21" t="s">
+      <c r="I16" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="J16" s="21" t="s">
+      <c r="J16" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="K16" s="21" t="s">
+      <c r="K16" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="L16" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="M16" s="21" t="s">
+      <c r="L16" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="M16" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="N16" s="21" t="s">
+      <c r="N16" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="O16" s="22" t="s">
+      <c r="O16" s="19" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
         <v>25</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C17" s="5" t="n">
+      <c r="C17" s="5">
         <v>30</v>
       </c>
-      <c r="D17" s="6" t="n">
+      <c r="D17" s="40">
         <v>43519</v>
       </c>
-      <c r="H17" s="23" t="s">
-        <v>6</v>
-      </c>
-      <c r="I17" s="24" t="n">
-        <f aca="false">SUMIFS(C:C,B:B,"Documenti di progetto",A:A,"Giovanni")</f>
-        <v>981</v>
-      </c>
-      <c r="J17" s="24" t="n">
-        <f aca="false">SUMIFS(C:C,B:B,"Documenti di processo",A:A,"Giovanni")</f>
+      <c r="H17" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="I17" s="21">
+        <f>SUMIFS(C:C,B:B,"Documenti di progetto",A:A,"Giovanni")</f>
+        <v>1041</v>
+      </c>
+      <c r="J17" s="21">
+        <f>SUMIFS(C:C,B:B,"Documenti di processo",A:A,"Giovanni")</f>
         <v>1112</v>
       </c>
-      <c r="K17" s="24" t="n">
-        <f aca="false">SUMIFS(C:C,B:B,"Manuale",A:A,"Giovanni")</f>
+      <c r="K17" s="21">
+        <f>SUMIFS(C:C,B:B,"Manuale",A:A,"Giovanni")</f>
         <v>174</v>
       </c>
-      <c r="L17" s="24" t="n">
-        <f aca="false">SUMIFS(C:C,B:B,"Sviluppo",A:A,"Giovanni")</f>
+      <c r="L17" s="21">
+        <f>SUMIFS(C:C,B:B,"Sviluppo",A:A,"Giovanni")</f>
         <v>0</v>
       </c>
-      <c r="M17" s="24" t="n">
-        <f aca="false">SUMIFS(C:C,B:B,"Testing",A:A,"Giovanni")</f>
+      <c r="M17" s="21">
+        <f>SUMIFS(C:C,B:B,"Testing",A:A,"Giovanni")</f>
         <v>0</v>
       </c>
-      <c r="N17" s="24" t="n">
-        <f aca="false">SUMIFS(C:C,B:B,"Ispezione codice",A:A,"Giovanni")</f>
-        <v>134</v>
-      </c>
-      <c r="O17" s="25" t="n">
-        <f aca="false">SUM(I17:N17)</f>
-        <v>2401</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N17" s="21">
+        <f>SUMIFS(C:C,B:B,"Ispezione codice",A:A,"Giovanni")</f>
+        <v>189</v>
+      </c>
+      <c r="O17" s="22">
+        <f>SUM(I17:N17)</f>
+        <v>2516</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
         <v>25</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="5" t="n">
+      <c r="C18" s="5">
         <v>100</v>
       </c>
-      <c r="D18" s="6" t="n">
+      <c r="D18" s="40">
         <v>43520</v>
       </c>
-      <c r="H18" s="23" t="s">
-        <v>25</v>
-      </c>
-      <c r="I18" s="24" t="n">
-        <f aca="false">SUMIFS(C:C,B:B,"Documenti di progetto",A:A,"Hristina")</f>
-        <v>150</v>
-      </c>
-      <c r="J18" s="24" t="n">
-        <f aca="false">SUMIFS(C:C,B:B,"Documenti di processo",A:A,"Hristina")</f>
+      <c r="H18" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="I18" s="21">
+        <f>SUMIFS(C:C,B:B,"Documenti di progetto",A:A,"Hristina")</f>
+        <v>180</v>
+      </c>
+      <c r="J18" s="21">
+        <f>SUMIFS(C:C,B:B,"Documenti di processo",A:A,"Hristina")</f>
         <v>282</v>
       </c>
-      <c r="K18" s="24" t="n">
-        <f aca="false">SUMIFS(C:C,B:B,"Manuale",A:A,"Hristina")</f>
+      <c r="K18" s="21">
+        <f>SUMIFS(C:C,B:B,"Manuale",A:A,"Hristina")</f>
         <v>0</v>
       </c>
-      <c r="L18" s="24" t="n">
-        <f aca="false">SUMIFS(C:C,B:B,"Sviluppo",A:A,"Hristina")</f>
+      <c r="L18" s="21">
+        <f>SUMIFS(C:C,B:B,"Sviluppo",A:A,"Hristina")</f>
         <v>2747</v>
       </c>
-      <c r="M18" s="24" t="n">
-        <f aca="false">SUMIFS(C:C,B:B,"Testing",A:A,"Hristina")</f>
+      <c r="M18" s="21">
+        <f>SUMIFS(C:C,B:B,"Testing",A:A,"Hristina")</f>
         <v>0</v>
       </c>
-      <c r="N18" s="24" t="n">
-        <f aca="false">SUMIFS(C:C,B:B,"Ispezione codice",A:A,"Hristina")</f>
-        <v>134</v>
-      </c>
-      <c r="O18" s="25" t="n">
-        <f aca="false">SUM(I18:N18)</f>
-        <v>3313</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N18" s="21">
+        <f>SUMIFS(C:C,B:B,"Ispezione codice",A:A,"Hristina")</f>
+        <v>189</v>
+      </c>
+      <c r="O18" s="22">
+        <f>SUM(I18:N18)</f>
+        <v>3398</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
         <v>25</v>
       </c>
       <c r="B19" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C19" s="5" t="n">
+      <c r="C19" s="5">
         <v>125</v>
       </c>
-      <c r="D19" s="6" t="n">
+      <c r="D19" s="40">
         <v>43522</v>
       </c>
-      <c r="H19" s="23" t="s">
+      <c r="H19" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="I19" s="24" t="n">
-        <f aca="false">SUMIFS(C:C,B:B,"Documenti di progetto",A:A,"Luca")</f>
-        <v>782</v>
-      </c>
-      <c r="J19" s="24" t="n">
-        <f aca="false">SUMIFS(C:C,B:B,"Documenti di processo",A:A,"Luca")</f>
+      <c r="I19" s="21">
+        <f>SUMIFS(C:C,B:B,"Documenti di progetto",A:A,"Luca")</f>
+        <v>842</v>
+      </c>
+      <c r="J19" s="21">
+        <f>SUMIFS(C:C,B:B,"Documenti di processo",A:A,"Luca")</f>
         <v>852</v>
       </c>
-      <c r="K19" s="24" t="n">
-        <f aca="false">SUMIFS(C:C,B:B,"Manuale",A:A,"Luca")</f>
+      <c r="K19" s="21">
+        <f>SUMIFS(C:C,B:B,"Manuale",A:A,"Luca")</f>
         <v>0</v>
       </c>
-      <c r="L19" s="24" t="n">
-        <f aca="false">SUMIFS(C:C,B:B,"Sviluppo",A:A,"Luca")</f>
+      <c r="L19" s="21">
+        <f>SUMIFS(C:C,B:B,"Sviluppo",A:A,"Luca")</f>
         <v>60</v>
       </c>
-      <c r="M19" s="24" t="n">
-        <f aca="false">SUMIFS(C:C,B:B,"Testing",A:A,"Luca")</f>
+      <c r="M19" s="21">
+        <f>SUMIFS(C:C,B:B,"Testing",A:A,"Luca")</f>
         <v>90</v>
       </c>
-      <c r="N19" s="24" t="n">
-        <f aca="false">SUMIFS(C:C,B:B,"Ispezione codice",A:A,"Luca")</f>
-        <v>134</v>
-      </c>
-      <c r="O19" s="25" t="n">
-        <f aca="false">SUM(I19:N19)</f>
-        <v>1918</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N19" s="21">
+        <f>SUMIFS(C:C,B:B,"Ispezione codice",A:A,"Luca")</f>
+        <v>189</v>
+      </c>
+      <c r="O19" s="22">
+        <f>SUM(I19:N19)</f>
+        <v>2033</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
         <v>25</v>
       </c>
       <c r="B20" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C20" s="5" t="n">
+      <c r="C20" s="5">
         <v>170</v>
       </c>
-      <c r="D20" s="6" t="n">
+      <c r="D20" s="40">
         <v>43523</v>
       </c>
-      <c r="H20" s="23" t="s">
-        <v>16</v>
-      </c>
-      <c r="I20" s="24" t="n">
-        <f aca="false">SUMIFS(C:C,B:B,"Documenti di progetto",A:A,"Viktorija")</f>
-        <v>435</v>
-      </c>
-      <c r="J20" s="24" t="n">
-        <f aca="false">SUMIFS(C:C,B:B,"Documenti di processo",A:A,"Viktorija")</f>
+      <c r="H20" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="I20" s="21">
+        <f>SUMIFS(C:C,B:B,"Documenti di progetto",A:A,"Viktorija")</f>
+        <v>465</v>
+      </c>
+      <c r="J20" s="21">
+        <f>SUMIFS(C:C,B:B,"Documenti di processo",A:A,"Viktorija")</f>
         <v>90</v>
       </c>
-      <c r="K20" s="24" t="n">
-        <f aca="false">SUMIFS(C:C,B:B,"Manuale",A:A,"Viktorija")</f>
+      <c r="K20" s="21">
+        <f>SUMIFS(C:C,B:B,"Manuale",A:A,"Viktorija")</f>
         <v>0</v>
       </c>
-      <c r="L20" s="24" t="n">
-        <f aca="false">SUMIFS(C:C,B:B,"Sviluppo",A:A,"Viktorija")</f>
+      <c r="L20" s="21">
+        <f>SUMIFS(C:C,B:B,"Sviluppo",A:A,"Viktorija")</f>
         <v>2672</v>
       </c>
-      <c r="M20" s="24" t="n">
-        <f aca="false">SUMIFS(C:C,B:B,"Testing",A:A,"Viktorija")</f>
+      <c r="M20" s="21">
+        <f>SUMIFS(C:C,B:B,"Testing",A:A,"Viktorija")</f>
         <v>0</v>
       </c>
-      <c r="N20" s="24" t="n">
-        <f aca="false">SUMIFS(C:C,B:B,"Ispezione codice",A:A,"Viktorija")</f>
-        <v>134</v>
-      </c>
-      <c r="O20" s="25" t="n">
-        <f aca="false">SUM(I20:N20)</f>
-        <v>3331</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N20" s="21">
+        <f>SUMIFS(C:C,B:B,"Ispezione codice",A:A,"Viktorija")</f>
+        <v>189</v>
+      </c>
+      <c r="O20" s="22">
+        <f>SUM(I20:N20)</f>
+        <v>3416</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
         <v>25</v>
       </c>
       <c r="B21" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C21" s="5" t="n">
+      <c r="C21" s="5">
         <v>65</v>
       </c>
-      <c r="D21" s="6" t="n">
+      <c r="D21" s="40">
         <v>43524</v>
       </c>
-      <c r="H21" s="26" t="s">
+      <c r="H21" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="I21" s="27" t="n">
-        <f aca="false">AVERAGE(I17:I20)</f>
-        <v>587</v>
-      </c>
-      <c r="J21" s="28" t="n">
-        <f aca="false">AVERAGE(J17:J20)</f>
+      <c r="I21" s="24">
+        <f t="shared" ref="I21:N21" si="0">AVERAGE(I17:I20)</f>
+        <v>632</v>
+      </c>
+      <c r="J21" s="25">
+        <f t="shared" si="0"/>
         <v>584</v>
       </c>
-      <c r="K21" s="28" t="n">
-        <f aca="false">AVERAGE(K17:K20)</f>
+      <c r="K21" s="25">
+        <f t="shared" si="0"/>
         <v>43.5</v>
       </c>
-      <c r="L21" s="28" t="n">
-        <f aca="false">AVERAGE(L17:L20)</f>
+      <c r="L21" s="25">
+        <f t="shared" si="0"/>
         <v>1369.75</v>
       </c>
-      <c r="M21" s="28" t="n">
-        <f aca="false">AVERAGE(M17:M20)</f>
+      <c r="M21" s="25">
+        <f t="shared" si="0"/>
         <v>22.5</v>
       </c>
-      <c r="N21" s="29" t="n">
-        <f aca="false">AVERAGE(N17:N20)</f>
-        <v>134</v>
-      </c>
-      <c r="O21" s="30" t="n">
-        <f aca="false">SUM(O17:O20)</f>
-        <v>10963</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N21" s="26">
+        <f t="shared" si="0"/>
+        <v>189</v>
+      </c>
+      <c r="O21" s="27">
+        <f>SUM(O17:O20)</f>
+        <v>11363</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
         <v>16</v>
       </c>
       <c r="B22" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C22" s="5" t="n">
+      <c r="C22" s="5">
         <v>60</v>
       </c>
-      <c r="D22" s="6" t="n">
+      <c r="D22" s="40">
         <v>43487</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A23" s="5" t="s">
         <v>16</v>
       </c>
       <c r="B23" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C23" s="5" t="n">
+      <c r="C23" s="5">
         <v>103</v>
       </c>
-      <c r="D23" s="6" t="n">
+      <c r="D23" s="40">
         <v>43506</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
         <v>16</v>
       </c>
       <c r="B24" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C24" s="5" t="n">
+      <c r="C24" s="5">
         <v>100</v>
       </c>
-      <c r="D24" s="6" t="n">
+      <c r="D24" s="40">
         <v>43520</v>
       </c>
-      <c r="H24" s="31" t="s">
+      <c r="H24" s="44" t="s">
         <v>28</v>
       </c>
-      <c r="I24" s="31"/>
-      <c r="J24" s="31"/>
-      <c r="K24" s="31"/>
-      <c r="L24" s="31"/>
-      <c r="M24" s="31"/>
-      <c r="N24" s="31"/>
-      <c r="O24" s="31"/>
-    </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I24" s="44"/>
+      <c r="J24" s="44"/>
+      <c r="K24" s="44"/>
+      <c r="L24" s="44"/>
+      <c r="M24" s="44"/>
+      <c r="N24" s="44"/>
+      <c r="O24" s="44"/>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A25" s="5" t="s">
         <v>16</v>
       </c>
       <c r="B25" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C25" s="5" t="n">
+      <c r="C25" s="5">
         <v>170</v>
       </c>
-      <c r="D25" s="6" t="n">
+      <c r="D25" s="40">
         <v>43523</v>
       </c>
-      <c r="H25" s="32" t="s">
+      <c r="H25" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="I25" s="33" t="s">
+      <c r="I25" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="J25" s="33" t="s">
+      <c r="J25" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="K25" s="33" t="s">
+      <c r="K25" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="L25" s="33" t="s">
-        <v>15</v>
-      </c>
-      <c r="M25" s="33" t="s">
+      <c r="L25" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="M25" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="N25" s="33" t="s">
+      <c r="N25" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="O25" s="34" t="s">
+      <c r="O25" s="30" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="s">
         <v>16</v>
       </c>
       <c r="B26" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C26" s="5" t="n">
+      <c r="C26" s="5">
         <v>45</v>
       </c>
-      <c r="D26" s="6" t="n">
+      <c r="D26" s="40">
         <v>43524</v>
       </c>
-      <c r="H26" s="35" t="s">
-        <v>6</v>
-      </c>
-      <c r="I26" s="36" t="n">
-        <f aca="false">I17/O17</f>
-        <v>0.408579758433986</v>
-      </c>
-      <c r="J26" s="36" t="n">
-        <f aca="false">J17/O17</f>
-        <v>0.46314035818409</v>
-      </c>
-      <c r="K26" s="36" t="n">
-        <f aca="false">K17/O17</f>
-        <v>0.0724698042482299</v>
-      </c>
-      <c r="L26" s="36" t="n">
-        <f aca="false">L17/O17</f>
+      <c r="H26" s="31" t="s">
+        <v>6</v>
+      </c>
+      <c r="I26" s="32">
+        <f>I17/O17</f>
+        <v>0.41375198728139906</v>
+      </c>
+      <c r="J26" s="32">
+        <f>J17/O17</f>
+        <v>0.44197138314785372</v>
+      </c>
+      <c r="K26" s="32">
+        <f>K17/O17</f>
+        <v>6.9157392686804445E-2</v>
+      </c>
+      <c r="L26" s="32">
+        <f>L17/O17</f>
         <v>0</v>
       </c>
-      <c r="M26" s="36" t="n">
-        <f aca="false">M17/O17</f>
+      <c r="M26" s="32">
+        <f>M17/O17</f>
         <v>0</v>
       </c>
-      <c r="N26" s="36" t="n">
-        <f aca="false">N17/O17</f>
-        <v>0.0558100791336943</v>
-      </c>
-      <c r="O26" s="37" t="n">
-        <f aca="false">SUM(I26:N26)</f>
+      <c r="N26" s="32">
+        <f>N17/O17</f>
+        <v>7.5119236883942772E-2</v>
+      </c>
+      <c r="O26" s="33">
+        <f>SUM(I26:N26)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A27" s="5" t="s">
         <v>16</v>
       </c>
       <c r="B27" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C27" s="5" t="n">
-        <v>25</v>
-      </c>
-      <c r="D27" s="6" t="n">
+      <c r="C27" s="5">
+        <v>25</v>
+      </c>
+      <c r="D27" s="40">
         <v>43530</v>
       </c>
-      <c r="H27" s="35" t="s">
-        <v>25</v>
-      </c>
-      <c r="I27" s="36" t="n">
-        <f aca="false">I18/O18</f>
-        <v>0.0452761847268337</v>
-      </c>
-      <c r="J27" s="36" t="n">
-        <f aca="false">J18/O18</f>
-        <v>0.0851192272864473</v>
-      </c>
-      <c r="K27" s="36" t="n">
-        <f aca="false">K18/O18</f>
+      <c r="H27" s="31" t="s">
+        <v>25</v>
+      </c>
+      <c r="I27" s="32">
+        <f>I18/O18</f>
+        <v>5.2972336668628606E-2</v>
+      </c>
+      <c r="J27" s="32">
+        <f>J18/O18</f>
+        <v>8.2989994114184812E-2</v>
+      </c>
+      <c r="K27" s="32">
+        <f>K18/O18</f>
         <v>0</v>
       </c>
-      <c r="L27" s="36" t="n">
-        <f aca="false">L18/O18</f>
-        <v>0.829157862964081</v>
-      </c>
-      <c r="M27" s="36" t="n">
-        <f aca="false">M18/O18</f>
+      <c r="L27" s="32">
+        <f>L18/O18</f>
+        <v>0.80841671571512652</v>
+      </c>
+      <c r="M27" s="32">
+        <f>M18/O18</f>
         <v>0</v>
       </c>
-      <c r="N27" s="36" t="n">
-        <f aca="false">N18/O18</f>
-        <v>0.0404467250226381</v>
-      </c>
-      <c r="O27" s="37" t="n">
-        <f aca="false">SUM(I27:N27)</f>
+      <c r="N27" s="32">
+        <f>N18/O18</f>
+        <v>5.5620953502060033E-2</v>
+      </c>
+      <c r="O27" s="33">
+        <f>SUM(I27:N27)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A28" s="5" t="s">
         <v>19</v>
       </c>
       <c r="B28" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C28" s="5" t="n">
-        <v>15</v>
-      </c>
-      <c r="D28" s="6" t="n">
+      <c r="C28" s="5">
+        <v>15</v>
+      </c>
+      <c r="D28" s="40">
         <v>43532</v>
       </c>
-      <c r="H28" s="35" t="s">
+      <c r="H28" s="31" t="s">
         <v>19</v>
       </c>
-      <c r="I28" s="36" t="n">
-        <f aca="false">I19/O19</f>
-        <v>0.407716371220021</v>
-      </c>
-      <c r="J28" s="36" t="n">
-        <f aca="false">J19/O19</f>
-        <v>0.444212721584984</v>
-      </c>
-      <c r="K28" s="36" t="n">
-        <f aca="false">K19/O19</f>
+      <c r="I28" s="32">
+        <f>I19/O19</f>
+        <v>0.41416625676340385</v>
+      </c>
+      <c r="J28" s="32">
+        <f>J19/O19</f>
+        <v>0.41908509591736348</v>
+      </c>
+      <c r="K28" s="32">
+        <f>K19/O19</f>
         <v>0</v>
       </c>
-      <c r="L28" s="36" t="n">
-        <f aca="false">L19/O19</f>
-        <v>0.0312825860271116</v>
-      </c>
-      <c r="M28" s="36" t="n">
-        <f aca="false">M19/O19</f>
-        <v>0.0469238790406674</v>
-      </c>
-      <c r="N28" s="36" t="n">
-        <f aca="false">N19/O19</f>
-        <v>0.0698644421272159</v>
-      </c>
-      <c r="O28" s="37" t="n">
-        <f aca="false">SUM(I28:N28)</f>
+      <c r="L28" s="32">
+        <f>L19/O19</f>
+        <v>2.9513034923757994E-2</v>
+      </c>
+      <c r="M28" s="32">
+        <f>M19/O19</f>
+        <v>4.4269552385636991E-2</v>
+      </c>
+      <c r="N28" s="32">
+        <f>N19/O19</f>
+        <v>9.2966060009837675E-2</v>
+      </c>
+      <c r="O28" s="33">
+        <f>SUM(I28:N28)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A29" s="5" t="s">
         <v>6</v>
       </c>
       <c r="B29" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C29" s="5" t="n">
+      <c r="C29" s="5">
         <v>47</v>
       </c>
-      <c r="D29" s="6" t="n">
+      <c r="D29" s="40">
         <v>43532</v>
       </c>
-      <c r="H29" s="35" t="s">
-        <v>16</v>
-      </c>
-      <c r="I29" s="36" t="n">
-        <f aca="false">I20/O20</f>
-        <v>0.130591413989793</v>
-      </c>
-      <c r="J29" s="36" t="n">
-        <f aca="false">J20/O20</f>
-        <v>0.0270189132392675</v>
-      </c>
-      <c r="K29" s="36" t="n">
-        <f aca="false">K20/O20</f>
+      <c r="H29" s="31" t="s">
+        <v>16</v>
+      </c>
+      <c r="I29" s="32">
+        <f>I20/O20</f>
+        <v>0.1361241217798595</v>
+      </c>
+      <c r="J29" s="32">
+        <f>J20/O20</f>
+        <v>2.6346604215456676E-2</v>
+      </c>
+      <c r="K29" s="32">
+        <f>K20/O20</f>
         <v>0</v>
       </c>
-      <c r="L29" s="36" t="n">
-        <f aca="false">L20/O20</f>
-        <v>0.802161513059141</v>
-      </c>
-      <c r="M29" s="36" t="n">
-        <f aca="false">M20/O20</f>
+      <c r="L29" s="32">
+        <f>L20/O20</f>
+        <v>0.7822014051522248</v>
+      </c>
+      <c r="M29" s="32">
+        <f>M20/O20</f>
         <v>0</v>
       </c>
-      <c r="N29" s="36" t="n">
-        <f aca="false">N20/O20</f>
-        <v>0.0402281597117983</v>
-      </c>
-      <c r="O29" s="38" t="n">
-        <f aca="false">SUM(I29:N29)</f>
+      <c r="N29" s="32">
+        <f>N20/O20</f>
+        <v>5.5327868852459015E-2</v>
+      </c>
+      <c r="O29" s="34">
+        <f>SUM(I29:N29)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A30" s="5" t="s">
         <v>25</v>
       </c>
       <c r="B30" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C30" s="5" t="n">
-        <v>15</v>
-      </c>
-      <c r="D30" s="6" t="n">
+      <c r="C30" s="5">
+        <v>15</v>
+      </c>
+      <c r="D30" s="40">
         <v>43532</v>
       </c>
-      <c r="H30" s="39" t="s">
+      <c r="H30" s="35" t="s">
         <v>27</v>
       </c>
-      <c r="I30" s="40" t="n">
-        <f aca="false">AVERAGE(I26:I29)</f>
-        <v>0.248040932092658</v>
-      </c>
-      <c r="J30" s="40" t="n">
-        <f aca="false">AVERAGE(J26:J29)</f>
-        <v>0.254872805073697</v>
-      </c>
-      <c r="K30" s="40" t="n">
-        <f aca="false">AVERAGE(K26:K29)</f>
-        <v>0.0181174510620575</v>
-      </c>
-      <c r="L30" s="40" t="n">
-        <f aca="false">AVERAGE(L26:L29)</f>
-        <v>0.415650490512584</v>
-      </c>
-      <c r="M30" s="40" t="n">
-        <f aca="false">AVERAGE(M26:M29)</f>
-        <v>0.0117309697601668</v>
-      </c>
-      <c r="N30" s="41" t="n">
-        <f aca="false">AVERAGE(N26:N29)</f>
-        <v>0.0515873514988366</v>
-      </c>
-      <c r="O30" s="42" t="n">
-        <f aca="false">SUM(I30:N30)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I30" s="36">
+        <f t="shared" ref="I30:N30" si="1">AVERAGE(I26:I29)</f>
+        <v>0.25425367562332274</v>
+      </c>
+      <c r="J30" s="36">
+        <f t="shared" si="1"/>
+        <v>0.24259826934871467</v>
+      </c>
+      <c r="K30" s="36">
+        <f t="shared" si="1"/>
+        <v>1.7289348171701111E-2</v>
+      </c>
+      <c r="L30" s="36">
+        <f t="shared" si="1"/>
+        <v>0.40503278894777733</v>
+      </c>
+      <c r="M30" s="36">
+        <f t="shared" si="1"/>
+        <v>1.1067388096409248E-2</v>
+      </c>
+      <c r="N30" s="37">
+        <f t="shared" si="1"/>
+        <v>6.9758529812074879E-2</v>
+      </c>
+      <c r="O30" s="38">
+        <f>SUM(I30:N30)</f>
+        <v>1.0000000000000002</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A31" s="5" t="s">
         <v>25</v>
       </c>
       <c r="B31" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C31" s="5" t="n">
+      <c r="C31" s="5">
         <v>55</v>
       </c>
-      <c r="D31" s="6" t="n">
+      <c r="D31" s="40">
         <v>43531</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A32" s="5" t="s">
         <v>25</v>
       </c>
       <c r="B32" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C32" s="5" t="n">
+      <c r="C32" s="5">
         <v>68</v>
       </c>
-      <c r="D32" s="6" t="n">
+      <c r="D32" s="40">
         <v>43532</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="5" t="s">
         <v>25</v>
       </c>
       <c r="B33" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C33" s="5" t="n">
+      <c r="C33" s="5">
         <v>129</v>
       </c>
-      <c r="D33" s="6" t="n">
+      <c r="D33" s="40">
         <v>43533</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="5" t="s">
         <v>25</v>
       </c>
       <c r="B34" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C34" s="5" t="n">
+      <c r="C34" s="5">
         <v>95</v>
       </c>
-      <c r="D34" s="6" t="n">
+      <c r="D34" s="40">
         <v>43534</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="5" t="s">
         <v>6</v>
       </c>
       <c r="B35" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C35" s="5" t="n">
+      <c r="C35" s="5">
         <v>74</v>
       </c>
-      <c r="D35" s="6" t="n">
+      <c r="D35" s="40">
         <v>43546</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="5" t="s">
         <v>6</v>
       </c>
       <c r="B36" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C36" s="5" t="n">
+      <c r="C36" s="5">
         <v>52</v>
       </c>
-      <c r="D36" s="6" t="n">
+      <c r="D36" s="40">
         <v>43546</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" s="5" t="s">
         <v>16</v>
       </c>
       <c r="B37" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C37" s="5" t="n">
+      <c r="C37" s="5">
         <v>196</v>
       </c>
-      <c r="D37" s="6" t="n">
+      <c r="D37" s="40">
         <v>43376</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" s="5" t="s">
         <v>16</v>
       </c>
       <c r="B38" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C38" s="5" t="n">
+      <c r="C38" s="5">
         <v>115</v>
       </c>
-      <c r="D38" s="6" t="n">
+      <c r="D38" s="40">
         <v>43407</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" s="5" t="s">
         <v>25</v>
       </c>
       <c r="B39" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C39" s="5" t="n">
+      <c r="C39" s="5">
         <v>10</v>
       </c>
-      <c r="D39" s="6" t="n">
+      <c r="D39" s="40">
         <v>43546</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" s="5" t="s">
         <v>19</v>
       </c>
       <c r="B40" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C40" s="5" t="n">
+      <c r="C40" s="5">
         <v>60</v>
       </c>
-      <c r="D40" s="6" t="n">
+      <c r="D40" s="40">
         <v>43553</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" s="5" t="s">
         <v>25</v>
       </c>
       <c r="B41" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C41" s="5" t="n">
+      <c r="C41" s="5">
         <v>60</v>
       </c>
-      <c r="D41" s="6" t="n">
+      <c r="D41" s="40">
         <v>43553</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" s="5" t="s">
         <v>16</v>
       </c>
       <c r="B42" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C42" s="5" t="n">
+      <c r="C42" s="5">
         <v>60</v>
       </c>
-      <c r="D42" s="6" t="n">
+      <c r="D42" s="40">
         <v>43553</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" s="5" t="s">
         <v>19</v>
       </c>
       <c r="B43" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C43" s="5" t="n">
+      <c r="C43" s="5">
         <v>60</v>
       </c>
-      <c r="D43" s="6" t="n">
+      <c r="D43" s="40">
         <v>43481</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" s="5" t="s">
         <v>19</v>
       </c>
       <c r="B44" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C44" s="5" t="n">
+      <c r="C44" s="5">
         <v>150</v>
       </c>
-      <c r="D44" s="6" t="n">
+      <c r="D44" s="40">
         <v>43442</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" s="5" t="s">
         <v>19</v>
       </c>
       <c r="B45" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C45" s="5" t="n">
+      <c r="C45" s="5">
         <v>180</v>
       </c>
-      <c r="D45" s="6" t="n">
+      <c r="D45" s="40">
         <v>43448</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" s="5" t="s">
         <v>19</v>
       </c>
       <c r="B46" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C46" s="5" t="n">
+      <c r="C46" s="5">
         <v>180</v>
       </c>
-      <c r="D46" s="6" t="n">
+      <c r="D46" s="40">
         <v>43468</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" s="5" t="s">
         <v>19</v>
       </c>
       <c r="B47" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C47" s="5" t="n">
+      <c r="C47" s="5">
         <v>120</v>
       </c>
-      <c r="D47" s="6" t="n">
+      <c r="D47" s="40">
         <v>43478</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" s="5" t="s">
         <v>6</v>
       </c>
       <c r="B48" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C48" s="5" t="n">
+      <c r="C48" s="5">
         <v>300</v>
       </c>
-      <c r="D48" s="6" t="n">
+      <c r="D48" s="40">
         <v>43449</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" s="5" t="s">
         <v>6</v>
       </c>
       <c r="B49" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C49" s="5" t="n">
+      <c r="C49" s="5">
         <v>150</v>
       </c>
-      <c r="D49" s="6" t="n">
+      <c r="D49" s="40">
         <v>43450</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" s="5" t="s">
         <v>19</v>
       </c>
       <c r="B50" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C50" s="5" t="n">
+      <c r="C50" s="5">
         <v>82</v>
       </c>
-      <c r="D50" s="6" t="n">
+      <c r="D50" s="40">
         <v>43558</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" s="5" t="s">
         <v>25</v>
       </c>
       <c r="B51" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C51" s="5" t="n">
+      <c r="C51" s="5">
         <v>82</v>
       </c>
-      <c r="D51" s="6" t="n">
+      <c r="D51" s="40">
         <v>43558</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" s="5" t="s">
         <v>6</v>
       </c>
       <c r="B52" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C52" s="5" t="n">
+      <c r="C52" s="5">
         <v>82</v>
       </c>
-      <c r="D52" s="6" t="n">
+      <c r="D52" s="40">
         <v>43558</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" s="5" t="s">
         <v>25</v>
       </c>
       <c r="B53" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C53" s="5" t="n">
+      <c r="C53" s="5">
         <v>85</v>
       </c>
-      <c r="D53" s="6" t="n">
+      <c r="D53" s="40">
         <v>43559</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" s="5" t="s">
         <v>19</v>
       </c>
       <c r="B54" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C54" s="5" t="n">
+      <c r="C54" s="5">
         <v>70</v>
       </c>
-      <c r="D54" s="6" t="n">
+      <c r="D54" s="40">
         <v>43571</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" s="5" t="s">
         <v>25</v>
       </c>
       <c r="B55" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C55" s="5" t="n">
+      <c r="C55" s="5">
         <v>70</v>
       </c>
-      <c r="D55" s="6" t="n">
+      <c r="D55" s="40">
         <v>43571</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" s="5" t="s">
         <v>19</v>
       </c>
       <c r="B56" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C56" s="5" t="n">
+      <c r="C56" s="5">
         <v>120</v>
       </c>
-      <c r="D56" s="6" t="n">
+      <c r="D56" s="40">
         <v>43572</v>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" s="5" t="s">
         <v>19</v>
       </c>
       <c r="B57" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C57" s="5" t="n">
+      <c r="C57" s="5">
         <v>100</v>
       </c>
-      <c r="D57" s="6" t="n">
+      <c r="D57" s="40">
         <v>43574</v>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" s="5" t="s">
         <v>6</v>
       </c>
       <c r="B58" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C58" s="5" t="n">
+      <c r="C58" s="5">
         <v>42</v>
       </c>
-      <c r="D58" s="6" t="n">
+      <c r="D58" s="40">
         <v>43577</v>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" s="5" t="s">
         <v>6</v>
       </c>
       <c r="B59" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C59" s="5" t="n">
+      <c r="C59" s="5">
         <v>97</v>
       </c>
-      <c r="D59" s="6" t="n">
+      <c r="D59" s="40">
         <v>43578</v>
       </c>
     </row>
-    <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" s="5" t="s">
         <v>25</v>
       </c>
       <c r="B60" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C60" s="5" t="n">
+      <c r="C60" s="5">
         <v>30</v>
       </c>
-      <c r="D60" s="6" t="n">
+      <c r="D60" s="40">
         <v>43578</v>
       </c>
     </row>
-    <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" s="5" t="s">
         <v>6</v>
       </c>
       <c r="B61" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C61" s="5" t="n">
+      <c r="C61" s="5">
         <v>107</v>
       </c>
-      <c r="D61" s="6" t="n">
+      <c r="D61" s="40">
         <v>43581</v>
       </c>
     </row>
-    <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" s="5" t="s">
         <v>6</v>
       </c>
       <c r="B62" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C62" s="5" t="n">
+      <c r="C62" s="5">
         <v>39</v>
       </c>
-      <c r="D62" s="6" t="n">
+      <c r="D62" s="40">
         <v>43584</v>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" s="5" t="s">
         <v>6</v>
       </c>
       <c r="B63" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C63" s="5" t="n">
+      <c r="C63" s="5">
         <v>22</v>
       </c>
-      <c r="D63" s="6" t="n">
+      <c r="D63" s="40">
         <v>43585</v>
       </c>
     </row>
-    <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" s="5" t="s">
         <v>19</v>
       </c>
       <c r="B64" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C64" s="5" t="n">
+      <c r="C64" s="5">
         <v>22</v>
       </c>
-      <c r="D64" s="6" t="n">
+      <c r="D64" s="40">
         <v>43585</v>
       </c>
     </row>
-    <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" s="5" t="s">
         <v>19</v>
       </c>
       <c r="B65" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C65" s="5" t="n">
-        <v>25</v>
-      </c>
-      <c r="D65" s="6" t="n">
+      <c r="C65" s="5">
+        <v>25</v>
+      </c>
+      <c r="D65" s="40">
         <v>43587</v>
       </c>
     </row>
-    <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66" s="5" t="s">
         <v>16</v>
       </c>
       <c r="B66" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C66" s="5" t="n">
-        <v>25</v>
-      </c>
-      <c r="D66" s="6" t="n">
+      <c r="C66" s="5">
+        <v>25</v>
+      </c>
+      <c r="D66" s="40">
         <v>43587</v>
       </c>
     </row>
-    <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67" s="5" t="s">
         <v>16</v>
       </c>
       <c r="B67" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C67" s="5" t="n">
+      <c r="C67" s="5">
         <v>136</v>
       </c>
-      <c r="D67" s="6" t="n">
+      <c r="D67" s="40">
         <v>43587</v>
       </c>
     </row>
-    <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68" s="5" t="s">
         <v>16</v>
       </c>
       <c r="B68" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C68" s="5" t="n">
+      <c r="C68" s="5">
         <v>35</v>
       </c>
-      <c r="D68" s="6" t="n">
+      <c r="D68" s="40">
         <v>43587</v>
       </c>
     </row>
-    <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69" s="5" t="s">
         <v>16</v>
       </c>
       <c r="B69" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C69" s="5" t="n">
+      <c r="C69" s="5">
         <v>135</v>
       </c>
-      <c r="D69" s="6" t="n">
+      <c r="D69" s="40">
         <v>43588</v>
       </c>
     </row>
-    <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70" s="5" t="s">
         <v>25</v>
       </c>
       <c r="B70" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C70" s="5" t="n">
+      <c r="C70" s="5">
         <v>135</v>
       </c>
-      <c r="D70" s="6" t="n">
+      <c r="D70" s="40">
         <v>43588</v>
       </c>
     </row>
-    <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71" s="5" t="s">
         <v>25</v>
       </c>
       <c r="B71" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C71" s="5" t="n">
+      <c r="C71" s="5">
         <v>40</v>
       </c>
-      <c r="D71" s="6" t="n">
+      <c r="D71" s="40">
         <v>43589</v>
       </c>
     </row>
-    <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72" s="5" t="s">
         <v>16</v>
       </c>
       <c r="B72" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C72" s="5" t="n">
+      <c r="C72" s="5">
         <v>40</v>
       </c>
-      <c r="D72" s="6" t="n">
+      <c r="D72" s="40">
         <v>43589</v>
       </c>
     </row>
-    <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73" s="5" t="s">
         <v>25</v>
       </c>
       <c r="B73" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C73" s="5" t="n">
+      <c r="C73" s="5">
         <v>78</v>
       </c>
-      <c r="D73" s="6" t="n">
+      <c r="D73" s="40">
         <v>43590</v>
       </c>
     </row>
-    <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74" s="5" t="s">
         <v>16</v>
       </c>
       <c r="B74" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C74" s="5" t="n">
+      <c r="C74" s="5">
         <v>78</v>
       </c>
-      <c r="D74" s="6" t="n">
+      <c r="D74" s="40">
         <v>43590</v>
       </c>
     </row>
-    <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75" s="5" t="s">
         <v>6</v>
       </c>
       <c r="B75" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C75" s="5" t="n">
+      <c r="C75" s="5">
         <v>45</v>
       </c>
-      <c r="D75" s="6" t="n">
+      <c r="D75" s="40">
         <v>43593</v>
       </c>
     </row>
-    <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76" s="5" t="s">
         <v>25</v>
       </c>
       <c r="B76" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C76" s="5" t="n">
+      <c r="C76" s="5">
         <v>45</v>
       </c>
-      <c r="D76" s="6" t="n">
+      <c r="D76" s="40">
         <v>43593</v>
       </c>
     </row>
-    <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" s="5" t="s">
         <v>19</v>
       </c>
       <c r="B77" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C77" s="5" t="n">
+      <c r="C77" s="5">
         <v>45</v>
       </c>
-      <c r="D77" s="6" t="n">
+      <c r="D77" s="40">
         <v>43593</v>
       </c>
     </row>
-    <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A78" s="5" t="s">
         <v>16</v>
       </c>
       <c r="B78" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C78" s="5" t="n">
+      <c r="C78" s="5">
         <v>45</v>
       </c>
-      <c r="D78" s="6" t="n">
+      <c r="D78" s="40">
         <v>43593</v>
       </c>
     </row>
-    <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A79" s="5" t="s">
         <v>25</v>
       </c>
       <c r="B79" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C79" s="5" t="n">
+      <c r="C79" s="5">
         <v>60</v>
       </c>
-      <c r="D79" s="6" t="n">
+      <c r="D79" s="40">
         <v>43593</v>
       </c>
     </row>
-    <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A80" s="5" t="s">
         <v>19</v>
       </c>
       <c r="B80" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C80" s="5" t="n">
+      <c r="C80" s="5">
         <v>60</v>
       </c>
-      <c r="D80" s="6" t="n">
+      <c r="D80" s="40">
         <v>43593</v>
       </c>
     </row>
-    <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A81" s="5" t="s">
         <v>16</v>
       </c>
       <c r="B81" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C81" s="5" t="n">
+      <c r="C81" s="5">
         <v>60</v>
       </c>
-      <c r="D81" s="6" t="n">
+      <c r="D81" s="40">
         <v>43593</v>
       </c>
     </row>
-    <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A82" s="5" t="s">
         <v>16</v>
       </c>
       <c r="B82" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C82" s="5" t="n">
+      <c r="C82" s="5">
         <v>116</v>
       </c>
-      <c r="D82" s="6" t="n">
+      <c r="D82" s="40">
         <v>43594</v>
       </c>
     </row>
-    <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A83" s="5" t="s">
         <v>25</v>
       </c>
       <c r="B83" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C83" s="5" t="n">
+      <c r="C83" s="5">
         <v>116</v>
       </c>
-      <c r="D83" s="6" t="n">
+      <c r="D83" s="40">
         <v>43594</v>
       </c>
     </row>
-    <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A84" s="5" t="s">
         <v>6</v>
       </c>
       <c r="B84" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C84" s="5" t="n">
+      <c r="C84" s="5">
         <v>47</v>
       </c>
-      <c r="D84" s="6" t="n">
+      <c r="D84" s="40">
         <v>43598</v>
       </c>
     </row>
-    <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A85" s="5" t="s">
         <v>6</v>
       </c>
       <c r="B85" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C85" s="5" t="n">
+      <c r="C85" s="5">
         <v>31</v>
       </c>
-      <c r="D85" s="6" t="n">
+      <c r="D85" s="40">
         <v>43598</v>
       </c>
     </row>
-    <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A86" s="5" t="s">
         <v>25</v>
       </c>
       <c r="B86" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C86" s="5" t="n">
+      <c r="C86" s="5">
         <v>160</v>
       </c>
-      <c r="D86" s="6" t="n">
+      <c r="D86" s="40">
         <v>43595</v>
       </c>
     </row>
-    <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A87" s="5" t="s">
         <v>16</v>
       </c>
       <c r="B87" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C87" s="5" t="n">
+      <c r="C87" s="5">
         <v>160</v>
       </c>
-      <c r="D87" s="6" t="n">
+      <c r="D87" s="40">
         <v>43595</v>
       </c>
     </row>
-    <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A88" s="5" t="s">
         <v>25</v>
       </c>
       <c r="B88" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C88" s="5" t="n">
+      <c r="C88" s="5">
         <v>240</v>
       </c>
-      <c r="D88" s="6" t="n">
+      <c r="D88" s="40">
         <v>43599</v>
       </c>
     </row>
-    <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A89" s="5" t="s">
         <v>16</v>
       </c>
       <c r="B89" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C89" s="5" t="n">
+      <c r="C89" s="5">
         <v>240</v>
       </c>
-      <c r="D89" s="6" t="n">
+      <c r="D89" s="40">
         <v>43599</v>
       </c>
     </row>
-    <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A90" s="5" t="s">
         <v>6</v>
       </c>
       <c r="B90" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C90" s="5" t="n">
+      <c r="C90" s="5">
         <v>40</v>
       </c>
-      <c r="D90" s="6" t="n">
+      <c r="D90" s="40">
         <v>43600</v>
       </c>
     </row>
-    <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A91" s="5" t="s">
         <v>19</v>
       </c>
       <c r="B91" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C91" s="5" t="n">
+      <c r="C91" s="5">
         <v>40</v>
       </c>
-      <c r="D91" s="6" t="n">
+      <c r="D91" s="40">
         <v>43600</v>
       </c>
     </row>
-    <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A92" s="5" t="s">
         <v>16</v>
       </c>
       <c r="B92" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C92" s="5" t="n">
+      <c r="C92" s="5">
         <v>40</v>
       </c>
-      <c r="D92" s="6" t="n">
+      <c r="D92" s="40">
         <v>43600</v>
       </c>
     </row>
-    <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A93" s="5" t="s">
         <v>25</v>
       </c>
       <c r="B93" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C93" s="5" t="n">
+      <c r="C93" s="5">
         <v>40</v>
       </c>
-      <c r="D93" s="6" t="n">
+      <c r="D93" s="40">
         <v>43600</v>
       </c>
     </row>
-    <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A94" s="5" t="s">
         <v>6</v>
       </c>
       <c r="B94" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C94" s="5" t="n">
+      <c r="C94" s="5">
         <v>20</v>
       </c>
-      <c r="D94" s="6" t="n">
+      <c r="D94" s="40">
         <v>43600</v>
       </c>
     </row>
-    <row r="95" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A95" s="5" t="s">
         <v>19</v>
       </c>
       <c r="B95" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C95" s="5" t="n">
+      <c r="C95" s="5">
         <v>20</v>
       </c>
-      <c r="D95" s="6" t="n">
+      <c r="D95" s="40">
         <v>43600</v>
       </c>
     </row>
-    <row r="96" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A96" s="5" t="s">
         <v>16</v>
       </c>
       <c r="B96" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C96" s="5" t="n">
+      <c r="C96" s="5">
         <v>20</v>
       </c>
-      <c r="D96" s="6" t="n">
+      <c r="D96" s="40">
         <v>43600</v>
       </c>
     </row>
-    <row r="97" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A97" s="5" t="s">
         <v>25</v>
       </c>
       <c r="B97" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C97" s="5" t="n">
+      <c r="C97" s="5">
         <v>20</v>
       </c>
-      <c r="D97" s="6" t="n">
+      <c r="D97" s="40">
         <v>43600</v>
       </c>
     </row>
-    <row r="98" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A98" s="5" t="s">
         <v>25</v>
       </c>
       <c r="B98" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C98" s="5" t="n">
+      <c r="C98" s="5">
         <v>210</v>
       </c>
-      <c r="D98" s="6" t="n">
+      <c r="D98" s="40">
         <v>43603</v>
       </c>
     </row>
-    <row r="99" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A99" s="5" t="s">
         <v>16</v>
       </c>
       <c r="B99" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C99" s="5" t="n">
+      <c r="C99" s="5">
         <v>210</v>
       </c>
-      <c r="D99" s="6" t="n">
+      <c r="D99" s="40">
         <v>43603</v>
       </c>
     </row>
-    <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A100" s="5" t="s">
         <v>25</v>
       </c>
       <c r="B100" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C100" s="5" t="n">
+      <c r="C100" s="5">
         <v>65</v>
       </c>
-      <c r="D100" s="6" t="n">
+      <c r="D100" s="40">
         <v>43604</v>
       </c>
     </row>
-    <row r="101" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A101" s="5" t="s">
         <v>16</v>
       </c>
       <c r="B101" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C101" s="5" t="n">
+      <c r="C101" s="5">
         <v>65</v>
       </c>
-      <c r="D101" s="6" t="n">
+      <c r="D101" s="40">
         <v>43604</v>
       </c>
     </row>
-    <row r="102" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A102" s="5" t="s">
         <v>16</v>
       </c>
       <c r="B102" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C102" s="5" t="n">
+      <c r="C102" s="5">
         <v>110</v>
       </c>
-      <c r="D102" s="6" t="n">
+      <c r="D102" s="40">
         <v>43604</v>
       </c>
     </row>
-    <row r="103" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A103" s="5" t="s">
         <v>16</v>
       </c>
       <c r="B103" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C103" s="5" t="n">
+      <c r="C103" s="5">
         <v>20</v>
       </c>
-      <c r="D103" s="6" t="n">
+      <c r="D103" s="40">
         <v>43605</v>
       </c>
     </row>
-    <row r="104" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A104" s="5" t="s">
         <v>25</v>
       </c>
       <c r="B104" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C104" s="5" t="n">
-        <v>15</v>
-      </c>
-      <c r="D104" s="6" t="n">
+      <c r="C104" s="5">
+        <v>15</v>
+      </c>
+      <c r="D104" s="40">
         <v>43606</v>
       </c>
     </row>
-    <row r="105" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A105" s="5" t="s">
         <v>6</v>
       </c>
       <c r="B105" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C105" s="5" t="n">
+      <c r="C105" s="5">
         <v>30</v>
       </c>
-      <c r="D105" s="6" t="n">
+      <c r="D105" s="40">
         <v>43607</v>
       </c>
     </row>
-    <row r="106" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A106" s="5" t="s">
         <v>16</v>
       </c>
       <c r="B106" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C106" s="5" t="n">
+      <c r="C106" s="5">
         <v>30</v>
       </c>
-      <c r="D106" s="6" t="n">
+      <c r="D106" s="40">
         <v>43607</v>
       </c>
     </row>
-    <row r="107" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A107" s="5" t="s">
         <v>25</v>
       </c>
       <c r="B107" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C107" s="5" t="n">
+      <c r="C107" s="5">
         <v>30</v>
       </c>
-      <c r="D107" s="6" t="n">
+      <c r="D107" s="40">
         <v>43607</v>
       </c>
     </row>
-    <row r="108" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A108" s="5" t="s">
         <v>6</v>
       </c>
       <c r="B108" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C108" s="5" t="n">
+      <c r="C108" s="5">
         <v>30</v>
       </c>
-      <c r="D108" s="6" t="n">
+      <c r="D108" s="40">
         <v>43607</v>
       </c>
     </row>
-    <row r="109" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A109" s="5" t="s">
         <v>16</v>
       </c>
       <c r="B109" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C109" s="5" t="n">
+      <c r="C109" s="5">
         <v>30</v>
       </c>
-      <c r="D109" s="6" t="n">
+      <c r="D109" s="40">
         <v>43607</v>
       </c>
     </row>
-    <row r="110" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A110" s="5" t="s">
         <v>25</v>
       </c>
       <c r="B110" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C110" s="5" t="n">
+      <c r="C110" s="5">
         <v>30</v>
       </c>
-      <c r="D110" s="6" t="n">
+      <c r="D110" s="40">
         <v>43607</v>
       </c>
     </row>
-    <row r="111" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A111" s="5" t="s">
         <v>16</v>
       </c>
       <c r="B111" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C111" s="5" t="n">
+      <c r="C111" s="5">
         <v>130</v>
       </c>
-      <c r="D111" s="6" t="n">
+      <c r="D111" s="40">
         <v>43607</v>
       </c>
     </row>
-    <row r="112" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A112" s="5" t="s">
         <v>25</v>
       </c>
       <c r="B112" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C112" s="5" t="n">
+      <c r="C112" s="5">
         <v>130</v>
       </c>
-      <c r="D112" s="6" t="n">
+      <c r="D112" s="40">
         <v>43607</v>
       </c>
     </row>
-    <row r="113" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A113" s="5" t="s">
         <v>25</v>
       </c>
       <c r="B113" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C113" s="5" t="n">
+      <c r="C113" s="5">
         <v>20</v>
       </c>
-      <c r="D113" s="6" t="n">
+      <c r="D113" s="40">
         <v>43607</v>
       </c>
     </row>
-    <row r="114" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A114" s="5" t="s">
         <v>6</v>
       </c>
       <c r="B114" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C114" s="5" t="n">
+      <c r="C114" s="5">
         <v>68</v>
       </c>
-      <c r="D114" s="6" t="n">
+      <c r="D114" s="40">
         <v>43608</v>
       </c>
     </row>
-    <row r="115" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A115" s="5" t="s">
         <v>6</v>
       </c>
       <c r="B115" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C115" s="5" t="n">
+      <c r="C115" s="5">
         <v>23</v>
       </c>
-      <c r="D115" s="6" t="n">
+      <c r="D115" s="40">
         <v>43609</v>
       </c>
     </row>
-    <row r="116" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A116" s="5" t="s">
         <v>16</v>
       </c>
       <c r="B116" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C116" s="5" t="n">
+      <c r="C116" s="5">
         <v>85</v>
       </c>
-      <c r="D116" s="6" t="n">
+      <c r="D116" s="40">
         <v>43608</v>
       </c>
     </row>
-    <row r="117" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A117" s="5" t="s">
         <v>25</v>
       </c>
       <c r="B117" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C117" s="5" t="n">
+      <c r="C117" s="5">
         <v>85</v>
       </c>
-      <c r="D117" s="6" t="n">
+      <c r="D117" s="40">
         <v>43608</v>
       </c>
     </row>
-    <row r="118" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A118" s="5" t="s">
         <v>25</v>
       </c>
       <c r="B118" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C118" s="5" t="n">
+      <c r="C118" s="5">
         <v>73</v>
       </c>
-      <c r="D118" s="6" t="n">
+      <c r="D118" s="40">
         <v>43609</v>
       </c>
     </row>
-    <row r="119" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A119" s="5" t="s">
         <v>19</v>
       </c>
       <c r="B119" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C119" s="5" t="n">
+      <c r="C119" s="5">
         <v>30</v>
       </c>
-      <c r="D119" s="6" t="n">
+      <c r="D119" s="40">
         <v>43614</v>
       </c>
     </row>
-    <row r="120" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A120" s="5" t="s">
         <v>16</v>
       </c>
       <c r="B120" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C120" s="5" t="n">
+      <c r="C120" s="5">
         <v>30</v>
       </c>
-      <c r="D120" s="6" t="n">
+      <c r="D120" s="40">
         <v>43614</v>
       </c>
     </row>
-    <row r="121" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A121" s="5" t="s">
         <v>6</v>
       </c>
       <c r="B121" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C121" s="5" t="n">
+      <c r="C121" s="5">
         <v>30</v>
       </c>
-      <c r="D121" s="6" t="n">
+      <c r="D121" s="40">
         <v>43614</v>
       </c>
     </row>
-    <row r="122" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A122" s="5" t="s">
         <v>19</v>
       </c>
       <c r="B122" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C122" s="5" t="n">
+      <c r="C122" s="5">
         <v>84</v>
       </c>
-      <c r="D122" s="6" t="n">
+      <c r="D122" s="40">
         <v>43614</v>
       </c>
     </row>
-    <row r="123" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A123" s="5" t="s">
         <v>16</v>
       </c>
       <c r="B123" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C123" s="5" t="n">
+      <c r="C123" s="5">
         <v>84</v>
       </c>
-      <c r="D123" s="6" t="n">
+      <c r="D123" s="40">
         <v>43614</v>
       </c>
     </row>
-    <row r="124" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A124" s="5" t="s">
         <v>6</v>
       </c>
       <c r="B124" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C124" s="5" t="n">
+      <c r="C124" s="5">
         <v>84</v>
       </c>
-      <c r="D124" s="6" t="n">
+      <c r="D124" s="40">
         <v>43614</v>
       </c>
     </row>
-    <row r="125" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A125" s="5" t="s">
         <v>25</v>
       </c>
       <c r="B125" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C125" s="5" t="n">
+      <c r="C125" s="5">
         <v>84</v>
       </c>
-      <c r="D125" s="6" t="n">
+      <c r="D125" s="40">
         <v>43614</v>
       </c>
     </row>
-    <row r="126" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A126" s="5" t="s">
         <v>6</v>
       </c>
       <c r="B126" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C126" s="5" t="n">
+      <c r="C126" s="5">
         <v>64</v>
       </c>
-      <c r="D126" s="43" t="s">
+      <c r="D126" s="41" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="127" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A127" s="5" t="s">
         <v>6</v>
       </c>
       <c r="B127" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C127" s="5" t="n">
+      <c r="C127" s="5">
         <v>98</v>
       </c>
-      <c r="D127" s="43" t="s">
+      <c r="D127" s="41" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="128" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A128" s="5" t="s">
         <v>19</v>
       </c>
       <c r="B128" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C128" s="5" t="n">
+      <c r="C128" s="5">
         <v>60</v>
       </c>
-      <c r="D128" s="43" t="n">
+      <c r="D128" s="41">
         <v>43471</v>
       </c>
     </row>
-    <row r="129" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="129" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A129" s="5" t="s">
         <v>16</v>
       </c>
       <c r="B129" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C129" s="5" t="n">
+      <c r="C129" s="5">
         <v>165</v>
       </c>
-      <c r="D129" s="44" t="n">
+      <c r="D129" s="41">
         <v>43616</v>
       </c>
     </row>
-    <row r="130" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="130" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A130" s="5" t="s">
         <v>25</v>
       </c>
       <c r="B130" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C130" s="5" t="n">
+      <c r="C130" s="5">
         <v>165</v>
       </c>
-      <c r="D130" s="44" t="n">
+      <c r="D130" s="41">
         <v>43616</v>
       </c>
     </row>
-    <row r="131" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="131" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A131" s="5" t="s">
         <v>16</v>
       </c>
       <c r="B131" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C131" s="5" t="n">
+      <c r="C131" s="5">
         <v>118</v>
       </c>
-      <c r="D131" s="43" t="n">
+      <c r="D131" s="41">
         <v>43618</v>
       </c>
     </row>
-    <row r="132" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="132" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A132" s="5" t="s">
         <v>25</v>
       </c>
       <c r="B132" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C132" s="5" t="n">
+      <c r="C132" s="5">
         <v>118</v>
       </c>
-      <c r="D132" s="43" t="n">
+      <c r="D132" s="41">
         <v>43618</v>
       </c>
     </row>
-    <row r="133" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="133" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A133" s="5" t="s">
         <v>25</v>
       </c>
       <c r="B133" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C133" s="5" t="n">
+      <c r="C133" s="5">
         <v>20</v>
       </c>
-      <c r="D133" s="45" t="n">
+      <c r="D133" s="40">
         <v>43530</v>
       </c>
     </row>
-    <row r="134" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="134" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A134" s="5" t="s">
         <v>19</v>
       </c>
       <c r="B134" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C134" s="5" t="n">
+      <c r="C134" s="5">
         <v>30</v>
       </c>
-      <c r="D134" s="44" t="n">
+      <c r="D134" s="41">
         <v>43619</v>
       </c>
     </row>
-    <row r="135" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="135" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A135" s="5" t="s">
         <v>19</v>
       </c>
       <c r="B135" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C135" s="5" t="n">
+      <c r="C135" s="5">
         <v>30</v>
       </c>
-      <c r="D135" s="44" t="n">
+      <c r="D135" s="41">
         <v>43619</v>
       </c>
     </row>
-    <row r="136" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="136" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A136" s="5" t="s">
         <v>19</v>
       </c>
       <c r="B136" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C136" s="5" t="n">
+      <c r="C136" s="5">
         <v>35</v>
       </c>
-      <c r="D136" s="44" t="n">
+      <c r="D136" s="41">
         <v>43619</v>
       </c>
     </row>
-    <row r="137" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="137" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A137" s="5" t="s">
         <v>25</v>
       </c>
       <c r="B137" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C137" s="5" t="n">
+      <c r="C137" s="5">
         <v>180</v>
       </c>
-      <c r="D137" s="44" t="n">
+      <c r="D137" s="41">
         <v>43620</v>
       </c>
     </row>
-    <row r="138" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="138" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A138" s="5" t="s">
         <v>16</v>
       </c>
       <c r="B138" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C138" s="5" t="n">
+      <c r="C138" s="5">
         <v>180</v>
       </c>
-      <c r="D138" s="44" t="n">
+      <c r="D138" s="41">
         <v>43620</v>
       </c>
     </row>
-    <row r="139" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A139" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="B139" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="C139" s="0" t="n">
+    <row r="139" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A139" s="39" t="s">
+        <v>25</v>
+      </c>
+      <c r="B139" s="39" t="s">
+        <v>7</v>
+      </c>
+      <c r="C139" s="39">
         <v>10</v>
       </c>
-      <c r="D139" s="46" t="n">
+      <c r="D139" s="40">
         <v>43620</v>
       </c>
+    </row>
+    <row r="140" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A140" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B140" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C140" s="5">
+        <v>55</v>
+      </c>
+      <c r="D140" s="40">
+        <v>43621</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A141" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B141" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C141" s="5">
+        <v>55</v>
+      </c>
+      <c r="D141" s="40">
+        <v>43621</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A142" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B142" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C142" s="5">
+        <v>55</v>
+      </c>
+      <c r="D142" s="40">
+        <v>43621</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A143" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B143" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C143" s="5">
+        <v>55</v>
+      </c>
+      <c r="D143" s="40">
+        <v>43621</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A144" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B144" s="39" t="s">
+        <v>7</v>
+      </c>
+      <c r="C144" s="5">
+        <v>60</v>
+      </c>
+      <c r="D144" s="40">
+        <v>43621</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A145" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B145" s="39" t="s">
+        <v>7</v>
+      </c>
+      <c r="C145" s="5">
+        <v>30</v>
+      </c>
+      <c r="D145" s="40">
+        <v>43621</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A146" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B146" s="39" t="s">
+        <v>7</v>
+      </c>
+      <c r="C146" s="5">
+        <v>60</v>
+      </c>
+      <c r="D146" s="40">
+        <v>43621</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A147" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B147" s="39" t="s">
+        <v>7</v>
+      </c>
+      <c r="C147" s="5">
+        <v>30</v>
+      </c>
+      <c r="D147" s="40">
+        <v>43621</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A148" s="39"/>
+      <c r="B148" s="39"/>
+      <c r="C148" s="39"/>
+      <c r="D148" s="39"/>
+    </row>
+    <row r="149" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A149" s="39"/>
+      <c r="B149" s="39"/>
+      <c r="C149" s="39"/>
+      <c r="D149" s="39"/>
+    </row>
+    <row r="150" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A150" s="39"/>
+      <c r="B150" s="39"/>
+      <c r="C150" s="39"/>
+      <c r="D150" s="39"/>
+    </row>
+    <row r="151" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A151" s="39"/>
+      <c r="B151" s="39"/>
+      <c r="C151" s="39"/>
+      <c r="D151" s="39"/>
+    </row>
+    <row r="152" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A152" s="39"/>
+      <c r="B152" s="39"/>
+      <c r="C152" s="39"/>
+      <c r="D152" s="39"/>
+    </row>
+    <row r="153" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A153" s="39"/>
+      <c r="B153" s="39"/>
+      <c r="C153" s="39"/>
+      <c r="D153" s="39"/>
+    </row>
+    <row r="154" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A154" s="39"/>
+      <c r="B154" s="39"/>
+      <c r="C154" s="39"/>
+      <c r="D154" s="39"/>
+    </row>
+    <row r="155" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A155" s="39"/>
+      <c r="B155" s="39"/>
+      <c r="C155" s="39"/>
+      <c r="D155" s="39"/>
+    </row>
+    <row r="156" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A156" s="39"/>
+      <c r="B156" s="39"/>
+      <c r="C156" s="39"/>
+      <c r="D156" s="39"/>
+    </row>
+    <row r="157" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A157" s="39"/>
+      <c r="B157" s="39"/>
+      <c r="C157" s="39"/>
+      <c r="D157" s="39"/>
+    </row>
+    <row r="158" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A158" s="39"/>
+      <c r="B158" s="39"/>
+      <c r="C158" s="39"/>
+      <c r="D158" s="39"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -2977,12 +3379,7 @@
     <mergeCell ref="H15:O15"/>
     <mergeCell ref="H24:O24"/>
   </mergeCells>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Aggiunte test chain e documenti per i risultati dei test
Fatti tutti i requisiti funzionali TRANNE il Calendario
</commit_message>
<xml_diff>
--- a/Documentazione/Attività sul progetto/DocAttivProg.xlsx
+++ b/Documentazione/Attività sul progetto/DocAttivProg.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="30">
   <si>
     <t>Le categorie sono: Ispezione Codice, Documenti di progetto, Documenti di processo, Manuale, Sviluppo, Testing</t>
   </si>
@@ -281,15 +281,6 @@
   </cellStyleXfs>
   <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -389,6 +380,15 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -740,8 +740,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O158"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A132" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F152" sqref="F152"/>
+    <sheetView tabSelected="1" topLeftCell="A130" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G156" sqref="G156"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -758,2631 +758,2639 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="F2" s="6" t="s">
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="F2" s="3" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H3" s="5"/>
+      <c r="H3" s="2"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="8">
+      <c r="A4" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="5">
         <v>98</v>
       </c>
-      <c r="D4" s="9">
+      <c r="D4" s="6">
         <v>43484</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="H4" s="42" t="s">
         <v>8</v>
       </c>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
+      <c r="I4" s="42"/>
+      <c r="J4" s="42"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="8">
+      <c r="A5" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="5">
         <v>149</v>
       </c>
-      <c r="D5" s="9">
+      <c r="D5" s="6">
         <v>43493</v>
       </c>
-      <c r="H5" s="10" t="s">
+      <c r="H5" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="I5" s="11" t="s">
+      <c r="I5" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="J5" s="11" t="s">
+      <c r="J5" s="8" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="8" t="s">
+      <c r="A6" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="8">
+      <c r="C6" s="5">
         <v>135</v>
       </c>
-      <c r="D6" s="9">
+      <c r="D6" s="6">
         <v>43494</v>
       </c>
-      <c r="H6" s="12" t="s">
+      <c r="H6" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="I6" s="13">
+      <c r="I6" s="10">
         <f>SUMIF(B:B,"Ispezione codice",C:C)</f>
         <v>756</v>
       </c>
-      <c r="J6" s="14">
+      <c r="J6" s="11">
         <f>I6/I12</f>
-        <v>6.3518736346832472E-2</v>
+        <v>6.3226561846617041E-2</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" s="8">
+      <c r="A7" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="5">
         <v>53</v>
       </c>
-      <c r="D7" s="9">
+      <c r="D7" s="6">
         <v>43494</v>
       </c>
-      <c r="H7" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="I7" s="13">
+      <c r="H7" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="I7" s="10">
         <f>SUMIF(B:B,"Documenti di progetto",C:C)</f>
-        <v>2822</v>
-      </c>
-      <c r="J7" s="14">
+        <v>2877</v>
+      </c>
+      <c r="J7" s="11">
         <f>(I7/I12)</f>
-        <v>0.23710300789783229</v>
+        <v>0.24061219369407041</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" s="8">
+      <c r="A8" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="5">
         <v>87</v>
       </c>
-      <c r="D8" s="9">
+      <c r="D8" s="6">
         <v>43495</v>
       </c>
-      <c r="H8" s="12" t="s">
+      <c r="H8" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="I8" s="13">
+      <c r="I8" s="10">
         <f>SUMIF(B:B,"Documenti di processo",C:C)</f>
         <v>2336</v>
       </c>
-      <c r="J8" s="14">
+      <c r="J8" s="11">
         <f>I8/I12</f>
-        <v>0.19626953453201143</v>
+        <v>0.19536673078531405</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" s="8" t="s">
+      <c r="A9" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="8">
+      <c r="C9" s="5">
         <v>74</v>
       </c>
-      <c r="D9" s="9">
+      <c r="D9" s="6">
         <v>43495</v>
       </c>
-      <c r="H9" s="12" t="s">
+      <c r="H9" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="I9" s="13">
+      <c r="I9" s="10">
         <f>SUMIF(B:B,"Manuale",C:C)</f>
         <v>174</v>
       </c>
-      <c r="J9" s="14">
+      <c r="J9" s="11">
         <f>I9/I12</f>
-        <v>1.4619391698874138E-2</v>
+        <v>1.4552145186919796E-2</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B10" s="8" t="s">
+      <c r="A10" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="8">
+      <c r="C10" s="5">
         <v>32</v>
       </c>
-      <c r="D10" s="9">
+      <c r="D10" s="6">
         <v>43499</v>
       </c>
-      <c r="H10" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="I10" s="13">
+      <c r="H10" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="I10" s="10">
         <f>SUMIF(B:B,"Sviluppo",C:C)</f>
         <v>5724</v>
       </c>
-      <c r="J10" s="14">
+      <c r="J10" s="11">
         <f>I10/I12</f>
-        <v>0.48092757519744583</v>
+        <v>0.47871539683867192</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B11" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C11" s="8">
+      <c r="A11" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="5">
         <v>75</v>
       </c>
-      <c r="D11" s="9">
+      <c r="D11" s="6">
         <v>43497</v>
       </c>
-      <c r="H11" s="15" t="s">
+      <c r="H11" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="I11" s="16">
+      <c r="I11" s="13">
         <f>SUMIF(B:B,"Testing",C:C)</f>
         <v>90</v>
       </c>
-      <c r="J11" s="17">
+      <c r="J11" s="14">
         <f>I11/I12</f>
-        <v>7.5617543270038645E-3</v>
+        <v>7.5269716484067913E-3</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B12" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C12" s="8">
+      <c r="A12" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" s="5">
         <v>55</v>
       </c>
-      <c r="D12" s="9">
+      <c r="D12" s="6">
         <v>43503</v>
       </c>
-      <c r="H12" s="18" t="s">
+      <c r="H12" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="I12" s="19">
+      <c r="I12" s="16">
         <f>SUM(I6:I11)</f>
-        <v>11902</v>
-      </c>
-      <c r="J12" s="20">
+        <v>11957</v>
+      </c>
+      <c r="J12" s="17">
         <f>SUM(J6:J11)</f>
         <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A13" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B13" s="8" t="s">
+      <c r="A13" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="8">
+      <c r="C13" s="5">
         <v>127</v>
       </c>
-      <c r="D13" s="9">
+      <c r="D13" s="6">
         <v>43505</v>
       </c>
-      <c r="H13" s="5"/>
+      <c r="H13" s="2"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A14" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B14" s="8" t="s">
+      <c r="A14" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="8">
+      <c r="C14" s="5">
         <v>24</v>
       </c>
-      <c r="D14" s="9">
+      <c r="D14" s="6">
         <v>43509</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A15" s="8" t="s">
+      <c r="A15" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B15" s="8" t="s">
+      <c r="B15" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="8">
+      <c r="C15" s="5">
         <v>195</v>
       </c>
-      <c r="D15" s="9">
+      <c r="D15" s="6">
         <v>43521</v>
       </c>
-      <c r="H15" s="2" t="s">
+      <c r="H15" s="43" t="s">
         <v>20</v>
       </c>
-      <c r="I15" s="2"/>
-      <c r="J15" s="2"/>
-      <c r="K15" s="2"/>
-      <c r="L15" s="2"/>
-      <c r="M15" s="2"/>
-      <c r="N15" s="2"/>
-      <c r="O15" s="2"/>
+      <c r="I15" s="43"/>
+      <c r="J15" s="43"/>
+      <c r="K15" s="43"/>
+      <c r="L15" s="43"/>
+      <c r="M15" s="43"/>
+      <c r="N15" s="43"/>
+      <c r="O15" s="43"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A16" s="8" t="s">
+      <c r="A16" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="8" t="s">
+      <c r="B16" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C16" s="8">
+      <c r="C16" s="5">
         <v>105</v>
       </c>
-      <c r="D16" s="9">
+      <c r="D16" s="6">
         <v>43523</v>
       </c>
-      <c r="H16" s="21" t="s">
+      <c r="H16" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="I16" s="22" t="s">
+      <c r="I16" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="J16" s="22" t="s">
+      <c r="J16" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="K16" s="22" t="s">
+      <c r="K16" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="L16" s="22" t="s">
-        <v>15</v>
-      </c>
-      <c r="M16" s="22" t="s">
+      <c r="L16" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="M16" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="N16" s="22" t="s">
+      <c r="N16" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="O16" s="23" t="s">
+      <c r="O16" s="20" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A17" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B17" s="8" t="s">
+      <c r="A17" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B17" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C17" s="8">
+      <c r="C17" s="5">
         <v>30</v>
       </c>
-      <c r="D17" s="9">
+      <c r="D17" s="6">
         <v>43519</v>
       </c>
-      <c r="H17" s="24" t="s">
-        <v>6</v>
-      </c>
-      <c r="I17" s="25">
+      <c r="H17" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="I17" s="22">
         <f>SUMIFS(C:C,B:B,"Documenti di progetto",A:A,"Giovanni")</f>
         <v>1041</v>
       </c>
-      <c r="J17" s="25">
+      <c r="J17" s="22">
         <f>SUMIFS(C:C,B:B,"Documenti di processo",A:A,"Giovanni")</f>
         <v>1112</v>
       </c>
-      <c r="K17" s="25">
+      <c r="K17" s="22">
         <f>SUMIFS(C:C,B:B,"Manuale",A:A,"Giovanni")</f>
         <v>174</v>
       </c>
-      <c r="L17" s="25">
+      <c r="L17" s="22">
         <f>SUMIFS(C:C,B:B,"Sviluppo",A:A,"Giovanni")</f>
         <v>0</v>
       </c>
-      <c r="M17" s="25">
+      <c r="M17" s="22">
         <f>SUMIFS(C:C,B:B,"Testing",A:A,"Giovanni")</f>
         <v>0</v>
       </c>
-      <c r="N17" s="25">
+      <c r="N17" s="22">
         <f>SUMIFS(C:C,B:B,"Ispezione codice",A:A,"Giovanni")</f>
         <v>189</v>
       </c>
-      <c r="O17" s="26">
+      <c r="O17" s="23">
         <f>SUM(I17:N17)</f>
         <v>2516</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A18" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B18" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C18" s="8">
+      <c r="A18" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18" s="5">
         <v>100</v>
       </c>
-      <c r="D18" s="9">
+      <c r="D18" s="6">
         <v>43520</v>
       </c>
-      <c r="H18" s="24" t="s">
-        <v>25</v>
-      </c>
-      <c r="I18" s="25">
+      <c r="H18" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="I18" s="22">
         <f>SUMIFS(C:C,B:B,"Documenti di progetto",A:A,"Hristina")</f>
         <v>190</v>
       </c>
-      <c r="J18" s="25">
+      <c r="J18" s="22">
         <f>SUMIFS(C:C,B:B,"Documenti di processo",A:A,"Hristina")</f>
         <v>282</v>
       </c>
-      <c r="K18" s="25">
+      <c r="K18" s="22">
         <f>SUMIFS(C:C,B:B,"Manuale",A:A,"Hristina")</f>
         <v>0</v>
       </c>
-      <c r="L18" s="25">
+      <c r="L18" s="22">
         <f>SUMIFS(C:C,B:B,"Sviluppo",A:A,"Hristina")</f>
         <v>2962</v>
       </c>
-      <c r="M18" s="25">
+      <c r="M18" s="22">
         <f>SUMIFS(C:C,B:B,"Testing",A:A,"Hristina")</f>
         <v>0</v>
       </c>
-      <c r="N18" s="25">
+      <c r="N18" s="22">
         <f>SUMIFS(C:C,B:B,"Ispezione codice",A:A,"Hristina")</f>
         <v>189</v>
       </c>
-      <c r="O18" s="26">
+      <c r="O18" s="23">
         <f>SUM(I18:N18)</f>
         <v>3623</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A19" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B19" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C19" s="8">
+      <c r="A19" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C19" s="5">
         <v>125</v>
       </c>
-      <c r="D19" s="9">
+      <c r="D19" s="6">
         <v>43522</v>
       </c>
-      <c r="H19" s="24" t="s">
+      <c r="H19" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="I19" s="25">
+      <c r="I19" s="22">
         <f>SUMIFS(C:C,B:B,"Documenti di progetto",A:A,"Luca")</f>
-        <v>952</v>
-      </c>
-      <c r="J19" s="25">
+        <v>1007</v>
+      </c>
+      <c r="J19" s="22">
         <f>SUMIFS(C:C,B:B,"Documenti di processo",A:A,"Luca")</f>
         <v>852</v>
       </c>
-      <c r="K19" s="25">
+      <c r="K19" s="22">
         <f>SUMIFS(C:C,B:B,"Manuale",A:A,"Luca")</f>
         <v>0</v>
       </c>
-      <c r="L19" s="25">
+      <c r="L19" s="22">
         <f>SUMIFS(C:C,B:B,"Sviluppo",A:A,"Luca")</f>
         <v>60</v>
       </c>
-      <c r="M19" s="25">
+      <c r="M19" s="22">
         <f>SUMIFS(C:C,B:B,"Testing",A:A,"Luca")</f>
         <v>90</v>
       </c>
-      <c r="N19" s="25">
+      <c r="N19" s="22">
         <f>SUMIFS(C:C,B:B,"Ispezione codice",A:A,"Luca")</f>
         <v>189</v>
       </c>
-      <c r="O19" s="26">
+      <c r="O19" s="23">
         <f>SUM(I19:N19)</f>
-        <v>2143</v>
+        <v>2198</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A20" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B20" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C20" s="8">
+      <c r="A20" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C20" s="5">
         <v>170</v>
       </c>
-      <c r="D20" s="9">
+      <c r="D20" s="6">
         <v>43523</v>
       </c>
-      <c r="H20" s="24" t="s">
-        <v>16</v>
-      </c>
-      <c r="I20" s="25">
+      <c r="H20" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="I20" s="22">
         <f>SUMIFS(C:C,B:B,"Documenti di progetto",A:A,"Viktorija")</f>
         <v>639</v>
       </c>
-      <c r="J20" s="25">
+      <c r="J20" s="22">
         <f>SUMIFS(C:C,B:B,"Documenti di processo",A:A,"Viktorija")</f>
         <v>90</v>
       </c>
-      <c r="K20" s="25">
+      <c r="K20" s="22">
         <f>SUMIFS(C:C,B:B,"Manuale",A:A,"Viktorija")</f>
         <v>0</v>
       </c>
-      <c r="L20" s="25">
+      <c r="L20" s="22">
         <f>SUMIFS(C:C,B:B,"Sviluppo",A:A,"Viktorija")</f>
         <v>2702</v>
       </c>
-      <c r="M20" s="25">
+      <c r="M20" s="22">
         <f>SUMIFS(C:C,B:B,"Testing",A:A,"Viktorija")</f>
         <v>0</v>
       </c>
-      <c r="N20" s="25">
+      <c r="N20" s="22">
         <f>SUMIFS(C:C,B:B,"Ispezione codice",A:A,"Viktorija")</f>
         <v>189</v>
       </c>
-      <c r="O20" s="26">
+      <c r="O20" s="23">
         <f>SUM(I20:N20)</f>
         <v>3620</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A21" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B21" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C21" s="8">
+      <c r="A21" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C21" s="5">
         <v>65</v>
       </c>
-      <c r="D21" s="9">
+      <c r="D21" s="6">
         <v>43524</v>
       </c>
-      <c r="H21" s="27" t="s">
+      <c r="H21" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="I21" s="28">
+      <c r="I21" s="25">
         <f t="shared" ref="I21:N21" si="0">AVERAGE(I17:I20)</f>
-        <v>705.5</v>
-      </c>
-      <c r="J21" s="29">
+        <v>719.25</v>
+      </c>
+      <c r="J21" s="26">
         <f t="shared" si="0"/>
         <v>584</v>
       </c>
-      <c r="K21" s="29">
+      <c r="K21" s="26">
         <f t="shared" si="0"/>
         <v>43.5</v>
       </c>
-      <c r="L21" s="29">
+      <c r="L21" s="26">
         <f t="shared" si="0"/>
         <v>1431</v>
       </c>
-      <c r="M21" s="29">
+      <c r="M21" s="26">
         <f t="shared" si="0"/>
         <v>22.5</v>
       </c>
-      <c r="N21" s="30">
+      <c r="N21" s="27">
         <f t="shared" si="0"/>
         <v>189</v>
       </c>
-      <c r="O21" s="31">
+      <c r="O21" s="28">
         <f>SUM(O17:O20)</f>
-        <v>11902</v>
+        <v>11957</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A22" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B22" s="8" t="s">
+      <c r="A22" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B22" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C22" s="8">
+      <c r="C22" s="5">
         <v>60</v>
       </c>
-      <c r="D22" s="9">
+      <c r="D22" s="6">
         <v>43487</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A23" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B23" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C23" s="8">
+      <c r="A23" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C23" s="5">
         <v>103</v>
       </c>
-      <c r="D23" s="9">
+      <c r="D23" s="6">
         <v>43506</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A24" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B24" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C24" s="8">
+      <c r="A24" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C24" s="5">
         <v>100</v>
       </c>
-      <c r="D24" s="9">
+      <c r="D24" s="6">
         <v>43520</v>
       </c>
-      <c r="H24" s="1" t="s">
+      <c r="H24" s="44" t="s">
         <v>28</v>
       </c>
-      <c r="I24" s="1"/>
-      <c r="J24" s="1"/>
-      <c r="K24" s="1"/>
-      <c r="L24" s="1"/>
-      <c r="M24" s="1"/>
-      <c r="N24" s="1"/>
-      <c r="O24" s="1"/>
+      <c r="I24" s="44"/>
+      <c r="J24" s="44"/>
+      <c r="K24" s="44"/>
+      <c r="L24" s="44"/>
+      <c r="M24" s="44"/>
+      <c r="N24" s="44"/>
+      <c r="O24" s="44"/>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A25" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B25" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C25" s="8">
+      <c r="A25" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C25" s="5">
         <v>170</v>
       </c>
-      <c r="D25" s="9">
+      <c r="D25" s="6">
         <v>43523</v>
       </c>
-      <c r="H25" s="32" t="s">
+      <c r="H25" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="I25" s="33" t="s">
+      <c r="I25" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="J25" s="33" t="s">
+      <c r="J25" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="K25" s="33" t="s">
+      <c r="K25" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="L25" s="33" t="s">
-        <v>15</v>
-      </c>
-      <c r="M25" s="33" t="s">
+      <c r="L25" s="30" t="s">
+        <v>15</v>
+      </c>
+      <c r="M25" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="N25" s="33" t="s">
+      <c r="N25" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="O25" s="34" t="s">
+      <c r="O25" s="31" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A26" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B26" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C26" s="8">
+      <c r="A26" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C26" s="5">
         <v>45</v>
       </c>
-      <c r="D26" s="9">
+      <c r="D26" s="6">
         <v>43524</v>
       </c>
-      <c r="H26" s="35" t="s">
-        <v>6</v>
-      </c>
-      <c r="I26" s="36">
+      <c r="H26" s="32" t="s">
+        <v>6</v>
+      </c>
+      <c r="I26" s="33">
         <f>I17/O17</f>
         <v>0.41375198728139906</v>
       </c>
-      <c r="J26" s="36">
+      <c r="J26" s="33">
         <f>J17/O17</f>
         <v>0.44197138314785372</v>
       </c>
-      <c r="K26" s="36">
+      <c r="K26" s="33">
         <f>K17/O17</f>
         <v>6.9157392686804445E-2</v>
       </c>
-      <c r="L26" s="36">
+      <c r="L26" s="33">
         <f>L17/O17</f>
         <v>0</v>
       </c>
-      <c r="M26" s="36">
+      <c r="M26" s="33">
         <f>M17/O17</f>
         <v>0</v>
       </c>
-      <c r="N26" s="36">
+      <c r="N26" s="33">
         <f>N17/O17</f>
         <v>7.5119236883942772E-2</v>
       </c>
-      <c r="O26" s="37">
+      <c r="O26" s="34">
         <f>SUM(I26:N26)</f>
         <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A27" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B27" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C27" s="8">
-        <v>25</v>
-      </c>
-      <c r="D27" s="9">
+      <c r="A27" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C27" s="5">
+        <v>25</v>
+      </c>
+      <c r="D27" s="6">
         <v>43530</v>
       </c>
-      <c r="H27" s="35" t="s">
-        <v>25</v>
-      </c>
-      <c r="I27" s="36">
+      <c r="H27" s="32" t="s">
+        <v>25</v>
+      </c>
+      <c r="I27" s="33">
         <f>I18/O18</f>
         <v>5.2442727021805136E-2</v>
       </c>
-      <c r="J27" s="36">
+      <c r="J27" s="33">
         <f>J18/O18</f>
         <v>7.7836047474468678E-2</v>
       </c>
-      <c r="K27" s="36">
+      <c r="K27" s="33">
         <f>K18/O18</f>
         <v>0</v>
       </c>
-      <c r="L27" s="36">
+      <c r="L27" s="33">
         <f>L18/O18</f>
         <v>0.8175545128346674</v>
       </c>
-      <c r="M27" s="36">
+      <c r="M27" s="33">
         <f>M18/O18</f>
         <v>0</v>
       </c>
-      <c r="N27" s="36">
+      <c r="N27" s="33">
         <f>N18/O18</f>
         <v>5.2166712669058792E-2</v>
       </c>
-      <c r="O27" s="37">
+      <c r="O27" s="34">
         <f>SUM(I27:N27)</f>
         <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A28" s="8" t="s">
+      <c r="A28" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B28" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C28" s="8">
-        <v>15</v>
-      </c>
-      <c r="D28" s="9">
+      <c r="B28" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C28" s="5">
+        <v>15</v>
+      </c>
+      <c r="D28" s="6">
         <v>43532</v>
       </c>
-      <c r="H28" s="35" t="s">
+      <c r="H28" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="I28" s="36">
+      <c r="I28" s="33">
         <f>I19/O19</f>
-        <v>0.44423705086327581</v>
-      </c>
-      <c r="J28" s="36">
+        <v>0.45814376706096449</v>
+      </c>
+      <c r="J28" s="33">
         <f>J19/O19</f>
-        <v>0.39757349510032663</v>
-      </c>
-      <c r="K28" s="36">
+        <v>0.38762511373976344</v>
+      </c>
+      <c r="K28" s="33">
         <f>K19/O19</f>
         <v>0</v>
       </c>
-      <c r="L28" s="36">
+      <c r="L28" s="33">
         <f>L19/O19</f>
-        <v>2.7998133457769483E-2</v>
-      </c>
-      <c r="M28" s="36">
+        <v>2.7297543221110099E-2</v>
+      </c>
+      <c r="M28" s="33">
         <f>M19/O19</f>
-        <v>4.1997200186654225E-2</v>
-      </c>
-      <c r="N28" s="36">
+        <v>4.0946314831665151E-2</v>
+      </c>
+      <c r="N28" s="33">
         <f>N19/O19</f>
-        <v>8.8194120391973871E-2</v>
-      </c>
-      <c r="O28" s="37">
+        <v>8.598726114649681E-2</v>
+      </c>
+      <c r="O28" s="34">
         <f>SUM(I28:N28)</f>
         <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A29" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B29" s="8" t="s">
+      <c r="A29" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B29" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C29" s="8">
+      <c r="C29" s="5">
         <v>47</v>
       </c>
-      <c r="D29" s="9">
+      <c r="D29" s="6">
         <v>43532</v>
       </c>
-      <c r="H29" s="35" t="s">
-        <v>16</v>
-      </c>
-      <c r="I29" s="36">
+      <c r="H29" s="32" t="s">
+        <v>16</v>
+      </c>
+      <c r="I29" s="33">
         <f>I20/O20</f>
         <v>0.17651933701657457</v>
       </c>
-      <c r="J29" s="36">
+      <c r="J29" s="33">
         <f>J20/O20</f>
         <v>2.4861878453038673E-2</v>
       </c>
-      <c r="K29" s="36">
+      <c r="K29" s="33">
         <f>K20/O20</f>
         <v>0</v>
       </c>
-      <c r="L29" s="36">
+      <c r="L29" s="33">
         <f>L20/O20</f>
         <v>0.74640883977900552</v>
       </c>
-      <c r="M29" s="36">
+      <c r="M29" s="33">
         <f>M20/O20</f>
         <v>0</v>
       </c>
-      <c r="N29" s="36">
+      <c r="N29" s="33">
         <f>N20/O20</f>
         <v>5.2209944751381215E-2</v>
       </c>
-      <c r="O29" s="38">
+      <c r="O29" s="35">
         <f>SUM(I29:N29)</f>
         <v>0.99999999999999989</v>
       </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A30" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B30" s="8" t="s">
+      <c r="A30" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B30" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C30" s="8">
-        <v>15</v>
-      </c>
-      <c r="D30" s="9">
+      <c r="C30" s="5">
+        <v>15</v>
+      </c>
+      <c r="D30" s="6">
         <v>43532</v>
       </c>
-      <c r="H30" s="39" t="s">
+      <c r="H30" s="36" t="s">
         <v>27</v>
       </c>
-      <c r="I30" s="40">
+      <c r="I30" s="37">
         <f t="shared" ref="I30:N30" si="1">AVERAGE(I26:I29)</f>
-        <v>0.27173777554576362</v>
-      </c>
-      <c r="J30" s="40">
+        <v>0.27521445459518579</v>
+      </c>
+      <c r="J30" s="37">
         <f t="shared" si="1"/>
-        <v>0.23556070104392193</v>
-      </c>
-      <c r="K30" s="40">
+        <v>0.23307360570378113</v>
+      </c>
+      <c r="K30" s="37">
         <f t="shared" si="1"/>
         <v>1.7289348171701111E-2</v>
       </c>
-      <c r="L30" s="40">
+      <c r="L30" s="37">
         <f t="shared" si="1"/>
-        <v>0.3979903715178606</v>
-      </c>
-      <c r="M30" s="40">
+        <v>0.39781522395869573</v>
+      </c>
+      <c r="M30" s="37">
         <f t="shared" si="1"/>
-        <v>1.0499300046663556E-2</v>
-      </c>
-      <c r="N30" s="41">
+        <v>1.0236578707916288E-2</v>
+      </c>
+      <c r="N30" s="38">
         <f t="shared" si="1"/>
-        <v>6.6922503674089168E-2</v>
-      </c>
-      <c r="O30" s="42">
+        <v>6.6370788862719909E-2</v>
+      </c>
+      <c r="O30" s="39">
         <f>SUM(I30:N30)</f>
-        <v>0.99999999999999989</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A31" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B31" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C31" s="8">
+      <c r="A31" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C31" s="5">
         <v>55</v>
       </c>
-      <c r="D31" s="9">
+      <c r="D31" s="6">
         <v>43531</v>
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A32" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B32" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C32" s="8">
+      <c r="A32" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C32" s="5">
         <v>68</v>
       </c>
-      <c r="D32" s="9">
+      <c r="D32" s="6">
         <v>43532</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B33" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C33" s="8">
+      <c r="A33" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C33" s="5">
         <v>129</v>
       </c>
-      <c r="D33" s="9">
+      <c r="D33" s="6">
         <v>43533</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B34" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C34" s="8">
+      <c r="A34" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C34" s="5">
         <v>95</v>
       </c>
-      <c r="D34" s="9">
+      <c r="D34" s="6">
         <v>43534</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B35" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C35" s="8">
+      <c r="A35" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C35" s="5">
         <v>74</v>
       </c>
-      <c r="D35" s="9">
+      <c r="D35" s="6">
         <v>43546</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B36" s="8" t="s">
+      <c r="A36" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B36" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C36" s="8">
+      <c r="C36" s="5">
         <v>52</v>
       </c>
-      <c r="D36" s="9">
+      <c r="D36" s="6">
         <v>43546</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B37" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C37" s="8">
+      <c r="A37" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C37" s="5">
         <v>196</v>
       </c>
-      <c r="D37" s="9">
+      <c r="D37" s="6">
         <v>43376</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B38" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C38" s="8">
+      <c r="A38" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C38" s="5">
         <v>115</v>
       </c>
-      <c r="D38" s="9">
+      <c r="D38" s="6">
         <v>43407</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B39" s="8" t="s">
+      <c r="A39" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B39" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C39" s="8">
+      <c r="C39" s="5">
         <v>10</v>
       </c>
-      <c r="D39" s="9">
+      <c r="D39" s="6">
         <v>43546</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="8" t="s">
+      <c r="A40" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B40" s="8" t="s">
+      <c r="B40" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C40" s="8">
+      <c r="C40" s="5">
         <v>60</v>
       </c>
-      <c r="D40" s="9">
+      <c r="D40" s="6">
         <v>43553</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B41" s="8" t="s">
+      <c r="A41" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B41" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C41" s="8">
+      <c r="C41" s="5">
         <v>60</v>
       </c>
-      <c r="D41" s="9">
+      <c r="D41" s="6">
         <v>43553</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B42" s="8" t="s">
+      <c r="A42" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B42" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C42" s="8">
+      <c r="C42" s="5">
         <v>60</v>
       </c>
-      <c r="D42" s="9">
+      <c r="D42" s="6">
         <v>43553</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="8" t="s">
+      <c r="A43" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B43" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C43" s="8">
+      <c r="B43" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C43" s="5">
         <v>60</v>
       </c>
-      <c r="D43" s="9">
+      <c r="D43" s="6">
         <v>43481</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="8" t="s">
+      <c r="A44" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B44" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C44" s="8">
+      <c r="B44" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C44" s="5">
         <v>150</v>
       </c>
-      <c r="D44" s="9">
+      <c r="D44" s="6">
         <v>43442</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="8" t="s">
+      <c r="A45" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B45" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C45" s="8">
+      <c r="B45" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C45" s="5">
         <v>180</v>
       </c>
-      <c r="D45" s="9">
+      <c r="D45" s="6">
         <v>43448</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="8" t="s">
+      <c r="A46" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B46" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C46" s="8">
+      <c r="B46" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C46" s="5">
         <v>180</v>
       </c>
-      <c r="D46" s="9">
+      <c r="D46" s="6">
         <v>43468</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="8" t="s">
+      <c r="A47" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B47" s="8" t="s">
+      <c r="B47" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C47" s="8">
+      <c r="C47" s="5">
         <v>120</v>
       </c>
-      <c r="D47" s="9">
+      <c r="D47" s="6">
         <v>43478</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B48" s="8" t="s">
+      <c r="A48" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B48" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C48" s="8">
+      <c r="C48" s="5">
         <v>300</v>
       </c>
-      <c r="D48" s="9">
+      <c r="D48" s="6">
         <v>43449</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B49" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C49" s="8">
+      <c r="A49" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B49" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C49" s="5">
         <v>150</v>
       </c>
-      <c r="D49" s="9">
+      <c r="D49" s="6">
         <v>43450</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="8" t="s">
+      <c r="A50" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B50" s="8" t="s">
+      <c r="B50" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C50" s="8">
+      <c r="C50" s="5">
         <v>82</v>
       </c>
-      <c r="D50" s="9">
+      <c r="D50" s="6">
         <v>43558</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B51" s="8" t="s">
+      <c r="A51" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B51" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C51" s="8">
+      <c r="C51" s="5">
         <v>82</v>
       </c>
-      <c r="D51" s="9">
+      <c r="D51" s="6">
         <v>43558</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B52" s="8" t="s">
+      <c r="A52" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B52" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C52" s="8">
+      <c r="C52" s="5">
         <v>82</v>
       </c>
-      <c r="D52" s="9">
+      <c r="D52" s="6">
         <v>43558</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B53" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C53" s="8">
+      <c r="A53" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B53" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C53" s="5">
         <v>85</v>
       </c>
-      <c r="D53" s="9">
+      <c r="D53" s="6">
         <v>43559</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="8" t="s">
+      <c r="A54" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B54" s="8" t="s">
+      <c r="B54" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C54" s="8">
+      <c r="C54" s="5">
         <v>70</v>
       </c>
-      <c r="D54" s="9">
+      <c r="D54" s="6">
         <v>43571</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B55" s="8" t="s">
+      <c r="A55" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B55" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C55" s="8">
+      <c r="C55" s="5">
         <v>70</v>
       </c>
-      <c r="D55" s="9">
+      <c r="D55" s="6">
         <v>43571</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="8" t="s">
+      <c r="A56" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B56" s="8" t="s">
+      <c r="B56" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C56" s="8">
+      <c r="C56" s="5">
         <v>120</v>
       </c>
-      <c r="D56" s="9">
+      <c r="D56" s="6">
         <v>43572</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="8" t="s">
+      <c r="A57" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B57" s="8" t="s">
+      <c r="B57" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C57" s="8">
+      <c r="C57" s="5">
         <v>100</v>
       </c>
-      <c r="D57" s="9">
+      <c r="D57" s="6">
         <v>43574</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B58" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C58" s="8">
+      <c r="A58" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B58" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C58" s="5">
         <v>42</v>
       </c>
-      <c r="D58" s="9">
+      <c r="D58" s="6">
         <v>43577</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B59" s="8" t="s">
+      <c r="A59" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B59" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C59" s="8">
+      <c r="C59" s="5">
         <v>97</v>
       </c>
-      <c r="D59" s="9">
+      <c r="D59" s="6">
         <v>43578</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B60" s="8" t="s">
+      <c r="A60" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B60" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C60" s="8">
+      <c r="C60" s="5">
         <v>30</v>
       </c>
-      <c r="D60" s="9">
+      <c r="D60" s="6">
         <v>43578</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B61" s="8" t="s">
+      <c r="A61" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B61" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C61" s="8">
+      <c r="C61" s="5">
         <v>107</v>
       </c>
-      <c r="D61" s="9">
+      <c r="D61" s="6">
         <v>43581</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B62" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C62" s="8">
+      <c r="A62" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B62" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C62" s="5">
         <v>39</v>
       </c>
-      <c r="D62" s="9">
+      <c r="D62" s="6">
         <v>43584</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B63" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C63" s="8">
+      <c r="A63" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B63" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C63" s="5">
         <v>22</v>
       </c>
-      <c r="D63" s="9">
+      <c r="D63" s="6">
         <v>43585</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" s="8" t="s">
+      <c r="A64" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B64" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C64" s="8">
+      <c r="B64" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C64" s="5">
         <v>22</v>
       </c>
-      <c r="D64" s="9">
+      <c r="D64" s="6">
         <v>43585</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" s="8" t="s">
+      <c r="A65" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B65" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C65" s="8">
-        <v>25</v>
-      </c>
-      <c r="D65" s="9">
+      <c r="B65" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C65" s="5">
+        <v>25</v>
+      </c>
+      <c r="D65" s="6">
         <v>43587</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B66" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C66" s="8">
-        <v>25</v>
-      </c>
-      <c r="D66" s="9">
+      <c r="A66" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B66" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C66" s="5">
+        <v>25</v>
+      </c>
+      <c r="D66" s="6">
         <v>43587</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B67" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C67" s="8">
+      <c r="A67" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B67" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C67" s="5">
         <v>136</v>
       </c>
-      <c r="D67" s="9">
+      <c r="D67" s="6">
         <v>43587</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B68" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C68" s="8">
+      <c r="A68" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B68" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C68" s="5">
         <v>35</v>
       </c>
-      <c r="D68" s="9">
+      <c r="D68" s="6">
         <v>43587</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B69" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C69" s="8">
+      <c r="A69" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B69" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C69" s="5">
         <v>135</v>
       </c>
-      <c r="D69" s="9">
+      <c r="D69" s="6">
         <v>43588</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A70" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B70" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C70" s="8">
+      <c r="A70" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B70" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C70" s="5">
         <v>135</v>
       </c>
-      <c r="D70" s="9">
+      <c r="D70" s="6">
         <v>43588</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B71" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C71" s="8">
+      <c r="A71" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B71" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C71" s="5">
         <v>40</v>
       </c>
-      <c r="D71" s="9">
+      <c r="D71" s="6">
         <v>43589</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B72" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C72" s="8">
+      <c r="A72" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B72" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C72" s="5">
         <v>40</v>
       </c>
-      <c r="D72" s="9">
+      <c r="D72" s="6">
         <v>43589</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B73" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C73" s="8">
+      <c r="A73" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B73" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C73" s="5">
         <v>78</v>
       </c>
-      <c r="D73" s="9">
+      <c r="D73" s="6">
         <v>43590</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A74" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B74" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C74" s="8">
+      <c r="A74" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B74" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C74" s="5">
         <v>78</v>
       </c>
-      <c r="D74" s="9">
+      <c r="D74" s="6">
         <v>43590</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B75" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C75" s="8">
+      <c r="A75" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B75" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C75" s="5">
         <v>45</v>
       </c>
-      <c r="D75" s="9">
+      <c r="D75" s="6">
         <v>43593</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B76" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C76" s="8">
+      <c r="A76" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B76" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C76" s="5">
         <v>45</v>
       </c>
-      <c r="D76" s="9">
+      <c r="D76" s="6">
         <v>43593</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" s="8" t="s">
+      <c r="A77" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B77" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C77" s="8">
+      <c r="B77" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C77" s="5">
         <v>45</v>
       </c>
-      <c r="D77" s="9">
+      <c r="D77" s="6">
         <v>43593</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B78" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C78" s="8">
+      <c r="A78" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B78" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C78" s="5">
         <v>45</v>
       </c>
-      <c r="D78" s="9">
+      <c r="D78" s="6">
         <v>43593</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B79" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C79" s="8">
+      <c r="A79" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B79" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C79" s="5">
         <v>60</v>
       </c>
-      <c r="D79" s="9">
+      <c r="D79" s="6">
         <v>43593</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" s="8" t="s">
+      <c r="A80" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B80" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C80" s="8">
+      <c r="B80" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C80" s="5">
         <v>60</v>
       </c>
-      <c r="D80" s="9">
+      <c r="D80" s="6">
         <v>43593</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A81" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B81" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C81" s="8">
+      <c r="A81" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B81" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C81" s="5">
         <v>60</v>
       </c>
-      <c r="D81" s="9">
+      <c r="D81" s="6">
         <v>43593</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A82" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B82" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C82" s="8">
+      <c r="A82" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B82" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C82" s="5">
         <v>116</v>
       </c>
-      <c r="D82" s="9">
+      <c r="D82" s="6">
         <v>43594</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A83" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B83" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C83" s="8">
+      <c r="A83" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B83" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C83" s="5">
         <v>116</v>
       </c>
-      <c r="D83" s="9">
+      <c r="D83" s="6">
         <v>43594</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A84" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B84" s="8" t="s">
+      <c r="A84" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B84" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C84" s="8">
+      <c r="C84" s="5">
         <v>47</v>
       </c>
-      <c r="D84" s="9">
+      <c r="D84" s="6">
         <v>43598</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A85" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B85" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C85" s="8">
+      <c r="A85" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B85" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C85" s="5">
         <v>31</v>
       </c>
-      <c r="D85" s="9">
+      <c r="D85" s="6">
         <v>43598</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A86" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B86" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C86" s="8">
+      <c r="A86" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B86" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C86" s="5">
         <v>160</v>
       </c>
-      <c r="D86" s="9">
+      <c r="D86" s="6">
         <v>43595</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A87" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B87" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C87" s="8">
+      <c r="A87" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B87" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C87" s="5">
         <v>160</v>
       </c>
-      <c r="D87" s="9">
+      <c r="D87" s="6">
         <v>43595</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A88" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B88" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C88" s="8">
+      <c r="A88" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B88" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C88" s="5">
         <v>240</v>
       </c>
-      <c r="D88" s="9">
+      <c r="D88" s="6">
         <v>43599</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A89" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B89" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C89" s="8">
+      <c r="A89" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B89" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C89" s="5">
         <v>240</v>
       </c>
-      <c r="D89" s="9">
+      <c r="D89" s="6">
         <v>43599</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A90" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B90" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C90" s="8">
+      <c r="A90" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B90" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C90" s="5">
         <v>40</v>
       </c>
-      <c r="D90" s="9">
+      <c r="D90" s="6">
         <v>43600</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A91" s="8" t="s">
+      <c r="A91" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B91" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C91" s="8">
+      <c r="B91" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C91" s="5">
         <v>40</v>
       </c>
-      <c r="D91" s="9">
+      <c r="D91" s="6">
         <v>43600</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A92" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B92" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C92" s="8">
+      <c r="A92" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B92" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C92" s="5">
         <v>40</v>
       </c>
-      <c r="D92" s="9">
+      <c r="D92" s="6">
         <v>43600</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A93" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B93" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C93" s="8">
+      <c r="A93" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B93" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C93" s="5">
         <v>40</v>
       </c>
-      <c r="D93" s="9">
+      <c r="D93" s="6">
         <v>43600</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A94" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B94" s="8" t="s">
+      <c r="A94" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B94" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C94" s="8">
+      <c r="C94" s="5">
         <v>20</v>
       </c>
-      <c r="D94" s="9">
+      <c r="D94" s="6">
         <v>43600</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A95" s="8" t="s">
+      <c r="A95" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B95" s="8" t="s">
+      <c r="B95" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C95" s="8">
+      <c r="C95" s="5">
         <v>20</v>
       </c>
-      <c r="D95" s="9">
+      <c r="D95" s="6">
         <v>43600</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A96" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B96" s="8" t="s">
+      <c r="A96" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B96" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C96" s="8">
+      <c r="C96" s="5">
         <v>20</v>
       </c>
-      <c r="D96" s="9">
+      <c r="D96" s="6">
         <v>43600</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A97" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B97" s="8" t="s">
+      <c r="A97" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B97" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C97" s="8">
+      <c r="C97" s="5">
         <v>20</v>
       </c>
-      <c r="D97" s="9">
+      <c r="D97" s="6">
         <v>43600</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A98" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B98" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C98" s="8">
+      <c r="A98" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B98" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C98" s="5">
         <v>210</v>
       </c>
-      <c r="D98" s="9">
+      <c r="D98" s="6">
         <v>43603</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A99" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B99" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C99" s="8">
+      <c r="A99" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B99" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C99" s="5">
         <v>210</v>
       </c>
-      <c r="D99" s="9">
+      <c r="D99" s="6">
         <v>43603</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A100" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B100" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C100" s="8">
+      <c r="A100" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B100" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C100" s="5">
         <v>65</v>
       </c>
-      <c r="D100" s="9">
+      <c r="D100" s="6">
         <v>43604</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A101" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B101" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C101" s="8">
+      <c r="A101" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B101" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C101" s="5">
         <v>65</v>
       </c>
-      <c r="D101" s="9">
+      <c r="D101" s="6">
         <v>43604</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A102" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B102" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C102" s="8">
+      <c r="A102" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B102" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C102" s="5">
         <v>110</v>
       </c>
-      <c r="D102" s="9">
+      <c r="D102" s="6">
         <v>43604</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A103" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B103" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C103" s="8">
+      <c r="A103" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B103" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C103" s="5">
         <v>20</v>
       </c>
-      <c r="D103" s="9">
+      <c r="D103" s="6">
         <v>43605</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A104" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B104" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C104" s="8">
-        <v>15</v>
-      </c>
-      <c r="D104" s="9">
+      <c r="A104" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B104" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C104" s="5">
+        <v>15</v>
+      </c>
+      <c r="D104" s="6">
         <v>43606</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A105" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B105" s="8" t="s">
+      <c r="A105" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B105" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C105" s="8">
+      <c r="C105" s="5">
         <v>30</v>
       </c>
-      <c r="D105" s="9">
+      <c r="D105" s="6">
         <v>43607</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A106" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B106" s="8" t="s">
+      <c r="A106" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B106" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C106" s="8">
+      <c r="C106" s="5">
         <v>30</v>
       </c>
-      <c r="D106" s="9">
+      <c r="D106" s="6">
         <v>43607</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A107" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B107" s="8" t="s">
+      <c r="A107" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B107" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C107" s="8">
+      <c r="C107" s="5">
         <v>30</v>
       </c>
-      <c r="D107" s="9">
+      <c r="D107" s="6">
         <v>43607</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A108" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B108" s="8" t="s">
+      <c r="A108" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B108" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C108" s="8">
+      <c r="C108" s="5">
         <v>30</v>
       </c>
-      <c r="D108" s="9">
+      <c r="D108" s="6">
         <v>43607</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A109" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B109" s="8" t="s">
+      <c r="A109" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B109" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C109" s="8">
+      <c r="C109" s="5">
         <v>30</v>
       </c>
-      <c r="D109" s="9">
+      <c r="D109" s="6">
         <v>43607</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A110" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B110" s="8" t="s">
+      <c r="A110" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B110" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C110" s="8">
+      <c r="C110" s="5">
         <v>30</v>
       </c>
-      <c r="D110" s="9">
+      <c r="D110" s="6">
         <v>43607</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A111" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B111" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C111" s="8">
+      <c r="A111" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B111" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C111" s="5">
         <v>130</v>
       </c>
-      <c r="D111" s="9">
+      <c r="D111" s="6">
         <v>43607</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A112" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B112" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C112" s="8">
+      <c r="A112" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B112" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C112" s="5">
         <v>130</v>
       </c>
-      <c r="D112" s="9">
+      <c r="D112" s="6">
         <v>43607</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A113" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B113" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C113" s="8">
+      <c r="A113" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B113" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C113" s="5">
         <v>20</v>
       </c>
-      <c r="D113" s="9">
+      <c r="D113" s="6">
         <v>43607</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A114" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B114" s="8" t="s">
+      <c r="A114" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B114" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C114" s="8">
+      <c r="C114" s="5">
         <v>68</v>
       </c>
-      <c r="D114" s="9">
+      <c r="D114" s="6">
         <v>43608</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A115" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B115" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C115" s="8">
+      <c r="A115" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B115" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C115" s="5">
         <v>23</v>
       </c>
-      <c r="D115" s="9">
+      <c r="D115" s="6">
         <v>43609</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A116" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B116" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C116" s="8">
+      <c r="A116" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B116" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C116" s="5">
         <v>85</v>
       </c>
-      <c r="D116" s="9">
+      <c r="D116" s="6">
         <v>43608</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A117" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B117" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C117" s="8">
+      <c r="A117" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B117" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C117" s="5">
         <v>85</v>
       </c>
-      <c r="D117" s="9">
+      <c r="D117" s="6">
         <v>43608</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A118" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B118" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C118" s="8">
+      <c r="A118" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B118" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C118" s="5">
         <v>73</v>
       </c>
-      <c r="D118" s="9">
+      <c r="D118" s="6">
         <v>43609</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A119" s="8" t="s">
+      <c r="A119" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B119" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C119" s="8">
+      <c r="B119" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C119" s="5">
         <v>30</v>
       </c>
-      <c r="D119" s="9">
+      <c r="D119" s="6">
         <v>43614</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A120" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B120" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C120" s="8">
+      <c r="A120" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B120" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C120" s="5">
         <v>30</v>
       </c>
-      <c r="D120" s="9">
+      <c r="D120" s="6">
         <v>43614</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A121" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B121" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C121" s="8">
+      <c r="A121" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B121" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C121" s="5">
         <v>30</v>
       </c>
-      <c r="D121" s="9">
+      <c r="D121" s="6">
         <v>43614</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A122" s="8" t="s">
+      <c r="A122" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B122" s="8" t="s">
+      <c r="B122" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C122" s="8">
+      <c r="C122" s="5">
         <v>84</v>
       </c>
-      <c r="D122" s="9">
+      <c r="D122" s="6">
         <v>43614</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A123" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B123" s="8" t="s">
+      <c r="A123" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B123" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C123" s="8">
+      <c r="C123" s="5">
         <v>84</v>
       </c>
-      <c r="D123" s="9">
+      <c r="D123" s="6">
         <v>43614</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A124" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B124" s="8" t="s">
+      <c r="A124" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B124" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C124" s="8">
+      <c r="C124" s="5">
         <v>84</v>
       </c>
-      <c r="D124" s="9">
+      <c r="D124" s="6">
         <v>43614</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A125" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B125" s="8" t="s">
+      <c r="A125" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B125" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C125" s="8">
+      <c r="C125" s="5">
         <v>84</v>
       </c>
-      <c r="D125" s="9">
+      <c r="D125" s="6">
         <v>43614</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A126" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B126" s="8" t="s">
+      <c r="A126" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B126" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C126" s="8">
+      <c r="C126" s="5">
         <v>64</v>
       </c>
-      <c r="D126" s="43" t="s">
+      <c r="D126" s="40" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A127" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B127" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C127" s="8">
+      <c r="A127" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B127" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C127" s="5">
         <v>98</v>
       </c>
-      <c r="D127" s="43" t="s">
+      <c r="D127" s="40" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A128" s="8" t="s">
+      <c r="A128" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B128" s="8" t="s">
+      <c r="B128" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C128" s="8">
+      <c r="C128" s="5">
         <v>60</v>
       </c>
-      <c r="D128" s="43">
+      <c r="D128" s="40">
         <v>43471</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A129" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B129" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C129" s="8">
+      <c r="A129" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B129" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C129" s="5">
         <v>165</v>
       </c>
-      <c r="D129" s="43">
+      <c r="D129" s="40">
         <v>43616</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A130" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B130" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C130" s="8">
+      <c r="A130" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B130" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C130" s="5">
         <v>165</v>
       </c>
-      <c r="D130" s="43">
+      <c r="D130" s="40">
         <v>43616</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A131" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B131" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C131" s="8">
+      <c r="A131" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B131" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C131" s="5">
         <v>118</v>
       </c>
-      <c r="D131" s="43">
+      <c r="D131" s="40">
         <v>43618</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A132" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B132" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C132" s="8">
+      <c r="A132" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B132" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C132" s="5">
         <v>118</v>
       </c>
-      <c r="D132" s="43">
+      <c r="D132" s="40">
         <v>43618</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A133" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B133" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C133" s="8">
+      <c r="A133" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B133" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C133" s="5">
         <v>20</v>
       </c>
-      <c r="D133" s="9">
+      <c r="D133" s="6">
         <v>43530</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A134" s="8" t="s">
+      <c r="A134" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B134" s="8" t="s">
+      <c r="B134" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C134" s="8">
+      <c r="C134" s="5">
         <v>30</v>
       </c>
-      <c r="D134" s="43">
+      <c r="D134" s="40">
         <v>43619</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A135" s="8" t="s">
+      <c r="A135" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B135" s="8" t="s">
+      <c r="B135" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C135" s="8">
+      <c r="C135" s="5">
         <v>30</v>
       </c>
-      <c r="D135" s="43">
+      <c r="D135" s="40">
         <v>43619</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A136" s="8" t="s">
+      <c r="A136" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B136" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C136" s="8">
+      <c r="B136" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C136" s="5">
         <v>35</v>
       </c>
-      <c r="D136" s="43">
+      <c r="D136" s="40">
         <v>43619</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A137" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B137" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C137" s="8">
+      <c r="A137" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B137" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C137" s="5">
         <v>180</v>
       </c>
-      <c r="D137" s="43">
+      <c r="D137" s="40">
         <v>43620</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A138" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B138" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C138" s="8">
+      <c r="A138" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B138" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C138" s="5">
         <v>180</v>
       </c>
-      <c r="D138" s="43">
+      <c r="D138" s="40">
         <v>43620</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A139" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B139" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C139" s="8">
+      <c r="A139" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B139" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C139" s="5">
         <v>10</v>
       </c>
-      <c r="D139" s="9">
+      <c r="D139" s="6">
         <v>43620</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A140" s="8" t="s">
+      <c r="A140" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B140" s="8" t="s">
+      <c r="B140" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C140" s="8">
+      <c r="C140" s="5">
         <v>55</v>
       </c>
-      <c r="D140" s="9">
+      <c r="D140" s="6">
         <v>43621</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A141" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B141" s="8" t="s">
+      <c r="A141" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B141" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C141" s="8">
+      <c r="C141" s="5">
         <v>55</v>
       </c>
-      <c r="D141" s="9">
+      <c r="D141" s="6">
         <v>43621</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A142" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B142" s="8" t="s">
+      <c r="A142" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B142" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C142" s="8">
+      <c r="C142" s="5">
         <v>55</v>
       </c>
-      <c r="D142" s="9">
+      <c r="D142" s="6">
         <v>43621</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A143" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B143" s="8" t="s">
+      <c r="A143" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B143" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C143" s="8">
+      <c r="C143" s="5">
         <v>55</v>
       </c>
-      <c r="D143" s="9">
+      <c r="D143" s="6">
         <v>43621</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A144" s="8" t="s">
+      <c r="A144" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B144" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C144" s="8">
+      <c r="B144" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C144" s="5">
         <v>60</v>
       </c>
-      <c r="D144" s="9">
+      <c r="D144" s="6">
         <v>43621</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A145" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B145" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C145" s="8">
+      <c r="A145" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B145" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C145" s="5">
         <v>30</v>
       </c>
-      <c r="D145" s="9">
+      <c r="D145" s="6">
         <v>43621</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A146" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B146" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C146" s="8">
+      <c r="A146" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B146" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C146" s="5">
         <v>60</v>
       </c>
-      <c r="D146" s="9">
+      <c r="D146" s="6">
         <v>43621</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A147" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B147" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C147" s="8">
+      <c r="A147" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B147" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C147" s="5">
         <v>30</v>
       </c>
-      <c r="D147" s="9">
+      <c r="D147" s="6">
         <v>43621</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A148" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B148" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C148" s="8">
+      <c r="A148" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B148" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C148" s="5">
         <v>30</v>
       </c>
-      <c r="D148" s="9">
+      <c r="D148" s="6">
         <v>43621</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A149" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B149" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C149" s="8">
+      <c r="A149" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B149" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C149" s="5">
         <v>30</v>
       </c>
-      <c r="D149" s="9">
+      <c r="D149" s="6">
         <v>43621</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A150" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B150" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C150" s="8">
+      <c r="A150" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B150" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C150" s="5">
         <v>174</v>
       </c>
-      <c r="D150" s="9">
+      <c r="D150" s="6">
         <v>43622</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A151" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B151" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C151" s="8">
+      <c r="A151" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B151" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C151" s="5">
         <v>185</v>
       </c>
-      <c r="D151" s="44">
+      <c r="D151" s="41">
         <v>43622</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A152" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B152" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C152" s="8">
+      <c r="A152" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B152" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C152" s="5">
         <v>10</v>
       </c>
-      <c r="D152" s="44">
+      <c r="D152" s="41">
         <v>43622</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A153" s="8" t="s">
+      <c r="A153" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B153" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C153" s="8">
+      <c r="B153" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C153" s="5">
         <v>110</v>
       </c>
-      <c r="D153" s="44">
-        <v>43623</v>
+      <c r="D153" s="41">
+        <v>43622</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A154" s="8"/>
-      <c r="B154" s="8"/>
-      <c r="C154" s="8"/>
-      <c r="D154" s="8"/>
+      <c r="A154" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B154" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C154" s="5">
+        <v>55</v>
+      </c>
+      <c r="D154" s="41">
+        <v>43622</v>
+      </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A155" s="8"/>
-      <c r="B155" s="8"/>
-      <c r="C155" s="8"/>
-      <c r="D155" s="8"/>
+      <c r="A155" s="5"/>
+      <c r="B155" s="5"/>
+      <c r="C155" s="5"/>
+      <c r="D155" s="5"/>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A156" s="8"/>
-      <c r="B156" s="8"/>
-      <c r="C156" s="8"/>
-      <c r="D156" s="8"/>
+      <c r="A156" s="5"/>
+      <c r="B156" s="5"/>
+      <c r="C156" s="5"/>
+      <c r="D156" s="5"/>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A157" s="8"/>
-      <c r="B157" s="8"/>
-      <c r="C157" s="8"/>
-      <c r="D157" s="8"/>
+      <c r="A157" s="5"/>
+      <c r="B157" s="5"/>
+      <c r="C157" s="5"/>
+      <c r="D157" s="5"/>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A158" s="8"/>
-      <c r="B158" s="8"/>
-      <c r="C158" s="8"/>
-      <c r="D158" s="8"/>
+      <c r="A158" s="5"/>
+      <c r="B158" s="5"/>
+      <c r="C158" s="5"/>
+      <c r="D158" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
Documento dei requisiti versione 1.00
Dettagliati meglio i requisiti del calendario.
</commit_message>
<xml_diff>
--- a/Documentazione/Attività sul progetto/DocAttivProg.xlsx
+++ b/Documentazione/Attività sul progetto/DocAttivProg.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="31">
   <si>
     <t>Le categorie sono: Ispezione Codice, Documenti di progetto, Documenti di processo, Manuale, Sviluppo, Testing</t>
   </si>
@@ -778,8 +778,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O171"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A139" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G162" sqref="G162"/>
+    <sheetView tabSelected="1" topLeftCell="A142" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H163" sqref="H163"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -886,7 +886,7 @@
       </c>
       <c r="J6" s="10">
         <f>I6/I12</f>
-        <v>6.3935059914959416E-2</v>
+        <v>6.3590926566705119E-2</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
@@ -907,11 +907,11 @@
       </c>
       <c r="I7" s="9">
         <f>SUMIF(B:B,"Documenti di progetto",C:C)</f>
-        <v>2926</v>
+        <v>2996</v>
       </c>
       <c r="J7" s="10">
         <f>(I7/I12)</f>
-        <v>0.22620796289137998</v>
+        <v>0.23037293348712035</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
@@ -936,7 +936,7 @@
       </c>
       <c r="J8" s="10">
         <f>I8/I12</f>
-        <v>0.18654812524159259</v>
+        <v>0.18554402153018071</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
@@ -961,7 +961,7 @@
       </c>
       <c r="J9" s="10">
         <f>I9/I12</f>
-        <v>3.6335523772709703E-2</v>
+        <v>3.613994617454825E-2</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
@@ -986,7 +986,7 @@
       </c>
       <c r="J10" s="10">
         <f>I10/I12</f>
-        <v>0.46841901816776188</v>
+        <v>0.4658977316416763</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
@@ -1011,7 +1011,7 @@
       </c>
       <c r="J11" s="13">
         <f>I11/I12</f>
-        <v>1.8554310011596443E-2</v>
+        <v>1.845444059976932E-2</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
@@ -1032,7 +1032,7 @@
       </c>
       <c r="I12" s="15">
         <f>SUM(I6:I11)</f>
-        <v>12935</v>
+        <v>13005</v>
       </c>
       <c r="J12" s="16">
         <f>SUM(J6:J11)</f>
@@ -1238,7 +1238,7 @@
       </c>
       <c r="I19" s="21">
         <f>SUMIFS(C:C,B:B,"Documenti di progetto",A:A,"Luca")</f>
-        <v>1007</v>
+        <v>1077</v>
       </c>
       <c r="J19" s="21">
         <f>SUMIFS(C:C,B:B,"Documenti di processo",A:A,"Luca")</f>
@@ -1262,7 +1262,7 @@
       </c>
       <c r="O19" s="22">
         <f>SUM(I19:N19)</f>
-        <v>2273</v>
+        <v>2343</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
@@ -1328,7 +1328,7 @@
       </c>
       <c r="I21" s="24">
         <f t="shared" ref="I21:N21" si="0">AVERAGE(I17:I20)</f>
-        <v>731.5</v>
+        <v>749</v>
       </c>
       <c r="J21" s="25">
         <f t="shared" si="0"/>
@@ -1352,7 +1352,7 @@
       </c>
       <c r="O21" s="27">
         <f>SUM(O17:O20)</f>
-        <v>12935</v>
+        <v>13005</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
@@ -1553,11 +1553,11 @@
       </c>
       <c r="I28" s="32">
         <f>I19/O19</f>
-        <v>0.44302683677958643</v>
+        <v>0.45966709346991036</v>
       </c>
       <c r="J28" s="32">
         <f>J19/O19</f>
-        <v>0.37483501979762429</v>
+        <v>0.36363636363636365</v>
       </c>
       <c r="K28" s="32">
         <f>K19/O19</f>
@@ -1565,19 +1565,19 @@
       </c>
       <c r="L28" s="32">
         <f>L19/O19</f>
-        <v>2.6396832380114386E-2</v>
+        <v>2.5608194622279128E-2</v>
       </c>
       <c r="M28" s="32">
         <f>M19/O19</f>
-        <v>7.2591289045314561E-2</v>
+        <v>7.0422535211267609E-2</v>
       </c>
       <c r="N28" s="32">
         <f>N19/O19</f>
-        <v>8.315002199736031E-2</v>
+        <v>8.0665813060179253E-2</v>
       </c>
       <c r="O28" s="33">
         <f>SUM(I28:N28)</f>
-        <v>0.99999999999999989</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
@@ -1643,11 +1643,11 @@
       </c>
       <c r="I30" s="36">
         <f t="shared" ref="I30:N30" si="1">AVERAGE(I26:I29)</f>
-        <v>0.2553974554369689</v>
+        <v>0.25955751960954987</v>
       </c>
       <c r="J30" s="36">
         <f t="shared" si="1"/>
-        <v>0.21651602778416382</v>
+        <v>0.21371636374384864</v>
       </c>
       <c r="K30" s="36">
         <f t="shared" si="1"/>
@@ -1655,19 +1655,19 @@
       </c>
       <c r="L30" s="36">
         <f t="shared" si="1"/>
-        <v>0.39907021745215016</v>
+        <v>0.39887305801269135</v>
       </c>
       <c r="M30" s="36">
         <f t="shared" si="1"/>
-        <v>2.3049783045642366E-2</v>
+        <v>2.2507594587130628E-2</v>
       </c>
       <c r="N30" s="37">
         <f t="shared" si="1"/>
-        <v>6.7046344038610373E-2</v>
+        <v>6.6425291804315112E-2</v>
       </c>
       <c r="O30" s="38">
         <f>SUM(I30:N30)</f>
-        <v>0.99999999999999978</v>
+        <v>0.99999999999999989</v>
       </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
@@ -3575,10 +3575,18 @@
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A167" s="5"/>
-      <c r="B167" s="5"/>
-      <c r="C167" s="5"/>
-      <c r="D167" s="5"/>
+      <c r="A167" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B167" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C167" s="5">
+        <v>70</v>
+      </c>
+      <c r="D167" s="39">
+        <v>43628</v>
+      </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A168" s="5"/>

</xml_diff>

<commit_message>
Modificato nome doc risultati test e fatti alcuni test
</commit_message>
<xml_diff>
--- a/Documentazione/Attività sul progetto/DocAttivProg.xlsx
+++ b/Documentazione/Attività sul progetto/DocAttivProg.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="31">
   <si>
     <t>Le categorie sono: Ispezione Codice, Documenti di progetto, Documenti di processo, Manuale, Sviluppo, Testing</t>
   </si>
@@ -779,7 +779,7 @@
   <dimension ref="A1:O171"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A142" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H163" sqref="H163"/>
+      <selection activeCell="I164" sqref="I164"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -886,7 +886,7 @@
       </c>
       <c r="J6" s="10">
         <f>I6/I12</f>
-        <v>6.3590926566705119E-2</v>
+        <v>6.3033536585365854E-2</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
@@ -911,7 +911,7 @@
       </c>
       <c r="J7" s="10">
         <f>(I7/I12)</f>
-        <v>0.23037293348712035</v>
+        <v>0.22835365853658537</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
@@ -936,7 +936,7 @@
       </c>
       <c r="J8" s="10">
         <f>I8/I12</f>
-        <v>0.18554402153018071</v>
+        <v>0.18391768292682928</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
@@ -961,7 +961,7 @@
       </c>
       <c r="J9" s="10">
         <f>I9/I12</f>
-        <v>3.613994617454825E-2</v>
+        <v>3.5823170731707314E-2</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
@@ -986,7 +986,7 @@
       </c>
       <c r="J10" s="10">
         <f>I10/I12</f>
-        <v>0.4658977316416763</v>
+        <v>0.46181402439024388</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
@@ -1007,11 +1007,11 @@
       </c>
       <c r="I11" s="12">
         <f>SUMIF(B:B,"Testing",C:C)</f>
-        <v>240</v>
+        <v>355</v>
       </c>
       <c r="J11" s="13">
         <f>I11/I12</f>
-        <v>1.845444059976932E-2</v>
+        <v>2.7057926829268292E-2</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
@@ -1032,7 +1032,7 @@
       </c>
       <c r="I12" s="15">
         <f>SUM(I6:I11)</f>
-        <v>13005</v>
+        <v>13120</v>
       </c>
       <c r="J12" s="16">
         <f>SUM(J6:J11)</f>
@@ -1254,7 +1254,7 @@
       </c>
       <c r="M19" s="21">
         <f>SUMIFS(C:C,B:B,"Testing",A:A,"Luca")</f>
-        <v>165</v>
+        <v>280</v>
       </c>
       <c r="N19" s="21">
         <f>SUMIFS(C:C,B:B,"Ispezione codice",A:A,"Luca")</f>
@@ -1262,7 +1262,7 @@
       </c>
       <c r="O19" s="22">
         <f>SUM(I19:N19)</f>
-        <v>2343</v>
+        <v>2458</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
@@ -1344,7 +1344,7 @@
       </c>
       <c r="M21" s="25">
         <f t="shared" si="0"/>
-        <v>60</v>
+        <v>88.75</v>
       </c>
       <c r="N21" s="26">
         <f t="shared" si="0"/>
@@ -1352,7 +1352,7 @@
       </c>
       <c r="O21" s="27">
         <f>SUM(O17:O20)</f>
-        <v>13005</v>
+        <v>13120</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
@@ -1553,11 +1553,11 @@
       </c>
       <c r="I28" s="32">
         <f>I19/O19</f>
-        <v>0.45966709346991036</v>
+        <v>0.43816110659072416</v>
       </c>
       <c r="J28" s="32">
         <f>J19/O19</f>
-        <v>0.36363636363636365</v>
+        <v>0.34662327095199347</v>
       </c>
       <c r="K28" s="32">
         <f>K19/O19</f>
@@ -1565,15 +1565,15 @@
       </c>
       <c r="L28" s="32">
         <f>L19/O19</f>
-        <v>2.5608194622279128E-2</v>
+        <v>2.4410089503661515E-2</v>
       </c>
       <c r="M28" s="32">
         <f>M19/O19</f>
-        <v>7.0422535211267609E-2</v>
+        <v>0.11391375101708706</v>
       </c>
       <c r="N28" s="32">
         <f>N19/O19</f>
-        <v>8.0665813060179253E-2</v>
+        <v>7.6891781936533773E-2</v>
       </c>
       <c r="O28" s="33">
         <f>SUM(I28:N28)</f>
@@ -1643,11 +1643,11 @@
       </c>
       <c r="I30" s="36">
         <f t="shared" ref="I30:N30" si="1">AVERAGE(I26:I29)</f>
-        <v>0.25955751960954987</v>
+        <v>0.25418102288975331</v>
       </c>
       <c r="J30" s="36">
         <f t="shared" si="1"/>
-        <v>0.21371636374384864</v>
+        <v>0.20946309057275611</v>
       </c>
       <c r="K30" s="36">
         <f t="shared" si="1"/>
@@ -1655,15 +1655,15 @@
       </c>
       <c r="L30" s="36">
         <f t="shared" si="1"/>
-        <v>0.39887305801269135</v>
+        <v>0.39857353173303695</v>
       </c>
       <c r="M30" s="36">
         <f t="shared" si="1"/>
-        <v>2.2507594587130628E-2</v>
+        <v>3.3380398538585487E-2</v>
       </c>
       <c r="N30" s="37">
         <f t="shared" si="1"/>
-        <v>6.6425291804315112E-2</v>
+        <v>6.5481784023403738E-2</v>
       </c>
       <c r="O30" s="38">
         <f>SUM(I30:N30)</f>
@@ -3589,10 +3589,18 @@
       </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A168" s="5"/>
-      <c r="B168" s="5"/>
-      <c r="C168" s="5"/>
-      <c r="D168" s="5"/>
+      <c r="A168" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B168" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C168" s="5">
+        <v>115</v>
+      </c>
+      <c r="D168" s="39">
+        <v>43628</v>
+      </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A169" s="5"/>

</xml_diff>

<commit_message>
aggiunta versione corretta manuale nel codice, correzione CMv1.00, creazione doc avanz 12/06/19
</commit_message>
<xml_diff>
--- a/Documentazione/Attività sul progetto/DocAttivProg.xlsx
+++ b/Documentazione/Attività sul progetto/DocAttivProg.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LUCA\Documents\Universita\INGEGNERIA DEL SOFTWARE\Progetto\Documentazione\Attività sul progetto\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\UniUD\Laurea Magistrale\Ingegneria del Software 2\Progetto-Ingegneria-Del-Sw-2\Documentazione\Attività sul progetto\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AB2DB19-EEFD-4E73-8DB2-F820442F08BB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330" tabRatio="500"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913" iterateDelta="1E-4"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="31">
   <si>
     <t>Le categorie sono: Ispezione Codice, Documenti di progetto, Documenti di processo, Manuale, Sviluppo, Testing</t>
   </si>
@@ -128,7 +129,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -775,39 +776,39 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O171"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H165" sqref="H165"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.5703125" customWidth="1"/>
-    <col min="2" max="2" width="23.42578125" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" customWidth="1"/>
-    <col min="4" max="4" width="10.85546875" customWidth="1"/>
-    <col min="5" max="7" width="8.7109375" customWidth="1"/>
-    <col min="8" max="8" width="26.28515625" customWidth="1"/>
-    <col min="9" max="11" width="17.28515625" customWidth="1"/>
-    <col min="12" max="14" width="17.42578125" customWidth="1"/>
-    <col min="15" max="1025" width="8.7109375" customWidth="1"/>
+    <col min="1" max="1" width="15.5546875" customWidth="1"/>
+    <col min="2" max="2" width="23.44140625" customWidth="1"/>
+    <col min="3" max="3" width="15.5546875" customWidth="1"/>
+    <col min="4" max="4" width="10.88671875" customWidth="1"/>
+    <col min="5" max="7" width="8.6640625" customWidth="1"/>
+    <col min="8" max="8" width="26.33203125" customWidth="1"/>
+    <col min="9" max="11" width="17.33203125" customWidth="1"/>
+    <col min="12" max="14" width="17.44140625" customWidth="1"/>
+    <col min="15" max="1025" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="F1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="F2" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
@@ -822,7 +823,7 @@
       </c>
       <c r="H3" s="2"/>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>6</v>
       </c>
@@ -841,7 +842,7 @@
       <c r="I4" s="41"/>
       <c r="J4" s="41"/>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>6</v>
       </c>
@@ -864,7 +865,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>6</v>
       </c>
@@ -886,10 +887,10 @@
       </c>
       <c r="J6" s="10">
         <f>I6/I12</f>
-        <v>6.2203836028582177E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+        <v>6.209641087250338E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>6</v>
       </c>
@@ -911,10 +912,10 @@
       </c>
       <c r="J7" s="10">
         <f>(I7/I12)</f>
-        <v>0.22534787514103047</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+        <v>0.22495870250788408</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>6</v>
       </c>
@@ -932,14 +933,14 @@
       </c>
       <c r="I8" s="9">
         <f>SUMIF(B:B,"Documenti di processo",C:C)</f>
-        <v>2413</v>
+        <v>2436</v>
       </c>
       <c r="J8" s="10">
         <f>I8/I12</f>
-        <v>0.18149680330951484</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+        <v>0.18291034689893376</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>6</v>
       </c>
@@ -961,10 +962,10 @@
       </c>
       <c r="J9" s="10">
         <f>I9/I12</f>
-        <v>3.5351635953365927E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+        <v>3.5290584171797569E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>6</v>
       </c>
@@ -986,10 +987,10 @@
       </c>
       <c r="J10" s="10">
         <f>I10/I12</f>
-        <v>0.45573523881158329</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+        <v>0.45494819041898182</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>16</v>
       </c>
@@ -1011,10 +1012,10 @@
       </c>
       <c r="J11" s="13">
         <f>I11/I12</f>
-        <v>3.9864610755923277E-2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+        <v>3.9795765129899387E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>16</v>
       </c>
@@ -1032,14 +1033,14 @@
       </c>
       <c r="I12" s="15">
         <f>SUM(I6:I11)</f>
-        <v>13295</v>
+        <v>13318</v>
       </c>
       <c r="J12" s="16">
         <f>SUM(J6:J11)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
         <v>6</v>
       </c>
@@ -1054,7 +1055,7 @@
       </c>
       <c r="H13" s="2"/>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
         <v>6</v>
       </c>
@@ -1068,7 +1069,7 @@
         <v>43509</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
         <v>19</v>
       </c>
@@ -1092,7 +1093,7 @@
       <c r="N15" s="42"/>
       <c r="O15" s="42"/>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
         <v>19</v>
       </c>
@@ -1130,7 +1131,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
         <v>25</v>
       </c>
@@ -1152,7 +1153,7 @@
       </c>
       <c r="J17" s="21">
         <f>SUMIFS(C:C,B:B,"Documenti di processo",A:A,"Giovanni")</f>
-        <v>1189</v>
+        <v>1212</v>
       </c>
       <c r="K17" s="21">
         <f>SUMIFS(C:C,B:B,"Manuale",A:A,"Giovanni")</f>
@@ -1172,10 +1173,10 @@
       </c>
       <c r="O17" s="22">
         <f>SUM(I17:N17)</f>
-        <v>3019</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+        <v>3042</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
         <v>25</v>
       </c>
@@ -1220,7 +1221,7 @@
         <v>3818</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
         <v>25</v>
       </c>
@@ -1265,7 +1266,7 @@
         <v>2633</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
         <v>25</v>
       </c>
@@ -1310,7 +1311,7 @@
         <v>3825</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
         <v>25</v>
       </c>
@@ -1332,7 +1333,7 @@
       </c>
       <c r="J21" s="25">
         <f t="shared" si="0"/>
-        <v>603.25</v>
+        <v>609</v>
       </c>
       <c r="K21" s="25">
         <f t="shared" si="0"/>
@@ -1352,10 +1353,10 @@
       </c>
       <c r="O21" s="27">
         <f>SUM(O17:O20)</f>
-        <v>13295</v>
-      </c>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+        <v>13318</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
         <v>16</v>
       </c>
@@ -1369,7 +1370,7 @@
         <v>43487</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A23" s="5" t="s">
         <v>16</v>
       </c>
@@ -1383,7 +1384,7 @@
         <v>43506</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
         <v>16</v>
       </c>
@@ -1407,7 +1408,7 @@
       <c r="N24" s="43"/>
       <c r="O24" s="43"/>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A25" s="5" t="s">
         <v>16</v>
       </c>
@@ -1445,7 +1446,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="s">
         <v>16</v>
       </c>
@@ -1463,15 +1464,15 @@
       </c>
       <c r="I26" s="32">
         <f>I17/O17</f>
-        <v>0.36435905929115603</v>
+        <v>0.36160420775805391</v>
       </c>
       <c r="J26" s="32">
         <f>J17/O17</f>
-        <v>0.39383901954289502</v>
+        <v>0.39842209072978302</v>
       </c>
       <c r="K26" s="32">
         <f>K17/O17</f>
-        <v>0.15568068896985757</v>
+        <v>0.15450361604207757</v>
       </c>
       <c r="L26" s="32">
         <f>L17/O17</f>
@@ -1483,14 +1484,14 @@
       </c>
       <c r="N26" s="32">
         <f>N17/O17</f>
-        <v>8.6121232196091427E-2</v>
+        <v>8.5470085470085472E-2</v>
       </c>
       <c r="O26" s="33">
         <f>SUM(I26:N26)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A27" s="5" t="s">
         <v>16</v>
       </c>
@@ -1535,7 +1536,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A28" s="5" t="s">
         <v>19</v>
       </c>
@@ -1580,7 +1581,7 @@
         <v>0.99999999999999989</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A29" s="5" t="s">
         <v>6</v>
       </c>
@@ -1625,7 +1626,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A30" s="5" t="s">
         <v>25</v>
       </c>
@@ -1643,15 +1644,15 @@
       </c>
       <c r="I30" s="36">
         <f t="shared" ref="I30:N30" si="1">AVERAGE(I26:I29)</f>
-        <v>0.24690052596102402</v>
+        <v>0.24621181307774853</v>
       </c>
       <c r="J30" s="36">
         <f t="shared" si="1"/>
-        <v>0.20370358882412348</v>
+        <v>0.2048493566208455</v>
       </c>
       <c r="K30" s="36">
         <f t="shared" si="1"/>
-        <v>3.8920172242464392E-2</v>
+        <v>3.8625904010519393E-2</v>
       </c>
       <c r="L30" s="36">
         <f t="shared" si="1"/>
@@ -1663,14 +1664,14 @@
       </c>
       <c r="N30" s="37">
         <f t="shared" si="1"/>
-        <v>6.4204148072122547E-2</v>
+        <v>6.4041361390621054E-2</v>
       </c>
       <c r="O30" s="38">
         <f>SUM(I30:N30)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A31" s="5" t="s">
         <v>25</v>
       </c>
@@ -1684,7 +1685,7 @@
         <v>43531</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A32" s="5" t="s">
         <v>25</v>
       </c>
@@ -1698,7 +1699,7 @@
         <v>43532</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="5" t="s">
         <v>25</v>
       </c>
@@ -1712,7 +1713,7 @@
         <v>43533</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="5" t="s">
         <v>25</v>
       </c>
@@ -1726,7 +1727,7 @@
         <v>43534</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="5" t="s">
         <v>6</v>
       </c>
@@ -1740,7 +1741,7 @@
         <v>43546</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="5" t="s">
         <v>6</v>
       </c>
@@ -1754,7 +1755,7 @@
         <v>43546</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" s="5" t="s">
         <v>16</v>
       </c>
@@ -1768,7 +1769,7 @@
         <v>43376</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" s="5" t="s">
         <v>16</v>
       </c>
@@ -1782,7 +1783,7 @@
         <v>43407</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" s="5" t="s">
         <v>25</v>
       </c>
@@ -1796,7 +1797,7 @@
         <v>43546</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" s="5" t="s">
         <v>19</v>
       </c>
@@ -1810,7 +1811,7 @@
         <v>43553</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" s="5" t="s">
         <v>25</v>
       </c>
@@ -1824,7 +1825,7 @@
         <v>43553</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" s="5" t="s">
         <v>16</v>
       </c>
@@ -1838,7 +1839,7 @@
         <v>43553</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" s="5" t="s">
         <v>19</v>
       </c>
@@ -1852,7 +1853,7 @@
         <v>43481</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" s="5" t="s">
         <v>19</v>
       </c>
@@ -1866,7 +1867,7 @@
         <v>43442</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" s="5" t="s">
         <v>19</v>
       </c>
@@ -1880,7 +1881,7 @@
         <v>43448</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" s="5" t="s">
         <v>19</v>
       </c>
@@ -1894,7 +1895,7 @@
         <v>43468</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" s="5" t="s">
         <v>19</v>
       </c>
@@ -1908,7 +1909,7 @@
         <v>43478</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" s="5" t="s">
         <v>6</v>
       </c>
@@ -1922,7 +1923,7 @@
         <v>43449</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" s="5" t="s">
         <v>6</v>
       </c>
@@ -1936,7 +1937,7 @@
         <v>43450</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" s="5" t="s">
         <v>19</v>
       </c>
@@ -1950,7 +1951,7 @@
         <v>43558</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" s="5" t="s">
         <v>25</v>
       </c>
@@ -1964,7 +1965,7 @@
         <v>43558</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" s="5" t="s">
         <v>6</v>
       </c>
@@ -1978,7 +1979,7 @@
         <v>43558</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" s="5" t="s">
         <v>25</v>
       </c>
@@ -1992,7 +1993,7 @@
         <v>43559</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" s="5" t="s">
         <v>19</v>
       </c>
@@ -2006,7 +2007,7 @@
         <v>43571</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" s="5" t="s">
         <v>25</v>
       </c>
@@ -2020,7 +2021,7 @@
         <v>43571</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" s="5" t="s">
         <v>19</v>
       </c>
@@ -2034,7 +2035,7 @@
         <v>43572</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" s="5" t="s">
         <v>19</v>
       </c>
@@ -2048,7 +2049,7 @@
         <v>43574</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" s="5" t="s">
         <v>6</v>
       </c>
@@ -2062,7 +2063,7 @@
         <v>43577</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" s="5" t="s">
         <v>6</v>
       </c>
@@ -2076,7 +2077,7 @@
         <v>43578</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" s="5" t="s">
         <v>25</v>
       </c>
@@ -2090,7 +2091,7 @@
         <v>43578</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" s="5" t="s">
         <v>6</v>
       </c>
@@ -2104,7 +2105,7 @@
         <v>43581</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" s="5" t="s">
         <v>6</v>
       </c>
@@ -2118,7 +2119,7 @@
         <v>43584</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" s="5" t="s">
         <v>6</v>
       </c>
@@ -2132,7 +2133,7 @@
         <v>43585</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" s="5" t="s">
         <v>19</v>
       </c>
@@ -2146,7 +2147,7 @@
         <v>43585</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" s="5" t="s">
         <v>19</v>
       </c>
@@ -2160,7 +2161,7 @@
         <v>43587</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66" s="5" t="s">
         <v>16</v>
       </c>
@@ -2174,7 +2175,7 @@
         <v>43587</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67" s="5" t="s">
         <v>16</v>
       </c>
@@ -2188,7 +2189,7 @@
         <v>43587</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68" s="5" t="s">
         <v>16</v>
       </c>
@@ -2202,7 +2203,7 @@
         <v>43587</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69" s="5" t="s">
         <v>16</v>
       </c>
@@ -2216,7 +2217,7 @@
         <v>43588</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70" s="5" t="s">
         <v>25</v>
       </c>
@@ -2230,7 +2231,7 @@
         <v>43588</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71" s="5" t="s">
         <v>25</v>
       </c>
@@ -2244,7 +2245,7 @@
         <v>43589</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72" s="5" t="s">
         <v>16</v>
       </c>
@@ -2258,7 +2259,7 @@
         <v>43589</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73" s="5" t="s">
         <v>25</v>
       </c>
@@ -2272,7 +2273,7 @@
         <v>43590</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74" s="5" t="s">
         <v>16</v>
       </c>
@@ -2286,7 +2287,7 @@
         <v>43590</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75" s="5" t="s">
         <v>6</v>
       </c>
@@ -2300,7 +2301,7 @@
         <v>43593</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76" s="5" t="s">
         <v>25</v>
       </c>
@@ -2314,7 +2315,7 @@
         <v>43593</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" s="5" t="s">
         <v>19</v>
       </c>
@@ -2328,7 +2329,7 @@
         <v>43593</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A78" s="5" t="s">
         <v>16</v>
       </c>
@@ -2342,7 +2343,7 @@
         <v>43593</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A79" s="5" t="s">
         <v>25</v>
       </c>
@@ -2356,7 +2357,7 @@
         <v>43593</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A80" s="5" t="s">
         <v>19</v>
       </c>
@@ -2370,7 +2371,7 @@
         <v>43593</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A81" s="5" t="s">
         <v>16</v>
       </c>
@@ -2384,7 +2385,7 @@
         <v>43593</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A82" s="5" t="s">
         <v>16</v>
       </c>
@@ -2398,7 +2399,7 @@
         <v>43594</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A83" s="5" t="s">
         <v>25</v>
       </c>
@@ -2412,7 +2413,7 @@
         <v>43594</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A84" s="5" t="s">
         <v>6</v>
       </c>
@@ -2426,7 +2427,7 @@
         <v>43598</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A85" s="5" t="s">
         <v>6</v>
       </c>
@@ -2440,7 +2441,7 @@
         <v>43598</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A86" s="5" t="s">
         <v>25</v>
       </c>
@@ -2454,7 +2455,7 @@
         <v>43595</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A87" s="5" t="s">
         <v>16</v>
       </c>
@@ -2468,7 +2469,7 @@
         <v>43595</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A88" s="5" t="s">
         <v>25</v>
       </c>
@@ -2482,7 +2483,7 @@
         <v>43599</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A89" s="5" t="s">
         <v>16</v>
       </c>
@@ -2496,7 +2497,7 @@
         <v>43599</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A90" s="5" t="s">
         <v>6</v>
       </c>
@@ -2510,7 +2511,7 @@
         <v>43600</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A91" s="5" t="s">
         <v>19</v>
       </c>
@@ -2524,7 +2525,7 @@
         <v>43600</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A92" s="5" t="s">
         <v>16</v>
       </c>
@@ -2538,7 +2539,7 @@
         <v>43600</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A93" s="5" t="s">
         <v>25</v>
       </c>
@@ -2552,7 +2553,7 @@
         <v>43600</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A94" s="5" t="s">
         <v>6</v>
       </c>
@@ -2566,7 +2567,7 @@
         <v>43600</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A95" s="5" t="s">
         <v>19</v>
       </c>
@@ -2580,7 +2581,7 @@
         <v>43600</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A96" s="5" t="s">
         <v>16</v>
       </c>
@@ -2594,7 +2595,7 @@
         <v>43600</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A97" s="5" t="s">
         <v>25</v>
       </c>
@@ -2608,7 +2609,7 @@
         <v>43600</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A98" s="5" t="s">
         <v>25</v>
       </c>
@@ -2622,7 +2623,7 @@
         <v>43603</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A99" s="5" t="s">
         <v>16</v>
       </c>
@@ -2636,7 +2637,7 @@
         <v>43603</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A100" s="5" t="s">
         <v>25</v>
       </c>
@@ -2650,7 +2651,7 @@
         <v>43604</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A101" s="5" t="s">
         <v>16</v>
       </c>
@@ -2664,7 +2665,7 @@
         <v>43604</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A102" s="5" t="s">
         <v>16</v>
       </c>
@@ -2678,7 +2679,7 @@
         <v>43604</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A103" s="5" t="s">
         <v>16</v>
       </c>
@@ -2692,7 +2693,7 @@
         <v>43605</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A104" s="5" t="s">
         <v>25</v>
       </c>
@@ -2706,7 +2707,7 @@
         <v>43606</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A105" s="5" t="s">
         <v>6</v>
       </c>
@@ -2720,7 +2721,7 @@
         <v>43607</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A106" s="5" t="s">
         <v>16</v>
       </c>
@@ -2734,7 +2735,7 @@
         <v>43607</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A107" s="5" t="s">
         <v>25</v>
       </c>
@@ -2748,7 +2749,7 @@
         <v>43607</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A108" s="5" t="s">
         <v>6</v>
       </c>
@@ -2762,7 +2763,7 @@
         <v>43607</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A109" s="5" t="s">
         <v>16</v>
       </c>
@@ -2776,7 +2777,7 @@
         <v>43607</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A110" s="5" t="s">
         <v>25</v>
       </c>
@@ -2790,7 +2791,7 @@
         <v>43607</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A111" s="5" t="s">
         <v>16</v>
       </c>
@@ -2804,7 +2805,7 @@
         <v>43607</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A112" s="5" t="s">
         <v>25</v>
       </c>
@@ -2818,7 +2819,7 @@
         <v>43607</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A113" s="5" t="s">
         <v>25</v>
       </c>
@@ -2832,7 +2833,7 @@
         <v>43607</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A114" s="5" t="s">
         <v>6</v>
       </c>
@@ -2846,7 +2847,7 @@
         <v>43608</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A115" s="5" t="s">
         <v>6</v>
       </c>
@@ -2860,7 +2861,7 @@
         <v>43609</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A116" s="5" t="s">
         <v>16</v>
       </c>
@@ -2874,7 +2875,7 @@
         <v>43608</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A117" s="5" t="s">
         <v>25</v>
       </c>
@@ -2888,7 +2889,7 @@
         <v>43608</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A118" s="5" t="s">
         <v>25</v>
       </c>
@@ -2902,7 +2903,7 @@
         <v>43609</v>
       </c>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A119" s="5" t="s">
         <v>19</v>
       </c>
@@ -2916,7 +2917,7 @@
         <v>43614</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A120" s="5" t="s">
         <v>16</v>
       </c>
@@ -2930,7 +2931,7 @@
         <v>43614</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A121" s="5" t="s">
         <v>6</v>
       </c>
@@ -2944,7 +2945,7 @@
         <v>43614</v>
       </c>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A122" s="5" t="s">
         <v>19</v>
       </c>
@@ -2958,7 +2959,7 @@
         <v>43614</v>
       </c>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A123" s="5" t="s">
         <v>16</v>
       </c>
@@ -2972,7 +2973,7 @@
         <v>43614</v>
       </c>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A124" s="5" t="s">
         <v>6</v>
       </c>
@@ -2986,7 +2987,7 @@
         <v>43614</v>
       </c>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A125" s="5" t="s">
         <v>25</v>
       </c>
@@ -3000,7 +3001,7 @@
         <v>43614</v>
       </c>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A126" s="5" t="s">
         <v>6</v>
       </c>
@@ -3014,7 +3015,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A127" s="5" t="s">
         <v>6</v>
       </c>
@@ -3028,7 +3029,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A128" s="5" t="s">
         <v>19</v>
       </c>
@@ -3042,7 +3043,7 @@
         <v>43471</v>
       </c>
     </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A129" s="5" t="s">
         <v>16</v>
       </c>
@@ -3056,7 +3057,7 @@
         <v>43616</v>
       </c>
     </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A130" s="5" t="s">
         <v>25</v>
       </c>
@@ -3070,7 +3071,7 @@
         <v>43616</v>
       </c>
     </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A131" s="5" t="s">
         <v>16</v>
       </c>
@@ -3084,7 +3085,7 @@
         <v>43618</v>
       </c>
     </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A132" s="5" t="s">
         <v>25</v>
       </c>
@@ -3098,7 +3099,7 @@
         <v>43618</v>
       </c>
     </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A133" s="5" t="s">
         <v>25</v>
       </c>
@@ -3112,7 +3113,7 @@
         <v>43530</v>
       </c>
     </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A134" s="5" t="s">
         <v>19</v>
       </c>
@@ -3126,7 +3127,7 @@
         <v>43619</v>
       </c>
     </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A135" s="5" t="s">
         <v>19</v>
       </c>
@@ -3140,7 +3141,7 @@
         <v>43619</v>
       </c>
     </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A136" s="5" t="s">
         <v>19</v>
       </c>
@@ -3154,7 +3155,7 @@
         <v>43619</v>
       </c>
     </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A137" s="5" t="s">
         <v>25</v>
       </c>
@@ -3168,7 +3169,7 @@
         <v>43620</v>
       </c>
     </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A138" s="5" t="s">
         <v>16</v>
       </c>
@@ -3182,7 +3183,7 @@
         <v>43620</v>
       </c>
     </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A139" s="5" t="s">
         <v>25</v>
       </c>
@@ -3196,7 +3197,7 @@
         <v>43620</v>
       </c>
     </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A140" s="5" t="s">
         <v>19</v>
       </c>
@@ -3210,7 +3211,7 @@
         <v>43621</v>
       </c>
     </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A141" s="5" t="s">
         <v>16</v>
       </c>
@@ -3224,7 +3225,7 @@
         <v>43621</v>
       </c>
     </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A142" s="5" t="s">
         <v>6</v>
       </c>
@@ -3238,7 +3239,7 @@
         <v>43621</v>
       </c>
     </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A143" s="5" t="s">
         <v>25</v>
       </c>
@@ -3252,7 +3253,7 @@
         <v>43621</v>
       </c>
     </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A144" s="5" t="s">
         <v>19</v>
       </c>
@@ -3266,7 +3267,7 @@
         <v>43621</v>
       </c>
     </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A145" s="5" t="s">
         <v>16</v>
       </c>
@@ -3280,7 +3281,7 @@
         <v>43621</v>
       </c>
     </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A146" s="5" t="s">
         <v>6</v>
       </c>
@@ -3294,7 +3295,7 @@
         <v>43621</v>
       </c>
     </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A147" s="5" t="s">
         <v>25</v>
       </c>
@@ -3308,7 +3309,7 @@
         <v>43621</v>
       </c>
     </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A148" s="5" t="s">
         <v>16</v>
       </c>
@@ -3322,7 +3323,7 @@
         <v>43621</v>
       </c>
     </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A149" s="5" t="s">
         <v>25</v>
       </c>
@@ -3336,7 +3337,7 @@
         <v>43621</v>
       </c>
     </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A150" s="5" t="s">
         <v>16</v>
       </c>
@@ -3350,7 +3351,7 @@
         <v>43622</v>
       </c>
     </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A151" s="5" t="s">
         <v>25</v>
       </c>
@@ -3364,7 +3365,7 @@
         <v>43622</v>
       </c>
     </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A152" s="5" t="s">
         <v>25</v>
       </c>
@@ -3378,7 +3379,7 @@
         <v>43622</v>
       </c>
     </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A153" s="5" t="s">
         <v>19</v>
       </c>
@@ -3392,7 +3393,7 @@
         <v>43622</v>
       </c>
     </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A154" s="5" t="s">
         <v>19</v>
       </c>
@@ -3406,7 +3407,7 @@
         <v>43622</v>
       </c>
     </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A155" s="5" t="s">
         <v>6</v>
       </c>
@@ -3420,7 +3421,7 @@
         <v>43623</v>
       </c>
     </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A156" s="5" t="s">
         <v>6</v>
       </c>
@@ -3434,7 +3435,7 @@
         <v>43625</v>
       </c>
     </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A157" s="5" t="s">
         <v>6</v>
       </c>
@@ -3448,7 +3449,7 @@
         <v>43625</v>
       </c>
     </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A158" s="5" t="s">
         <v>25</v>
       </c>
@@ -3462,7 +3463,7 @@
         <v>43625</v>
       </c>
     </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A159" s="5" t="s">
         <v>6</v>
       </c>
@@ -3476,7 +3477,7 @@
         <v>43625</v>
       </c>
     </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A160" s="5" t="s">
         <v>25</v>
       </c>
@@ -3490,7 +3491,7 @@
         <v>43626</v>
       </c>
     </row>
-    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A161" s="5" t="s">
         <v>16</v>
       </c>
@@ -3504,7 +3505,7 @@
         <v>43626</v>
       </c>
     </row>
-    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A162" s="5" t="s">
         <v>6</v>
       </c>
@@ -3518,7 +3519,7 @@
         <v>43626</v>
       </c>
     </row>
-    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A163" s="5" t="s">
         <v>6</v>
       </c>
@@ -3532,7 +3533,7 @@
         <v>43626</v>
       </c>
     </row>
-    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A164" s="5" t="s">
         <v>6</v>
       </c>
@@ -3546,7 +3547,7 @@
         <v>43626</v>
       </c>
     </row>
-    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A165" s="5" t="s">
         <v>19</v>
       </c>
@@ -3560,7 +3561,7 @@
         <v>43627</v>
       </c>
     </row>
-    <row r="166" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A166" s="5" t="s">
         <v>16</v>
       </c>
@@ -3574,7 +3575,7 @@
         <v>43627</v>
       </c>
     </row>
-    <row r="167" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A167" s="5" t="s">
         <v>19</v>
       </c>
@@ -3588,7 +3589,7 @@
         <v>43628</v>
       </c>
     </row>
-    <row r="168" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A168" s="5" t="s">
         <v>19</v>
       </c>
@@ -3602,7 +3603,7 @@
         <v>43628</v>
       </c>
     </row>
-    <row r="169" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A169" s="5" t="s">
         <v>19</v>
       </c>
@@ -3616,13 +3617,21 @@
         <v>43628</v>
       </c>
     </row>
-    <row r="170" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A170" s="5"/>
-      <c r="B170" s="5"/>
-      <c r="C170" s="5"/>
-      <c r="D170" s="5"/>
-    </row>
-    <row r="171" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A170" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B170" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C170" s="5">
+        <v>23</v>
+      </c>
+      <c r="D170" s="39">
+        <v>43628</v>
+      </c>
+    </row>
+    <row r="171" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A171" s="5"/>
       <c r="B171" s="5"/>
       <c r="C171" s="5"/>

</xml_diff>

<commit_message>
Aggiornati test result con ultimi fix
</commit_message>
<xml_diff>
--- a/Documentazione/Attività sul progetto/DocAttivProg.xlsx
+++ b/Documentazione/Attività sul progetto/DocAttivProg.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\UniUD\Laurea Magistrale\Ingegneria del Software 2\Progetto-Ingegneria-Del-Sw-2\Documentazione\Attività sul progetto\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LUCA\Documents\Universita\INGEGNERIA DEL SOFTWARE\Progetto\Documentazione\Attività sul progetto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AB2DB19-EEFD-4E73-8DB2-F820442F08BB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" iterateDelta="1E-4"/>
+  <calcPr calcId="162913" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -31,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="31">
   <si>
     <t>Le categorie sono: Ispezione Codice, Documenti di progetto, Documenti di processo, Manuale, Sviluppo, Testing</t>
   </si>
@@ -129,7 +128,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -285,7 +284,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -394,6 +393,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -776,39 +776,39 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O171"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:O229"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="G183" sqref="G183"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.5546875" customWidth="1"/>
-    <col min="2" max="2" width="23.44140625" customWidth="1"/>
-    <col min="3" max="3" width="15.5546875" customWidth="1"/>
-    <col min="4" max="4" width="10.88671875" customWidth="1"/>
-    <col min="5" max="7" width="8.6640625" customWidth="1"/>
-    <col min="8" max="8" width="26.33203125" customWidth="1"/>
-    <col min="9" max="11" width="17.33203125" customWidth="1"/>
-    <col min="12" max="14" width="17.44140625" customWidth="1"/>
-    <col min="15" max="1025" width="8.6640625" customWidth="1"/>
+    <col min="1" max="1" width="15.5703125" customWidth="1"/>
+    <col min="2" max="2" width="23.42578125" customWidth="1"/>
+    <col min="3" max="3" width="15.5703125" customWidth="1"/>
+    <col min="4" max="4" width="10.85546875" customWidth="1"/>
+    <col min="5" max="7" width="8.7109375" customWidth="1"/>
+    <col min="8" max="8" width="26.28515625" customWidth="1"/>
+    <col min="9" max="11" width="17.28515625" customWidth="1"/>
+    <col min="12" max="14" width="17.42578125" customWidth="1"/>
+    <col min="15" max="1025" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="F1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="F2" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
@@ -823,7 +823,7 @@
       </c>
       <c r="H3" s="2"/>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>6</v>
       </c>
@@ -842,7 +842,7 @@
       <c r="I4" s="41"/>
       <c r="J4" s="41"/>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>6</v>
       </c>
@@ -865,7 +865,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>6</v>
       </c>
@@ -887,10 +887,10 @@
       </c>
       <c r="J6" s="10">
         <f>I6/I12</f>
-        <v>6.209641087250338E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+        <v>6.1956847467785438E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>6</v>
       </c>
@@ -912,10 +912,10 @@
       </c>
       <c r="J7" s="10">
         <f>(I7/I12)</f>
-        <v>0.22495870250788408</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+        <v>0.22445310158825293</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>6</v>
       </c>
@@ -937,10 +937,10 @@
       </c>
       <c r="J8" s="10">
         <f>I8/I12</f>
-        <v>0.18291034689893376</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+        <v>0.18249925082409349</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>6</v>
       </c>
@@ -962,10 +962,10 @@
       </c>
       <c r="J9" s="10">
         <f>I9/I12</f>
-        <v>3.5290584171797569E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+        <v>3.5211267605633804E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>6</v>
       </c>
@@ -987,10 +987,10 @@
       </c>
       <c r="J10" s="10">
         <f>I10/I12</f>
-        <v>0.45494819041898182</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+        <v>0.45392568175007492</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>16</v>
       </c>
@@ -1008,14 +1008,14 @@
       </c>
       <c r="I11" s="12">
         <f>SUMIF(B:B,"Testing",C:C)</f>
-        <v>530</v>
+        <v>560</v>
       </c>
       <c r="J11" s="13">
         <f>I11/I12</f>
-        <v>3.9795765129899387E-2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+        <v>4.1953850764159424E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>16</v>
       </c>
@@ -1033,14 +1033,14 @@
       </c>
       <c r="I12" s="15">
         <f>SUM(I6:I11)</f>
-        <v>13318</v>
+        <v>13348</v>
       </c>
       <c r="J12" s="16">
         <f>SUM(J6:J11)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>6</v>
       </c>
@@ -1055,7 +1055,7 @@
       </c>
       <c r="H13" s="2"/>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>6</v>
       </c>
@@ -1069,7 +1069,7 @@
         <v>43509</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>19</v>
       </c>
@@ -1093,7 +1093,7 @@
       <c r="N15" s="42"/>
       <c r="O15" s="42"/>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>19</v>
       </c>
@@ -1131,7 +1131,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>25</v>
       </c>
@@ -1176,7 +1176,7 @@
         <v>3042</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>25</v>
       </c>
@@ -1221,7 +1221,7 @@
         <v>3818</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>25</v>
       </c>
@@ -1255,7 +1255,7 @@
       </c>
       <c r="M19" s="21">
         <f>SUMIFS(C:C,B:B,"Testing",A:A,"Luca")</f>
-        <v>455</v>
+        <v>485</v>
       </c>
       <c r="N19" s="21">
         <f>SUMIFS(C:C,B:B,"Ispezione codice",A:A,"Luca")</f>
@@ -1263,10 +1263,10 @@
       </c>
       <c r="O19" s="22">
         <f>SUM(I19:N19)</f>
-        <v>2633</v>
-      </c>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
+        <v>2663</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>25</v>
       </c>
@@ -1311,7 +1311,7 @@
         <v>3825</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>25</v>
       </c>
@@ -1345,7 +1345,7 @@
       </c>
       <c r="M21" s="25">
         <f t="shared" si="0"/>
-        <v>132.5</v>
+        <v>140</v>
       </c>
       <c r="N21" s="26">
         <f t="shared" si="0"/>
@@ -1353,10 +1353,10 @@
       </c>
       <c r="O21" s="27">
         <f>SUM(O17:O20)</f>
-        <v>13318</v>
-      </c>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
+        <v>13348</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>16</v>
       </c>
@@ -1370,7 +1370,7 @@
         <v>43487</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
         <v>16</v>
       </c>
@@ -1384,7 +1384,7 @@
         <v>43506</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
         <v>16</v>
       </c>
@@ -1408,7 +1408,7 @@
       <c r="N24" s="43"/>
       <c r="O24" s="43"/>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
         <v>16</v>
       </c>
@@ -1446,7 +1446,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
         <v>16</v>
       </c>
@@ -1491,7 +1491,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
         <v>16</v>
       </c>
@@ -1536,7 +1536,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
         <v>19</v>
       </c>
@@ -1554,11 +1554,11 @@
       </c>
       <c r="I28" s="32">
         <f>I19/O19</f>
-        <v>0.40903911887580707</v>
+        <v>0.40443109275253475</v>
       </c>
       <c r="J28" s="32">
         <f>J19/O19</f>
-        <v>0.32358526395746295</v>
+        <v>0.31993991738640631</v>
       </c>
       <c r="K28" s="32">
         <f>K19/O19</f>
@@ -1566,22 +1566,22 @@
       </c>
       <c r="L28" s="32">
         <f>L19/O19</f>
-        <v>2.2787694644891759E-2</v>
+        <v>2.2530980097634247E-2</v>
       </c>
       <c r="M28" s="32">
         <f>M19/O19</f>
-        <v>0.17280668439042918</v>
+        <v>0.18212542245587682</v>
       </c>
       <c r="N28" s="32">
         <f>N19/O19</f>
-        <v>7.1781238131409034E-2</v>
+        <v>7.097258730754788E-2</v>
       </c>
       <c r="O28" s="33">
         <f>SUM(I28:N28)</f>
-        <v>0.99999999999999989</v>
-      </c>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
         <v>6</v>
       </c>
@@ -1626,7 +1626,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
         <v>25</v>
       </c>
@@ -1644,11 +1644,11 @@
       </c>
       <c r="I30" s="36">
         <f t="shared" ref="I30:N30" si="1">AVERAGE(I26:I29)</f>
-        <v>0.24621181307774853</v>
+        <v>0.24505980654693044</v>
       </c>
       <c r="J30" s="36">
         <f t="shared" si="1"/>
-        <v>0.2048493566208455</v>
+        <v>0.20393801997808134</v>
       </c>
       <c r="K30" s="36">
         <f t="shared" si="1"/>
@@ -1656,22 +1656,22 @@
       </c>
       <c r="L30" s="36">
         <f t="shared" si="1"/>
-        <v>0.39816793301834452</v>
+        <v>0.39810375438153012</v>
       </c>
       <c r="M30" s="36">
         <f t="shared" si="1"/>
-        <v>4.8103631881921016E-2</v>
+        <v>5.0433316398282926E-2</v>
       </c>
       <c r="N30" s="37">
         <f t="shared" si="1"/>
-        <v>6.4041361390621054E-2</v>
+        <v>6.3839198684655762E-2</v>
       </c>
       <c r="O30" s="38">
         <f>SUM(I30:N30)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
         <v>25</v>
       </c>
@@ -1685,7 +1685,7 @@
         <v>43531</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
         <v>25</v>
       </c>
@@ -1699,7 +1699,7 @@
         <v>43532</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
         <v>25</v>
       </c>
@@ -1713,7 +1713,7 @@
         <v>43533</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
         <v>25</v>
       </c>
@@ -1727,7 +1727,7 @@
         <v>43534</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
         <v>6</v>
       </c>
@@ -1741,7 +1741,7 @@
         <v>43546</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
         <v>6</v>
       </c>
@@ -1755,7 +1755,7 @@
         <v>43546</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
         <v>16</v>
       </c>
@@ -1769,7 +1769,7 @@
         <v>43376</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
         <v>16</v>
       </c>
@@ -1783,7 +1783,7 @@
         <v>43407</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
         <v>25</v>
       </c>
@@ -1797,7 +1797,7 @@
         <v>43546</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
         <v>19</v>
       </c>
@@ -1811,7 +1811,7 @@
         <v>43553</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
         <v>25</v>
       </c>
@@ -1825,7 +1825,7 @@
         <v>43553</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
         <v>16</v>
       </c>
@@ -1839,7 +1839,7 @@
         <v>43553</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
         <v>19</v>
       </c>
@@ -1853,7 +1853,7 @@
         <v>43481</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
         <v>19</v>
       </c>
@@ -1867,7 +1867,7 @@
         <v>43442</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
         <v>19</v>
       </c>
@@ -1881,7 +1881,7 @@
         <v>43448</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="5" t="s">
         <v>19</v>
       </c>
@@ -1895,7 +1895,7 @@
         <v>43468</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
         <v>19</v>
       </c>
@@ -1909,7 +1909,7 @@
         <v>43478</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
         <v>6</v>
       </c>
@@ -1923,7 +1923,7 @@
         <v>43449</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="5" t="s">
         <v>6</v>
       </c>
@@ -1937,7 +1937,7 @@
         <v>43450</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="5" t="s">
         <v>19</v>
       </c>
@@ -1951,7 +1951,7 @@
         <v>43558</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="5" t="s">
         <v>25</v>
       </c>
@@ -1965,7 +1965,7 @@
         <v>43558</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="5" t="s">
         <v>6</v>
       </c>
@@ -1979,7 +1979,7 @@
         <v>43558</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="5" t="s">
         <v>25</v>
       </c>
@@ -1993,7 +1993,7 @@
         <v>43559</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="5" t="s">
         <v>19</v>
       </c>
@@ -2007,7 +2007,7 @@
         <v>43571</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="5" t="s">
         <v>25</v>
       </c>
@@ -2021,7 +2021,7 @@
         <v>43571</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="5" t="s">
         <v>19</v>
       </c>
@@ -2035,7 +2035,7 @@
         <v>43572</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="5" t="s">
         <v>19</v>
       </c>
@@ -2049,7 +2049,7 @@
         <v>43574</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="5" t="s">
         <v>6</v>
       </c>
@@ -2063,7 +2063,7 @@
         <v>43577</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="5" t="s">
         <v>6</v>
       </c>
@@ -2077,7 +2077,7 @@
         <v>43578</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="5" t="s">
         <v>25</v>
       </c>
@@ -2091,7 +2091,7 @@
         <v>43578</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="5" t="s">
         <v>6</v>
       </c>
@@ -2105,7 +2105,7 @@
         <v>43581</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="5" t="s">
         <v>6</v>
       </c>
@@ -2119,7 +2119,7 @@
         <v>43584</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="5" t="s">
         <v>6</v>
       </c>
@@ -2133,7 +2133,7 @@
         <v>43585</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="5" t="s">
         <v>19</v>
       </c>
@@ -2147,7 +2147,7 @@
         <v>43585</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="5" t="s">
         <v>19</v>
       </c>
@@ -2161,7 +2161,7 @@
         <v>43587</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="5" t="s">
         <v>16</v>
       </c>
@@ -2175,7 +2175,7 @@
         <v>43587</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="5" t="s">
         <v>16</v>
       </c>
@@ -2189,7 +2189,7 @@
         <v>43587</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="5" t="s">
         <v>16</v>
       </c>
@@ -2203,7 +2203,7 @@
         <v>43587</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="5" t="s">
         <v>16</v>
       </c>
@@ -2217,7 +2217,7 @@
         <v>43588</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="5" t="s">
         <v>25</v>
       </c>
@@ -2231,7 +2231,7 @@
         <v>43588</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="5" t="s">
         <v>25</v>
       </c>
@@ -2245,7 +2245,7 @@
         <v>43589</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="5" t="s">
         <v>16</v>
       </c>
@@ -2259,7 +2259,7 @@
         <v>43589</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="5" t="s">
         <v>25</v>
       </c>
@@ -2273,7 +2273,7 @@
         <v>43590</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="5" t="s">
         <v>16</v>
       </c>
@@ -2287,7 +2287,7 @@
         <v>43590</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="5" t="s">
         <v>6</v>
       </c>
@@ -2301,7 +2301,7 @@
         <v>43593</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="5" t="s">
         <v>25</v>
       </c>
@@ -2315,7 +2315,7 @@
         <v>43593</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="5" t="s">
         <v>19</v>
       </c>
@@ -2329,7 +2329,7 @@
         <v>43593</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="5" t="s">
         <v>16</v>
       </c>
@@ -2343,7 +2343,7 @@
         <v>43593</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="5" t="s">
         <v>25</v>
       </c>
@@ -2357,7 +2357,7 @@
         <v>43593</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="5" t="s">
         <v>19</v>
       </c>
@@ -2371,7 +2371,7 @@
         <v>43593</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="5" t="s">
         <v>16</v>
       </c>
@@ -2385,7 +2385,7 @@
         <v>43593</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="5" t="s">
         <v>16</v>
       </c>
@@ -2399,7 +2399,7 @@
         <v>43594</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="5" t="s">
         <v>25</v>
       </c>
@@ -2413,7 +2413,7 @@
         <v>43594</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="5" t="s">
         <v>6</v>
       </c>
@@ -2427,7 +2427,7 @@
         <v>43598</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" s="5" t="s">
         <v>6</v>
       </c>
@@ -2441,7 +2441,7 @@
         <v>43598</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" s="5" t="s">
         <v>25</v>
       </c>
@@ -2455,7 +2455,7 @@
         <v>43595</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" s="5" t="s">
         <v>16</v>
       </c>
@@ -2469,7 +2469,7 @@
         <v>43595</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" s="5" t="s">
         <v>25</v>
       </c>
@@ -2483,7 +2483,7 @@
         <v>43599</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" s="5" t="s">
         <v>16</v>
       </c>
@@ -2497,7 +2497,7 @@
         <v>43599</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" s="5" t="s">
         <v>6</v>
       </c>
@@ -2511,7 +2511,7 @@
         <v>43600</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" s="5" t="s">
         <v>19</v>
       </c>
@@ -2525,7 +2525,7 @@
         <v>43600</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" s="5" t="s">
         <v>16</v>
       </c>
@@ -2539,7 +2539,7 @@
         <v>43600</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" s="5" t="s">
         <v>25</v>
       </c>
@@ -2553,7 +2553,7 @@
         <v>43600</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" s="5" t="s">
         <v>6</v>
       </c>
@@ -2567,7 +2567,7 @@
         <v>43600</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" s="5" t="s">
         <v>19</v>
       </c>
@@ -2581,7 +2581,7 @@
         <v>43600</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" s="5" t="s">
         <v>16</v>
       </c>
@@ -2595,7 +2595,7 @@
         <v>43600</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" s="5" t="s">
         <v>25</v>
       </c>
@@ -2609,7 +2609,7 @@
         <v>43600</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" s="5" t="s">
         <v>25</v>
       </c>
@@ -2623,7 +2623,7 @@
         <v>43603</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" s="5" t="s">
         <v>16</v>
       </c>
@@ -2637,7 +2637,7 @@
         <v>43603</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" s="5" t="s">
         <v>25</v>
       </c>
@@ -2651,7 +2651,7 @@
         <v>43604</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" s="5" t="s">
         <v>16</v>
       </c>
@@ -2665,7 +2665,7 @@
         <v>43604</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" s="5" t="s">
         <v>16</v>
       </c>
@@ -2679,7 +2679,7 @@
         <v>43604</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" s="5" t="s">
         <v>16</v>
       </c>
@@ -2693,7 +2693,7 @@
         <v>43605</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" s="5" t="s">
         <v>25</v>
       </c>
@@ -2707,7 +2707,7 @@
         <v>43606</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" s="5" t="s">
         <v>6</v>
       </c>
@@ -2721,7 +2721,7 @@
         <v>43607</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" s="5" t="s">
         <v>16</v>
       </c>
@@ -2735,7 +2735,7 @@
         <v>43607</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" s="5" t="s">
         <v>25</v>
       </c>
@@ -2749,7 +2749,7 @@
         <v>43607</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" s="5" t="s">
         <v>6</v>
       </c>
@@ -2763,7 +2763,7 @@
         <v>43607</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" s="5" t="s">
         <v>16</v>
       </c>
@@ -2777,7 +2777,7 @@
         <v>43607</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" s="5" t="s">
         <v>25</v>
       </c>
@@ -2791,7 +2791,7 @@
         <v>43607</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" s="5" t="s">
         <v>16</v>
       </c>
@@ -2805,7 +2805,7 @@
         <v>43607</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" s="5" t="s">
         <v>25</v>
       </c>
@@ -2819,7 +2819,7 @@
         <v>43607</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" s="5" t="s">
         <v>25</v>
       </c>
@@ -2833,7 +2833,7 @@
         <v>43607</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" s="5" t="s">
         <v>6</v>
       </c>
@@ -2847,7 +2847,7 @@
         <v>43608</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" s="5" t="s">
         <v>6</v>
       </c>
@@ -2861,7 +2861,7 @@
         <v>43609</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" s="5" t="s">
         <v>16</v>
       </c>
@@ -2875,7 +2875,7 @@
         <v>43608</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" s="5" t="s">
         <v>25</v>
       </c>
@@ -2889,7 +2889,7 @@
         <v>43608</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" s="5" t="s">
         <v>25</v>
       </c>
@@ -2903,7 +2903,7 @@
         <v>43609</v>
       </c>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" s="5" t="s">
         <v>19</v>
       </c>
@@ -2917,7 +2917,7 @@
         <v>43614</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" s="5" t="s">
         <v>16</v>
       </c>
@@ -2931,7 +2931,7 @@
         <v>43614</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" s="5" t="s">
         <v>6</v>
       </c>
@@ -2945,7 +2945,7 @@
         <v>43614</v>
       </c>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" s="5" t="s">
         <v>19</v>
       </c>
@@ -2959,7 +2959,7 @@
         <v>43614</v>
       </c>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" s="5" t="s">
         <v>16</v>
       </c>
@@ -2973,7 +2973,7 @@
         <v>43614</v>
       </c>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" s="5" t="s">
         <v>6</v>
       </c>
@@ -2987,7 +2987,7 @@
         <v>43614</v>
       </c>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" s="5" t="s">
         <v>25</v>
       </c>
@@ -3001,7 +3001,7 @@
         <v>43614</v>
       </c>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" s="5" t="s">
         <v>6</v>
       </c>
@@ -3015,7 +3015,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" s="5" t="s">
         <v>6</v>
       </c>
@@ -3029,7 +3029,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" s="5" t="s">
         <v>19</v>
       </c>
@@ -3043,7 +3043,7 @@
         <v>43471</v>
       </c>
     </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" s="5" t="s">
         <v>16</v>
       </c>
@@ -3057,7 +3057,7 @@
         <v>43616</v>
       </c>
     </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" s="5" t="s">
         <v>25</v>
       </c>
@@ -3071,7 +3071,7 @@
         <v>43616</v>
       </c>
     </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" s="5" t="s">
         <v>16</v>
       </c>
@@ -3085,7 +3085,7 @@
         <v>43618</v>
       </c>
     </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132" s="5" t="s">
         <v>25</v>
       </c>
@@ -3099,7 +3099,7 @@
         <v>43618</v>
       </c>
     </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133" s="5" t="s">
         <v>25</v>
       </c>
@@ -3113,7 +3113,7 @@
         <v>43530</v>
       </c>
     </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134" s="5" t="s">
         <v>19</v>
       </c>
@@ -3127,7 +3127,7 @@
         <v>43619</v>
       </c>
     </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135" s="5" t="s">
         <v>19</v>
       </c>
@@ -3141,7 +3141,7 @@
         <v>43619</v>
       </c>
     </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136" s="5" t="s">
         <v>19</v>
       </c>
@@ -3155,7 +3155,7 @@
         <v>43619</v>
       </c>
     </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A137" s="5" t="s">
         <v>25</v>
       </c>
@@ -3169,7 +3169,7 @@
         <v>43620</v>
       </c>
     </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A138" s="5" t="s">
         <v>16</v>
       </c>
@@ -3183,7 +3183,7 @@
         <v>43620</v>
       </c>
     </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A139" s="5" t="s">
         <v>25</v>
       </c>
@@ -3197,7 +3197,7 @@
         <v>43620</v>
       </c>
     </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A140" s="5" t="s">
         <v>19</v>
       </c>
@@ -3211,7 +3211,7 @@
         <v>43621</v>
       </c>
     </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A141" s="5" t="s">
         <v>16</v>
       </c>
@@ -3225,7 +3225,7 @@
         <v>43621</v>
       </c>
     </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A142" s="5" t="s">
         <v>6</v>
       </c>
@@ -3239,7 +3239,7 @@
         <v>43621</v>
       </c>
     </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A143" s="5" t="s">
         <v>25</v>
       </c>
@@ -3253,7 +3253,7 @@
         <v>43621</v>
       </c>
     </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A144" s="5" t="s">
         <v>19</v>
       </c>
@@ -3267,7 +3267,7 @@
         <v>43621</v>
       </c>
     </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A145" s="5" t="s">
         <v>16</v>
       </c>
@@ -3281,7 +3281,7 @@
         <v>43621</v>
       </c>
     </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A146" s="5" t="s">
         <v>6</v>
       </c>
@@ -3295,7 +3295,7 @@
         <v>43621</v>
       </c>
     </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A147" s="5" t="s">
         <v>25</v>
       </c>
@@ -3309,7 +3309,7 @@
         <v>43621</v>
       </c>
     </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A148" s="5" t="s">
         <v>16</v>
       </c>
@@ -3323,7 +3323,7 @@
         <v>43621</v>
       </c>
     </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A149" s="5" t="s">
         <v>25</v>
       </c>
@@ -3337,7 +3337,7 @@
         <v>43621</v>
       </c>
     </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A150" s="5" t="s">
         <v>16</v>
       </c>
@@ -3351,7 +3351,7 @@
         <v>43622</v>
       </c>
     </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A151" s="5" t="s">
         <v>25</v>
       </c>
@@ -3365,7 +3365,7 @@
         <v>43622</v>
       </c>
     </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A152" s="5" t="s">
         <v>25</v>
       </c>
@@ -3379,7 +3379,7 @@
         <v>43622</v>
       </c>
     </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A153" s="5" t="s">
         <v>19</v>
       </c>
@@ -3393,7 +3393,7 @@
         <v>43622</v>
       </c>
     </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A154" s="5" t="s">
         <v>19</v>
       </c>
@@ -3407,7 +3407,7 @@
         <v>43622</v>
       </c>
     </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A155" s="5" t="s">
         <v>6</v>
       </c>
@@ -3421,7 +3421,7 @@
         <v>43623</v>
       </c>
     </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A156" s="5" t="s">
         <v>6</v>
       </c>
@@ -3435,7 +3435,7 @@
         <v>43625</v>
       </c>
     </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A157" s="5" t="s">
         <v>6</v>
       </c>
@@ -3449,7 +3449,7 @@
         <v>43625</v>
       </c>
     </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A158" s="5" t="s">
         <v>25</v>
       </c>
@@ -3463,7 +3463,7 @@
         <v>43625</v>
       </c>
     </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A159" s="5" t="s">
         <v>6</v>
       </c>
@@ -3477,7 +3477,7 @@
         <v>43625</v>
       </c>
     </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A160" s="5" t="s">
         <v>25</v>
       </c>
@@ -3491,7 +3491,7 @@
         <v>43626</v>
       </c>
     </row>
-    <row r="161" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A161" s="5" t="s">
         <v>16</v>
       </c>
@@ -3505,7 +3505,7 @@
         <v>43626</v>
       </c>
     </row>
-    <row r="162" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A162" s="5" t="s">
         <v>6</v>
       </c>
@@ -3519,7 +3519,7 @@
         <v>43626</v>
       </c>
     </row>
-    <row r="163" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A163" s="5" t="s">
         <v>6</v>
       </c>
@@ -3533,7 +3533,7 @@
         <v>43626</v>
       </c>
     </row>
-    <row r="164" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A164" s="5" t="s">
         <v>6</v>
       </c>
@@ -3547,7 +3547,7 @@
         <v>43626</v>
       </c>
     </row>
-    <row r="165" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A165" s="5" t="s">
         <v>19</v>
       </c>
@@ -3561,7 +3561,7 @@
         <v>43627</v>
       </c>
     </row>
-    <row r="166" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A166" s="5" t="s">
         <v>16</v>
       </c>
@@ -3575,7 +3575,7 @@
         <v>43627</v>
       </c>
     </row>
-    <row r="167" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A167" s="5" t="s">
         <v>19</v>
       </c>
@@ -3589,7 +3589,7 @@
         <v>43628</v>
       </c>
     </row>
-    <row r="168" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A168" s="5" t="s">
         <v>19</v>
       </c>
@@ -3603,7 +3603,7 @@
         <v>43628</v>
       </c>
     </row>
-    <row r="169" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A169" s="5" t="s">
         <v>19</v>
       </c>
@@ -3617,7 +3617,7 @@
         <v>43628</v>
       </c>
     </row>
-    <row r="170" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A170" s="5" t="s">
         <v>6</v>
       </c>
@@ -3631,11 +3631,367 @@
         <v>43628</v>
       </c>
     </row>
-    <row r="171" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A171" s="5"/>
-      <c r="B171" s="5"/>
-      <c r="C171" s="5"/>
-      <c r="D171" s="5"/>
+    <row r="171" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A171" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B171" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C171" s="5">
+        <v>30</v>
+      </c>
+      <c r="D171" s="39">
+        <v>43628</v>
+      </c>
+    </row>
+    <row r="172" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A172" s="44"/>
+      <c r="B172" s="44"/>
+      <c r="C172" s="44"/>
+      <c r="D172" s="44"/>
+    </row>
+    <row r="173" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A173" s="44"/>
+      <c r="B173" s="44"/>
+      <c r="C173" s="44"/>
+      <c r="D173" s="44"/>
+    </row>
+    <row r="174" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A174" s="44"/>
+      <c r="B174" s="44"/>
+      <c r="C174" s="44"/>
+      <c r="D174" s="44"/>
+    </row>
+    <row r="175" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A175" s="44"/>
+      <c r="B175" s="44"/>
+      <c r="C175" s="44"/>
+      <c r="D175" s="44"/>
+    </row>
+    <row r="176" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A176" s="44"/>
+      <c r="B176" s="44"/>
+      <c r="C176" s="44"/>
+      <c r="D176" s="44"/>
+    </row>
+    <row r="177" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A177" s="44"/>
+      <c r="B177" s="44"/>
+      <c r="C177" s="44"/>
+      <c r="D177" s="44"/>
+    </row>
+    <row r="178" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A178" s="44"/>
+      <c r="B178" s="44"/>
+      <c r="C178" s="44"/>
+      <c r="D178" s="44"/>
+    </row>
+    <row r="179" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A179" s="44"/>
+      <c r="B179" s="44"/>
+      <c r="C179" s="44"/>
+      <c r="D179" s="44"/>
+    </row>
+    <row r="180" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A180" s="44"/>
+      <c r="B180" s="44"/>
+      <c r="C180" s="44"/>
+      <c r="D180" s="44"/>
+    </row>
+    <row r="181" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A181" s="44"/>
+      <c r="B181" s="44"/>
+      <c r="C181" s="44"/>
+      <c r="D181" s="44"/>
+    </row>
+    <row r="182" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A182" s="44"/>
+      <c r="B182" s="44"/>
+      <c r="C182" s="44"/>
+      <c r="D182" s="44"/>
+    </row>
+    <row r="183" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A183" s="44"/>
+      <c r="B183" s="44"/>
+      <c r="C183" s="44"/>
+      <c r="D183" s="44"/>
+    </row>
+    <row r="184" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A184" s="44"/>
+      <c r="B184" s="44"/>
+      <c r="C184" s="44"/>
+      <c r="D184" s="44"/>
+    </row>
+    <row r="185" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A185" s="44"/>
+      <c r="B185" s="44"/>
+      <c r="C185" s="44"/>
+      <c r="D185" s="44"/>
+    </row>
+    <row r="186" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A186" s="44"/>
+      <c r="B186" s="44"/>
+      <c r="C186" s="44"/>
+      <c r="D186" s="44"/>
+    </row>
+    <row r="187" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A187" s="44"/>
+      <c r="B187" s="44"/>
+      <c r="C187" s="44"/>
+      <c r="D187" s="44"/>
+    </row>
+    <row r="188" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A188" s="44"/>
+      <c r="B188" s="44"/>
+      <c r="C188" s="44"/>
+      <c r="D188" s="44"/>
+    </row>
+    <row r="189" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A189" s="44"/>
+      <c r="B189" s="44"/>
+      <c r="C189" s="44"/>
+      <c r="D189" s="44"/>
+    </row>
+    <row r="190" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A190" s="44"/>
+      <c r="B190" s="44"/>
+      <c r="C190" s="44"/>
+      <c r="D190" s="44"/>
+    </row>
+    <row r="191" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A191" s="44"/>
+      <c r="B191" s="44"/>
+      <c r="C191" s="44"/>
+      <c r="D191" s="44"/>
+    </row>
+    <row r="192" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A192" s="44"/>
+      <c r="B192" s="44"/>
+      <c r="C192" s="44"/>
+      <c r="D192" s="44"/>
+    </row>
+    <row r="193" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A193" s="44"/>
+      <c r="B193" s="44"/>
+      <c r="C193" s="44"/>
+      <c r="D193" s="44"/>
+    </row>
+    <row r="194" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A194" s="44"/>
+      <c r="B194" s="44"/>
+      <c r="C194" s="44"/>
+      <c r="D194" s="44"/>
+    </row>
+    <row r="195" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A195" s="44"/>
+      <c r="B195" s="44"/>
+      <c r="C195" s="44"/>
+      <c r="D195" s="44"/>
+    </row>
+    <row r="196" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A196" s="44"/>
+      <c r="B196" s="44"/>
+      <c r="C196" s="44"/>
+      <c r="D196" s="44"/>
+    </row>
+    <row r="197" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A197" s="44"/>
+      <c r="B197" s="44"/>
+      <c r="C197" s="44"/>
+      <c r="D197" s="44"/>
+    </row>
+    <row r="198" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A198" s="44"/>
+      <c r="B198" s="44"/>
+      <c r="C198" s="44"/>
+      <c r="D198" s="44"/>
+    </row>
+    <row r="199" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A199" s="44"/>
+      <c r="B199" s="44"/>
+      <c r="C199" s="44"/>
+      <c r="D199" s="44"/>
+    </row>
+    <row r="200" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A200" s="44"/>
+      <c r="B200" s="44"/>
+      <c r="C200" s="44"/>
+      <c r="D200" s="44"/>
+    </row>
+    <row r="201" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A201" s="44"/>
+      <c r="B201" s="44"/>
+      <c r="C201" s="44"/>
+      <c r="D201" s="44"/>
+    </row>
+    <row r="202" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A202" s="44"/>
+      <c r="B202" s="44"/>
+      <c r="C202" s="44"/>
+      <c r="D202" s="44"/>
+    </row>
+    <row r="203" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A203" s="44"/>
+      <c r="B203" s="44"/>
+      <c r="C203" s="44"/>
+      <c r="D203" s="44"/>
+    </row>
+    <row r="204" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A204" s="44"/>
+      <c r="B204" s="44"/>
+      <c r="C204" s="44"/>
+      <c r="D204" s="44"/>
+    </row>
+    <row r="205" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A205" s="44"/>
+      <c r="B205" s="44"/>
+      <c r="C205" s="44"/>
+      <c r="D205" s="44"/>
+    </row>
+    <row r="206" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A206" s="44"/>
+      <c r="B206" s="44"/>
+      <c r="C206" s="44"/>
+      <c r="D206" s="44"/>
+    </row>
+    <row r="207" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A207" s="44"/>
+      <c r="B207" s="44"/>
+      <c r="C207" s="44"/>
+      <c r="D207" s="44"/>
+    </row>
+    <row r="208" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A208" s="44"/>
+      <c r="B208" s="44"/>
+      <c r="C208" s="44"/>
+      <c r="D208" s="44"/>
+    </row>
+    <row r="209" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A209" s="44"/>
+      <c r="B209" s="44"/>
+      <c r="C209" s="44"/>
+      <c r="D209" s="44"/>
+    </row>
+    <row r="210" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A210" s="44"/>
+      <c r="B210" s="44"/>
+      <c r="C210" s="44"/>
+      <c r="D210" s="44"/>
+    </row>
+    <row r="211" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A211" s="44"/>
+      <c r="B211" s="44"/>
+      <c r="C211" s="44"/>
+      <c r="D211" s="44"/>
+    </row>
+    <row r="212" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A212" s="44"/>
+      <c r="B212" s="44"/>
+      <c r="C212" s="44"/>
+      <c r="D212" s="44"/>
+    </row>
+    <row r="213" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A213" s="44"/>
+      <c r="B213" s="44"/>
+      <c r="C213" s="44"/>
+      <c r="D213" s="44"/>
+    </row>
+    <row r="214" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A214" s="44"/>
+      <c r="B214" s="44"/>
+      <c r="C214" s="44"/>
+      <c r="D214" s="44"/>
+    </row>
+    <row r="215" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A215" s="44"/>
+      <c r="B215" s="44"/>
+      <c r="C215" s="44"/>
+      <c r="D215" s="44"/>
+    </row>
+    <row r="216" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A216" s="44"/>
+      <c r="B216" s="44"/>
+      <c r="C216" s="44"/>
+      <c r="D216" s="44"/>
+    </row>
+    <row r="217" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A217" s="44"/>
+      <c r="B217" s="44"/>
+      <c r="C217" s="44"/>
+      <c r="D217" s="44"/>
+    </row>
+    <row r="218" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A218" s="44"/>
+      <c r="B218" s="44"/>
+      <c r="C218" s="44"/>
+      <c r="D218" s="44"/>
+    </row>
+    <row r="219" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A219" s="44"/>
+      <c r="B219" s="44"/>
+      <c r="C219" s="44"/>
+      <c r="D219" s="44"/>
+    </row>
+    <row r="220" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A220" s="44"/>
+      <c r="B220" s="44"/>
+      <c r="C220" s="44"/>
+      <c r="D220" s="44"/>
+    </row>
+    <row r="221" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A221" s="44"/>
+      <c r="B221" s="44"/>
+      <c r="C221" s="44"/>
+      <c r="D221" s="44"/>
+    </row>
+    <row r="222" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A222" s="44"/>
+      <c r="B222" s="44"/>
+      <c r="C222" s="44"/>
+      <c r="D222" s="44"/>
+    </row>
+    <row r="223" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A223" s="44"/>
+      <c r="B223" s="44"/>
+      <c r="C223" s="44"/>
+      <c r="D223" s="44"/>
+    </row>
+    <row r="224" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A224" s="44"/>
+      <c r="B224" s="44"/>
+      <c r="C224" s="44"/>
+      <c r="D224" s="44"/>
+    </row>
+    <row r="225" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A225" s="44"/>
+      <c r="B225" s="44"/>
+      <c r="C225" s="44"/>
+      <c r="D225" s="44"/>
+    </row>
+    <row r="226" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A226" s="44"/>
+      <c r="B226" s="44"/>
+      <c r="C226" s="44"/>
+      <c r="D226" s="44"/>
+    </row>
+    <row r="227" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A227" s="44"/>
+      <c r="B227" s="44"/>
+      <c r="C227" s="44"/>
+      <c r="D227" s="44"/>
+    </row>
+    <row r="228" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A228" s="44"/>
+      <c r="B228" s="44"/>
+      <c r="C228" s="44"/>
+      <c r="D228" s="44"/>
+    </row>
+    <row r="229" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A229" s="44"/>
+      <c r="B229" s="44"/>
+      <c r="C229" s="44"/>
+      <c r="D229" s="44"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
Fix bottone indietro da show e da modifica
</commit_message>
<xml_diff>
--- a/Documentazione/Attività sul progetto/DocAttivProg.xlsx
+++ b/Documentazione/Attività sul progetto/DocAttivProg.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="31">
   <si>
     <t>Le categorie sono: Ispezione Codice, Documenti di progetto, Documenti di processo, Manuale, Sviluppo, Testing</t>
   </si>
@@ -780,7 +780,7 @@
   <dimension ref="A1:O229"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A151" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F177" sqref="F177"/>
+      <selection activeCell="H171" sqref="H171"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -887,7 +887,7 @@
       </c>
       <c r="J6" s="10">
         <f>I6/I12</f>
-        <v>6.1601489757914338E-2</v>
+        <v>6.1423054070112892E-2</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
@@ -912,7 +912,7 @@
       </c>
       <c r="J7" s="10">
         <f>(I7/I12)</f>
-        <v>0.2231657355679702</v>
+        <v>0.22251931075460488</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
@@ -937,7 +937,7 @@
       </c>
       <c r="J8" s="10">
         <f>I8/I12</f>
-        <v>0.18145251396648043</v>
+        <v>0.18092691622103388</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
@@ -962,7 +962,7 @@
       </c>
       <c r="J9" s="10">
         <f>I9/I12</f>
-        <v>3.5009310986964616E-2</v>
+        <v>3.490790255496138E-2</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
@@ -983,11 +983,11 @@
       </c>
       <c r="I10" s="9">
         <f>SUMIF(B:B,"Sviluppo",C:C)</f>
-        <v>6136</v>
+        <v>6175</v>
       </c>
       <c r="J10" s="10">
         <f>I10/I12</f>
-        <v>0.45705772811918061</v>
+        <v>0.45863042186571601</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
@@ -1012,7 +1012,7 @@
       </c>
       <c r="J11" s="13">
         <f>I11/I12</f>
-        <v>4.1713221601489756E-2</v>
+        <v>4.1592394533571005E-2</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
@@ -1033,7 +1033,7 @@
       </c>
       <c r="I12" s="15">
         <f>SUM(I6:I11)</f>
-        <v>13425</v>
+        <v>13464</v>
       </c>
       <c r="J12" s="16">
         <f>SUM(J6:J11)</f>
@@ -1251,7 +1251,7 @@
       </c>
       <c r="L19" s="21">
         <f>SUMIFS(C:C,B:B,"Sviluppo",A:A,"Luca")</f>
-        <v>137</v>
+        <v>176</v>
       </c>
       <c r="M19" s="21">
         <f>SUMIFS(C:C,B:B,"Testing",A:A,"Luca")</f>
@@ -1263,7 +1263,7 @@
       </c>
       <c r="O19" s="22">
         <f>SUM(I19:N19)</f>
-        <v>2740</v>
+        <v>2779</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
@@ -1341,7 +1341,7 @@
       </c>
       <c r="L21" s="25">
         <f t="shared" si="0"/>
-        <v>1534</v>
+        <v>1543.75</v>
       </c>
       <c r="M21" s="25">
         <f t="shared" si="0"/>
@@ -1353,7 +1353,7 @@
       </c>
       <c r="O21" s="27">
         <f>SUM(O17:O20)</f>
-        <v>13425</v>
+        <v>13464</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
@@ -1554,11 +1554,11 @@
       </c>
       <c r="I28" s="32">
         <f>I19/O19</f>
-        <v>0.39306569343065695</v>
+        <v>0.38754947822957897</v>
       </c>
       <c r="J28" s="32">
         <f>J19/O19</f>
-        <v>0.31094890510948903</v>
+        <v>0.30658510255487587</v>
       </c>
       <c r="K28" s="32">
         <f>K19/O19</f>
@@ -1566,15 +1566,15 @@
       </c>
       <c r="L28" s="32">
         <f>L19/O19</f>
-        <v>0.05</v>
+        <v>6.333213386110112E-2</v>
       </c>
       <c r="M28" s="32">
         <f>M19/O19</f>
-        <v>0.177007299270073</v>
+        <v>0.17452320978769342</v>
       </c>
       <c r="N28" s="32">
         <f>N19/O19</f>
-        <v>6.8978102189781024E-2</v>
+        <v>6.8010075566750636E-2</v>
       </c>
       <c r="O28" s="33">
         <f>SUM(I28:N28)</f>
@@ -1644,11 +1644,11 @@
       </c>
       <c r="I30" s="36">
         <f t="shared" ref="I30:N30" si="1">AVERAGE(I26:I29)</f>
-        <v>0.24221845671646097</v>
+        <v>0.24083940291619149</v>
       </c>
       <c r="J30" s="36">
         <f t="shared" si="1"/>
-        <v>0.201690266908852</v>
+        <v>0.2005993162701987</v>
       </c>
       <c r="K30" s="36">
         <f t="shared" si="1"/>
@@ -1656,15 +1656,15 @@
       </c>
       <c r="L30" s="36">
         <f t="shared" si="1"/>
-        <v>0.4049710093571216</v>
+        <v>0.40830404282239685</v>
       </c>
       <c r="M30" s="36">
         <f t="shared" si="1"/>
-        <v>4.9153785601831979E-2</v>
+        <v>4.8532763231237078E-2</v>
       </c>
       <c r="N30" s="37">
         <f t="shared" si="1"/>
-        <v>6.3340577405214066E-2</v>
+        <v>6.3098570749456462E-2</v>
       </c>
       <c r="O30" s="38">
         <f>SUM(I30:N30)</f>
@@ -3660,10 +3660,18 @@
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A173" s="41"/>
-      <c r="B173" s="41"/>
-      <c r="C173" s="41"/>
-      <c r="D173" s="41"/>
+      <c r="A173" s="41" t="s">
+        <v>19</v>
+      </c>
+      <c r="B173" s="41" t="s">
+        <v>15</v>
+      </c>
+      <c r="C173" s="41">
+        <v>39</v>
+      </c>
+      <c r="D173" s="40">
+        <v>43629</v>
+      </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A174" s="41"/>

</xml_diff>

<commit_message>
Test per le cose fixate
</commit_message>
<xml_diff>
--- a/Documentazione/Attività sul progetto/DocAttivProg.xlsx
+++ b/Documentazione/Attività sul progetto/DocAttivProg.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="31">
   <si>
     <t>Le categorie sono: Ispezione Codice, Documenti di progetto, Documenti di processo, Manuale, Sviluppo, Testing</t>
   </si>
@@ -780,7 +780,7 @@
   <dimension ref="A1:O229"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A151" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H171" sqref="H171"/>
+      <selection activeCell="I170" sqref="I170"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -887,7 +887,7 @@
       </c>
       <c r="J6" s="10">
         <f>I6/I12</f>
-        <v>6.1423054070112892E-2</v>
+        <v>6.1241113744075829E-2</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
@@ -912,7 +912,7 @@
       </c>
       <c r="J7" s="10">
         <f>(I7/I12)</f>
-        <v>0.22251931075460488</v>
+        <v>0.22186018957345971</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
@@ -937,7 +937,7 @@
       </c>
       <c r="J8" s="10">
         <f>I8/I12</f>
-        <v>0.18092691622103388</v>
+        <v>0.18039099526066352</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
@@ -962,7 +962,7 @@
       </c>
       <c r="J9" s="10">
         <f>I9/I12</f>
-        <v>3.490790255496138E-2</v>
+        <v>3.4804502369668248E-2</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
@@ -987,7 +987,7 @@
       </c>
       <c r="J10" s="10">
         <f>I10/I12</f>
-        <v>0.45863042186571601</v>
+        <v>0.45727191943127959</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
@@ -1008,11 +1008,11 @@
       </c>
       <c r="I11" s="12">
         <f>SUMIF(B:B,"Testing",C:C)</f>
-        <v>560</v>
+        <v>600</v>
       </c>
       <c r="J11" s="13">
         <f>I11/I12</f>
-        <v>4.1592394533571005E-2</v>
+        <v>4.4431279620853081E-2</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
@@ -1033,7 +1033,7 @@
       </c>
       <c r="I12" s="15">
         <f>SUM(I6:I11)</f>
-        <v>13464</v>
+        <v>13504</v>
       </c>
       <c r="J12" s="16">
         <f>SUM(J6:J11)</f>
@@ -1255,7 +1255,7 @@
       </c>
       <c r="M19" s="21">
         <f>SUMIFS(C:C,B:B,"Testing",A:A,"Luca")</f>
-        <v>485</v>
+        <v>525</v>
       </c>
       <c r="N19" s="21">
         <f>SUMIFS(C:C,B:B,"Ispezione codice",A:A,"Luca")</f>
@@ -1263,7 +1263,7 @@
       </c>
       <c r="O19" s="22">
         <f>SUM(I19:N19)</f>
-        <v>2779</v>
+        <v>2819</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
@@ -1345,7 +1345,7 @@
       </c>
       <c r="M21" s="25">
         <f t="shared" si="0"/>
-        <v>140</v>
+        <v>150</v>
       </c>
       <c r="N21" s="26">
         <f t="shared" si="0"/>
@@ -1353,7 +1353,7 @@
       </c>
       <c r="O21" s="27">
         <f>SUM(O17:O20)</f>
-        <v>13464</v>
+        <v>13504</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
@@ -1554,11 +1554,11 @@
       </c>
       <c r="I28" s="32">
         <f>I19/O19</f>
-        <v>0.38754947822957897</v>
+        <v>0.382050372472508</v>
       </c>
       <c r="J28" s="32">
         <f>J19/O19</f>
-        <v>0.30658510255487587</v>
+        <v>0.30223483504788934</v>
       </c>
       <c r="K28" s="32">
         <f>K19/O19</f>
@@ -1566,15 +1566,15 @@
       </c>
       <c r="L28" s="32">
         <f>L19/O19</f>
-        <v>6.333213386110112E-2</v>
+        <v>6.2433487052146151E-2</v>
       </c>
       <c r="M28" s="32">
         <f>M19/O19</f>
-        <v>0.17452320978769342</v>
+        <v>0.18623625399077687</v>
       </c>
       <c r="N28" s="32">
         <f>N19/O19</f>
-        <v>6.8010075566750636E-2</v>
+        <v>6.7045051436679673E-2</v>
       </c>
       <c r="O28" s="33">
         <f>SUM(I28:N28)</f>
@@ -1644,11 +1644,11 @@
       </c>
       <c r="I30" s="36">
         <f t="shared" ref="I30:N30" si="1">AVERAGE(I26:I29)</f>
-        <v>0.24083940291619149</v>
+        <v>0.23946462647692374</v>
       </c>
       <c r="J30" s="36">
         <f t="shared" si="1"/>
-        <v>0.2005993162701987</v>
+        <v>0.19951174939345209</v>
       </c>
       <c r="K30" s="36">
         <f t="shared" si="1"/>
@@ -1656,15 +1656,15 @@
       </c>
       <c r="L30" s="36">
         <f t="shared" si="1"/>
-        <v>0.40830404282239685</v>
+        <v>0.40807938112015807</v>
       </c>
       <c r="M30" s="36">
         <f t="shared" si="1"/>
-        <v>4.8532763231237078E-2</v>
+        <v>5.1461024282007939E-2</v>
       </c>
       <c r="N30" s="37">
         <f t="shared" si="1"/>
-        <v>6.3098570749456462E-2</v>
+        <v>6.2857314716938728E-2</v>
       </c>
       <c r="O30" s="38">
         <f>SUM(I30:N30)</f>
@@ -3674,10 +3674,18 @@
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A174" s="41"/>
-      <c r="B174" s="41"/>
-      <c r="C174" s="41"/>
-      <c r="D174" s="41"/>
+      <c r="A174" s="41" t="s">
+        <v>19</v>
+      </c>
+      <c r="B174" s="41" t="s">
+        <v>17</v>
+      </c>
+      <c r="C174" s="41">
+        <v>40</v>
+      </c>
+      <c r="D174" s="40">
+        <v>43629</v>
+      </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A175" s="41"/>

</xml_diff>

<commit_message>
Modifiche errori nei VerbInt, modifiche al CM e al Manuale. Eliminazione file di Test dummy
</commit_message>
<xml_diff>
--- a/Documentazione/Attività sul progetto/DocAttivProg.xlsx
+++ b/Documentazione/Attività sul progetto/DocAttivProg.xlsx
@@ -1,21 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LUCA\Documents\Universita\INGEGNERIA DEL SOFTWARE\Progetto\Documentazione\Attività sul progetto\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\UniUD\Laurea Magistrale\Ingegneria del Software 2\Progetto-Ingegneria-Del-Sw-2\Documentazione\Attività sul progetto\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46941D95-569D-4FA9-A638-7BA3456A6A8B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913" iterateDelta="1E-4"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
     </ext>
@@ -24,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="31">
   <si>
     <t>Le categorie sono: Ispezione Codice, Documenti di progetto, Documenti di processo, Manuale, Sviluppo, Testing</t>
   </si>
@@ -122,10 +129,9 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yyyy"/>
-    <numFmt numFmtId="165" formatCode="mm/dd/yy"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -381,8 +387,6 @@
     <xf numFmtId="9" fontId="0" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -392,6 +396,8 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -740,39 +746,39 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O230"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A161" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F178" sqref="F178"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.5703125" customWidth="1"/>
-    <col min="2" max="2" width="23.42578125" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" customWidth="1"/>
-    <col min="4" max="4" width="10.85546875" customWidth="1"/>
-    <col min="5" max="7" width="8.7109375" customWidth="1"/>
-    <col min="8" max="8" width="26.28515625" customWidth="1"/>
-    <col min="9" max="11" width="17.28515625" customWidth="1"/>
-    <col min="12" max="14" width="17.42578125" customWidth="1"/>
-    <col min="15" max="1025" width="8.7109375" customWidth="1"/>
+    <col min="1" max="1" width="15.5546875" customWidth="1"/>
+    <col min="2" max="2" width="23.44140625" customWidth="1"/>
+    <col min="3" max="3" width="15.5546875" customWidth="1"/>
+    <col min="4" max="4" width="10.88671875" customWidth="1"/>
+    <col min="5" max="7" width="8.6640625" customWidth="1"/>
+    <col min="8" max="8" width="26.33203125" customWidth="1"/>
+    <col min="9" max="11" width="17.33203125" customWidth="1"/>
+    <col min="12" max="14" width="17.44140625" customWidth="1"/>
+    <col min="15" max="1025" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="F1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="F2" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
@@ -787,7 +793,7 @@
       </c>
       <c r="H3" s="2"/>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>6</v>
       </c>
@@ -797,16 +803,16 @@
       <c r="C4" s="5">
         <v>98</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4" s="43">
         <v>43484</v>
       </c>
-      <c r="H4" s="42" t="s">
+      <c r="H4" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="I4" s="42"/>
-      <c r="J4" s="42"/>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="I4" s="40"/>
+      <c r="J4" s="40"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>6</v>
       </c>
@@ -816,7 +822,7 @@
       <c r="C5" s="5">
         <v>149</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="43">
         <v>43493</v>
       </c>
       <c r="H5" s="7" t="s">
@@ -829,7 +835,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>6</v>
       </c>
@@ -839,7 +845,7 @@
       <c r="C6" s="5">
         <v>135</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6" s="43">
         <v>43494</v>
       </c>
       <c r="H6" s="9" t="s">
@@ -851,10 +857,10 @@
       </c>
       <c r="J6" s="11">
         <f>I6/I12</f>
-        <v>6.7071847189060133E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+        <v>6.672905269219695E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>6</v>
       </c>
@@ -864,7 +870,7 @@
       <c r="C7" s="5">
         <v>53</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D7" s="43">
         <v>43494</v>
       </c>
       <c r="H7" s="9" t="s">
@@ -872,14 +878,14 @@
       </c>
       <c r="I7" s="10">
         <f>SUMIF(B:B,"Documenti di progetto",C:C)</f>
-        <v>2996</v>
+        <v>3036</v>
       </c>
       <c r="J7" s="11">
         <f>(I7/I12)</f>
-        <v>0.21677157948050069</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+        <v>0.2185430463576159</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>6</v>
       </c>
@@ -889,7 +895,7 @@
       <c r="C8" s="5">
         <v>87</v>
       </c>
-      <c r="D8" s="6">
+      <c r="D8" s="43">
         <v>43495</v>
       </c>
       <c r="H8" s="9" t="s">
@@ -897,14 +903,14 @@
       </c>
       <c r="I8" s="10">
         <f>SUMIF(B:B,"Documenti di processo",C:C)</f>
-        <v>2496</v>
+        <v>2527</v>
       </c>
       <c r="J8" s="11">
         <f>I8/I12</f>
-        <v>0.18059474712394183</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+        <v>0.18190325367117766</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>6</v>
       </c>
@@ -914,7 +920,7 @@
       <c r="C9" s="5">
         <v>74</v>
       </c>
-      <c r="D9" s="6">
+      <c r="D9" s="43">
         <v>43495</v>
       </c>
       <c r="H9" s="9" t="s">
@@ -926,10 +932,10 @@
       </c>
       <c r="J9" s="11">
         <f>I9/I12</f>
-        <v>3.4006222415165328E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+        <v>3.3832421537575583E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>6</v>
       </c>
@@ -939,7 +945,7 @@
       <c r="C10" s="5">
         <v>32</v>
       </c>
-      <c r="D10" s="6">
+      <c r="D10" s="43">
         <v>43499</v>
       </c>
       <c r="H10" s="9" t="s">
@@ -951,10 +957,10 @@
       </c>
       <c r="J10" s="11">
         <f>I10/I12</f>
-        <v>0.45669633166919904</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+        <v>0.45436222286207889</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>16</v>
       </c>
@@ -964,7 +970,7 @@
       <c r="C11" s="5">
         <v>75</v>
       </c>
-      <c r="D11" s="6">
+      <c r="D11" s="43">
         <v>43497</v>
       </c>
       <c r="H11" s="12" t="s">
@@ -976,10 +982,10 @@
       </c>
       <c r="J11" s="14">
         <f>I11/I12</f>
-        <v>4.4859272122132983E-2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+        <v>4.4630002879355021E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>16</v>
       </c>
@@ -989,7 +995,7 @@
       <c r="C12" s="5">
         <v>55</v>
       </c>
-      <c r="D12" s="6">
+      <c r="D12" s="43">
         <v>43503</v>
       </c>
       <c r="H12" s="15" t="s">
@@ -997,14 +1003,14 @@
       </c>
       <c r="I12" s="16">
         <f>SUM(I6:I11)</f>
-        <v>13821</v>
+        <v>13892</v>
       </c>
       <c r="J12" s="17">
         <f>SUM(J6:J11)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
         <v>6</v>
       </c>
@@ -1014,12 +1020,12 @@
       <c r="C13" s="5">
         <v>127</v>
       </c>
-      <c r="D13" s="6">
+      <c r="D13" s="43">
         <v>43505</v>
       </c>
       <c r="H13" s="2"/>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
         <v>6</v>
       </c>
@@ -1029,11 +1035,11 @@
       <c r="C14" s="5">
         <v>24</v>
       </c>
-      <c r="D14" s="6">
+      <c r="D14" s="43">
         <v>43509</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
         <v>19</v>
       </c>
@@ -1043,21 +1049,21 @@
       <c r="C15" s="5">
         <v>195</v>
       </c>
-      <c r="D15" s="6">
+      <c r="D15" s="43">
         <v>43521</v>
       </c>
-      <c r="H15" s="43" t="s">
+      <c r="H15" s="41" t="s">
         <v>20</v>
       </c>
-      <c r="I15" s="43"/>
-      <c r="J15" s="43"/>
-      <c r="K15" s="43"/>
-      <c r="L15" s="43"/>
-      <c r="M15" s="43"/>
-      <c r="N15" s="43"/>
-      <c r="O15" s="43"/>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="I15" s="41"/>
+      <c r="J15" s="41"/>
+      <c r="K15" s="41"/>
+      <c r="L15" s="41"/>
+      <c r="M15" s="41"/>
+      <c r="N15" s="41"/>
+      <c r="O15" s="41"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
         <v>19</v>
       </c>
@@ -1067,7 +1073,7 @@
       <c r="C16" s="5">
         <v>105</v>
       </c>
-      <c r="D16" s="6">
+      <c r="D16" s="43">
         <v>43523</v>
       </c>
       <c r="H16" s="18" t="s">
@@ -1095,7 +1101,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
         <v>25</v>
       </c>
@@ -1105,7 +1111,7 @@
       <c r="C17" s="5">
         <v>30</v>
       </c>
-      <c r="D17" s="6">
+      <c r="D17" s="43">
         <v>43519</v>
       </c>
       <c r="H17" s="21" t="s">
@@ -1113,11 +1119,11 @@
       </c>
       <c r="I17" s="22">
         <f>SUMIFS(C:C,B:B,"Documenti di progetto",A:A,"Giovanni")</f>
-        <v>1100</v>
+        <v>1140</v>
       </c>
       <c r="J17" s="22">
         <f>SUMIFS(C:C,B:B,"Documenti di processo",A:A,"Giovanni")</f>
-        <v>1212</v>
+        <v>1243</v>
       </c>
       <c r="K17" s="22">
         <f>SUMIFS(C:C,B:B,"Manuale",A:A,"Giovanni")</f>
@@ -1137,10 +1143,10 @@
       </c>
       <c r="O17" s="23">
         <f>SUM(I17:N17)</f>
-        <v>3042</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+        <v>3113</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
         <v>25</v>
       </c>
@@ -1150,7 +1156,7 @@
       <c r="C18" s="5">
         <v>100</v>
       </c>
-      <c r="D18" s="6">
+      <c r="D18" s="43">
         <v>43520</v>
       </c>
       <c r="H18" s="21" t="s">
@@ -1185,7 +1191,7 @@
         <v>3955</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
         <v>25</v>
       </c>
@@ -1195,7 +1201,7 @@
       <c r="C19" s="5">
         <v>125</v>
       </c>
-      <c r="D19" s="6">
+      <c r="D19" s="43">
         <v>43522</v>
       </c>
       <c r="H19" s="21" t="s">
@@ -1230,7 +1236,7 @@
         <v>2999</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
         <v>25</v>
       </c>
@@ -1240,7 +1246,7 @@
       <c r="C20" s="5">
         <v>170</v>
       </c>
-      <c r="D20" s="6">
+      <c r="D20" s="43">
         <v>43523</v>
       </c>
       <c r="H20" s="21" t="s">
@@ -1275,7 +1281,7 @@
         <v>3825</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
         <v>25</v>
       </c>
@@ -1285,7 +1291,7 @@
       <c r="C21" s="5">
         <v>65</v>
       </c>
-      <c r="D21" s="6">
+      <c r="D21" s="43">
         <v>43524</v>
       </c>
       <c r="H21" s="24" t="s">
@@ -1293,11 +1299,11 @@
       </c>
       <c r="I21" s="25">
         <f t="shared" ref="I21:N21" si="0">AVERAGE(I17:I20)</f>
-        <v>749</v>
+        <v>759</v>
       </c>
       <c r="J21" s="26">
         <f t="shared" si="0"/>
-        <v>624</v>
+        <v>631.75</v>
       </c>
       <c r="K21" s="26">
         <f t="shared" si="0"/>
@@ -1317,10 +1323,10 @@
       </c>
       <c r="O21" s="28">
         <f>SUM(O17:O20)</f>
-        <v>13821</v>
-      </c>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+        <v>13892</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
         <v>16</v>
       </c>
@@ -1330,11 +1336,11 @@
       <c r="C22" s="5">
         <v>60</v>
       </c>
-      <c r="D22" s="6">
+      <c r="D22" s="43">
         <v>43487</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A23" s="5" t="s">
         <v>16</v>
       </c>
@@ -1344,11 +1350,11 @@
       <c r="C23" s="5">
         <v>103</v>
       </c>
-      <c r="D23" s="6">
+      <c r="D23" s="43">
         <v>43506</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
         <v>16</v>
       </c>
@@ -1358,21 +1364,21 @@
       <c r="C24" s="5">
         <v>100</v>
       </c>
-      <c r="D24" s="6">
+      <c r="D24" s="43">
         <v>43520</v>
       </c>
-      <c r="H24" s="44" t="s">
+      <c r="H24" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="I24" s="44"/>
-      <c r="J24" s="44"/>
-      <c r="K24" s="44"/>
-      <c r="L24" s="44"/>
-      <c r="M24" s="44"/>
-      <c r="N24" s="44"/>
-      <c r="O24" s="44"/>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="I24" s="42"/>
+      <c r="J24" s="42"/>
+      <c r="K24" s="42"/>
+      <c r="L24" s="42"/>
+      <c r="M24" s="42"/>
+      <c r="N24" s="42"/>
+      <c r="O24" s="42"/>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A25" s="5" t="s">
         <v>16</v>
       </c>
@@ -1382,7 +1388,7 @@
       <c r="C25" s="5">
         <v>170</v>
       </c>
-      <c r="D25" s="6">
+      <c r="D25" s="43">
         <v>43523</v>
       </c>
       <c r="H25" s="29" t="s">
@@ -1410,7 +1416,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="s">
         <v>16</v>
       </c>
@@ -1420,7 +1426,7 @@
       <c r="C26" s="5">
         <v>45</v>
       </c>
-      <c r="D26" s="6">
+      <c r="D26" s="43">
         <v>43524</v>
       </c>
       <c r="H26" s="32" t="s">
@@ -1428,15 +1434,15 @@
       </c>
       <c r="I26" s="33">
         <f>I17/O17</f>
-        <v>0.36160420775805391</v>
+        <v>0.36620623193061358</v>
       </c>
       <c r="J26" s="33">
         <f>J17/O17</f>
-        <v>0.39842209072978302</v>
+        <v>0.39929328621908128</v>
       </c>
       <c r="K26" s="33">
         <f>K17/O17</f>
-        <v>0.15450361604207757</v>
+        <v>0.15097976228718279</v>
       </c>
       <c r="L26" s="33">
         <f>L17/O17</f>
@@ -1448,14 +1454,14 @@
       </c>
       <c r="N26" s="33">
         <f>N17/O17</f>
-        <v>8.5470085470085472E-2</v>
+        <v>8.3520719563122389E-2</v>
       </c>
       <c r="O26" s="34">
         <f>SUM(I26:N26)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A27" s="5" t="s">
         <v>16</v>
       </c>
@@ -1465,7 +1471,7 @@
       <c r="C27" s="5">
         <v>25</v>
       </c>
-      <c r="D27" s="6">
+      <c r="D27" s="43">
         <v>43530</v>
       </c>
       <c r="H27" s="32" t="s">
@@ -1500,7 +1506,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A28" s="5" t="s">
         <v>19</v>
       </c>
@@ -1510,7 +1516,7 @@
       <c r="C28" s="5">
         <v>15</v>
       </c>
-      <c r="D28" s="6">
+      <c r="D28" s="43">
         <v>43532</v>
       </c>
       <c r="H28" s="32" t="s">
@@ -1545,7 +1551,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A29" s="5" t="s">
         <v>6</v>
       </c>
@@ -1555,7 +1561,7 @@
       <c r="C29" s="5">
         <v>47</v>
       </c>
-      <c r="D29" s="6">
+      <c r="D29" s="43">
         <v>43532</v>
       </c>
       <c r="H29" s="32" t="s">
@@ -1590,7 +1596,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A30" s="5" t="s">
         <v>25</v>
       </c>
@@ -1600,7 +1606,7 @@
       <c r="C30" s="5">
         <v>15</v>
       </c>
-      <c r="D30" s="6">
+      <c r="D30" s="43">
         <v>43532</v>
       </c>
       <c r="H30" s="36" t="s">
@@ -1608,15 +1614,15 @@
       </c>
       <c r="I30" s="37">
         <f t="shared" ref="I30:N30" si="1">AVERAGE(I26:I29)</f>
-        <v>0.23332368699252548</v>
+        <v>0.23447419303566541</v>
       </c>
       <c r="J30" s="37">
         <f t="shared" si="1"/>
-        <v>0.19933875469877962</v>
+        <v>0.19955655357110416</v>
       </c>
       <c r="K30" s="37">
         <f t="shared" si="1"/>
-        <v>3.8625904010519393E-2</v>
+        <v>3.7744940571795699E-2</v>
       </c>
       <c r="L30" s="37">
         <f t="shared" si="1"/>
@@ -1628,14 +1634,14 @@
       </c>
       <c r="N30" s="38">
         <f t="shared" si="1"/>
-        <v>6.9758728986788532E-2</v>
+        <v>6.9271387510047744E-2</v>
       </c>
       <c r="O30" s="39">
         <f>SUM(I30:N30)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A31" s="5" t="s">
         <v>25</v>
       </c>
@@ -1645,11 +1651,11 @@
       <c r="C31" s="5">
         <v>55</v>
       </c>
-      <c r="D31" s="6">
+      <c r="D31" s="43">
         <v>43531</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A32" s="5" t="s">
         <v>25</v>
       </c>
@@ -1659,11 +1665,11 @@
       <c r="C32" s="5">
         <v>68</v>
       </c>
-      <c r="D32" s="6">
+      <c r="D32" s="43">
         <v>43532</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="5" t="s">
         <v>25</v>
       </c>
@@ -1673,11 +1679,11 @@
       <c r="C33" s="5">
         <v>129</v>
       </c>
-      <c r="D33" s="6">
+      <c r="D33" s="43">
         <v>43533</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="5" t="s">
         <v>25</v>
       </c>
@@ -1687,11 +1693,11 @@
       <c r="C34" s="5">
         <v>95</v>
       </c>
-      <c r="D34" s="6">
+      <c r="D34" s="43">
         <v>43534</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="5" t="s">
         <v>6</v>
       </c>
@@ -1701,11 +1707,11 @@
       <c r="C35" s="5">
         <v>74</v>
       </c>
-      <c r="D35" s="6">
+      <c r="D35" s="43">
         <v>43546</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="5" t="s">
         <v>6</v>
       </c>
@@ -1715,11 +1721,11 @@
       <c r="C36" s="5">
         <v>52</v>
       </c>
-      <c r="D36" s="6">
+      <c r="D36" s="43">
         <v>43546</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" s="5" t="s">
         <v>16</v>
       </c>
@@ -1729,11 +1735,11 @@
       <c r="C37" s="5">
         <v>196</v>
       </c>
-      <c r="D37" s="6">
+      <c r="D37" s="43">
         <v>43376</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" s="5" t="s">
         <v>16</v>
       </c>
@@ -1743,11 +1749,11 @@
       <c r="C38" s="5">
         <v>115</v>
       </c>
-      <c r="D38" s="6">
+      <c r="D38" s="43">
         <v>43407</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" s="5" t="s">
         <v>25</v>
       </c>
@@ -1757,11 +1763,11 @@
       <c r="C39" s="5">
         <v>10</v>
       </c>
-      <c r="D39" s="6">
+      <c r="D39" s="43">
         <v>43546</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" s="5" t="s">
         <v>19</v>
       </c>
@@ -1771,11 +1777,11 @@
       <c r="C40" s="5">
         <v>60</v>
       </c>
-      <c r="D40" s="6">
+      <c r="D40" s="43">
         <v>43553</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" s="5" t="s">
         <v>25</v>
       </c>
@@ -1785,11 +1791,11 @@
       <c r="C41" s="5">
         <v>60</v>
       </c>
-      <c r="D41" s="6">
+      <c r="D41" s="43">
         <v>43553</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" s="5" t="s">
         <v>16</v>
       </c>
@@ -1799,11 +1805,11 @@
       <c r="C42" s="5">
         <v>60</v>
       </c>
-      <c r="D42" s="6">
+      <c r="D42" s="43">
         <v>43553</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" s="5" t="s">
         <v>19</v>
       </c>
@@ -1813,11 +1819,11 @@
       <c r="C43" s="5">
         <v>60</v>
       </c>
-      <c r="D43" s="6">
+      <c r="D43" s="43">
         <v>43481</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" s="5" t="s">
         <v>19</v>
       </c>
@@ -1827,11 +1833,11 @@
       <c r="C44" s="5">
         <v>150</v>
       </c>
-      <c r="D44" s="6">
+      <c r="D44" s="43">
         <v>43442</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" s="5" t="s">
         <v>19</v>
       </c>
@@ -1841,11 +1847,11 @@
       <c r="C45" s="5">
         <v>180</v>
       </c>
-      <c r="D45" s="6">
+      <c r="D45" s="43">
         <v>43448</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" s="5" t="s">
         <v>19</v>
       </c>
@@ -1855,11 +1861,11 @@
       <c r="C46" s="5">
         <v>180</v>
       </c>
-      <c r="D46" s="6">
+      <c r="D46" s="43">
         <v>43468</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" s="5" t="s">
         <v>19</v>
       </c>
@@ -1869,11 +1875,11 @@
       <c r="C47" s="5">
         <v>120</v>
       </c>
-      <c r="D47" s="6">
+      <c r="D47" s="43">
         <v>43478</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" s="5" t="s">
         <v>6</v>
       </c>
@@ -1883,11 +1889,11 @@
       <c r="C48" s="5">
         <v>300</v>
       </c>
-      <c r="D48" s="6">
+      <c r="D48" s="43">
         <v>43449</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" s="5" t="s">
         <v>6</v>
       </c>
@@ -1897,11 +1903,11 @@
       <c r="C49" s="5">
         <v>150</v>
       </c>
-      <c r="D49" s="6">
+      <c r="D49" s="43">
         <v>43450</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" s="5" t="s">
         <v>19</v>
       </c>
@@ -1911,11 +1917,11 @@
       <c r="C50" s="5">
         <v>82</v>
       </c>
-      <c r="D50" s="6">
+      <c r="D50" s="43">
         <v>43558</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" s="5" t="s">
         <v>25</v>
       </c>
@@ -1925,11 +1931,11 @@
       <c r="C51" s="5">
         <v>82</v>
       </c>
-      <c r="D51" s="6">
+      <c r="D51" s="43">
         <v>43558</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" s="5" t="s">
         <v>6</v>
       </c>
@@ -1939,11 +1945,11 @@
       <c r="C52" s="5">
         <v>82</v>
       </c>
-      <c r="D52" s="6">
+      <c r="D52" s="43">
         <v>43558</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" s="5" t="s">
         <v>25</v>
       </c>
@@ -1953,11 +1959,11 @@
       <c r="C53" s="5">
         <v>85</v>
       </c>
-      <c r="D53" s="6">
+      <c r="D53" s="43">
         <v>43559</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" s="5" t="s">
         <v>19</v>
       </c>
@@ -1967,11 +1973,11 @@
       <c r="C54" s="5">
         <v>70</v>
       </c>
-      <c r="D54" s="6">
+      <c r="D54" s="43">
         <v>43571</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" s="5" t="s">
         <v>25</v>
       </c>
@@ -1981,11 +1987,11 @@
       <c r="C55" s="5">
         <v>70</v>
       </c>
-      <c r="D55" s="6">
+      <c r="D55" s="43">
         <v>43571</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" s="5" t="s">
         <v>19</v>
       </c>
@@ -1995,11 +2001,11 @@
       <c r="C56" s="5">
         <v>120</v>
       </c>
-      <c r="D56" s="6">
+      <c r="D56" s="43">
         <v>43572</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" s="5" t="s">
         <v>19</v>
       </c>
@@ -2009,11 +2015,11 @@
       <c r="C57" s="5">
         <v>100</v>
       </c>
-      <c r="D57" s="6">
+      <c r="D57" s="43">
         <v>43574</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" s="5" t="s">
         <v>6</v>
       </c>
@@ -2023,11 +2029,11 @@
       <c r="C58" s="5">
         <v>42</v>
       </c>
-      <c r="D58" s="6">
+      <c r="D58" s="43">
         <v>43577</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" s="5" t="s">
         <v>6</v>
       </c>
@@ -2037,11 +2043,11 @@
       <c r="C59" s="5">
         <v>97</v>
       </c>
-      <c r="D59" s="6">
+      <c r="D59" s="43">
         <v>43578</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" s="5" t="s">
         <v>25</v>
       </c>
@@ -2051,11 +2057,11 @@
       <c r="C60" s="5">
         <v>30</v>
       </c>
-      <c r="D60" s="6">
+      <c r="D60" s="43">
         <v>43578</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" s="5" t="s">
         <v>6</v>
       </c>
@@ -2065,11 +2071,11 @@
       <c r="C61" s="5">
         <v>107</v>
       </c>
-      <c r="D61" s="6">
+      <c r="D61" s="43">
         <v>43581</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" s="5" t="s">
         <v>6</v>
       </c>
@@ -2079,11 +2085,11 @@
       <c r="C62" s="5">
         <v>39</v>
       </c>
-      <c r="D62" s="6">
+      <c r="D62" s="43">
         <v>43584</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" s="5" t="s">
         <v>6</v>
       </c>
@@ -2093,11 +2099,11 @@
       <c r="C63" s="5">
         <v>22</v>
       </c>
-      <c r="D63" s="6">
+      <c r="D63" s="43">
         <v>43585</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" s="5" t="s">
         <v>19</v>
       </c>
@@ -2107,11 +2113,11 @@
       <c r="C64" s="5">
         <v>22</v>
       </c>
-      <c r="D64" s="6">
+      <c r="D64" s="43">
         <v>43585</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" s="5" t="s">
         <v>19</v>
       </c>
@@ -2121,11 +2127,11 @@
       <c r="C65" s="5">
         <v>25</v>
       </c>
-      <c r="D65" s="6">
+      <c r="D65" s="43">
         <v>43587</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66" s="5" t="s">
         <v>16</v>
       </c>
@@ -2135,11 +2141,11 @@
       <c r="C66" s="5">
         <v>25</v>
       </c>
-      <c r="D66" s="6">
+      <c r="D66" s="43">
         <v>43587</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67" s="5" t="s">
         <v>16</v>
       </c>
@@ -2149,11 +2155,11 @@
       <c r="C67" s="5">
         <v>136</v>
       </c>
-      <c r="D67" s="6">
+      <c r="D67" s="43">
         <v>43587</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68" s="5" t="s">
         <v>16</v>
       </c>
@@ -2163,11 +2169,11 @@
       <c r="C68" s="5">
         <v>35</v>
       </c>
-      <c r="D68" s="6">
+      <c r="D68" s="43">
         <v>43587</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69" s="5" t="s">
         <v>16</v>
       </c>
@@ -2177,11 +2183,11 @@
       <c r="C69" s="5">
         <v>135</v>
       </c>
-      <c r="D69" s="6">
+      <c r="D69" s="43">
         <v>43588</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70" s="5" t="s">
         <v>25</v>
       </c>
@@ -2191,11 +2197,11 @@
       <c r="C70" s="5">
         <v>135</v>
       </c>
-      <c r="D70" s="6">
+      <c r="D70" s="43">
         <v>43588</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71" s="5" t="s">
         <v>25</v>
       </c>
@@ -2205,11 +2211,11 @@
       <c r="C71" s="5">
         <v>40</v>
       </c>
-      <c r="D71" s="6">
+      <c r="D71" s="43">
         <v>43589</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72" s="5" t="s">
         <v>16</v>
       </c>
@@ -2219,11 +2225,11 @@
       <c r="C72" s="5">
         <v>40</v>
       </c>
-      <c r="D72" s="6">
+      <c r="D72" s="43">
         <v>43589</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73" s="5" t="s">
         <v>25</v>
       </c>
@@ -2233,11 +2239,11 @@
       <c r="C73" s="5">
         <v>78</v>
       </c>
-      <c r="D73" s="6">
+      <c r="D73" s="43">
         <v>43590</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74" s="5" t="s">
         <v>16</v>
       </c>
@@ -2247,11 +2253,11 @@
       <c r="C74" s="5">
         <v>78</v>
       </c>
-      <c r="D74" s="6">
+      <c r="D74" s="43">
         <v>43590</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75" s="5" t="s">
         <v>6</v>
       </c>
@@ -2261,11 +2267,11 @@
       <c r="C75" s="5">
         <v>45</v>
       </c>
-      <c r="D75" s="6">
+      <c r="D75" s="43">
         <v>43593</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76" s="5" t="s">
         <v>25</v>
       </c>
@@ -2275,11 +2281,11 @@
       <c r="C76" s="5">
         <v>45</v>
       </c>
-      <c r="D76" s="6">
+      <c r="D76" s="43">
         <v>43593</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" s="5" t="s">
         <v>19</v>
       </c>
@@ -2289,11 +2295,11 @@
       <c r="C77" s="5">
         <v>45</v>
       </c>
-      <c r="D77" s="6">
+      <c r="D77" s="43">
         <v>43593</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A78" s="5" t="s">
         <v>16</v>
       </c>
@@ -2303,11 +2309,11 @@
       <c r="C78" s="5">
         <v>45</v>
       </c>
-      <c r="D78" s="6">
+      <c r="D78" s="43">
         <v>43593</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A79" s="5" t="s">
         <v>25</v>
       </c>
@@ -2317,11 +2323,11 @@
       <c r="C79" s="5">
         <v>60</v>
       </c>
-      <c r="D79" s="6">
+      <c r="D79" s="43">
         <v>43593</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A80" s="5" t="s">
         <v>19</v>
       </c>
@@ -2331,11 +2337,11 @@
       <c r="C80" s="5">
         <v>60</v>
       </c>
-      <c r="D80" s="6">
+      <c r="D80" s="43">
         <v>43593</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A81" s="5" t="s">
         <v>16</v>
       </c>
@@ -2345,11 +2351,11 @@
       <c r="C81" s="5">
         <v>60</v>
       </c>
-      <c r="D81" s="6">
+      <c r="D81" s="43">
         <v>43593</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A82" s="5" t="s">
         <v>16</v>
       </c>
@@ -2359,11 +2365,11 @@
       <c r="C82" s="5">
         <v>116</v>
       </c>
-      <c r="D82" s="6">
+      <c r="D82" s="43">
         <v>43594</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A83" s="5" t="s">
         <v>25</v>
       </c>
@@ -2373,11 +2379,11 @@
       <c r="C83" s="5">
         <v>116</v>
       </c>
-      <c r="D83" s="6">
+      <c r="D83" s="43">
         <v>43594</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A84" s="5" t="s">
         <v>6</v>
       </c>
@@ -2387,11 +2393,11 @@
       <c r="C84" s="5">
         <v>47</v>
       </c>
-      <c r="D84" s="6">
+      <c r="D84" s="43">
         <v>43598</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A85" s="5" t="s">
         <v>6</v>
       </c>
@@ -2401,11 +2407,11 @@
       <c r="C85" s="5">
         <v>31</v>
       </c>
-      <c r="D85" s="6">
+      <c r="D85" s="43">
         <v>43598</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A86" s="5" t="s">
         <v>25</v>
       </c>
@@ -2415,11 +2421,11 @@
       <c r="C86" s="5">
         <v>160</v>
       </c>
-      <c r="D86" s="6">
+      <c r="D86" s="43">
         <v>43595</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A87" s="5" t="s">
         <v>16</v>
       </c>
@@ -2429,11 +2435,11 @@
       <c r="C87" s="5">
         <v>160</v>
       </c>
-      <c r="D87" s="6">
+      <c r="D87" s="43">
         <v>43595</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A88" s="5" t="s">
         <v>25</v>
       </c>
@@ -2443,11 +2449,11 @@
       <c r="C88" s="5">
         <v>240</v>
       </c>
-      <c r="D88" s="6">
+      <c r="D88" s="43">
         <v>43599</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A89" s="5" t="s">
         <v>16</v>
       </c>
@@ -2457,11 +2463,11 @@
       <c r="C89" s="5">
         <v>240</v>
       </c>
-      <c r="D89" s="6">
+      <c r="D89" s="43">
         <v>43599</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A90" s="5" t="s">
         <v>6</v>
       </c>
@@ -2471,11 +2477,11 @@
       <c r="C90" s="5">
         <v>40</v>
       </c>
-      <c r="D90" s="6">
+      <c r="D90" s="43">
         <v>43600</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A91" s="5" t="s">
         <v>19</v>
       </c>
@@ -2485,11 +2491,11 @@
       <c r="C91" s="5">
         <v>40</v>
       </c>
-      <c r="D91" s="6">
+      <c r="D91" s="43">
         <v>43600</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A92" s="5" t="s">
         <v>16</v>
       </c>
@@ -2499,11 +2505,11 @@
       <c r="C92" s="5">
         <v>40</v>
       </c>
-      <c r="D92" s="6">
+      <c r="D92" s="43">
         <v>43600</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A93" s="5" t="s">
         <v>25</v>
       </c>
@@ -2513,11 +2519,11 @@
       <c r="C93" s="5">
         <v>40</v>
       </c>
-      <c r="D93" s="6">
+      <c r="D93" s="43">
         <v>43600</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A94" s="5" t="s">
         <v>6</v>
       </c>
@@ -2527,11 +2533,11 @@
       <c r="C94" s="5">
         <v>20</v>
       </c>
-      <c r="D94" s="6">
+      <c r="D94" s="43">
         <v>43600</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A95" s="5" t="s">
         <v>19</v>
       </c>
@@ -2541,11 +2547,11 @@
       <c r="C95" s="5">
         <v>20</v>
       </c>
-      <c r="D95" s="6">
+      <c r="D95" s="43">
         <v>43600</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A96" s="5" t="s">
         <v>16</v>
       </c>
@@ -2555,11 +2561,11 @@
       <c r="C96" s="5">
         <v>20</v>
       </c>
-      <c r="D96" s="6">
+      <c r="D96" s="43">
         <v>43600</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A97" s="5" t="s">
         <v>25</v>
       </c>
@@ -2569,11 +2575,11 @@
       <c r="C97" s="5">
         <v>20</v>
       </c>
-      <c r="D97" s="6">
+      <c r="D97" s="43">
         <v>43600</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A98" s="5" t="s">
         <v>25</v>
       </c>
@@ -2583,11 +2589,11 @@
       <c r="C98" s="5">
         <v>210</v>
       </c>
-      <c r="D98" s="6">
+      <c r="D98" s="43">
         <v>43603</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A99" s="5" t="s">
         <v>16</v>
       </c>
@@ -2597,11 +2603,11 @@
       <c r="C99" s="5">
         <v>210</v>
       </c>
-      <c r="D99" s="6">
+      <c r="D99" s="43">
         <v>43603</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A100" s="5" t="s">
         <v>25</v>
       </c>
@@ -2611,11 +2617,11 @@
       <c r="C100" s="5">
         <v>65</v>
       </c>
-      <c r="D100" s="6">
+      <c r="D100" s="43">
         <v>43604</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A101" s="5" t="s">
         <v>16</v>
       </c>
@@ -2625,11 +2631,11 @@
       <c r="C101" s="5">
         <v>65</v>
       </c>
-      <c r="D101" s="6">
+      <c r="D101" s="43">
         <v>43604</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A102" s="5" t="s">
         <v>16</v>
       </c>
@@ -2639,11 +2645,11 @@
       <c r="C102" s="5">
         <v>110</v>
       </c>
-      <c r="D102" s="6">
+      <c r="D102" s="43">
         <v>43604</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A103" s="5" t="s">
         <v>16</v>
       </c>
@@ -2653,11 +2659,11 @@
       <c r="C103" s="5">
         <v>20</v>
       </c>
-      <c r="D103" s="6">
+      <c r="D103" s="43">
         <v>43605</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A104" s="5" t="s">
         <v>25</v>
       </c>
@@ -2667,11 +2673,11 @@
       <c r="C104" s="5">
         <v>15</v>
       </c>
-      <c r="D104" s="6">
+      <c r="D104" s="43">
         <v>43606</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A105" s="5" t="s">
         <v>6</v>
       </c>
@@ -2681,11 +2687,11 @@
       <c r="C105" s="5">
         <v>30</v>
       </c>
-      <c r="D105" s="6">
+      <c r="D105" s="43">
         <v>43607</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A106" s="5" t="s">
         <v>16</v>
       </c>
@@ -2695,11 +2701,11 @@
       <c r="C106" s="5">
         <v>30</v>
       </c>
-      <c r="D106" s="6">
+      <c r="D106" s="43">
         <v>43607</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A107" s="5" t="s">
         <v>25</v>
       </c>
@@ -2709,11 +2715,11 @@
       <c r="C107" s="5">
         <v>30</v>
       </c>
-      <c r="D107" s="6">
+      <c r="D107" s="43">
         <v>43607</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A108" s="5" t="s">
         <v>6</v>
       </c>
@@ -2723,11 +2729,11 @@
       <c r="C108" s="5">
         <v>30</v>
       </c>
-      <c r="D108" s="6">
+      <c r="D108" s="43">
         <v>43607</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A109" s="5" t="s">
         <v>16</v>
       </c>
@@ -2737,11 +2743,11 @@
       <c r="C109" s="5">
         <v>30</v>
       </c>
-      <c r="D109" s="6">
+      <c r="D109" s="43">
         <v>43607</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A110" s="5" t="s">
         <v>25</v>
       </c>
@@ -2751,11 +2757,11 @@
       <c r="C110" s="5">
         <v>30</v>
       </c>
-      <c r="D110" s="6">
+      <c r="D110" s="43">
         <v>43607</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A111" s="5" t="s">
         <v>16</v>
       </c>
@@ -2765,11 +2771,11 @@
       <c r="C111" s="5">
         <v>130</v>
       </c>
-      <c r="D111" s="6">
+      <c r="D111" s="43">
         <v>43607</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A112" s="5" t="s">
         <v>25</v>
       </c>
@@ -2779,11 +2785,11 @@
       <c r="C112" s="5">
         <v>130</v>
       </c>
-      <c r="D112" s="6">
+      <c r="D112" s="43">
         <v>43607</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A113" s="5" t="s">
         <v>25</v>
       </c>
@@ -2793,11 +2799,11 @@
       <c r="C113" s="5">
         <v>20</v>
       </c>
-      <c r="D113" s="6">
+      <c r="D113" s="43">
         <v>43607</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A114" s="5" t="s">
         <v>6</v>
       </c>
@@ -2807,11 +2813,11 @@
       <c r="C114" s="5">
         <v>68</v>
       </c>
-      <c r="D114" s="6">
+      <c r="D114" s="43">
         <v>43608</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A115" s="5" t="s">
         <v>6</v>
       </c>
@@ -2821,11 +2827,11 @@
       <c r="C115" s="5">
         <v>23</v>
       </c>
-      <c r="D115" s="6">
+      <c r="D115" s="43">
         <v>43609</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A116" s="5" t="s">
         <v>16</v>
       </c>
@@ -2835,11 +2841,11 @@
       <c r="C116" s="5">
         <v>85</v>
       </c>
-      <c r="D116" s="6">
+      <c r="D116" s="43">
         <v>43608</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A117" s="5" t="s">
         <v>25</v>
       </c>
@@ -2849,11 +2855,11 @@
       <c r="C117" s="5">
         <v>85</v>
       </c>
-      <c r="D117" s="6">
+      <c r="D117" s="43">
         <v>43608</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A118" s="5" t="s">
         <v>25</v>
       </c>
@@ -2863,11 +2869,11 @@
       <c r="C118" s="5">
         <v>73</v>
       </c>
-      <c r="D118" s="6">
+      <c r="D118" s="43">
         <v>43609</v>
       </c>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A119" s="5" t="s">
         <v>19</v>
       </c>
@@ -2877,11 +2883,11 @@
       <c r="C119" s="5">
         <v>30</v>
       </c>
-      <c r="D119" s="6">
+      <c r="D119" s="43">
         <v>43614</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A120" s="5" t="s">
         <v>16</v>
       </c>
@@ -2891,11 +2897,11 @@
       <c r="C120" s="5">
         <v>30</v>
       </c>
-      <c r="D120" s="6">
+      <c r="D120" s="43">
         <v>43614</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A121" s="5" t="s">
         <v>6</v>
       </c>
@@ -2905,11 +2911,11 @@
       <c r="C121" s="5">
         <v>30</v>
       </c>
-      <c r="D121" s="6">
+      <c r="D121" s="43">
         <v>43614</v>
       </c>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A122" s="5" t="s">
         <v>19</v>
       </c>
@@ -2919,11 +2925,11 @@
       <c r="C122" s="5">
         <v>84</v>
       </c>
-      <c r="D122" s="6">
+      <c r="D122" s="43">
         <v>43614</v>
       </c>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A123" s="5" t="s">
         <v>16</v>
       </c>
@@ -2933,11 +2939,11 @@
       <c r="C123" s="5">
         <v>84</v>
       </c>
-      <c r="D123" s="6">
+      <c r="D123" s="43">
         <v>43614</v>
       </c>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A124" s="5" t="s">
         <v>6</v>
       </c>
@@ -2947,11 +2953,11 @@
       <c r="C124" s="5">
         <v>84</v>
       </c>
-      <c r="D124" s="6">
+      <c r="D124" s="43">
         <v>43614</v>
       </c>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A125" s="5" t="s">
         <v>25</v>
       </c>
@@ -2961,11 +2967,11 @@
       <c r="C125" s="5">
         <v>84</v>
       </c>
-      <c r="D125" s="6">
+      <c r="D125" s="43">
         <v>43614</v>
       </c>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A126" s="5" t="s">
         <v>6</v>
       </c>
@@ -2975,11 +2981,11 @@
       <c r="C126" s="5">
         <v>64</v>
       </c>
-      <c r="D126" s="40" t="s">
+      <c r="D126" s="44" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A127" s="5" t="s">
         <v>6</v>
       </c>
@@ -2989,11 +2995,11 @@
       <c r="C127" s="5">
         <v>98</v>
       </c>
-      <c r="D127" s="40" t="s">
+      <c r="D127" s="44" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A128" s="5" t="s">
         <v>19</v>
       </c>
@@ -3003,11 +3009,11 @@
       <c r="C128" s="5">
         <v>60</v>
       </c>
-      <c r="D128" s="40">
+      <c r="D128" s="44">
         <v>43471</v>
       </c>
     </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A129" s="5" t="s">
         <v>16</v>
       </c>
@@ -3017,11 +3023,11 @@
       <c r="C129" s="5">
         <v>165</v>
       </c>
-      <c r="D129" s="40">
+      <c r="D129" s="44">
         <v>43616</v>
       </c>
     </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A130" s="5" t="s">
         <v>25</v>
       </c>
@@ -3031,11 +3037,11 @@
       <c r="C130" s="5">
         <v>165</v>
       </c>
-      <c r="D130" s="40">
+      <c r="D130" s="44">
         <v>43616</v>
       </c>
     </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A131" s="5" t="s">
         <v>16</v>
       </c>
@@ -3045,11 +3051,11 @@
       <c r="C131" s="5">
         <v>118</v>
       </c>
-      <c r="D131" s="40">
+      <c r="D131" s="44">
         <v>43618</v>
       </c>
     </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A132" s="5" t="s">
         <v>25</v>
       </c>
@@ -3059,11 +3065,11 @@
       <c r="C132" s="5">
         <v>118</v>
       </c>
-      <c r="D132" s="40">
+      <c r="D132" s="44">
         <v>43618</v>
       </c>
     </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A133" s="5" t="s">
         <v>25</v>
       </c>
@@ -3073,11 +3079,11 @@
       <c r="C133" s="5">
         <v>20</v>
       </c>
-      <c r="D133" s="6">
+      <c r="D133" s="43">
         <v>43530</v>
       </c>
     </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A134" s="5" t="s">
         <v>19</v>
       </c>
@@ -3087,11 +3093,11 @@
       <c r="C134" s="5">
         <v>30</v>
       </c>
-      <c r="D134" s="40">
+      <c r="D134" s="44">
         <v>43619</v>
       </c>
     </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A135" s="5" t="s">
         <v>19</v>
       </c>
@@ -3101,11 +3107,11 @@
       <c r="C135" s="5">
         <v>30</v>
       </c>
-      <c r="D135" s="40">
+      <c r="D135" s="44">
         <v>43619</v>
       </c>
     </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A136" s="5" t="s">
         <v>19</v>
       </c>
@@ -3115,11 +3121,11 @@
       <c r="C136" s="5">
         <v>35</v>
       </c>
-      <c r="D136" s="40">
+      <c r="D136" s="44">
         <v>43619</v>
       </c>
     </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A137" s="5" t="s">
         <v>25</v>
       </c>
@@ -3129,11 +3135,11 @@
       <c r="C137" s="5">
         <v>180</v>
       </c>
-      <c r="D137" s="40">
+      <c r="D137" s="44">
         <v>43620</v>
       </c>
     </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A138" s="5" t="s">
         <v>16</v>
       </c>
@@ -3143,11 +3149,11 @@
       <c r="C138" s="5">
         <v>180</v>
       </c>
-      <c r="D138" s="40">
+      <c r="D138" s="44">
         <v>43620</v>
       </c>
     </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A139" s="5" t="s">
         <v>25</v>
       </c>
@@ -3157,11 +3163,11 @@
       <c r="C139" s="5">
         <v>10</v>
       </c>
-      <c r="D139" s="6">
+      <c r="D139" s="43">
         <v>43620</v>
       </c>
     </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A140" s="5" t="s">
         <v>19</v>
       </c>
@@ -3171,11 +3177,11 @@
       <c r="C140" s="5">
         <v>55</v>
       </c>
-      <c r="D140" s="6">
+      <c r="D140" s="43">
         <v>43621</v>
       </c>
     </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A141" s="5" t="s">
         <v>16</v>
       </c>
@@ -3185,11 +3191,11 @@
       <c r="C141" s="5">
         <v>55</v>
       </c>
-      <c r="D141" s="6">
+      <c r="D141" s="43">
         <v>43621</v>
       </c>
     </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A142" s="5" t="s">
         <v>6</v>
       </c>
@@ -3199,11 +3205,11 @@
       <c r="C142" s="5">
         <v>55</v>
       </c>
-      <c r="D142" s="6">
+      <c r="D142" s="43">
         <v>43621</v>
       </c>
     </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A143" s="5" t="s">
         <v>25</v>
       </c>
@@ -3213,11 +3219,11 @@
       <c r="C143" s="5">
         <v>55</v>
       </c>
-      <c r="D143" s="6">
+      <c r="D143" s="43">
         <v>43621</v>
       </c>
     </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A144" s="5" t="s">
         <v>19</v>
       </c>
@@ -3227,11 +3233,11 @@
       <c r="C144" s="5">
         <v>60</v>
       </c>
-      <c r="D144" s="6">
+      <c r="D144" s="43">
         <v>43621</v>
       </c>
     </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A145" s="5" t="s">
         <v>16</v>
       </c>
@@ -3241,11 +3247,11 @@
       <c r="C145" s="5">
         <v>30</v>
       </c>
-      <c r="D145" s="6">
+      <c r="D145" s="43">
         <v>43621</v>
       </c>
     </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A146" s="5" t="s">
         <v>6</v>
       </c>
@@ -3255,11 +3261,11 @@
       <c r="C146" s="5">
         <v>87</v>
       </c>
-      <c r="D146" s="6">
+      <c r="D146" s="43">
         <v>43621</v>
       </c>
     </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A147" s="5" t="s">
         <v>25</v>
       </c>
@@ -3269,11 +3275,11 @@
       <c r="C147" s="5">
         <v>30</v>
       </c>
-      <c r="D147" s="6">
+      <c r="D147" s="43">
         <v>43621</v>
       </c>
     </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A148" s="5" t="s">
         <v>16</v>
       </c>
@@ -3283,11 +3289,11 @@
       <c r="C148" s="5">
         <v>30</v>
       </c>
-      <c r="D148" s="6">
+      <c r="D148" s="43">
         <v>43621</v>
       </c>
     </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A149" s="5" t="s">
         <v>25</v>
       </c>
@@ -3297,11 +3303,11 @@
       <c r="C149" s="5">
         <v>30</v>
       </c>
-      <c r="D149" s="6">
+      <c r="D149" s="43">
         <v>43621</v>
       </c>
     </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A150" s="5" t="s">
         <v>16</v>
       </c>
@@ -3311,11 +3317,11 @@
       <c r="C150" s="5">
         <v>174</v>
       </c>
-      <c r="D150" s="6">
+      <c r="D150" s="43">
         <v>43622</v>
       </c>
     </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A151" s="5" t="s">
         <v>25</v>
       </c>
@@ -3325,11 +3331,11 @@
       <c r="C151" s="5">
         <v>185</v>
       </c>
-      <c r="D151" s="6">
+      <c r="D151" s="43">
         <v>43622</v>
       </c>
     </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A152" s="5" t="s">
         <v>25</v>
       </c>
@@ -3339,11 +3345,11 @@
       <c r="C152" s="5">
         <v>10</v>
       </c>
-      <c r="D152" s="6">
+      <c r="D152" s="43">
         <v>43622</v>
       </c>
     </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A153" s="5" t="s">
         <v>19</v>
       </c>
@@ -3353,11 +3359,11 @@
       <c r="C153" s="5">
         <v>110</v>
       </c>
-      <c r="D153" s="6">
+      <c r="D153" s="43">
         <v>43622</v>
       </c>
     </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A154" s="5" t="s">
         <v>19</v>
       </c>
@@ -3367,11 +3373,11 @@
       <c r="C154" s="5">
         <v>55</v>
       </c>
-      <c r="D154" s="6">
+      <c r="D154" s="43">
         <v>43622</v>
       </c>
     </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A155" s="5" t="s">
         <v>6</v>
       </c>
@@ -3381,11 +3387,11 @@
       <c r="C155" s="5">
         <v>30</v>
       </c>
-      <c r="D155" s="40">
+      <c r="D155" s="44">
         <v>43623</v>
       </c>
     </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A156" s="5" t="s">
         <v>6</v>
       </c>
@@ -3395,11 +3401,11 @@
       <c r="C156" s="5">
         <v>40</v>
       </c>
-      <c r="D156" s="40">
+      <c r="D156" s="44">
         <v>43625</v>
       </c>
     </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A157" s="5" t="s">
         <v>6</v>
       </c>
@@ -3409,11 +3415,11 @@
       <c r="C157" s="5">
         <v>271</v>
       </c>
-      <c r="D157" s="40">
+      <c r="D157" s="44">
         <v>43625</v>
       </c>
     </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A158" s="5" t="s">
         <v>25</v>
       </c>
@@ -3423,11 +3429,11 @@
       <c r="C158" s="5">
         <v>75</v>
       </c>
-      <c r="D158" s="40">
+      <c r="D158" s="44">
         <v>43625</v>
       </c>
     </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A159" s="5" t="s">
         <v>6</v>
       </c>
@@ -3437,11 +3443,11 @@
       <c r="C159" s="5">
         <v>47</v>
       </c>
-      <c r="D159" s="40">
+      <c r="D159" s="44">
         <v>43625</v>
       </c>
     </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A160" s="5" t="s">
         <v>25</v>
       </c>
@@ -3451,11 +3457,11 @@
       <c r="C160" s="5">
         <v>130</v>
       </c>
-      <c r="D160" s="6">
+      <c r="D160" s="43">
         <v>43626</v>
       </c>
     </row>
-    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A161" s="5" t="s">
         <v>16</v>
       </c>
@@ -3465,11 +3471,11 @@
       <c r="C161" s="5">
         <v>130</v>
       </c>
-      <c r="D161" s="6">
+      <c r="D161" s="43">
         <v>43626</v>
       </c>
     </row>
-    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A162" s="5" t="s">
         <v>6</v>
       </c>
@@ -3479,11 +3485,11 @@
       <c r="C162" s="5">
         <v>25</v>
       </c>
-      <c r="D162" s="40">
+      <c r="D162" s="44">
         <v>43626</v>
       </c>
     </row>
-    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A163" s="5" t="s">
         <v>6</v>
       </c>
@@ -3493,11 +3499,11 @@
       <c r="C163" s="5">
         <v>31</v>
       </c>
-      <c r="D163" s="40">
+      <c r="D163" s="44">
         <v>43626</v>
       </c>
     </row>
-    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A164" s="5" t="s">
         <v>6</v>
       </c>
@@ -3507,11 +3513,11 @@
       <c r="C164" s="5">
         <v>32</v>
       </c>
-      <c r="D164" s="40">
+      <c r="D164" s="44">
         <v>43626</v>
       </c>
     </row>
-    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A165" s="5" t="s">
         <v>19</v>
       </c>
@@ -3521,11 +3527,11 @@
       <c r="C165" s="5">
         <v>75</v>
       </c>
-      <c r="D165" s="40">
+      <c r="D165" s="44">
         <v>43627</v>
       </c>
     </row>
-    <row r="166" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A166" s="5" t="s">
         <v>16</v>
       </c>
@@ -3535,11 +3541,11 @@
       <c r="C166" s="5">
         <v>75</v>
       </c>
-      <c r="D166" s="40">
+      <c r="D166" s="44">
         <v>43627</v>
       </c>
     </row>
-    <row r="167" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A167" s="5" t="s">
         <v>19</v>
       </c>
@@ -3549,11 +3555,11 @@
       <c r="C167" s="5">
         <v>70</v>
       </c>
-      <c r="D167" s="40">
+      <c r="D167" s="44">
         <v>43628</v>
       </c>
     </row>
-    <row r="168" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A168" s="5" t="s">
         <v>25</v>
       </c>
@@ -3563,11 +3569,11 @@
       <c r="C168" s="5">
         <v>112</v>
       </c>
-      <c r="D168" s="40">
+      <c r="D168" s="44">
         <v>43628</v>
       </c>
     </row>
-    <row r="169" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A169" s="5" t="s">
         <v>19</v>
       </c>
@@ -3577,11 +3583,11 @@
       <c r="C169" s="5">
         <v>115</v>
       </c>
-      <c r="D169" s="40">
+      <c r="D169" s="44">
         <v>43628</v>
       </c>
     </row>
-    <row r="170" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A170" s="5" t="s">
         <v>19</v>
       </c>
@@ -3591,11 +3597,11 @@
       <c r="C170" s="5">
         <v>175</v>
       </c>
-      <c r="D170" s="40">
+      <c r="D170" s="44">
         <v>43628</v>
       </c>
     </row>
-    <row r="171" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A171" s="5" t="s">
         <v>6</v>
       </c>
@@ -3605,11 +3611,11 @@
       <c r="C171" s="5">
         <v>23</v>
       </c>
-      <c r="D171" s="40">
+      <c r="D171" s="44">
         <v>43628</v>
       </c>
     </row>
-    <row r="172" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A172" s="5" t="s">
         <v>19</v>
       </c>
@@ -3619,11 +3625,11 @@
       <c r="C172" s="5">
         <v>30</v>
       </c>
-      <c r="D172" s="40">
+      <c r="D172" s="44">
         <v>43628</v>
       </c>
     </row>
-    <row r="173" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A173" s="5" t="s">
         <v>19</v>
       </c>
@@ -3633,11 +3639,11 @@
       <c r="C173" s="5">
         <v>77</v>
       </c>
-      <c r="D173" s="6">
+      <c r="D173" s="43">
         <v>43629</v>
       </c>
     </row>
-    <row r="174" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A174" s="5" t="s">
         <v>19</v>
       </c>
@@ -3647,11 +3653,11 @@
       <c r="C174" s="5">
         <v>39</v>
       </c>
-      <c r="D174" s="6">
+      <c r="D174" s="43">
         <v>43629</v>
       </c>
     </row>
-    <row r="175" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A175" s="5" t="s">
         <v>19</v>
       </c>
@@ -3661,11 +3667,11 @@
       <c r="C175" s="5">
         <v>40</v>
       </c>
-      <c r="D175" s="6">
+      <c r="D175" s="43">
         <v>43629</v>
       </c>
     </row>
-    <row r="176" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A176" s="5" t="s">
         <v>25</v>
       </c>
@@ -3675,11 +3681,11 @@
       <c r="C176" s="5">
         <v>25</v>
       </c>
-      <c r="D176" s="41">
+      <c r="D176" s="43">
         <v>43629</v>
       </c>
     </row>
-    <row r="177" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A177" s="5" t="s">
         <v>19</v>
       </c>
@@ -3689,11 +3695,11 @@
       <c r="C177" s="5">
         <v>20</v>
       </c>
-      <c r="D177" s="6">
+      <c r="D177" s="43">
         <v>43629</v>
       </c>
     </row>
-    <row r="178" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A178" s="5" t="s">
         <v>19</v>
       </c>
@@ -3703,11 +3709,11 @@
       <c r="C178" s="5">
         <v>60</v>
       </c>
-      <c r="D178" s="6">
+      <c r="D178" s="43">
         <v>43630</v>
       </c>
     </row>
-    <row r="179" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A179" s="5" t="s">
         <v>19</v>
       </c>
@@ -3717,311 +3723,327 @@
       <c r="C179" s="5">
         <v>100</v>
       </c>
-      <c r="D179" s="6">
+      <c r="D179" s="43">
         <v>43630</v>
       </c>
     </row>
-    <row r="180" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A180" s="5"/>
-      <c r="B180" s="5"/>
-      <c r="C180" s="5"/>
-      <c r="D180" s="6"/>
-    </row>
-    <row r="181" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A181" s="5"/>
-      <c r="B181" s="5"/>
-      <c r="C181" s="5"/>
-      <c r="D181" s="6"/>
-    </row>
-    <row r="182" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A180" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B180" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C180" s="5">
+        <v>31</v>
+      </c>
+      <c r="D180" s="43">
+        <v>43630</v>
+      </c>
+    </row>
+    <row r="181" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A181" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B181" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C181" s="5">
+        <v>40</v>
+      </c>
+      <c r="D181" s="43">
+        <v>43630</v>
+      </c>
+    </row>
+    <row r="182" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A182" s="5"/>
       <c r="B182" s="5"/>
       <c r="C182" s="5"/>
       <c r="D182" s="6"/>
     </row>
-    <row r="183" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A183" s="5"/>
       <c r="B183" s="5"/>
       <c r="C183" s="5"/>
       <c r="D183" s="6"/>
     </row>
-    <row r="184" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A184" s="5"/>
       <c r="B184" s="5"/>
       <c r="C184" s="5"/>
       <c r="D184" s="6"/>
     </row>
-    <row r="185" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A185" s="5"/>
       <c r="B185" s="5"/>
       <c r="C185" s="5"/>
       <c r="D185" s="6"/>
     </row>
-    <row r="186" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A186" s="5"/>
       <c r="B186" s="5"/>
       <c r="C186" s="5"/>
       <c r="D186" s="6"/>
     </row>
-    <row r="187" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A187" s="5"/>
       <c r="B187" s="5"/>
       <c r="C187" s="5"/>
       <c r="D187" s="5"/>
     </row>
-    <row r="188" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A188" s="5"/>
       <c r="B188" s="5"/>
       <c r="C188" s="5"/>
       <c r="D188" s="5"/>
     </row>
-    <row r="189" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A189" s="5"/>
       <c r="B189" s="5"/>
       <c r="C189" s="5"/>
       <c r="D189" s="5"/>
     </row>
-    <row r="190" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A190" s="5"/>
       <c r="B190" s="5"/>
       <c r="C190" s="5"/>
       <c r="D190" s="5"/>
     </row>
-    <row r="191" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A191" s="5"/>
       <c r="B191" s="5"/>
       <c r="C191" s="5"/>
       <c r="D191" s="5"/>
     </row>
-    <row r="192" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A192" s="5"/>
       <c r="B192" s="5"/>
       <c r="C192" s="5"/>
       <c r="D192" s="5"/>
     </row>
-    <row r="193" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A193" s="5"/>
       <c r="B193" s="5"/>
       <c r="C193" s="5"/>
       <c r="D193" s="5"/>
     </row>
-    <row r="194" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A194" s="5"/>
       <c r="B194" s="5"/>
       <c r="C194" s="5"/>
       <c r="D194" s="5"/>
     </row>
-    <row r="195" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A195" s="5"/>
       <c r="B195" s="5"/>
       <c r="C195" s="5"/>
       <c r="D195" s="5"/>
     </row>
-    <row r="196" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A196" s="5"/>
       <c r="B196" s="5"/>
       <c r="C196" s="5"/>
       <c r="D196" s="5"/>
     </row>
-    <row r="197" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A197" s="5"/>
       <c r="B197" s="5"/>
       <c r="C197" s="5"/>
       <c r="D197" s="5"/>
     </row>
-    <row r="198" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A198" s="5"/>
       <c r="B198" s="5"/>
       <c r="C198" s="5"/>
       <c r="D198" s="5"/>
     </row>
-    <row r="199" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A199" s="5"/>
       <c r="B199" s="5"/>
       <c r="C199" s="5"/>
       <c r="D199" s="5"/>
     </row>
-    <row r="200" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A200" s="5"/>
       <c r="B200" s="5"/>
       <c r="C200" s="5"/>
       <c r="D200" s="5"/>
     </row>
-    <row r="201" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A201" s="5"/>
       <c r="B201" s="5"/>
       <c r="C201" s="5"/>
       <c r="D201" s="5"/>
     </row>
-    <row r="202" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A202" s="5"/>
       <c r="B202" s="5"/>
       <c r="C202" s="5"/>
       <c r="D202" s="5"/>
     </row>
-    <row r="203" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A203" s="5"/>
       <c r="B203" s="5"/>
       <c r="C203" s="5"/>
       <c r="D203" s="5"/>
     </row>
-    <row r="204" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A204" s="5"/>
       <c r="B204" s="5"/>
       <c r="C204" s="5"/>
       <c r="D204" s="5"/>
     </row>
-    <row r="205" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A205" s="5"/>
       <c r="B205" s="5"/>
       <c r="C205" s="5"/>
       <c r="D205" s="5"/>
     </row>
-    <row r="206" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A206" s="5"/>
       <c r="B206" s="5"/>
       <c r="C206" s="5"/>
       <c r="D206" s="5"/>
     </row>
-    <row r="207" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A207" s="5"/>
       <c r="B207" s="5"/>
       <c r="C207" s="5"/>
       <c r="D207" s="5"/>
     </row>
-    <row r="208" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A208" s="5"/>
       <c r="B208" s="5"/>
       <c r="C208" s="5"/>
       <c r="D208" s="5"/>
     </row>
-    <row r="209" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A209" s="5"/>
       <c r="B209" s="5"/>
       <c r="C209" s="5"/>
       <c r="D209" s="5"/>
     </row>
-    <row r="210" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A210" s="5"/>
       <c r="B210" s="5"/>
       <c r="C210" s="5"/>
       <c r="D210" s="5"/>
     </row>
-    <row r="211" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A211" s="5"/>
       <c r="B211" s="5"/>
       <c r="C211" s="5"/>
       <c r="D211" s="5"/>
     </row>
-    <row r="212" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A212" s="5"/>
       <c r="B212" s="5"/>
       <c r="C212" s="5"/>
       <c r="D212" s="5"/>
     </row>
-    <row r="213" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A213" s="5"/>
       <c r="B213" s="5"/>
       <c r="C213" s="5"/>
       <c r="D213" s="5"/>
     </row>
-    <row r="214" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A214" s="5"/>
       <c r="B214" s="5"/>
       <c r="C214" s="5"/>
       <c r="D214" s="5"/>
     </row>
-    <row r="215" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A215" s="5"/>
       <c r="B215" s="5"/>
       <c r="C215" s="5"/>
       <c r="D215" s="5"/>
     </row>
-    <row r="216" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A216" s="5"/>
       <c r="B216" s="5"/>
       <c r="C216" s="5"/>
       <c r="D216" s="5"/>
     </row>
-    <row r="217" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A217" s="5"/>
       <c r="B217" s="5"/>
       <c r="C217" s="5"/>
       <c r="D217" s="5"/>
     </row>
-    <row r="218" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A218" s="5"/>
       <c r="B218" s="5"/>
       <c r="C218" s="5"/>
       <c r="D218" s="5"/>
     </row>
-    <row r="219" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A219" s="5"/>
       <c r="B219" s="5"/>
       <c r="C219" s="5"/>
       <c r="D219" s="5"/>
     </row>
-    <row r="220" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A220" s="5"/>
       <c r="B220" s="5"/>
       <c r="C220" s="5"/>
       <c r="D220" s="5"/>
     </row>
-    <row r="221" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A221" s="5"/>
       <c r="B221" s="5"/>
       <c r="C221" s="5"/>
       <c r="D221" s="5"/>
     </row>
-    <row r="222" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A222" s="5"/>
       <c r="B222" s="5"/>
       <c r="C222" s="5"/>
       <c r="D222" s="5"/>
     </row>
-    <row r="223" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A223" s="5"/>
       <c r="B223" s="5"/>
       <c r="C223" s="5"/>
       <c r="D223" s="5"/>
     </row>
-    <row r="224" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A224" s="5"/>
       <c r="B224" s="5"/>
       <c r="C224" s="5"/>
       <c r="D224" s="5"/>
     </row>
-    <row r="225" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A225" s="5"/>
       <c r="B225" s="5"/>
       <c r="C225" s="5"/>
       <c r="D225" s="5"/>
     </row>
-    <row r="226" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A226" s="5"/>
       <c r="B226" s="5"/>
       <c r="C226" s="5"/>
       <c r="D226" s="5"/>
     </row>
-    <row r="227" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A227" s="5"/>
       <c r="B227" s="5"/>
       <c r="C227" s="5"/>
       <c r="D227" s="5"/>
     </row>
-    <row r="228" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A228" s="5"/>
       <c r="B228" s="5"/>
       <c r="C228" s="5"/>
       <c r="D228" s="5"/>
     </row>
-    <row r="229" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A229" s="5"/>
       <c r="B229" s="5"/>
       <c r="C229" s="5"/>
       <c r="D229" s="5"/>
     </row>
-    <row r="230" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A230" s="5"/>
       <c r="B230" s="5"/>
       <c r="C230" s="5"/>
@@ -4034,6 +4056,6 @@
     <mergeCell ref="H24:O24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Aumento leggibilità codice e test sul manuale
</commit_message>
<xml_diff>
--- a/Documentazione/Attività sul progetto/DocAttivProg.xlsx
+++ b/Documentazione/Attività sul progetto/DocAttivProg.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\UniUD\Laurea Magistrale\Ingegneria del Software 2\Progetto-Ingegneria-Del-Sw-2\Documentazione\Attività sul progetto\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LUCA\Documents\Universita\INGEGNERIA DEL SOFTWARE\Progetto\Documentazione\Attività sul progetto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46941D95-569D-4FA9-A638-7BA3456A6A8B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" iterateDelta="1E-4"/>
+  <calcPr calcId="162913" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -31,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="31">
   <si>
     <t>Le categorie sono: Ispezione Codice, Documenti di progetto, Documenti di processo, Manuale, Sviluppo, Testing</t>
   </si>
@@ -129,7 +128,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yyyy"/>
   </numFmts>
@@ -387,6 +386,8 @@
     <xf numFmtId="9" fontId="0" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -396,8 +397,6 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -746,39 +745,39 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O230"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+      <selection activeCell="F186" sqref="F186"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.5546875" customWidth="1"/>
-    <col min="2" max="2" width="23.44140625" customWidth="1"/>
-    <col min="3" max="3" width="15.5546875" customWidth="1"/>
-    <col min="4" max="4" width="10.88671875" customWidth="1"/>
-    <col min="5" max="7" width="8.6640625" customWidth="1"/>
-    <col min="8" max="8" width="26.33203125" customWidth="1"/>
-    <col min="9" max="11" width="17.33203125" customWidth="1"/>
-    <col min="12" max="14" width="17.44140625" customWidth="1"/>
-    <col min="15" max="1025" width="8.6640625" customWidth="1"/>
+    <col min="1" max="1" width="15.5703125" customWidth="1"/>
+    <col min="2" max="2" width="23.42578125" customWidth="1"/>
+    <col min="3" max="3" width="15.5703125" customWidth="1"/>
+    <col min="4" max="4" width="10.85546875" customWidth="1"/>
+    <col min="5" max="7" width="8.7109375" customWidth="1"/>
+    <col min="8" max="8" width="26.28515625" customWidth="1"/>
+    <col min="9" max="11" width="17.28515625" customWidth="1"/>
+    <col min="12" max="14" width="17.42578125" customWidth="1"/>
+    <col min="15" max="1025" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="F1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="F2" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
@@ -793,7 +792,7 @@
       </c>
       <c r="H3" s="2"/>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>6</v>
       </c>
@@ -803,16 +802,16 @@
       <c r="C4" s="5">
         <v>98</v>
       </c>
-      <c r="D4" s="43">
+      <c r="D4" s="40">
         <v>43484</v>
       </c>
-      <c r="H4" s="40" t="s">
+      <c r="H4" s="42" t="s">
         <v>8</v>
       </c>
-      <c r="I4" s="40"/>
-      <c r="J4" s="40"/>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="I4" s="42"/>
+      <c r="J4" s="42"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>6</v>
       </c>
@@ -822,7 +821,7 @@
       <c r="C5" s="5">
         <v>149</v>
       </c>
-      <c r="D5" s="43">
+      <c r="D5" s="40">
         <v>43493</v>
       </c>
       <c r="H5" s="7" t="s">
@@ -835,7 +834,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>6</v>
       </c>
@@ -845,7 +844,7 @@
       <c r="C6" s="5">
         <v>135</v>
       </c>
-      <c r="D6" s="43">
+      <c r="D6" s="40">
         <v>43494</v>
       </c>
       <c r="H6" s="9" t="s">
@@ -853,14 +852,14 @@
       </c>
       <c r="I6" s="10">
         <f>SUMIF(B:B,"Ispezione codice",C:C)</f>
-        <v>927</v>
+        <v>957</v>
       </c>
       <c r="J6" s="11">
         <f>I6/I12</f>
-        <v>6.672905269219695E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+        <v>6.8740123545467602E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>6</v>
       </c>
@@ -870,7 +869,7 @@
       <c r="C7" s="5">
         <v>53</v>
       </c>
-      <c r="D7" s="43">
+      <c r="D7" s="40">
         <v>43494</v>
       </c>
       <c r="H7" s="9" t="s">
@@ -882,10 +881,10 @@
       </c>
       <c r="J7" s="11">
         <f>(I7/I12)</f>
-        <v>0.2185430463576159</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+        <v>0.21807211607527655</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>6</v>
       </c>
@@ -895,7 +894,7 @@
       <c r="C8" s="5">
         <v>87</v>
       </c>
-      <c r="D8" s="43">
+      <c r="D8" s="40">
         <v>43495</v>
       </c>
       <c r="H8" s="9" t="s">
@@ -907,10 +906,10 @@
       </c>
       <c r="J8" s="11">
         <f>I8/I12</f>
-        <v>0.18190325367117766</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+        <v>0.181511277115357</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>6</v>
       </c>
@@ -920,7 +919,7 @@
       <c r="C9" s="5">
         <v>74</v>
       </c>
-      <c r="D9" s="43">
+      <c r="D9" s="40">
         <v>43495</v>
       </c>
       <c r="H9" s="9" t="s">
@@ -932,10 +931,10 @@
       </c>
       <c r="J9" s="11">
         <f>I9/I12</f>
-        <v>3.3832421537575583E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+        <v>3.3759517310731214E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>6</v>
       </c>
@@ -945,7 +944,7 @@
       <c r="C10" s="5">
         <v>32</v>
       </c>
-      <c r="D10" s="43">
+      <c r="D10" s="40">
         <v>43499</v>
       </c>
       <c r="H10" s="9" t="s">
@@ -957,10 +956,10 @@
       </c>
       <c r="J10" s="11">
         <f>I10/I12</f>
-        <v>0.45436222286207889</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+        <v>0.45338313460709667</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>16</v>
       </c>
@@ -970,7 +969,7 @@
       <c r="C11" s="5">
         <v>75</v>
       </c>
-      <c r="D11" s="43">
+      <c r="D11" s="40">
         <v>43497</v>
       </c>
       <c r="H11" s="12" t="s">
@@ -982,10 +981,10 @@
       </c>
       <c r="J11" s="14">
         <f>I11/I12</f>
-        <v>4.4630002879355021E-2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+        <v>4.4533831346070966E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>16</v>
       </c>
@@ -995,7 +994,7 @@
       <c r="C12" s="5">
         <v>55</v>
       </c>
-      <c r="D12" s="43">
+      <c r="D12" s="40">
         <v>43503</v>
       </c>
       <c r="H12" s="15" t="s">
@@ -1003,14 +1002,14 @@
       </c>
       <c r="I12" s="16">
         <f>SUM(I6:I11)</f>
-        <v>13892</v>
+        <v>13922</v>
       </c>
       <c r="J12" s="17">
         <f>SUM(J6:J11)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>6</v>
       </c>
@@ -1020,12 +1019,12 @@
       <c r="C13" s="5">
         <v>127</v>
       </c>
-      <c r="D13" s="43">
+      <c r="D13" s="40">
         <v>43505</v>
       </c>
       <c r="H13" s="2"/>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>6</v>
       </c>
@@ -1035,11 +1034,11 @@
       <c r="C14" s="5">
         <v>24</v>
       </c>
-      <c r="D14" s="43">
+      <c r="D14" s="40">
         <v>43509</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>19</v>
       </c>
@@ -1049,21 +1048,21 @@
       <c r="C15" s="5">
         <v>195</v>
       </c>
-      <c r="D15" s="43">
+      <c r="D15" s="40">
         <v>43521</v>
       </c>
-      <c r="H15" s="41" t="s">
+      <c r="H15" s="43" t="s">
         <v>20</v>
       </c>
-      <c r="I15" s="41"/>
-      <c r="J15" s="41"/>
-      <c r="K15" s="41"/>
-      <c r="L15" s="41"/>
-      <c r="M15" s="41"/>
-      <c r="N15" s="41"/>
-      <c r="O15" s="41"/>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="I15" s="43"/>
+      <c r="J15" s="43"/>
+      <c r="K15" s="43"/>
+      <c r="L15" s="43"/>
+      <c r="M15" s="43"/>
+      <c r="N15" s="43"/>
+      <c r="O15" s="43"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>19</v>
       </c>
@@ -1073,7 +1072,7 @@
       <c r="C16" s="5">
         <v>105</v>
       </c>
-      <c r="D16" s="43">
+      <c r="D16" s="40">
         <v>43523</v>
       </c>
       <c r="H16" s="18" t="s">
@@ -1101,7 +1100,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>25</v>
       </c>
@@ -1111,7 +1110,7 @@
       <c r="C17" s="5">
         <v>30</v>
       </c>
-      <c r="D17" s="43">
+      <c r="D17" s="40">
         <v>43519</v>
       </c>
       <c r="H17" s="21" t="s">
@@ -1146,7 +1145,7 @@
         <v>3113</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>25</v>
       </c>
@@ -1156,7 +1155,7 @@
       <c r="C18" s="5">
         <v>100</v>
       </c>
-      <c r="D18" s="43">
+      <c r="D18" s="40">
         <v>43520</v>
       </c>
       <c r="H18" s="21" t="s">
@@ -1191,7 +1190,7 @@
         <v>3955</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>25</v>
       </c>
@@ -1201,7 +1200,7 @@
       <c r="C19" s="5">
         <v>125</v>
       </c>
-      <c r="D19" s="43">
+      <c r="D19" s="40">
         <v>43522</v>
       </c>
       <c r="H19" s="21" t="s">
@@ -1229,14 +1228,14 @@
       </c>
       <c r="N19" s="22">
         <f>SUMIFS(C:C,B:B,"Ispezione codice",A:A,"Luca")</f>
-        <v>289</v>
+        <v>319</v>
       </c>
       <c r="O19" s="23">
         <f>SUM(I19:N19)</f>
-        <v>2999</v>
-      </c>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
+        <v>3029</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>25</v>
       </c>
@@ -1246,7 +1245,7 @@
       <c r="C20" s="5">
         <v>170</v>
       </c>
-      <c r="D20" s="43">
+      <c r="D20" s="40">
         <v>43523</v>
       </c>
       <c r="H20" s="21" t="s">
@@ -1281,7 +1280,7 @@
         <v>3825</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>25</v>
       </c>
@@ -1291,7 +1290,7 @@
       <c r="C21" s="5">
         <v>65</v>
       </c>
-      <c r="D21" s="43">
+      <c r="D21" s="40">
         <v>43524</v>
       </c>
       <c r="H21" s="24" t="s">
@@ -1319,14 +1318,14 @@
       </c>
       <c r="N21" s="27">
         <f t="shared" si="0"/>
-        <v>231.75</v>
+        <v>239.25</v>
       </c>
       <c r="O21" s="28">
         <f>SUM(O17:O20)</f>
-        <v>13892</v>
-      </c>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
+        <v>13922</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>16</v>
       </c>
@@ -1336,11 +1335,11 @@
       <c r="C22" s="5">
         <v>60</v>
       </c>
-      <c r="D22" s="43">
+      <c r="D22" s="40">
         <v>43487</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
         <v>16</v>
       </c>
@@ -1350,11 +1349,11 @@
       <c r="C23" s="5">
         <v>103</v>
       </c>
-      <c r="D23" s="43">
+      <c r="D23" s="40">
         <v>43506</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
         <v>16</v>
       </c>
@@ -1364,21 +1363,21 @@
       <c r="C24" s="5">
         <v>100</v>
       </c>
-      <c r="D24" s="43">
+      <c r="D24" s="40">
         <v>43520</v>
       </c>
-      <c r="H24" s="42" t="s">
+      <c r="H24" s="44" t="s">
         <v>28</v>
       </c>
-      <c r="I24" s="42"/>
-      <c r="J24" s="42"/>
-      <c r="K24" s="42"/>
-      <c r="L24" s="42"/>
-      <c r="M24" s="42"/>
-      <c r="N24" s="42"/>
-      <c r="O24" s="42"/>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="I24" s="44"/>
+      <c r="J24" s="44"/>
+      <c r="K24" s="44"/>
+      <c r="L24" s="44"/>
+      <c r="M24" s="44"/>
+      <c r="N24" s="44"/>
+      <c r="O24" s="44"/>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
         <v>16</v>
       </c>
@@ -1388,7 +1387,7 @@
       <c r="C25" s="5">
         <v>170</v>
       </c>
-      <c r="D25" s="43">
+      <c r="D25" s="40">
         <v>43523</v>
       </c>
       <c r="H25" s="29" t="s">
@@ -1416,7 +1415,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
         <v>16</v>
       </c>
@@ -1426,7 +1425,7 @@
       <c r="C26" s="5">
         <v>45</v>
       </c>
-      <c r="D26" s="43">
+      <c r="D26" s="40">
         <v>43524</v>
       </c>
       <c r="H26" s="32" t="s">
@@ -1461,7 +1460,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
         <v>16</v>
       </c>
@@ -1471,7 +1470,7 @@
       <c r="C27" s="5">
         <v>25</v>
       </c>
-      <c r="D27" s="43">
+      <c r="D27" s="40">
         <v>43530</v>
       </c>
       <c r="H27" s="32" t="s">
@@ -1506,7 +1505,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
         <v>19</v>
       </c>
@@ -1516,7 +1515,7 @@
       <c r="C28" s="5">
         <v>15</v>
       </c>
-      <c r="D28" s="43">
+      <c r="D28" s="40">
         <v>43532</v>
       </c>
       <c r="H28" s="32" t="s">
@@ -1524,11 +1523,11 @@
       </c>
       <c r="I28" s="33">
         <f>I19/O19</f>
-        <v>0.35911970656885628</v>
+        <v>0.35556289204357872</v>
       </c>
       <c r="J28" s="33">
         <f>J19/O19</f>
-        <v>0.30410136712237412</v>
+        <v>0.30108946847144274</v>
       </c>
       <c r="K28" s="33">
         <f>K19/O19</f>
@@ -1536,22 +1535,22 @@
       </c>
       <c r="L28" s="33">
         <f>L19/O19</f>
-        <v>5.8686228742914306E-2</v>
+        <v>5.8104985143611752E-2</v>
       </c>
       <c r="M28" s="33">
         <f>M19/O19</f>
-        <v>0.18172724241413804</v>
+        <v>0.17992736876857049</v>
       </c>
       <c r="N28" s="33">
         <f>N19/O19</f>
-        <v>9.6365455151717239E-2</v>
+        <v>0.1053152855727963</v>
       </c>
       <c r="O28" s="34">
         <f>SUM(I28:N28)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
         <v>6</v>
       </c>
@@ -1561,7 +1560,7 @@
       <c r="C29" s="5">
         <v>47</v>
       </c>
-      <c r="D29" s="43">
+      <c r="D29" s="40">
         <v>43532</v>
       </c>
       <c r="H29" s="32" t="s">
@@ -1596,7 +1595,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
         <v>25</v>
       </c>
@@ -1606,7 +1605,7 @@
       <c r="C30" s="5">
         <v>15</v>
       </c>
-      <c r="D30" s="43">
+      <c r="D30" s="40">
         <v>43532</v>
       </c>
       <c r="H30" s="36" t="s">
@@ -1614,11 +1613,11 @@
       </c>
       <c r="I30" s="37">
         <f t="shared" ref="I30:N30" si="1">AVERAGE(I26:I29)</f>
-        <v>0.23447419303566541</v>
+        <v>0.23358498940434602</v>
       </c>
       <c r="J30" s="37">
         <f t="shared" si="1"/>
-        <v>0.19955655357110416</v>
+        <v>0.19880357890837133</v>
       </c>
       <c r="K30" s="37">
         <f t="shared" si="1"/>
@@ -1626,22 +1625,22 @@
       </c>
       <c r="L30" s="37">
         <f t="shared" si="1"/>
-        <v>0.40861915392353876</v>
+        <v>0.40847384302371309</v>
       </c>
       <c r="M30" s="37">
         <f t="shared" si="1"/>
-        <v>5.0333771387848239E-2</v>
+        <v>4.9883802976456351E-2</v>
       </c>
       <c r="N30" s="38">
         <f t="shared" si="1"/>
-        <v>6.9271387510047744E-2</v>
+        <v>7.1508845115317521E-2</v>
       </c>
       <c r="O30" s="39">
         <f>SUM(I30:N30)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
+        <v>0.99999999999999989</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
         <v>25</v>
       </c>
@@ -1651,11 +1650,11 @@
       <c r="C31" s="5">
         <v>55</v>
       </c>
-      <c r="D31" s="43">
+      <c r="D31" s="40">
         <v>43531</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
         <v>25</v>
       </c>
@@ -1665,11 +1664,11 @@
       <c r="C32" s="5">
         <v>68</v>
       </c>
-      <c r="D32" s="43">
+      <c r="D32" s="40">
         <v>43532</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
         <v>25</v>
       </c>
@@ -1679,11 +1678,11 @@
       <c r="C33" s="5">
         <v>129</v>
       </c>
-      <c r="D33" s="43">
+      <c r="D33" s="40">
         <v>43533</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
         <v>25</v>
       </c>
@@ -1693,11 +1692,11 @@
       <c r="C34" s="5">
         <v>95</v>
       </c>
-      <c r="D34" s="43">
+      <c r="D34" s="40">
         <v>43534</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
         <v>6</v>
       </c>
@@ -1707,11 +1706,11 @@
       <c r="C35" s="5">
         <v>74</v>
       </c>
-      <c r="D35" s="43">
+      <c r="D35" s="40">
         <v>43546</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
         <v>6</v>
       </c>
@@ -1721,11 +1720,11 @@
       <c r="C36" s="5">
         <v>52</v>
       </c>
-      <c r="D36" s="43">
+      <c r="D36" s="40">
         <v>43546</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
         <v>16</v>
       </c>
@@ -1735,11 +1734,11 @@
       <c r="C37" s="5">
         <v>196</v>
       </c>
-      <c r="D37" s="43">
+      <c r="D37" s="40">
         <v>43376</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
         <v>16</v>
       </c>
@@ -1749,11 +1748,11 @@
       <c r="C38" s="5">
         <v>115</v>
       </c>
-      <c r="D38" s="43">
+      <c r="D38" s="40">
         <v>43407</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
         <v>25</v>
       </c>
@@ -1763,11 +1762,11 @@
       <c r="C39" s="5">
         <v>10</v>
       </c>
-      <c r="D39" s="43">
+      <c r="D39" s="40">
         <v>43546</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
         <v>19</v>
       </c>
@@ -1777,11 +1776,11 @@
       <c r="C40" s="5">
         <v>60</v>
       </c>
-      <c r="D40" s="43">
+      <c r="D40" s="40">
         <v>43553</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
         <v>25</v>
       </c>
@@ -1791,11 +1790,11 @@
       <c r="C41" s="5">
         <v>60</v>
       </c>
-      <c r="D41" s="43">
+      <c r="D41" s="40">
         <v>43553</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
         <v>16</v>
       </c>
@@ -1805,11 +1804,11 @@
       <c r="C42" s="5">
         <v>60</v>
       </c>
-      <c r="D42" s="43">
+      <c r="D42" s="40">
         <v>43553</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
         <v>19</v>
       </c>
@@ -1819,11 +1818,11 @@
       <c r="C43" s="5">
         <v>60</v>
       </c>
-      <c r="D43" s="43">
+      <c r="D43" s="40">
         <v>43481</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
         <v>19</v>
       </c>
@@ -1833,11 +1832,11 @@
       <c r="C44" s="5">
         <v>150</v>
       </c>
-      <c r="D44" s="43">
+      <c r="D44" s="40">
         <v>43442</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
         <v>19</v>
       </c>
@@ -1847,11 +1846,11 @@
       <c r="C45" s="5">
         <v>180</v>
       </c>
-      <c r="D45" s="43">
+      <c r="D45" s="40">
         <v>43448</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="5" t="s">
         <v>19</v>
       </c>
@@ -1861,11 +1860,11 @@
       <c r="C46" s="5">
         <v>180</v>
       </c>
-      <c r="D46" s="43">
+      <c r="D46" s="40">
         <v>43468</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
         <v>19</v>
       </c>
@@ -1875,11 +1874,11 @@
       <c r="C47" s="5">
         <v>120</v>
       </c>
-      <c r="D47" s="43">
+      <c r="D47" s="40">
         <v>43478</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
         <v>6</v>
       </c>
@@ -1889,11 +1888,11 @@
       <c r="C48" s="5">
         <v>300</v>
       </c>
-      <c r="D48" s="43">
+      <c r="D48" s="40">
         <v>43449</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="5" t="s">
         <v>6</v>
       </c>
@@ -1903,11 +1902,11 @@
       <c r="C49" s="5">
         <v>150</v>
       </c>
-      <c r="D49" s="43">
+      <c r="D49" s="40">
         <v>43450</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="5" t="s">
         <v>19</v>
       </c>
@@ -1917,11 +1916,11 @@
       <c r="C50" s="5">
         <v>82</v>
       </c>
-      <c r="D50" s="43">
+      <c r="D50" s="40">
         <v>43558</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="5" t="s">
         <v>25</v>
       </c>
@@ -1931,11 +1930,11 @@
       <c r="C51" s="5">
         <v>82</v>
       </c>
-      <c r="D51" s="43">
+      <c r="D51" s="40">
         <v>43558</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="5" t="s">
         <v>6</v>
       </c>
@@ -1945,11 +1944,11 @@
       <c r="C52" s="5">
         <v>82</v>
       </c>
-      <c r="D52" s="43">
+      <c r="D52" s="40">
         <v>43558</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="5" t="s">
         <v>25</v>
       </c>
@@ -1959,11 +1958,11 @@
       <c r="C53" s="5">
         <v>85</v>
       </c>
-      <c r="D53" s="43">
+      <c r="D53" s="40">
         <v>43559</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="5" t="s">
         <v>19</v>
       </c>
@@ -1973,11 +1972,11 @@
       <c r="C54" s="5">
         <v>70</v>
       </c>
-      <c r="D54" s="43">
+      <c r="D54" s="40">
         <v>43571</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="5" t="s">
         <v>25</v>
       </c>
@@ -1987,11 +1986,11 @@
       <c r="C55" s="5">
         <v>70</v>
       </c>
-      <c r="D55" s="43">
+      <c r="D55" s="40">
         <v>43571</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="5" t="s">
         <v>19</v>
       </c>
@@ -2001,11 +2000,11 @@
       <c r="C56" s="5">
         <v>120</v>
       </c>
-      <c r="D56" s="43">
+      <c r="D56" s="40">
         <v>43572</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="5" t="s">
         <v>19</v>
       </c>
@@ -2015,11 +2014,11 @@
       <c r="C57" s="5">
         <v>100</v>
       </c>
-      <c r="D57" s="43">
+      <c r="D57" s="40">
         <v>43574</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="5" t="s">
         <v>6</v>
       </c>
@@ -2029,11 +2028,11 @@
       <c r="C58" s="5">
         <v>42</v>
       </c>
-      <c r="D58" s="43">
+      <c r="D58" s="40">
         <v>43577</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="5" t="s">
         <v>6</v>
       </c>
@@ -2043,11 +2042,11 @@
       <c r="C59" s="5">
         <v>97</v>
       </c>
-      <c r="D59" s="43">
+      <c r="D59" s="40">
         <v>43578</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="5" t="s">
         <v>25</v>
       </c>
@@ -2057,11 +2056,11 @@
       <c r="C60" s="5">
         <v>30</v>
       </c>
-      <c r="D60" s="43">
+      <c r="D60" s="40">
         <v>43578</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="5" t="s">
         <v>6</v>
       </c>
@@ -2071,11 +2070,11 @@
       <c r="C61" s="5">
         <v>107</v>
       </c>
-      <c r="D61" s="43">
+      <c r="D61" s="40">
         <v>43581</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="5" t="s">
         <v>6</v>
       </c>
@@ -2085,11 +2084,11 @@
       <c r="C62" s="5">
         <v>39</v>
       </c>
-      <c r="D62" s="43">
+      <c r="D62" s="40">
         <v>43584</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="5" t="s">
         <v>6</v>
       </c>
@@ -2099,11 +2098,11 @@
       <c r="C63" s="5">
         <v>22</v>
       </c>
-      <c r="D63" s="43">
+      <c r="D63" s="40">
         <v>43585</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="5" t="s">
         <v>19</v>
       </c>
@@ -2113,11 +2112,11 @@
       <c r="C64" s="5">
         <v>22</v>
       </c>
-      <c r="D64" s="43">
+      <c r="D64" s="40">
         <v>43585</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="5" t="s">
         <v>19</v>
       </c>
@@ -2127,11 +2126,11 @@
       <c r="C65" s="5">
         <v>25</v>
       </c>
-      <c r="D65" s="43">
+      <c r="D65" s="40">
         <v>43587</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="5" t="s">
         <v>16</v>
       </c>
@@ -2141,11 +2140,11 @@
       <c r="C66" s="5">
         <v>25</v>
       </c>
-      <c r="D66" s="43">
+      <c r="D66" s="40">
         <v>43587</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="5" t="s">
         <v>16</v>
       </c>
@@ -2155,11 +2154,11 @@
       <c r="C67" s="5">
         <v>136</v>
       </c>
-      <c r="D67" s="43">
+      <c r="D67" s="40">
         <v>43587</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="5" t="s">
         <v>16</v>
       </c>
@@ -2169,11 +2168,11 @@
       <c r="C68" s="5">
         <v>35</v>
       </c>
-      <c r="D68" s="43">
+      <c r="D68" s="40">
         <v>43587</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="5" t="s">
         <v>16</v>
       </c>
@@ -2183,11 +2182,11 @@
       <c r="C69" s="5">
         <v>135</v>
       </c>
-      <c r="D69" s="43">
+      <c r="D69" s="40">
         <v>43588</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="5" t="s">
         <v>25</v>
       </c>
@@ -2197,11 +2196,11 @@
       <c r="C70" s="5">
         <v>135</v>
       </c>
-      <c r="D70" s="43">
+      <c r="D70" s="40">
         <v>43588</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="5" t="s">
         <v>25</v>
       </c>
@@ -2211,11 +2210,11 @@
       <c r="C71" s="5">
         <v>40</v>
       </c>
-      <c r="D71" s="43">
+      <c r="D71" s="40">
         <v>43589</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="5" t="s">
         <v>16</v>
       </c>
@@ -2225,11 +2224,11 @@
       <c r="C72" s="5">
         <v>40</v>
       </c>
-      <c r="D72" s="43">
+      <c r="D72" s="40">
         <v>43589</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="5" t="s">
         <v>25</v>
       </c>
@@ -2239,11 +2238,11 @@
       <c r="C73" s="5">
         <v>78</v>
       </c>
-      <c r="D73" s="43">
+      <c r="D73" s="40">
         <v>43590</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="5" t="s">
         <v>16</v>
       </c>
@@ -2253,11 +2252,11 @@
       <c r="C74" s="5">
         <v>78</v>
       </c>
-      <c r="D74" s="43">
+      <c r="D74" s="40">
         <v>43590</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="5" t="s">
         <v>6</v>
       </c>
@@ -2267,11 +2266,11 @@
       <c r="C75" s="5">
         <v>45</v>
       </c>
-      <c r="D75" s="43">
+      <c r="D75" s="40">
         <v>43593</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="5" t="s">
         <v>25</v>
       </c>
@@ -2281,11 +2280,11 @@
       <c r="C76" s="5">
         <v>45</v>
       </c>
-      <c r="D76" s="43">
+      <c r="D76" s="40">
         <v>43593</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="5" t="s">
         <v>19</v>
       </c>
@@ -2295,11 +2294,11 @@
       <c r="C77" s="5">
         <v>45</v>
       </c>
-      <c r="D77" s="43">
+      <c r="D77" s="40">
         <v>43593</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="5" t="s">
         <v>16</v>
       </c>
@@ -2309,11 +2308,11 @@
       <c r="C78" s="5">
         <v>45</v>
       </c>
-      <c r="D78" s="43">
+      <c r="D78" s="40">
         <v>43593</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="5" t="s">
         <v>25</v>
       </c>
@@ -2323,11 +2322,11 @@
       <c r="C79" s="5">
         <v>60</v>
       </c>
-      <c r="D79" s="43">
+      <c r="D79" s="40">
         <v>43593</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="5" t="s">
         <v>19</v>
       </c>
@@ -2337,11 +2336,11 @@
       <c r="C80" s="5">
         <v>60</v>
       </c>
-      <c r="D80" s="43">
+      <c r="D80" s="40">
         <v>43593</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="5" t="s">
         <v>16</v>
       </c>
@@ -2351,11 +2350,11 @@
       <c r="C81" s="5">
         <v>60</v>
       </c>
-      <c r="D81" s="43">
+      <c r="D81" s="40">
         <v>43593</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="5" t="s">
         <v>16</v>
       </c>
@@ -2365,11 +2364,11 @@
       <c r="C82" s="5">
         <v>116</v>
       </c>
-      <c r="D82" s="43">
+      <c r="D82" s="40">
         <v>43594</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="5" t="s">
         <v>25</v>
       </c>
@@ -2379,11 +2378,11 @@
       <c r="C83" s="5">
         <v>116</v>
       </c>
-      <c r="D83" s="43">
+      <c r="D83" s="40">
         <v>43594</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="5" t="s">
         <v>6</v>
       </c>
@@ -2393,11 +2392,11 @@
       <c r="C84" s="5">
         <v>47</v>
       </c>
-      <c r="D84" s="43">
+      <c r="D84" s="40">
         <v>43598</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" s="5" t="s">
         <v>6</v>
       </c>
@@ -2407,11 +2406,11 @@
       <c r="C85" s="5">
         <v>31</v>
       </c>
-      <c r="D85" s="43">
+      <c r="D85" s="40">
         <v>43598</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" s="5" t="s">
         <v>25</v>
       </c>
@@ -2421,11 +2420,11 @@
       <c r="C86" s="5">
         <v>160</v>
       </c>
-      <c r="D86" s="43">
+      <c r="D86" s="40">
         <v>43595</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" s="5" t="s">
         <v>16</v>
       </c>
@@ -2435,11 +2434,11 @@
       <c r="C87" s="5">
         <v>160</v>
       </c>
-      <c r="D87" s="43">
+      <c r="D87" s="40">
         <v>43595</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" s="5" t="s">
         <v>25</v>
       </c>
@@ -2449,11 +2448,11 @@
       <c r="C88" s="5">
         <v>240</v>
       </c>
-      <c r="D88" s="43">
+      <c r="D88" s="40">
         <v>43599</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" s="5" t="s">
         <v>16</v>
       </c>
@@ -2463,11 +2462,11 @@
       <c r="C89" s="5">
         <v>240</v>
       </c>
-      <c r="D89" s="43">
+      <c r="D89" s="40">
         <v>43599</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" s="5" t="s">
         <v>6</v>
       </c>
@@ -2477,11 +2476,11 @@
       <c r="C90" s="5">
         <v>40</v>
       </c>
-      <c r="D90" s="43">
+      <c r="D90" s="40">
         <v>43600</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" s="5" t="s">
         <v>19</v>
       </c>
@@ -2491,11 +2490,11 @@
       <c r="C91" s="5">
         <v>40</v>
       </c>
-      <c r="D91" s="43">
+      <c r="D91" s="40">
         <v>43600</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" s="5" t="s">
         <v>16</v>
       </c>
@@ -2505,11 +2504,11 @@
       <c r="C92" s="5">
         <v>40</v>
       </c>
-      <c r="D92" s="43">
+      <c r="D92" s="40">
         <v>43600</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" s="5" t="s">
         <v>25</v>
       </c>
@@ -2519,11 +2518,11 @@
       <c r="C93" s="5">
         <v>40</v>
       </c>
-      <c r="D93" s="43">
+      <c r="D93" s="40">
         <v>43600</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" s="5" t="s">
         <v>6</v>
       </c>
@@ -2533,11 +2532,11 @@
       <c r="C94" s="5">
         <v>20</v>
       </c>
-      <c r="D94" s="43">
+      <c r="D94" s="40">
         <v>43600</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" s="5" t="s">
         <v>19</v>
       </c>
@@ -2547,11 +2546,11 @@
       <c r="C95" s="5">
         <v>20</v>
       </c>
-      <c r="D95" s="43">
+      <c r="D95" s="40">
         <v>43600</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" s="5" t="s">
         <v>16</v>
       </c>
@@ -2561,11 +2560,11 @@
       <c r="C96" s="5">
         <v>20</v>
       </c>
-      <c r="D96" s="43">
+      <c r="D96" s="40">
         <v>43600</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" s="5" t="s">
         <v>25</v>
       </c>
@@ -2575,11 +2574,11 @@
       <c r="C97" s="5">
         <v>20</v>
       </c>
-      <c r="D97" s="43">
+      <c r="D97" s="40">
         <v>43600</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" s="5" t="s">
         <v>25</v>
       </c>
@@ -2589,11 +2588,11 @@
       <c r="C98" s="5">
         <v>210</v>
       </c>
-      <c r="D98" s="43">
+      <c r="D98" s="40">
         <v>43603</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" s="5" t="s">
         <v>16</v>
       </c>
@@ -2603,11 +2602,11 @@
       <c r="C99" s="5">
         <v>210</v>
       </c>
-      <c r="D99" s="43">
+      <c r="D99" s="40">
         <v>43603</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" s="5" t="s">
         <v>25</v>
       </c>
@@ -2617,11 +2616,11 @@
       <c r="C100" s="5">
         <v>65</v>
       </c>
-      <c r="D100" s="43">
+      <c r="D100" s="40">
         <v>43604</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" s="5" t="s">
         <v>16</v>
       </c>
@@ -2631,11 +2630,11 @@
       <c r="C101" s="5">
         <v>65</v>
       </c>
-      <c r="D101" s="43">
+      <c r="D101" s="40">
         <v>43604</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" s="5" t="s">
         <v>16</v>
       </c>
@@ -2645,11 +2644,11 @@
       <c r="C102" s="5">
         <v>110</v>
       </c>
-      <c r="D102" s="43">
+      <c r="D102" s="40">
         <v>43604</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" s="5" t="s">
         <v>16</v>
       </c>
@@ -2659,11 +2658,11 @@
       <c r="C103" s="5">
         <v>20</v>
       </c>
-      <c r="D103" s="43">
+      <c r="D103" s="40">
         <v>43605</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" s="5" t="s">
         <v>25</v>
       </c>
@@ -2673,11 +2672,11 @@
       <c r="C104" s="5">
         <v>15</v>
       </c>
-      <c r="D104" s="43">
+      <c r="D104" s="40">
         <v>43606</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" s="5" t="s">
         <v>6</v>
       </c>
@@ -2687,11 +2686,11 @@
       <c r="C105" s="5">
         <v>30</v>
       </c>
-      <c r="D105" s="43">
+      <c r="D105" s="40">
         <v>43607</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" s="5" t="s">
         <v>16</v>
       </c>
@@ -2701,11 +2700,11 @@
       <c r="C106" s="5">
         <v>30</v>
       </c>
-      <c r="D106" s="43">
+      <c r="D106" s="40">
         <v>43607</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" s="5" t="s">
         <v>25</v>
       </c>
@@ -2715,11 +2714,11 @@
       <c r="C107" s="5">
         <v>30</v>
       </c>
-      <c r="D107" s="43">
+      <c r="D107" s="40">
         <v>43607</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" s="5" t="s">
         <v>6</v>
       </c>
@@ -2729,11 +2728,11 @@
       <c r="C108" s="5">
         <v>30</v>
       </c>
-      <c r="D108" s="43">
+      <c r="D108" s="40">
         <v>43607</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" s="5" t="s">
         <v>16</v>
       </c>
@@ -2743,11 +2742,11 @@
       <c r="C109" s="5">
         <v>30</v>
       </c>
-      <c r="D109" s="43">
+      <c r="D109" s="40">
         <v>43607</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" s="5" t="s">
         <v>25</v>
       </c>
@@ -2757,11 +2756,11 @@
       <c r="C110" s="5">
         <v>30</v>
       </c>
-      <c r="D110" s="43">
+      <c r="D110" s="40">
         <v>43607</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" s="5" t="s">
         <v>16</v>
       </c>
@@ -2771,11 +2770,11 @@
       <c r="C111" s="5">
         <v>130</v>
       </c>
-      <c r="D111" s="43">
+      <c r="D111" s="40">
         <v>43607</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" s="5" t="s">
         <v>25</v>
       </c>
@@ -2785,11 +2784,11 @@
       <c r="C112" s="5">
         <v>130</v>
       </c>
-      <c r="D112" s="43">
+      <c r="D112" s="40">
         <v>43607</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" s="5" t="s">
         <v>25</v>
       </c>
@@ -2799,11 +2798,11 @@
       <c r="C113" s="5">
         <v>20</v>
       </c>
-      <c r="D113" s="43">
+      <c r="D113" s="40">
         <v>43607</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" s="5" t="s">
         <v>6</v>
       </c>
@@ -2813,11 +2812,11 @@
       <c r="C114" s="5">
         <v>68</v>
       </c>
-      <c r="D114" s="43">
+      <c r="D114" s="40">
         <v>43608</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" s="5" t="s">
         <v>6</v>
       </c>
@@ -2827,11 +2826,11 @@
       <c r="C115" s="5">
         <v>23</v>
       </c>
-      <c r="D115" s="43">
+      <c r="D115" s="40">
         <v>43609</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" s="5" t="s">
         <v>16</v>
       </c>
@@ -2841,11 +2840,11 @@
       <c r="C116" s="5">
         <v>85</v>
       </c>
-      <c r="D116" s="43">
+      <c r="D116" s="40">
         <v>43608</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" s="5" t="s">
         <v>25</v>
       </c>
@@ -2855,11 +2854,11 @@
       <c r="C117" s="5">
         <v>85</v>
       </c>
-      <c r="D117" s="43">
+      <c r="D117" s="40">
         <v>43608</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" s="5" t="s">
         <v>25</v>
       </c>
@@ -2869,11 +2868,11 @@
       <c r="C118" s="5">
         <v>73</v>
       </c>
-      <c r="D118" s="43">
+      <c r="D118" s="40">
         <v>43609</v>
       </c>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" s="5" t="s">
         <v>19</v>
       </c>
@@ -2883,11 +2882,11 @@
       <c r="C119" s="5">
         <v>30</v>
       </c>
-      <c r="D119" s="43">
+      <c r="D119" s="40">
         <v>43614</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" s="5" t="s">
         <v>16</v>
       </c>
@@ -2897,11 +2896,11 @@
       <c r="C120" s="5">
         <v>30</v>
       </c>
-      <c r="D120" s="43">
+      <c r="D120" s="40">
         <v>43614</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" s="5" t="s">
         <v>6</v>
       </c>
@@ -2911,11 +2910,11 @@
       <c r="C121" s="5">
         <v>30</v>
       </c>
-      <c r="D121" s="43">
+      <c r="D121" s="40">
         <v>43614</v>
       </c>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" s="5" t="s">
         <v>19</v>
       </c>
@@ -2925,11 +2924,11 @@
       <c r="C122" s="5">
         <v>84</v>
       </c>
-      <c r="D122" s="43">
+      <c r="D122" s="40">
         <v>43614</v>
       </c>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" s="5" t="s">
         <v>16</v>
       </c>
@@ -2939,11 +2938,11 @@
       <c r="C123" s="5">
         <v>84</v>
       </c>
-      <c r="D123" s="43">
+      <c r="D123" s="40">
         <v>43614</v>
       </c>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" s="5" t="s">
         <v>6</v>
       </c>
@@ -2953,11 +2952,11 @@
       <c r="C124" s="5">
         <v>84</v>
       </c>
-      <c r="D124" s="43">
+      <c r="D124" s="40">
         <v>43614</v>
       </c>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" s="5" t="s">
         <v>25</v>
       </c>
@@ -2967,11 +2966,11 @@
       <c r="C125" s="5">
         <v>84</v>
       </c>
-      <c r="D125" s="43">
+      <c r="D125" s="40">
         <v>43614</v>
       </c>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" s="5" t="s">
         <v>6</v>
       </c>
@@ -2981,11 +2980,11 @@
       <c r="C126" s="5">
         <v>64</v>
       </c>
-      <c r="D126" s="44" t="s">
+      <c r="D126" s="41" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" s="5" t="s">
         <v>6</v>
       </c>
@@ -2995,11 +2994,11 @@
       <c r="C127" s="5">
         <v>98</v>
       </c>
-      <c r="D127" s="44" t="s">
+      <c r="D127" s="41" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" s="5" t="s">
         <v>19</v>
       </c>
@@ -3009,11 +3008,11 @@
       <c r="C128" s="5">
         <v>60</v>
       </c>
-      <c r="D128" s="44">
+      <c r="D128" s="41">
         <v>43471</v>
       </c>
     </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" s="5" t="s">
         <v>16</v>
       </c>
@@ -3023,11 +3022,11 @@
       <c r="C129" s="5">
         <v>165</v>
       </c>
-      <c r="D129" s="44">
+      <c r="D129" s="41">
         <v>43616</v>
       </c>
     </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" s="5" t="s">
         <v>25</v>
       </c>
@@ -3037,11 +3036,11 @@
       <c r="C130" s="5">
         <v>165</v>
       </c>
-      <c r="D130" s="44">
+      <c r="D130" s="41">
         <v>43616</v>
       </c>
     </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" s="5" t="s">
         <v>16</v>
       </c>
@@ -3051,11 +3050,11 @@
       <c r="C131" s="5">
         <v>118</v>
       </c>
-      <c r="D131" s="44">
+      <c r="D131" s="41">
         <v>43618</v>
       </c>
     </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132" s="5" t="s">
         <v>25</v>
       </c>
@@ -3065,11 +3064,11 @@
       <c r="C132" s="5">
         <v>118</v>
       </c>
-      <c r="D132" s="44">
+      <c r="D132" s="41">
         <v>43618</v>
       </c>
     </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133" s="5" t="s">
         <v>25</v>
       </c>
@@ -3079,11 +3078,11 @@
       <c r="C133" s="5">
         <v>20</v>
       </c>
-      <c r="D133" s="43">
+      <c r="D133" s="40">
         <v>43530</v>
       </c>
     </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134" s="5" t="s">
         <v>19</v>
       </c>
@@ -3093,11 +3092,11 @@
       <c r="C134" s="5">
         <v>30</v>
       </c>
-      <c r="D134" s="44">
+      <c r="D134" s="41">
         <v>43619</v>
       </c>
     </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135" s="5" t="s">
         <v>19</v>
       </c>
@@ -3107,11 +3106,11 @@
       <c r="C135" s="5">
         <v>30</v>
       </c>
-      <c r="D135" s="44">
+      <c r="D135" s="41">
         <v>43619</v>
       </c>
     </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136" s="5" t="s">
         <v>19</v>
       </c>
@@ -3121,11 +3120,11 @@
       <c r="C136" s="5">
         <v>35</v>
       </c>
-      <c r="D136" s="44">
+      <c r="D136" s="41">
         <v>43619</v>
       </c>
     </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A137" s="5" t="s">
         <v>25</v>
       </c>
@@ -3135,11 +3134,11 @@
       <c r="C137" s="5">
         <v>180</v>
       </c>
-      <c r="D137" s="44">
+      <c r="D137" s="41">
         <v>43620</v>
       </c>
     </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A138" s="5" t="s">
         <v>16</v>
       </c>
@@ -3149,11 +3148,11 @@
       <c r="C138" s="5">
         <v>180</v>
       </c>
-      <c r="D138" s="44">
+      <c r="D138" s="41">
         <v>43620</v>
       </c>
     </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A139" s="5" t="s">
         <v>25</v>
       </c>
@@ -3163,11 +3162,11 @@
       <c r="C139" s="5">
         <v>10</v>
       </c>
-      <c r="D139" s="43">
+      <c r="D139" s="40">
         <v>43620</v>
       </c>
     </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A140" s="5" t="s">
         <v>19</v>
       </c>
@@ -3177,11 +3176,11 @@
       <c r="C140" s="5">
         <v>55</v>
       </c>
-      <c r="D140" s="43">
+      <c r="D140" s="40">
         <v>43621</v>
       </c>
     </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A141" s="5" t="s">
         <v>16</v>
       </c>
@@ -3191,11 +3190,11 @@
       <c r="C141" s="5">
         <v>55</v>
       </c>
-      <c r="D141" s="43">
+      <c r="D141" s="40">
         <v>43621</v>
       </c>
     </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A142" s="5" t="s">
         <v>6</v>
       </c>
@@ -3205,11 +3204,11 @@
       <c r="C142" s="5">
         <v>55</v>
       </c>
-      <c r="D142" s="43">
+      <c r="D142" s="40">
         <v>43621</v>
       </c>
     </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A143" s="5" t="s">
         <v>25</v>
       </c>
@@ -3219,11 +3218,11 @@
       <c r="C143" s="5">
         <v>55</v>
       </c>
-      <c r="D143" s="43">
+      <c r="D143" s="40">
         <v>43621</v>
       </c>
     </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A144" s="5" t="s">
         <v>19</v>
       </c>
@@ -3233,11 +3232,11 @@
       <c r="C144" s="5">
         <v>60</v>
       </c>
-      <c r="D144" s="43">
+      <c r="D144" s="40">
         <v>43621</v>
       </c>
     </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A145" s="5" t="s">
         <v>16</v>
       </c>
@@ -3247,11 +3246,11 @@
       <c r="C145" s="5">
         <v>30</v>
       </c>
-      <c r="D145" s="43">
+      <c r="D145" s="40">
         <v>43621</v>
       </c>
     </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A146" s="5" t="s">
         <v>6</v>
       </c>
@@ -3261,11 +3260,11 @@
       <c r="C146" s="5">
         <v>87</v>
       </c>
-      <c r="D146" s="43">
+      <c r="D146" s="40">
         <v>43621</v>
       </c>
     </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A147" s="5" t="s">
         <v>25</v>
       </c>
@@ -3275,11 +3274,11 @@
       <c r="C147" s="5">
         <v>30</v>
       </c>
-      <c r="D147" s="43">
+      <c r="D147" s="40">
         <v>43621</v>
       </c>
     </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A148" s="5" t="s">
         <v>16</v>
       </c>
@@ -3289,11 +3288,11 @@
       <c r="C148" s="5">
         <v>30</v>
       </c>
-      <c r="D148" s="43">
+      <c r="D148" s="40">
         <v>43621</v>
       </c>
     </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A149" s="5" t="s">
         <v>25</v>
       </c>
@@ -3303,11 +3302,11 @@
       <c r="C149" s="5">
         <v>30</v>
       </c>
-      <c r="D149" s="43">
+      <c r="D149" s="40">
         <v>43621</v>
       </c>
     </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A150" s="5" t="s">
         <v>16</v>
       </c>
@@ -3317,11 +3316,11 @@
       <c r="C150" s="5">
         <v>174</v>
       </c>
-      <c r="D150" s="43">
+      <c r="D150" s="40">
         <v>43622</v>
       </c>
     </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A151" s="5" t="s">
         <v>25</v>
       </c>
@@ -3331,11 +3330,11 @@
       <c r="C151" s="5">
         <v>185</v>
       </c>
-      <c r="D151" s="43">
+      <c r="D151" s="40">
         <v>43622</v>
       </c>
     </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A152" s="5" t="s">
         <v>25</v>
       </c>
@@ -3345,11 +3344,11 @@
       <c r="C152" s="5">
         <v>10</v>
       </c>
-      <c r="D152" s="43">
+      <c r="D152" s="40">
         <v>43622</v>
       </c>
     </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A153" s="5" t="s">
         <v>19</v>
       </c>
@@ -3359,11 +3358,11 @@
       <c r="C153" s="5">
         <v>110</v>
       </c>
-      <c r="D153" s="43">
+      <c r="D153" s="40">
         <v>43622</v>
       </c>
     </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A154" s="5" t="s">
         <v>19</v>
       </c>
@@ -3373,11 +3372,11 @@
       <c r="C154" s="5">
         <v>55</v>
       </c>
-      <c r="D154" s="43">
+      <c r="D154" s="40">
         <v>43622</v>
       </c>
     </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A155" s="5" t="s">
         <v>6</v>
       </c>
@@ -3387,11 +3386,11 @@
       <c r="C155" s="5">
         <v>30</v>
       </c>
-      <c r="D155" s="44">
+      <c r="D155" s="41">
         <v>43623</v>
       </c>
     </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A156" s="5" t="s">
         <v>6</v>
       </c>
@@ -3401,11 +3400,11 @@
       <c r="C156" s="5">
         <v>40</v>
       </c>
-      <c r="D156" s="44">
+      <c r="D156" s="41">
         <v>43625</v>
       </c>
     </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A157" s="5" t="s">
         <v>6</v>
       </c>
@@ -3415,11 +3414,11 @@
       <c r="C157" s="5">
         <v>271</v>
       </c>
-      <c r="D157" s="44">
+      <c r="D157" s="41">
         <v>43625</v>
       </c>
     </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A158" s="5" t="s">
         <v>25</v>
       </c>
@@ -3429,11 +3428,11 @@
       <c r="C158" s="5">
         <v>75</v>
       </c>
-      <c r="D158" s="44">
+      <c r="D158" s="41">
         <v>43625</v>
       </c>
     </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A159" s="5" t="s">
         <v>6</v>
       </c>
@@ -3443,11 +3442,11 @@
       <c r="C159" s="5">
         <v>47</v>
       </c>
-      <c r="D159" s="44">
+      <c r="D159" s="41">
         <v>43625</v>
       </c>
     </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A160" s="5" t="s">
         <v>25</v>
       </c>
@@ -3457,11 +3456,11 @@
       <c r="C160" s="5">
         <v>130</v>
       </c>
-      <c r="D160" s="43">
+      <c r="D160" s="40">
         <v>43626</v>
       </c>
     </row>
-    <row r="161" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A161" s="5" t="s">
         <v>16</v>
       </c>
@@ -3471,11 +3470,11 @@
       <c r="C161" s="5">
         <v>130</v>
       </c>
-      <c r="D161" s="43">
+      <c r="D161" s="40">
         <v>43626</v>
       </c>
     </row>
-    <row r="162" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A162" s="5" t="s">
         <v>6</v>
       </c>
@@ -3485,11 +3484,11 @@
       <c r="C162" s="5">
         <v>25</v>
       </c>
-      <c r="D162" s="44">
+      <c r="D162" s="41">
         <v>43626</v>
       </c>
     </row>
-    <row r="163" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A163" s="5" t="s">
         <v>6</v>
       </c>
@@ -3499,11 +3498,11 @@
       <c r="C163" s="5">
         <v>31</v>
       </c>
-      <c r="D163" s="44">
+      <c r="D163" s="41">
         <v>43626</v>
       </c>
     </row>
-    <row r="164" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A164" s="5" t="s">
         <v>6</v>
       </c>
@@ -3513,11 +3512,11 @@
       <c r="C164" s="5">
         <v>32</v>
       </c>
-      <c r="D164" s="44">
+      <c r="D164" s="41">
         <v>43626</v>
       </c>
     </row>
-    <row r="165" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A165" s="5" t="s">
         <v>19</v>
       </c>
@@ -3527,11 +3526,11 @@
       <c r="C165" s="5">
         <v>75</v>
       </c>
-      <c r="D165" s="44">
+      <c r="D165" s="41">
         <v>43627</v>
       </c>
     </row>
-    <row r="166" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A166" s="5" t="s">
         <v>16</v>
       </c>
@@ -3541,11 +3540,11 @@
       <c r="C166" s="5">
         <v>75</v>
       </c>
-      <c r="D166" s="44">
+      <c r="D166" s="41">
         <v>43627</v>
       </c>
     </row>
-    <row r="167" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A167" s="5" t="s">
         <v>19</v>
       </c>
@@ -3555,11 +3554,11 @@
       <c r="C167" s="5">
         <v>70</v>
       </c>
-      <c r="D167" s="44">
+      <c r="D167" s="41">
         <v>43628</v>
       </c>
     </row>
-    <row r="168" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A168" s="5" t="s">
         <v>25</v>
       </c>
@@ -3569,11 +3568,11 @@
       <c r="C168" s="5">
         <v>112</v>
       </c>
-      <c r="D168" s="44">
+      <c r="D168" s="41">
         <v>43628</v>
       </c>
     </row>
-    <row r="169" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A169" s="5" t="s">
         <v>19</v>
       </c>
@@ -3583,11 +3582,11 @@
       <c r="C169" s="5">
         <v>115</v>
       </c>
-      <c r="D169" s="44">
+      <c r="D169" s="41">
         <v>43628</v>
       </c>
     </row>
-    <row r="170" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A170" s="5" t="s">
         <v>19</v>
       </c>
@@ -3597,11 +3596,11 @@
       <c r="C170" s="5">
         <v>175</v>
       </c>
-      <c r="D170" s="44">
+      <c r="D170" s="41">
         <v>43628</v>
       </c>
     </row>
-    <row r="171" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A171" s="5" t="s">
         <v>6</v>
       </c>
@@ -3611,11 +3610,11 @@
       <c r="C171" s="5">
         <v>23</v>
       </c>
-      <c r="D171" s="44">
+      <c r="D171" s="41">
         <v>43628</v>
       </c>
     </row>
-    <row r="172" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A172" s="5" t="s">
         <v>19</v>
       </c>
@@ -3625,11 +3624,11 @@
       <c r="C172" s="5">
         <v>30</v>
       </c>
-      <c r="D172" s="44">
+      <c r="D172" s="41">
         <v>43628</v>
       </c>
     </row>
-    <row r="173" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A173" s="5" t="s">
         <v>19</v>
       </c>
@@ -3639,11 +3638,11 @@
       <c r="C173" s="5">
         <v>77</v>
       </c>
-      <c r="D173" s="43">
+      <c r="D173" s="40">
         <v>43629</v>
       </c>
     </row>
-    <row r="174" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A174" s="5" t="s">
         <v>19</v>
       </c>
@@ -3653,11 +3652,11 @@
       <c r="C174" s="5">
         <v>39</v>
       </c>
-      <c r="D174" s="43">
+      <c r="D174" s="40">
         <v>43629</v>
       </c>
     </row>
-    <row r="175" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A175" s="5" t="s">
         <v>19</v>
       </c>
@@ -3667,11 +3666,11 @@
       <c r="C175" s="5">
         <v>40</v>
       </c>
-      <c r="D175" s="43">
+      <c r="D175" s="40">
         <v>43629</v>
       </c>
     </row>
-    <row r="176" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A176" s="5" t="s">
         <v>25</v>
       </c>
@@ -3681,11 +3680,11 @@
       <c r="C176" s="5">
         <v>25</v>
       </c>
-      <c r="D176" s="43">
+      <c r="D176" s="40">
         <v>43629</v>
       </c>
     </row>
-    <row r="177" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A177" s="5" t="s">
         <v>19</v>
       </c>
@@ -3695,11 +3694,11 @@
       <c r="C177" s="5">
         <v>20</v>
       </c>
-      <c r="D177" s="43">
+      <c r="D177" s="40">
         <v>43629</v>
       </c>
     </row>
-    <row r="178" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A178" s="5" t="s">
         <v>19</v>
       </c>
@@ -3709,11 +3708,11 @@
       <c r="C178" s="5">
         <v>60</v>
       </c>
-      <c r="D178" s="43">
+      <c r="D178" s="40">
         <v>43630</v>
       </c>
     </row>
-    <row r="179" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A179" s="5" t="s">
         <v>19</v>
       </c>
@@ -3723,11 +3722,11 @@
       <c r="C179" s="5">
         <v>100</v>
       </c>
-      <c r="D179" s="43">
+      <c r="D179" s="40">
         <v>43630</v>
       </c>
     </row>
-    <row r="180" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A180" s="5" t="s">
         <v>6</v>
       </c>
@@ -3737,11 +3736,11 @@
       <c r="C180" s="5">
         <v>31</v>
       </c>
-      <c r="D180" s="43">
+      <c r="D180" s="40">
         <v>43630</v>
       </c>
     </row>
-    <row r="181" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A181" s="5" t="s">
         <v>6</v>
       </c>
@@ -3751,299 +3750,307 @@
       <c r="C181" s="5">
         <v>40</v>
       </c>
-      <c r="D181" s="43">
+      <c r="D181" s="40">
         <v>43630</v>
       </c>
     </row>
-    <row r="182" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A182" s="5"/>
-      <c r="B182" s="5"/>
-      <c r="C182" s="5"/>
-      <c r="D182" s="6"/>
-    </row>
-    <row r="183" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A182" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B182" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C182" s="5">
+        <v>30</v>
+      </c>
+      <c r="D182" s="40">
+        <v>43631</v>
+      </c>
+    </row>
+    <row r="183" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A183" s="5"/>
       <c r="B183" s="5"/>
       <c r="C183" s="5"/>
       <c r="D183" s="6"/>
     </row>
-    <row r="184" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A184" s="5"/>
       <c r="B184" s="5"/>
       <c r="C184" s="5"/>
       <c r="D184" s="6"/>
     </row>
-    <row r="185" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A185" s="5"/>
       <c r="B185" s="5"/>
       <c r="C185" s="5"/>
       <c r="D185" s="6"/>
     </row>
-    <row r="186" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A186" s="5"/>
       <c r="B186" s="5"/>
       <c r="C186" s="5"/>
       <c r="D186" s="6"/>
     </row>
-    <row r="187" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A187" s="5"/>
       <c r="B187" s="5"/>
       <c r="C187" s="5"/>
       <c r="D187" s="5"/>
     </row>
-    <row r="188" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A188" s="5"/>
       <c r="B188" s="5"/>
       <c r="C188" s="5"/>
       <c r="D188" s="5"/>
     </row>
-    <row r="189" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A189" s="5"/>
       <c r="B189" s="5"/>
       <c r="C189" s="5"/>
       <c r="D189" s="5"/>
     </row>
-    <row r="190" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A190" s="5"/>
       <c r="B190" s="5"/>
       <c r="C190" s="5"/>
       <c r="D190" s="5"/>
     </row>
-    <row r="191" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A191" s="5"/>
       <c r="B191" s="5"/>
       <c r="C191" s="5"/>
       <c r="D191" s="5"/>
     </row>
-    <row r="192" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A192" s="5"/>
       <c r="B192" s="5"/>
       <c r="C192" s="5"/>
       <c r="D192" s="5"/>
     </row>
-    <row r="193" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A193" s="5"/>
       <c r="B193" s="5"/>
       <c r="C193" s="5"/>
       <c r="D193" s="5"/>
     </row>
-    <row r="194" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A194" s="5"/>
       <c r="B194" s="5"/>
       <c r="C194" s="5"/>
       <c r="D194" s="5"/>
     </row>
-    <row r="195" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A195" s="5"/>
       <c r="B195" s="5"/>
       <c r="C195" s="5"/>
       <c r="D195" s="5"/>
     </row>
-    <row r="196" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A196" s="5"/>
       <c r="B196" s="5"/>
       <c r="C196" s="5"/>
       <c r="D196" s="5"/>
     </row>
-    <row r="197" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A197" s="5"/>
       <c r="B197" s="5"/>
       <c r="C197" s="5"/>
       <c r="D197" s="5"/>
     </row>
-    <row r="198" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A198" s="5"/>
       <c r="B198" s="5"/>
       <c r="C198" s="5"/>
       <c r="D198" s="5"/>
     </row>
-    <row r="199" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A199" s="5"/>
       <c r="B199" s="5"/>
       <c r="C199" s="5"/>
       <c r="D199" s="5"/>
     </row>
-    <row r="200" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A200" s="5"/>
       <c r="B200" s="5"/>
       <c r="C200" s="5"/>
       <c r="D200" s="5"/>
     </row>
-    <row r="201" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A201" s="5"/>
       <c r="B201" s="5"/>
       <c r="C201" s="5"/>
       <c r="D201" s="5"/>
     </row>
-    <row r="202" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A202" s="5"/>
       <c r="B202" s="5"/>
       <c r="C202" s="5"/>
       <c r="D202" s="5"/>
     </row>
-    <row r="203" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A203" s="5"/>
       <c r="B203" s="5"/>
       <c r="C203" s="5"/>
       <c r="D203" s="5"/>
     </row>
-    <row r="204" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A204" s="5"/>
       <c r="B204" s="5"/>
       <c r="C204" s="5"/>
       <c r="D204" s="5"/>
     </row>
-    <row r="205" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A205" s="5"/>
       <c r="B205" s="5"/>
       <c r="C205" s="5"/>
       <c r="D205" s="5"/>
     </row>
-    <row r="206" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A206" s="5"/>
       <c r="B206" s="5"/>
       <c r="C206" s="5"/>
       <c r="D206" s="5"/>
     </row>
-    <row r="207" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A207" s="5"/>
       <c r="B207" s="5"/>
       <c r="C207" s="5"/>
       <c r="D207" s="5"/>
     </row>
-    <row r="208" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A208" s="5"/>
       <c r="B208" s="5"/>
       <c r="C208" s="5"/>
       <c r="D208" s="5"/>
     </row>
-    <row r="209" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A209" s="5"/>
       <c r="B209" s="5"/>
       <c r="C209" s="5"/>
       <c r="D209" s="5"/>
     </row>
-    <row r="210" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A210" s="5"/>
       <c r="B210" s="5"/>
       <c r="C210" s="5"/>
       <c r="D210" s="5"/>
     </row>
-    <row r="211" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A211" s="5"/>
       <c r="B211" s="5"/>
       <c r="C211" s="5"/>
       <c r="D211" s="5"/>
     </row>
-    <row r="212" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A212" s="5"/>
       <c r="B212" s="5"/>
       <c r="C212" s="5"/>
       <c r="D212" s="5"/>
     </row>
-    <row r="213" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A213" s="5"/>
       <c r="B213" s="5"/>
       <c r="C213" s="5"/>
       <c r="D213" s="5"/>
     </row>
-    <row r="214" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A214" s="5"/>
       <c r="B214" s="5"/>
       <c r="C214" s="5"/>
       <c r="D214" s="5"/>
     </row>
-    <row r="215" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A215" s="5"/>
       <c r="B215" s="5"/>
       <c r="C215" s="5"/>
       <c r="D215" s="5"/>
     </row>
-    <row r="216" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A216" s="5"/>
       <c r="B216" s="5"/>
       <c r="C216" s="5"/>
       <c r="D216" s="5"/>
     </row>
-    <row r="217" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A217" s="5"/>
       <c r="B217" s="5"/>
       <c r="C217" s="5"/>
       <c r="D217" s="5"/>
     </row>
-    <row r="218" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A218" s="5"/>
       <c r="B218" s="5"/>
       <c r="C218" s="5"/>
       <c r="D218" s="5"/>
     </row>
-    <row r="219" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A219" s="5"/>
       <c r="B219" s="5"/>
       <c r="C219" s="5"/>
       <c r="D219" s="5"/>
     </row>
-    <row r="220" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A220" s="5"/>
       <c r="B220" s="5"/>
       <c r="C220" s="5"/>
       <c r="D220" s="5"/>
     </row>
-    <row r="221" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A221" s="5"/>
       <c r="B221" s="5"/>
       <c r="C221" s="5"/>
       <c r="D221" s="5"/>
     </row>
-    <row r="222" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A222" s="5"/>
       <c r="B222" s="5"/>
       <c r="C222" s="5"/>
       <c r="D222" s="5"/>
     </row>
-    <row r="223" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A223" s="5"/>
       <c r="B223" s="5"/>
       <c r="C223" s="5"/>
       <c r="D223" s="5"/>
     </row>
-    <row r="224" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A224" s="5"/>
       <c r="B224" s="5"/>
       <c r="C224" s="5"/>
       <c r="D224" s="5"/>
     </row>
-    <row r="225" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A225" s="5"/>
       <c r="B225" s="5"/>
       <c r="C225" s="5"/>
       <c r="D225" s="5"/>
     </row>
-    <row r="226" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A226" s="5"/>
       <c r="B226" s="5"/>
       <c r="C226" s="5"/>
       <c r="D226" s="5"/>
     </row>
-    <row r="227" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A227" s="5"/>
       <c r="B227" s="5"/>
       <c r="C227" s="5"/>
       <c r="D227" s="5"/>
     </row>
-    <row r="228" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A228" s="5"/>
       <c r="B228" s="5"/>
       <c r="C228" s="5"/>
       <c r="D228" s="5"/>
     </row>
-    <row r="229" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A229" s="5"/>
       <c r="B229" s="5"/>
       <c r="C229" s="5"/>
       <c r="D229" s="5"/>
     </row>
-    <row r="230" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A230" s="5"/>
       <c r="B230" s="5"/>
       <c r="C230" s="5"/>

</xml_diff>